<commit_message>
Auto update stocks_data.xlsx [2025-11-20 03:57:39]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -493,6 +493,7 @@
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -536,6 +537,11 @@
           <t>2025/11/17</t>
         </is>
       </c>
+      <c r="I1" s="7" t="inlineStr">
+        <is>
+          <t>2025/11/20</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -578,6 +584,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="I2" s="8" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -604,6 +615,9 @@
       <c r="H3" s="9" t="n">
         <v>63.04</v>
       </c>
+      <c r="I3" s="9" t="n">
+        <v>62.05</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -629,6 +643,9 @@
       </c>
       <c r="H4" s="9" t="n">
         <v>3973.31</v>
+      </c>
+      <c r="I4" s="9" t="n">
+        <v>3961.71</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -640,6 +657,7 @@
       <c r="F5" s="4" t="n"/>
       <c r="G5" s="4" t="n"/>
       <c r="H5" s="7" t="n"/>
+      <c r="I5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -666,6 +684,9 @@
       <c r="H6" s="9" t="n">
         <v>49.48</v>
       </c>
+      <c r="I6" s="9" t="n">
+        <v>48.95</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -691,6 +712,9 @@
       </c>
       <c r="H7" s="9" t="n">
         <v>5533.35</v>
+      </c>
+      <c r="I7" s="9" t="n">
+        <v>5518.4</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -702,6 +726,7 @@
       <c r="F8" s="4" t="n"/>
       <c r="G8" s="4" t="n"/>
       <c r="H8" s="7" t="n"/>
+      <c r="I8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -728,6 +753,9 @@
       <c r="H9" s="9" t="n">
         <v>54.86</v>
       </c>
+      <c r="I9" s="9" t="n">
+        <v>54.37</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -753,6 +781,9 @@
       </c>
       <c r="H10" s="9" t="n">
         <v>4596.15</v>
+      </c>
+      <c r="I10" s="9" t="n">
+        <v>4602.83</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -764,6 +795,7 @@
       <c r="F11" s="4" t="n"/>
       <c r="G11" s="4" t="n"/>
       <c r="H11" s="7" t="n"/>
+      <c r="I11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -790,6 +822,9 @@
       <c r="H12" s="9" t="n">
         <v>57.09</v>
       </c>
+      <c r="I12" s="9" t="n">
+        <v>56.4</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -815,6 +850,9 @@
       </c>
       <c r="H13" s="9" t="n">
         <v>7220.73</v>
+      </c>
+      <c r="I13" s="9" t="n">
+        <v>7106.2</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -826,6 +864,7 @@
       <c r="F14" s="4" t="n"/>
       <c r="G14" s="4" t="n"/>
       <c r="H14" s="7" t="n"/>
+      <c r="I14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -852,6 +891,9 @@
       <c r="H15" s="9" t="n">
         <v>28.22</v>
       </c>
+      <c r="I15" s="9" t="n">
+        <v>26.88</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -877,6 +919,9 @@
       </c>
       <c r="H16" s="9" t="n">
         <v>2706.67</v>
+      </c>
+      <c r="I16" s="9" t="n">
+        <v>2682.5</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -888,6 +933,7 @@
       <c r="F17" s="4" t="n"/>
       <c r="G17" s="4" t="n"/>
       <c r="H17" s="7" t="n"/>
+      <c r="I17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -914,6 +960,9 @@
       <c r="H18" s="9" t="n">
         <v>96.06</v>
       </c>
+      <c r="I18" s="9" t="n">
+        <v>95.39</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -939,6 +988,9 @@
       </c>
       <c r="H19" s="9" t="n">
         <v>6734.11</v>
+      </c>
+      <c r="I19" s="9" t="n">
+        <v>6642.16</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -950,6 +1002,7 @@
       <c r="F20" s="4" t="n"/>
       <c r="G20" s="4" t="n"/>
       <c r="H20" s="7" t="n"/>
+      <c r="I20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -976,6 +1029,9 @@
       <c r="H21" s="9" t="n">
         <v>65.04000000000001</v>
       </c>
+      <c r="I21" s="9" t="n">
+        <v>68.22</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1001,6 +1057,9 @@
       </c>
       <c r="H22" s="9" t="n">
         <v>84700.5</v>
+      </c>
+      <c r="I22" s="9" t="n">
+        <v>85470.92</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1012,6 +1071,7 @@
       <c r="F23" s="4" t="n"/>
       <c r="G23" s="4" t="n"/>
       <c r="H23" s="7" t="n"/>
+      <c r="I23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1038,6 +1098,9 @@
       <c r="H24" s="9" t="n">
         <v>85.41</v>
       </c>
+      <c r="I24" s="9" t="n">
+        <v>81.56999999999999</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1063,6 +1126,9 @@
       </c>
       <c r="H25" s="9" t="n">
         <v>19909.14</v>
+      </c>
+      <c r="I25" s="9" t="n">
+        <v>23216.84</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1074,6 +1140,7 @@
       <c r="F26" s="4" t="n"/>
       <c r="G26" s="4" t="n"/>
       <c r="H26" s="7" t="n"/>
+      <c r="I26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1100,6 +1167,9 @@
       <c r="H27" s="9" t="n">
         <v>71.84999999999999</v>
       </c>
+      <c r="I27" s="9" t="n">
+        <v>66.56</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1125,6 +1195,9 @@
       </c>
       <c r="H28" s="9" t="n">
         <v>39894.54</v>
+      </c>
+      <c r="I28" s="9" t="n">
+        <v>50115.76</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1136,6 +1209,7 @@
       <c r="F29" s="4" t="n"/>
       <c r="G29" s="4" t="n"/>
       <c r="H29" s="7" t="n"/>
+      <c r="I29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1162,6 +1236,9 @@
       <c r="H30" s="9" t="n">
         <v>59.08</v>
       </c>
+      <c r="I30" s="9" t="n">
+        <v>46.33</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1187,6 +1264,9 @@
       </c>
       <c r="H31" s="9" t="n">
         <v>5751.84</v>
+      </c>
+      <c r="I31" s="9" t="n">
+        <v>5706.47</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1198,6 +1278,7 @@
       <c r="F32" s="4" t="n"/>
       <c r="G32" s="4" t="n"/>
       <c r="H32" s="7" t="n"/>
+      <c r="I32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1224,6 +1305,9 @@
       <c r="H33" s="9" t="n">
         <v>11.76</v>
       </c>
+      <c r="I33" s="9" t="n">
+        <v>10.84</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1249,6 +1333,9 @@
       </c>
       <c r="H34" s="9" t="n">
         <v>31971.95</v>
+      </c>
+      <c r="I34" s="9" t="n">
+        <v>31797.79</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1260,6 +1347,7 @@
       <c r="F35" s="4" t="n"/>
       <c r="G35" s="4" t="n"/>
       <c r="H35" s="7" t="n"/>
+      <c r="I35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1286,6 +1374,9 @@
       <c r="H36" s="9" t="n">
         <v>28.05</v>
       </c>
+      <c r="I36" s="9" t="n">
+        <v>27.48</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1311,6 +1402,9 @@
       </c>
       <c r="H37" s="9" t="n">
         <v>3241.89</v>
+      </c>
+      <c r="I37" s="9" t="n">
+        <v>3221.39</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1322,6 +1416,7 @@
       <c r="F38" s="4" t="n"/>
       <c r="G38" s="4" t="n"/>
       <c r="H38" s="7" t="n"/>
+      <c r="I38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1348,6 +1443,9 @@
       <c r="H39" s="9" t="n">
         <v>45.7</v>
       </c>
+      <c r="I39" s="9" t="n">
+        <v>44.97</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1373,6 +1471,9 @@
       </c>
       <c r="H40" s="9" t="n">
         <v>3086.67</v>
+      </c>
+      <c r="I40" s="9" t="n">
+        <v>3060.93</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1384,6 +1485,7 @@
       <c r="F41" s="4" t="n"/>
       <c r="G41" s="4" t="n"/>
       <c r="H41" s="7" t="n"/>
+      <c r="I41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1410,6 +1512,9 @@
       <c r="H42" s="9" t="n">
         <v>18.22</v>
       </c>
+      <c r="I42" s="9" t="n">
+        <v>16.34</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1435,6 +1540,9 @@
       </c>
       <c r="H43" s="9" t="n">
         <v>7139.25</v>
+      </c>
+      <c r="I43" s="9" t="n">
+        <v>7019.85</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1446,6 +1554,7 @@
       <c r="F44" s="4" t="n"/>
       <c r="G44" s="4" t="n"/>
       <c r="H44" s="7" t="n"/>
+      <c r="I44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1472,6 +1581,9 @@
       <c r="H45" s="9" t="n">
         <v>31.57</v>
       </c>
+      <c r="I45" s="9" t="n">
+        <v>28.7</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1497,6 +1609,9 @@
       </c>
       <c r="H46" s="9" t="n">
         <v>8691.709999999999</v>
+      </c>
+      <c r="I46" s="9" t="n">
+        <v>8604.700000000001</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1508,6 +1623,7 @@
       <c r="F47" s="4" t="n"/>
       <c r="G47" s="4" t="n"/>
       <c r="H47" s="7" t="n"/>
+      <c r="I47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1534,6 +1650,9 @@
       <c r="H48" s="9" t="n">
         <v>13.62</v>
       </c>
+      <c r="I48" s="9" t="n">
+        <v>12.48</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1559,6 +1678,9 @@
       </c>
       <c r="H49" s="9" t="n">
         <v>12878.88</v>
+      </c>
+      <c r="I49" s="9" t="n">
+        <v>12860.07</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1570,6 +1692,7 @@
       <c r="F50" s="4" t="n"/>
       <c r="G50" s="4" t="n"/>
       <c r="H50" s="7" t="n"/>
+      <c r="I50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1596,6 +1719,9 @@
       <c r="H51" s="9" t="n">
         <v>25.01</v>
       </c>
+      <c r="I51" s="9" t="n">
+        <v>22.51</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1621,6 +1747,9 @@
       </c>
       <c r="H52" s="9" t="n">
         <v>12336.81</v>
+      </c>
+      <c r="I52" s="9" t="n">
+        <v>12284.26</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1632,6 +1761,7 @@
       <c r="F53" s="4" t="n"/>
       <c r="G53" s="4" t="n"/>
       <c r="H53" s="7" t="n"/>
+      <c r="I53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1658,6 +1788,9 @@
       <c r="H54" s="9" t="n">
         <v>22.95</v>
       </c>
+      <c r="I54" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1683,6 +1816,9 @@
       </c>
       <c r="H55" s="9" t="n">
         <v>9969.459999999999</v>
+      </c>
+      <c r="I55" s="9" t="n">
+        <v>5595.66</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1694,6 +1830,7 @@
       <c r="F56" s="4" t="n"/>
       <c r="G56" s="4" t="n"/>
       <c r="H56" s="7" t="n"/>
+      <c r="I56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -1720,6 +1857,9 @@
       <c r="H57" s="9" t="n">
         <v>27.41</v>
       </c>
+      <c r="I57" s="9" t="n">
+        <v>27.22</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -1745,6 +1885,9 @@
       </c>
       <c r="H58" s="9" t="n">
         <v>16259.1</v>
+      </c>
+      <c r="I58" s="9" t="n">
+        <v>16227.71</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -1756,6 +1899,7 @@
       <c r="F59" s="4" t="n"/>
       <c r="G59" s="4" t="n"/>
       <c r="H59" s="7" t="n"/>
+      <c r="I59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -1782,6 +1926,9 @@
       <c r="H60" s="9" t="n">
         <v>32.67</v>
       </c>
+      <c r="I60" s="9" t="n">
+        <v>31.6</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -1806,6 +1953,9 @@
         <v>17526.85</v>
       </c>
       <c r="H61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="I61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1818,6 +1968,7 @@
       <c r="F62" s="4" t="n"/>
       <c r="G62" s="4" t="n"/>
       <c r="H62" s="7" t="n"/>
+      <c r="I62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -1844,6 +1995,9 @@
       <c r="H63" s="9" t="n">
         <v>20.09</v>
       </c>
+      <c r="I63" s="9" t="n">
+        <v>18.55</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -1869,6 +2023,9 @@
       </c>
       <c r="H64" s="9" t="n">
         <v>9989.68</v>
+      </c>
+      <c r="I64" s="9" t="n">
+        <v>9724.17</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -1880,6 +2037,7 @@
       <c r="F65" s="4" t="n"/>
       <c r="G65" s="4" t="n"/>
       <c r="H65" s="7" t="n"/>
+      <c r="I65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -1906,6 +2064,9 @@
       <c r="H66" s="9" t="n">
         <v>19.84</v>
       </c>
+      <c r="I66" s="9" t="n">
+        <v>15.64</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -1931,6 +2092,9 @@
       </c>
       <c r="H67" s="9" t="n">
         <v>10219.36</v>
+      </c>
+      <c r="I67" s="9" t="n">
+        <v>9999.030000000001</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -1942,6 +2106,7 @@
       <c r="F68" s="4" t="n"/>
       <c r="G68" s="4" t="n"/>
       <c r="H68" s="7" t="n"/>
+      <c r="I68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -1968,6 +2133,9 @@
       <c r="H69" s="9" t="n">
         <v>20.04</v>
       </c>
+      <c r="I69" s="9" t="n">
+        <v>20.27</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -1993,6 +2161,9 @@
       </c>
       <c r="H70" s="9" t="n">
         <v>3012.57</v>
+      </c>
+      <c r="I70" s="9" t="n">
+        <v>2949.42</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -2004,6 +2175,7 @@
       <c r="F71" s="4" t="n"/>
       <c r="G71" s="4" t="n"/>
       <c r="H71" s="7" t="n"/>
+      <c r="I71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2030,6 +2202,9 @@
       <c r="H72" s="9" t="n">
         <v>42.42</v>
       </c>
+      <c r="I72" s="9" t="n">
+        <v>39.93</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2055,6 +2230,9 @@
       </c>
       <c r="H73" s="9" t="n">
         <v>5743.57</v>
+      </c>
+      <c r="I73" s="9" t="n">
+        <v>5552.57</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -2066,6 +2244,7 @@
       <c r="F74" s="4" t="n"/>
       <c r="G74" s="4" t="n"/>
       <c r="H74" s="7" t="n"/>
+      <c r="I74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -2092,6 +2271,9 @@
       <c r="H75" s="9" t="n">
         <v>28.12</v>
       </c>
+      <c r="I75" s="9" t="n">
+        <v>25.67</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -2117,6 +2299,9 @@
       </c>
       <c r="H76" s="9" t="n">
         <v>9276.309999999999</v>
+      </c>
+      <c r="I76" s="9" t="n">
+        <v>9154.809999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -2128,6 +2313,7 @@
       <c r="F77" s="4" t="n"/>
       <c r="G77" s="4" t="n"/>
       <c r="H77" s="7" t="n"/>
+      <c r="I77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -2154,6 +2340,9 @@
       <c r="H78" s="9" t="n">
         <v>13.78</v>
       </c>
+      <c r="I78" s="9" t="n">
+        <v>13.75</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -2179,6 +2368,9 @@
       </c>
       <c r="H79" s="9" t="n">
         <v>1352.41</v>
+      </c>
+      <c r="I79" s="9" t="n">
+        <v>1346.27</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -2190,6 +2382,7 @@
       <c r="F80" s="4" t="n"/>
       <c r="G80" s="4" t="n"/>
       <c r="H80" s="7" t="n"/>
+      <c r="I80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -2216,6 +2409,9 @@
       <c r="H81" s="9" t="n">
         <v>56.98</v>
       </c>
+      <c r="I81" s="9" t="n">
+        <v>56.25</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -2241,6 +2437,9 @@
       </c>
       <c r="H82" s="9" t="n">
         <v>2999.85</v>
+      </c>
+      <c r="I82" s="9" t="n">
+        <v>2947.01</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -2252,6 +2451,7 @@
       <c r="F83" s="4" t="n"/>
       <c r="G83" s="4" t="n"/>
       <c r="H83" s="7" t="n"/>
+      <c r="I83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -2278,6 +2478,9 @@
       <c r="H84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="I84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -2303,6 +2506,9 @@
       </c>
       <c r="H85" s="9" t="n">
         <v>3040.05</v>
+      </c>
+      <c r="I85" s="9" t="n">
+        <v>2962.01</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -2314,6 +2520,7 @@
       <c r="F86" s="4" t="n"/>
       <c r="G86" s="4" t="n"/>
       <c r="H86" s="7" t="n"/>
+      <c r="I86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -2340,6 +2547,9 @@
       <c r="H87" s="9" t="n">
         <v>53.31</v>
       </c>
+      <c r="I87" s="9" t="n">
+        <v>52.59</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -2365,6 +2575,9 @@
       </c>
       <c r="H88" s="9" t="n">
         <v>4005.33</v>
+      </c>
+      <c r="I88" s="9" t="n">
+        <v>3096.58</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -2376,6 +2589,7 @@
       <c r="F89" s="4" t="n"/>
       <c r="G89" s="4" t="n"/>
       <c r="H89" s="7" t="n"/>
+      <c r="I89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -2402,6 +2616,9 @@
       <c r="H90" s="9" t="n">
         <v>45.31</v>
       </c>
+      <c r="I90" s="9" t="n">
+        <v>43.3</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -2427,6 +2644,9 @@
       </c>
       <c r="H91" s="9" t="n">
         <v>2026.1</v>
+      </c>
+      <c r="I91" s="9" t="n">
+        <v>2000.51</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -2438,6 +2658,7 @@
       <c r="F92" s="4" t="n"/>
       <c r="G92" s="4" t="n"/>
       <c r="H92" s="7" t="n"/>
+      <c r="I92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -2464,6 +2685,9 @@
       <c r="H93" s="9" t="n">
         <v>28.18</v>
       </c>
+      <c r="I93" s="9" t="n">
+        <v>27.42</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -2489,6 +2713,9 @@
       </c>
       <c r="H94" s="9" t="n">
         <v>14082.33</v>
+      </c>
+      <c r="I94" s="9" t="n">
+        <v>13704.57</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -2500,6 +2727,7 @@
       <c r="F95" s="4" t="n"/>
       <c r="G95" s="4" t="n"/>
       <c r="H95" s="7" t="n"/>
+      <c r="I95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -2526,6 +2754,9 @@
       <c r="H96" s="9" t="n">
         <v>84.89</v>
       </c>
+      <c r="I96" s="9" t="n">
+        <v>84.81</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -2551,6 +2782,9 @@
       </c>
       <c r="H97" s="9" t="n">
         <v>8772.93</v>
+      </c>
+      <c r="I97" s="9" t="n">
+        <v>8712.18</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -2562,6 +2796,7 @@
       <c r="F98" s="4" t="n"/>
       <c r="G98" s="4" t="n"/>
       <c r="H98" s="7" t="n"/>
+      <c r="I98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -2588,6 +2823,9 @@
       <c r="H99" s="9" t="n">
         <v>56.35</v>
       </c>
+      <c r="I99" s="9" t="n">
+        <v>56.5</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -2613,6 +2851,9 @@
       </c>
       <c r="H100" s="9" t="n">
         <v>12131.94</v>
+      </c>
+      <c r="I100" s="9" t="n">
+        <v>11944.72</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -2624,6 +2865,7 @@
       <c r="F101" s="4" t="n"/>
       <c r="G101" s="4" t="n"/>
       <c r="H101" s="7" t="n"/>
+      <c r="I101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -2650,6 +2892,9 @@
       <c r="H102" s="9" t="n">
         <v>6.1</v>
       </c>
+      <c r="I102" s="9" t="n">
+        <v>5.73</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -2675,6 +2920,9 @@
       </c>
       <c r="H103" s="9" t="n">
         <v>2290.06</v>
+      </c>
+      <c r="I103" s="9" t="n">
+        <v>2266.47</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -2686,6 +2934,7 @@
       <c r="F104" s="4" t="n"/>
       <c r="G104" s="4" t="n"/>
       <c r="H104" s="7" t="n"/>
+      <c r="I104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -2712,6 +2961,9 @@
       <c r="H105" s="9" t="n">
         <v>25.74</v>
       </c>
+      <c r="I105" s="9" t="n">
+        <v>25.59</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -2737,6 +2989,9 @@
       </c>
       <c r="H106" s="9" t="n">
         <v>860.3</v>
+      </c>
+      <c r="I106" s="9" t="n">
+        <v>865.4299999999999</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -2748,6 +3003,7 @@
       <c r="F107" s="4" t="n"/>
       <c r="G107" s="4" t="n"/>
       <c r="H107" s="7" t="n"/>
+      <c r="I107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -2774,6 +3030,9 @@
       <c r="H108" s="9" t="n">
         <v>29.67</v>
       </c>
+      <c r="I108" s="9" t="n">
+        <v>29.61</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -2799,6 +3058,9 @@
       </c>
       <c r="H109" s="9" t="n">
         <v>2836.05</v>
+      </c>
+      <c r="I109" s="9" t="n">
+        <v>2841.63</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -2810,6 +3072,7 @@
       <c r="F110" s="4" t="n"/>
       <c r="G110" s="4" t="n"/>
       <c r="H110" s="7" t="n"/>
+      <c r="I110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -2836,6 +3099,9 @@
       <c r="H111" s="9" t="n">
         <v>21.18</v>
       </c>
+      <c r="I111" s="9" t="n">
+        <v>20.59</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -2861,6 +3127,9 @@
       </c>
       <c r="H112" s="9" t="n">
         <v>3965.2</v>
+      </c>
+      <c r="I112" s="9" t="n">
+        <v>3899.86</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -2872,6 +3141,7 @@
       <c r="F113" s="4" t="n"/>
       <c r="G113" s="4" t="n"/>
       <c r="H113" s="7" t="n"/>
+      <c r="I113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -2898,6 +3168,9 @@
       <c r="H114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="I114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -2923,6 +3196,9 @@
       </c>
       <c r="H115" s="9" t="n">
         <v>3427</v>
+      </c>
+      <c r="I115" s="9" t="n">
+        <v>3366.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-24 04:11:32]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -494,6 +494,7 @@
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -542,6 +543,11 @@
           <t>2025/11/20</t>
         </is>
       </c>
+      <c r="J1" s="7" t="inlineStr">
+        <is>
+          <t>2025/11/24</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -589,6 +595,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="J2" s="8" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -618,6 +629,9 @@
       <c r="I3" s="9" t="n">
         <v>62.05</v>
       </c>
+      <c r="J3" s="9" t="n">
+        <v>60.18</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -646,6 +660,9 @@
       </c>
       <c r="I4" s="9" t="n">
         <v>3961.71</v>
+      </c>
+      <c r="J4" s="9" t="n">
+        <v>3821.68</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -658,6 +675,7 @@
       <c r="G5" s="4" t="n"/>
       <c r="H5" s="7" t="n"/>
       <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -687,6 +705,9 @@
       <c r="I6" s="9" t="n">
         <v>48.95</v>
       </c>
+      <c r="J6" s="9" t="n">
+        <v>46.74</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -715,6 +736,9 @@
       </c>
       <c r="I7" s="9" t="n">
         <v>5518.4</v>
+      </c>
+      <c r="J7" s="9" t="n">
+        <v>5300.7</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -727,6 +751,7 @@
       <c r="G8" s="4" t="n"/>
       <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
+      <c r="J8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -756,6 +781,9 @@
       <c r="I9" s="9" t="n">
         <v>54.37</v>
       </c>
+      <c r="J9" s="9" t="n">
+        <v>52.46</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -784,6 +812,9 @@
       </c>
       <c r="I10" s="9" t="n">
         <v>4602.83</v>
+      </c>
+      <c r="J10" s="9" t="n">
+        <v>4427.55</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -796,6 +827,7 @@
       <c r="G11" s="4" t="n"/>
       <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
+      <c r="J11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -825,6 +857,9 @@
       <c r="I12" s="9" t="n">
         <v>56.4</v>
       </c>
+      <c r="J12" s="9" t="n">
+        <v>54.44</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -853,6 +888,9 @@
       </c>
       <c r="I13" s="9" t="n">
         <v>7106.2</v>
+      </c>
+      <c r="J13" s="9" t="n">
+        <v>6804.37</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -865,6 +903,7 @@
       <c r="G14" s="4" t="n"/>
       <c r="H14" s="7" t="n"/>
       <c r="I14" s="7" t="n"/>
+      <c r="J14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -894,6 +933,9 @@
       <c r="I15" s="9" t="n">
         <v>26.88</v>
       </c>
+      <c r="J15" s="9" t="n">
+        <v>25.19</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -922,6 +964,9 @@
       </c>
       <c r="I16" s="9" t="n">
         <v>2682.5</v>
+      </c>
+      <c r="J16" s="9" t="n">
+        <v>2611.42</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -934,6 +979,7 @@
       <c r="G17" s="4" t="n"/>
       <c r="H17" s="7" t="n"/>
       <c r="I17" s="7" t="n"/>
+      <c r="J17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -963,6 +1009,9 @@
       <c r="I18" s="9" t="n">
         <v>95.39</v>
       </c>
+      <c r="J18" s="9" t="n">
+        <v>95.14</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -991,6 +1040,9 @@
       </c>
       <c r="I19" s="9" t="n">
         <v>6642.16</v>
+      </c>
+      <c r="J19" s="9" t="n">
+        <v>6602.99</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1003,6 +1055,7 @@
       <c r="G20" s="4" t="n"/>
       <c r="H20" s="7" t="n"/>
       <c r="I20" s="7" t="n"/>
+      <c r="J20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1032,6 +1085,9 @@
       <c r="I21" s="9" t="n">
         <v>68.22</v>
       </c>
+      <c r="J21" s="9" t="n">
+        <v>68.28</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1060,6 +1116,9 @@
       </c>
       <c r="I22" s="9" t="n">
         <v>85470.92</v>
+      </c>
+      <c r="J22" s="9" t="n">
+        <v>85382.7</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1072,6 +1131,7 @@
       <c r="G23" s="4" t="n"/>
       <c r="H23" s="7" t="n"/>
       <c r="I23" s="7" t="n"/>
+      <c r="J23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1101,6 +1161,9 @@
       <c r="I24" s="9" t="n">
         <v>81.56999999999999</v>
       </c>
+      <c r="J24" s="9" t="n">
+        <v>81.45999999999999</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1129,6 +1192,9 @@
       </c>
       <c r="I25" s="9" t="n">
         <v>23216.84</v>
+      </c>
+      <c r="J25" s="9" t="n">
+        <v>23091.87</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1141,6 +1207,7 @@
       <c r="G26" s="4" t="n"/>
       <c r="H26" s="7" t="n"/>
       <c r="I26" s="7" t="n"/>
+      <c r="J26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1170,6 +1237,9 @@
       <c r="I27" s="9" t="n">
         <v>66.56</v>
       </c>
+      <c r="J27" s="9" t="n">
+        <v>69.37</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1198,6 +1268,9 @@
       </c>
       <c r="I28" s="9" t="n">
         <v>50115.76</v>
+      </c>
+      <c r="J28" s="9" t="n">
+        <v>48625.83</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1210,6 +1283,7 @@
       <c r="G29" s="4" t="n"/>
       <c r="H29" s="7" t="n"/>
       <c r="I29" s="7" t="n"/>
+      <c r="J29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1239,6 +1313,9 @@
       <c r="I30" s="9" t="n">
         <v>46.33</v>
       </c>
+      <c r="J30" s="9" t="n">
+        <v>47.55</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1267,6 +1344,9 @@
       </c>
       <c r="I31" s="9" t="n">
         <v>5706.47</v>
+      </c>
+      <c r="J31" s="9" t="n">
+        <v>5530.63</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1279,6 +1359,7 @@
       <c r="G32" s="4" t="n"/>
       <c r="H32" s="7" t="n"/>
       <c r="I32" s="7" t="n"/>
+      <c r="J32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1308,6 +1389,9 @@
       <c r="I33" s="9" t="n">
         <v>10.84</v>
       </c>
+      <c r="J33" s="9" t="n">
+        <v>9.550000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1336,6 +1420,9 @@
       </c>
       <c r="I34" s="9" t="n">
         <v>31797.79</v>
+      </c>
+      <c r="J34" s="9" t="n">
+        <v>31126.79</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1348,6 +1435,7 @@
       <c r="G35" s="4" t="n"/>
       <c r="H35" s="7" t="n"/>
       <c r="I35" s="7" t="n"/>
+      <c r="J35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1377,6 +1465,9 @@
       <c r="I36" s="9" t="n">
         <v>27.48</v>
       </c>
+      <c r="J36" s="9" t="n">
+        <v>25.85</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1405,6 +1496,9 @@
       </c>
       <c r="I37" s="9" t="n">
         <v>3221.39</v>
+      </c>
+      <c r="J37" s="9" t="n">
+        <v>3045.56</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1417,6 +1511,7 @@
       <c r="G38" s="4" t="n"/>
       <c r="H38" s="7" t="n"/>
       <c r="I38" s="7" t="n"/>
+      <c r="J38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1446,6 +1541,9 @@
       <c r="I39" s="9" t="n">
         <v>44.97</v>
       </c>
+      <c r="J39" s="9" t="n">
+        <v>42.6</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1474,6 +1572,9 @@
       </c>
       <c r="I40" s="9" t="n">
         <v>3060.93</v>
+      </c>
+      <c r="J40" s="9" t="n">
+        <v>2897.68</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1486,6 +1587,7 @@
       <c r="G41" s="4" t="n"/>
       <c r="H41" s="7" t="n"/>
       <c r="I41" s="7" t="n"/>
+      <c r="J41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1515,6 +1617,9 @@
       <c r="I42" s="9" t="n">
         <v>16.34</v>
       </c>
+      <c r="J42" s="9" t="n">
+        <v>14.49</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1543,6 +1648,9 @@
       </c>
       <c r="I43" s="9" t="n">
         <v>7019.85</v>
+      </c>
+      <c r="J43" s="9" t="n">
+        <v>6893.92</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1555,6 +1663,7 @@
       <c r="G44" s="4" t="n"/>
       <c r="H44" s="7" t="n"/>
       <c r="I44" s="7" t="n"/>
+      <c r="J44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1584,6 +1693,9 @@
       <c r="I45" s="9" t="n">
         <v>28.7</v>
       </c>
+      <c r="J45" s="9" t="n">
+        <v>26.34</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1612,6 +1724,9 @@
       </c>
       <c r="I46" s="9" t="n">
         <v>8604.700000000001</v>
+      </c>
+      <c r="J46" s="9" t="n">
+        <v>8462.25</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1624,6 +1739,7 @@
       <c r="G47" s="4" t="n"/>
       <c r="H47" s="7" t="n"/>
       <c r="I47" s="7" t="n"/>
+      <c r="J47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1653,6 +1769,9 @@
       <c r="I48" s="9" t="n">
         <v>12.48</v>
       </c>
+      <c r="J48" s="9" t="n">
+        <v>11.21</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1681,6 +1800,9 @@
       </c>
       <c r="I49" s="9" t="n">
         <v>12860.07</v>
+      </c>
+      <c r="J49" s="9" t="n">
+        <v>12671.93</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1693,6 +1815,7 @@
       <c r="G50" s="4" t="n"/>
       <c r="H50" s="7" t="n"/>
       <c r="I50" s="7" t="n"/>
+      <c r="J50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1722,6 +1845,9 @@
       <c r="I51" s="9" t="n">
         <v>22.51</v>
       </c>
+      <c r="J51" s="9" t="n">
+        <v>22.2</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1750,6 +1876,9 @@
       </c>
       <c r="I52" s="9" t="n">
         <v>12284.26</v>
+      </c>
+      <c r="J52" s="9" t="n">
+        <v>12032.16</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1762,6 +1891,7 @@
       <c r="G53" s="4" t="n"/>
       <c r="H53" s="7" t="n"/>
       <c r="I53" s="7" t="n"/>
+      <c r="J53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1791,6 +1921,9 @@
       <c r="I54" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="J54" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1819,6 +1952,9 @@
       </c>
       <c r="I55" s="9" t="n">
         <v>5595.66</v>
+      </c>
+      <c r="J55" s="9" t="n">
+        <v>5459.33</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1831,6 +1967,7 @@
       <c r="G56" s="4" t="n"/>
       <c r="H56" s="7" t="n"/>
       <c r="I56" s="7" t="n"/>
+      <c r="J56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -1860,6 +1997,9 @@
       <c r="I57" s="9" t="n">
         <v>27.22</v>
       </c>
+      <c r="J57" s="9" t="n">
+        <v>26.82</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -1888,6 +2028,9 @@
       </c>
       <c r="I58" s="9" t="n">
         <v>16227.71</v>
+      </c>
+      <c r="J58" s="9" t="n">
+        <v>15973</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -1900,6 +2043,7 @@
       <c r="G59" s="4" t="n"/>
       <c r="H59" s="7" t="n"/>
       <c r="I59" s="7" t="n"/>
+      <c r="J59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -1929,6 +2073,9 @@
       <c r="I60" s="9" t="n">
         <v>31.6</v>
       </c>
+      <c r="J60" s="9" t="n">
+        <v>30.73</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -1956,6 +2103,9 @@
         <v>17526.85</v>
       </c>
       <c r="I61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="J61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -1969,6 +2119,7 @@
       <c r="G62" s="4" t="n"/>
       <c r="H62" s="7" t="n"/>
       <c r="I62" s="7" t="n"/>
+      <c r="J62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -1998,6 +2149,9 @@
       <c r="I63" s="9" t="n">
         <v>18.55</v>
       </c>
+      <c r="J63" s="9" t="n">
+        <v>17.84</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2026,6 +2180,9 @@
       </c>
       <c r="I64" s="9" t="n">
         <v>9724.17</v>
+      </c>
+      <c r="J64" s="9" t="n">
+        <v>9681.84</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -2038,6 +2195,7 @@
       <c r="G65" s="4" t="n"/>
       <c r="H65" s="7" t="n"/>
       <c r="I65" s="7" t="n"/>
+      <c r="J65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -2067,6 +2225,9 @@
       <c r="I66" s="9" t="n">
         <v>15.64</v>
       </c>
+      <c r="J66" s="9" t="n">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -2095,6 +2256,9 @@
       </c>
       <c r="I67" s="9" t="n">
         <v>9999.030000000001</v>
+      </c>
+      <c r="J67" s="9" t="n">
+        <v>9784.98</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -2107,6 +2271,7 @@
       <c r="G68" s="4" t="n"/>
       <c r="H68" s="7" t="n"/>
       <c r="I68" s="7" t="n"/>
+      <c r="J68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -2136,6 +2301,9 @@
       <c r="I69" s="9" t="n">
         <v>20.27</v>
       </c>
+      <c r="J69" s="9" t="n">
+        <v>19.43</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -2164,6 +2332,9 @@
       </c>
       <c r="I70" s="9" t="n">
         <v>2949.42</v>
+      </c>
+      <c r="J70" s="9" t="n">
+        <v>2946.79</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -2176,6 +2347,7 @@
       <c r="G71" s="4" t="n"/>
       <c r="H71" s="7" t="n"/>
       <c r="I71" s="7" t="n"/>
+      <c r="J71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2205,6 +2377,9 @@
       <c r="I72" s="9" t="n">
         <v>39.93</v>
       </c>
+      <c r="J72" s="9" t="n">
+        <v>36.97</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2233,6 +2408,9 @@
       </c>
       <c r="I73" s="9" t="n">
         <v>5552.57</v>
+      </c>
+      <c r="J73" s="9" t="n">
+        <v>5484.46</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -2245,6 +2423,7 @@
       <c r="G74" s="4" t="n"/>
       <c r="H74" s="7" t="n"/>
       <c r="I74" s="7" t="n"/>
+      <c r="J74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -2274,6 +2453,9 @@
       <c r="I75" s="9" t="n">
         <v>25.67</v>
       </c>
+      <c r="J75" s="9" t="n">
+        <v>24.07</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -2302,6 +2484,9 @@
       </c>
       <c r="I76" s="9" t="n">
         <v>9154.809999999999</v>
+      </c>
+      <c r="J76" s="9" t="n">
+        <v>8974.48</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -2314,6 +2499,7 @@
       <c r="G77" s="4" t="n"/>
       <c r="H77" s="7" t="n"/>
       <c r="I77" s="7" t="n"/>
+      <c r="J77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -2343,6 +2529,9 @@
       <c r="I78" s="9" t="n">
         <v>13.75</v>
       </c>
+      <c r="J78" s="9" t="n">
+        <v>13.35</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -2371,6 +2560,9 @@
       </c>
       <c r="I79" s="9" t="n">
         <v>1346.27</v>
+      </c>
+      <c r="J79" s="9" t="n">
+        <v>1311.44</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -2383,6 +2575,7 @@
       <c r="G80" s="4" t="n"/>
       <c r="H80" s="7" t="n"/>
       <c r="I80" s="7" t="n"/>
+      <c r="J80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -2412,6 +2605,9 @@
       <c r="I81" s="9" t="n">
         <v>56.25</v>
       </c>
+      <c r="J81" s="9" t="n">
+        <v>54.22</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -2440,6 +2636,9 @@
       </c>
       <c r="I82" s="9" t="n">
         <v>2947.01</v>
+      </c>
+      <c r="J82" s="9" t="n">
+        <v>2671.07</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -2452,6 +2651,7 @@
       <c r="G83" s="4" t="n"/>
       <c r="H83" s="7" t="n"/>
       <c r="I83" s="7" t="n"/>
+      <c r="J83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -2481,6 +2681,9 @@
       <c r="I84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="J84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -2509,6 +2712,9 @@
       </c>
       <c r="I85" s="9" t="n">
         <v>2962.01</v>
+      </c>
+      <c r="J85" s="9" t="n">
+        <v>2737.09</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -2521,6 +2727,7 @@
       <c r="G86" s="4" t="n"/>
       <c r="H86" s="7" t="n"/>
       <c r="I86" s="7" t="n"/>
+      <c r="J86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -2550,6 +2757,9 @@
       <c r="I87" s="9" t="n">
         <v>52.59</v>
       </c>
+      <c r="J87" s="9" t="n">
+        <v>49.61</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -2578,6 +2788,9 @@
       </c>
       <c r="I88" s="9" t="n">
         <v>3096.58</v>
+      </c>
+      <c r="J88" s="9" t="n">
+        <v>2866.82</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -2590,6 +2803,7 @@
       <c r="G89" s="4" t="n"/>
       <c r="H89" s="7" t="n"/>
       <c r="I89" s="7" t="n"/>
+      <c r="J89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -2619,6 +2833,9 @@
       <c r="I90" s="9" t="n">
         <v>43.3</v>
       </c>
+      <c r="J90" s="9" t="n">
+        <v>42.29</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -2647,6 +2864,9 @@
       </c>
       <c r="I91" s="9" t="n">
         <v>2000.51</v>
+      </c>
+      <c r="J91" s="9" t="n">
+        <v>1961.39</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -2659,6 +2879,7 @@
       <c r="G92" s="4" t="n"/>
       <c r="H92" s="7" t="n"/>
       <c r="I92" s="7" t="n"/>
+      <c r="J92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -2688,6 +2909,9 @@
       <c r="I93" s="9" t="n">
         <v>27.42</v>
       </c>
+      <c r="J93" s="9" t="n">
+        <v>27.15</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -2716,6 +2940,9 @@
       </c>
       <c r="I94" s="9" t="n">
         <v>13704.57</v>
+      </c>
+      <c r="J94" s="9" t="n">
+        <v>13260.42</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -2728,6 +2955,7 @@
       <c r="G95" s="4" t="n"/>
       <c r="H95" s="7" t="n"/>
       <c r="I95" s="7" t="n"/>
+      <c r="J95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -2757,6 +2985,9 @@
       <c r="I96" s="9" t="n">
         <v>84.81</v>
       </c>
+      <c r="J96" s="9" t="n">
+        <v>82.72</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -2785,6 +3016,9 @@
       </c>
       <c r="I97" s="9" t="n">
         <v>8712.18</v>
+      </c>
+      <c r="J97" s="9" t="n">
+        <v>8253.1</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -2797,6 +3031,7 @@
       <c r="G98" s="4" t="n"/>
       <c r="H98" s="7" t="n"/>
       <c r="I98" s="7" t="n"/>
+      <c r="J98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -2826,6 +3061,9 @@
       <c r="I99" s="9" t="n">
         <v>56.5</v>
       </c>
+      <c r="J99" s="9" t="n">
+        <v>55.43</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -2854,6 +3092,9 @@
       </c>
       <c r="I100" s="9" t="n">
         <v>11944.72</v>
+      </c>
+      <c r="J100" s="9" t="n">
+        <v>11942.92</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -2866,6 +3107,7 @@
       <c r="G101" s="4" t="n"/>
       <c r="H101" s="7" t="n"/>
       <c r="I101" s="7" t="n"/>
+      <c r="J101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -2895,6 +3137,9 @@
       <c r="I102" s="9" t="n">
         <v>5.73</v>
       </c>
+      <c r="J102" s="9" t="n">
+        <v>5.52</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -2923,6 +3168,9 @@
       </c>
       <c r="I103" s="9" t="n">
         <v>2266.47</v>
+      </c>
+      <c r="J103" s="9" t="n">
+        <v>2211.92</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -2935,6 +3183,7 @@
       <c r="G104" s="4" t="n"/>
       <c r="H104" s="7" t="n"/>
       <c r="I104" s="7" t="n"/>
+      <c r="J104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -2964,6 +3213,9 @@
       <c r="I105" s="9" t="n">
         <v>25.59</v>
       </c>
+      <c r="J105" s="9" t="n">
+        <v>25.14</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -2992,6 +3244,9 @@
       </c>
       <c r="I106" s="9" t="n">
         <v>865.4299999999999</v>
+      </c>
+      <c r="J106" s="9" t="n">
+        <v>825.27</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -3004,6 +3259,7 @@
       <c r="G107" s="4" t="n"/>
       <c r="H107" s="7" t="n"/>
       <c r="I107" s="7" t="n"/>
+      <c r="J107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -3033,6 +3289,9 @@
       <c r="I108" s="9" t="n">
         <v>29.61</v>
       </c>
+      <c r="J108" s="9" t="n">
+        <v>29.04</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -3061,6 +3320,9 @@
       </c>
       <c r="I109" s="9" t="n">
         <v>2841.63</v>
+      </c>
+      <c r="J109" s="9" t="n">
+        <v>2602.38</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -3073,6 +3335,7 @@
       <c r="G110" s="4" t="n"/>
       <c r="H110" s="7" t="n"/>
       <c r="I110" s="7" t="n"/>
+      <c r="J110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -3102,6 +3365,9 @@
       <c r="I111" s="9" t="n">
         <v>20.59</v>
       </c>
+      <c r="J111" s="9" t="n">
+        <v>19.63</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -3130,6 +3396,9 @@
       </c>
       <c r="I112" s="9" t="n">
         <v>3899.86</v>
+      </c>
+      <c r="J112" s="9" t="n">
+        <v>3795.3</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -3142,6 +3411,7 @@
       <c r="G113" s="4" t="n"/>
       <c r="H113" s="7" t="n"/>
       <c r="I113" s="7" t="n"/>
+      <c r="J113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -3171,6 +3441,9 @@
       <c r="I114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="J114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -3199,6 +3472,9 @@
       </c>
       <c r="I115" s="9" t="n">
         <v>3366.43</v>
+      </c>
+      <c r="J115" s="9" t="n">
+        <v>3255.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-11-27 03:58:20]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -495,6 +495,7 @@
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="15" customWidth="1" min="9" max="9"/>
     <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -548,6 +549,11 @@
           <t>2025/11/24</t>
         </is>
       </c>
+      <c r="K1" s="7" t="inlineStr">
+        <is>
+          <t>2025/11/27</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -600,6 +606,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="K2" s="8" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -632,6 +643,9 @@
       <c r="J3" s="9" t="n">
         <v>60.18</v>
       </c>
+      <c r="K3" s="9" t="n">
+        <v>60.84</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -663,6 +677,9 @@
       </c>
       <c r="J4" s="9" t="n">
         <v>3821.68</v>
+      </c>
+      <c r="K4" s="9" t="n">
+        <v>3883.01</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -676,6 +693,7 @@
       <c r="H5" s="7" t="n"/>
       <c r="I5" s="7" t="n"/>
       <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -708,6 +726,9 @@
       <c r="J6" s="9" t="n">
         <v>46.74</v>
       </c>
+      <c r="K6" s="9" t="n">
+        <v>47.52</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -739,6 +760,9 @@
       </c>
       <c r="J7" s="9" t="n">
         <v>5300.7</v>
+      </c>
+      <c r="K7" s="9" t="n">
+        <v>5438.34</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -752,6 +776,7 @@
       <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
+      <c r="K8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -784,6 +809,9 @@
       <c r="J9" s="9" t="n">
         <v>52.46</v>
       </c>
+      <c r="K9" s="9" t="n">
+        <v>52.69</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -815,6 +843,9 @@
       </c>
       <c r="J10" s="9" t="n">
         <v>4427.55</v>
+      </c>
+      <c r="K10" s="9" t="n">
+        <v>4531.83</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -828,6 +859,7 @@
       <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
       <c r="J11" s="7" t="n"/>
+      <c r="K11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -860,6 +892,9 @@
       <c r="J12" s="9" t="n">
         <v>54.44</v>
       </c>
+      <c r="K12" s="9" t="n">
+        <v>55.44</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -891,6 +926,9 @@
       </c>
       <c r="J13" s="9" t="n">
         <v>6804.37</v>
+      </c>
+      <c r="K13" s="9" t="n">
+        <v>6990.32</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -904,6 +942,7 @@
       <c r="H14" s="7" t="n"/>
       <c r="I14" s="7" t="n"/>
       <c r="J14" s="7" t="n"/>
+      <c r="K14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -936,6 +975,9 @@
       <c r="J15" s="9" t="n">
         <v>25.19</v>
       </c>
+      <c r="K15" s="9" t="n">
+        <v>26.21</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -967,6 +1009,9 @@
       </c>
       <c r="J16" s="9" t="n">
         <v>2611.42</v>
+      </c>
+      <c r="K16" s="9" t="n">
+        <v>2657.21</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -980,6 +1025,7 @@
       <c r="H17" s="7" t="n"/>
       <c r="I17" s="7" t="n"/>
       <c r="J17" s="7" t="n"/>
+      <c r="K17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1012,6 +1058,9 @@
       <c r="J18" s="9" t="n">
         <v>95.14</v>
       </c>
+      <c r="K18" s="9" t="n">
+        <v>96.53</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1043,6 +1092,9 @@
       </c>
       <c r="J19" s="9" t="n">
         <v>6602.99</v>
+      </c>
+      <c r="K19" s="9" t="n">
+        <v>6812.61</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1056,6 +1108,7 @@
       <c r="H20" s="7" t="n"/>
       <c r="I20" s="7" t="n"/>
       <c r="J20" s="7" t="n"/>
+      <c r="K20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1088,6 +1141,9 @@
       <c r="J21" s="9" t="n">
         <v>68.28</v>
       </c>
+      <c r="K21" s="9" t="n">
+        <v>69.8</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1119,6 +1175,9 @@
       </c>
       <c r="J22" s="9" t="n">
         <v>85382.7</v>
+      </c>
+      <c r="K22" s="9" t="n">
+        <v>85745.05</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1132,6 +1191,7 @@
       <c r="H23" s="7" t="n"/>
       <c r="I23" s="7" t="n"/>
       <c r="J23" s="7" t="n"/>
+      <c r="K23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1164,6 +1224,9 @@
       <c r="J24" s="9" t="n">
         <v>81.45999999999999</v>
       </c>
+      <c r="K24" s="9" t="n">
+        <v>81.62</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1195,6 +1258,9 @@
       </c>
       <c r="J25" s="9" t="n">
         <v>23091.87</v>
+      </c>
+      <c r="K25" s="9" t="n">
+        <v>23695.91</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1208,6 +1274,7 @@
       <c r="H26" s="7" t="n"/>
       <c r="I26" s="7" t="n"/>
       <c r="J26" s="7" t="n"/>
+      <c r="K26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1240,6 +1307,9 @@
       <c r="J27" s="9" t="n">
         <v>69.37</v>
       </c>
+      <c r="K27" s="9" t="n">
+        <v>67.17</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1271,6 +1341,9 @@
       </c>
       <c r="J28" s="9" t="n">
         <v>48625.83</v>
+      </c>
+      <c r="K28" s="9" t="n">
+        <v>50094.09</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1284,6 +1357,7 @@
       <c r="H29" s="7" t="n"/>
       <c r="I29" s="7" t="n"/>
       <c r="J29" s="7" t="n"/>
+      <c r="K29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1316,6 +1390,9 @@
       <c r="J30" s="9" t="n">
         <v>47.55</v>
       </c>
+      <c r="K30" s="9" t="n">
+        <v>47.93</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1347,6 +1424,9 @@
       </c>
       <c r="J31" s="9" t="n">
         <v>5530.63</v>
+      </c>
+      <c r="K31" s="9" t="n">
+        <v>5543.51</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1360,6 +1440,7 @@
       <c r="H32" s="7" t="n"/>
       <c r="I32" s="7" t="n"/>
       <c r="J32" s="7" t="n"/>
+      <c r="K32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1392,6 +1473,9 @@
       <c r="J33" s="9" t="n">
         <v>9.550000000000001</v>
       </c>
+      <c r="K33" s="9" t="n">
+        <v>10.13</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1423,6 +1507,9 @@
       </c>
       <c r="J34" s="9" t="n">
         <v>31126.79</v>
+      </c>
+      <c r="K34" s="9" t="n">
+        <v>31550.46</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1436,6 +1523,7 @@
       <c r="H35" s="7" t="n"/>
       <c r="I35" s="7" t="n"/>
       <c r="J35" s="7" t="n"/>
+      <c r="K35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1468,6 +1556,9 @@
       <c r="J36" s="9" t="n">
         <v>25.85</v>
       </c>
+      <c r="K36" s="9" t="n">
+        <v>27.02</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1499,6 +1590,9 @@
       </c>
       <c r="J37" s="9" t="n">
         <v>3045.56</v>
+      </c>
+      <c r="K37" s="9" t="n">
+        <v>3238.06</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1512,6 +1606,7 @@
       <c r="H38" s="7" t="n"/>
       <c r="I38" s="7" t="n"/>
       <c r="J38" s="7" t="n"/>
+      <c r="K38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1544,6 +1639,9 @@
       <c r="J39" s="9" t="n">
         <v>42.6</v>
       </c>
+      <c r="K39" s="9" t="n">
+        <v>41.66</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1575,6 +1673,9 @@
       </c>
       <c r="J40" s="9" t="n">
         <v>2897.68</v>
+      </c>
+      <c r="K40" s="9" t="n">
+        <v>3061.79</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1588,6 +1689,7 @@
       <c r="H41" s="7" t="n"/>
       <c r="I41" s="7" t="n"/>
       <c r="J41" s="7" t="n"/>
+      <c r="K41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1620,6 +1722,9 @@
       <c r="J42" s="9" t="n">
         <v>14.49</v>
       </c>
+      <c r="K42" s="9" t="n">
+        <v>15.05</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1651,6 +1756,9 @@
       </c>
       <c r="J43" s="9" t="n">
         <v>6893.92</v>
+      </c>
+      <c r="K43" s="9" t="n">
+        <v>6899.6</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1664,6 +1772,7 @@
       <c r="H44" s="7" t="n"/>
       <c r="I44" s="7" t="n"/>
       <c r="J44" s="7" t="n"/>
+      <c r="K44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1696,6 +1805,9 @@
       <c r="J45" s="9" t="n">
         <v>26.34</v>
       </c>
+      <c r="K45" s="9" t="n">
+        <v>27.83</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1727,6 +1839,9 @@
       </c>
       <c r="J46" s="9" t="n">
         <v>8462.25</v>
+      </c>
+      <c r="K46" s="9" t="n">
+        <v>8503.040000000001</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1740,6 +1855,7 @@
       <c r="H47" s="7" t="n"/>
       <c r="I47" s="7" t="n"/>
       <c r="J47" s="7" t="n"/>
+      <c r="K47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1772,6 +1888,9 @@
       <c r="J48" s="9" t="n">
         <v>11.21</v>
       </c>
+      <c r="K48" s="9" t="n">
+        <v>11.52</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1803,6 +1922,9 @@
       </c>
       <c r="J49" s="9" t="n">
         <v>12671.93</v>
+      </c>
+      <c r="K49" s="9" t="n">
+        <v>12753.32</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1816,6 +1938,7 @@
       <c r="H50" s="7" t="n"/>
       <c r="I50" s="7" t="n"/>
       <c r="J50" s="7" t="n"/>
+      <c r="K50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1848,6 +1971,9 @@
       <c r="J51" s="9" t="n">
         <v>22.2</v>
       </c>
+      <c r="K51" s="9" t="n">
+        <v>24.41</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -1879,6 +2005,9 @@
       </c>
       <c r="J52" s="9" t="n">
         <v>12032.16</v>
+      </c>
+      <c r="K52" s="9" t="n">
+        <v>12390.6</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1892,6 +2021,7 @@
       <c r="H53" s="7" t="n"/>
       <c r="I53" s="7" t="n"/>
       <c r="J53" s="7" t="n"/>
+      <c r="K53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -1924,6 +2054,9 @@
       <c r="J54" s="9" t="n">
         <v>0</v>
       </c>
+      <c r="K54" s="9" t="n">
+        <v>21.77</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -1955,6 +2088,9 @@
       </c>
       <c r="J55" s="9" t="n">
         <v>5459.33</v>
+      </c>
+      <c r="K55" s="9" t="n">
+        <v>9663.1</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1968,6 +2104,7 @@
       <c r="H56" s="7" t="n"/>
       <c r="I56" s="7" t="n"/>
       <c r="J56" s="7" t="n"/>
+      <c r="K56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2000,6 +2137,9 @@
       <c r="J57" s="9" t="n">
         <v>26.82</v>
       </c>
+      <c r="K57" s="9" t="n">
+        <v>26.61</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2031,6 +2171,9 @@
       </c>
       <c r="J58" s="9" t="n">
         <v>15973</v>
+      </c>
+      <c r="K58" s="9" t="n">
+        <v>15994.54</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -2044,6 +2187,7 @@
       <c r="H59" s="7" t="n"/>
       <c r="I59" s="7" t="n"/>
       <c r="J59" s="7" t="n"/>
+      <c r="K59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2076,6 +2220,9 @@
       <c r="J60" s="9" t="n">
         <v>30.73</v>
       </c>
+      <c r="K60" s="9" t="n">
+        <v>31.77</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -2106,6 +2253,9 @@
         <v>17526.85</v>
       </c>
       <c r="J61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="K61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -2120,6 +2270,7 @@
       <c r="H62" s="7" t="n"/>
       <c r="I62" s="7" t="n"/>
       <c r="J62" s="7" t="n"/>
+      <c r="K62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -2152,6 +2303,9 @@
       <c r="J63" s="9" t="n">
         <v>17.84</v>
       </c>
+      <c r="K63" s="9" t="n">
+        <v>19.71</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2183,6 +2337,9 @@
       </c>
       <c r="J64" s="9" t="n">
         <v>9681.84</v>
+      </c>
+      <c r="K64" s="9" t="n">
+        <v>9719.309999999999</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -2196,6 +2353,7 @@
       <c r="H65" s="7" t="n"/>
       <c r="I65" s="7" t="n"/>
       <c r="J65" s="7" t="n"/>
+      <c r="K65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -2228,6 +2386,9 @@
       <c r="J66" s="9" t="n">
         <v>13.8</v>
       </c>
+      <c r="K66" s="9" t="n">
+        <v>15.11</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -2259,6 +2420,9 @@
       </c>
       <c r="J67" s="9" t="n">
         <v>9784.98</v>
+      </c>
+      <c r="K67" s="9" t="n">
+        <v>9902.99</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -2272,6 +2436,7 @@
       <c r="H68" s="7" t="n"/>
       <c r="I68" s="7" t="n"/>
       <c r="J68" s="7" t="n"/>
+      <c r="K68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -2304,6 +2469,9 @@
       <c r="J69" s="9" t="n">
         <v>19.43</v>
       </c>
+      <c r="K69" s="9" t="n">
+        <v>22.23</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -2335,6 +2503,9 @@
       </c>
       <c r="J70" s="9" t="n">
         <v>2946.79</v>
+      </c>
+      <c r="K70" s="9" t="n">
+        <v>2990.37</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -2348,6 +2519,7 @@
       <c r="H71" s="7" t="n"/>
       <c r="I71" s="7" t="n"/>
       <c r="J71" s="7" t="n"/>
+      <c r="K71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2380,6 +2552,9 @@
       <c r="J72" s="9" t="n">
         <v>36.97</v>
       </c>
+      <c r="K72" s="9" t="n">
+        <v>42.23</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2411,6 +2586,9 @@
       </c>
       <c r="J73" s="9" t="n">
         <v>5484.46</v>
+      </c>
+      <c r="K73" s="9" t="n">
+        <v>5622.48</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -2424,6 +2602,7 @@
       <c r="H74" s="7" t="n"/>
       <c r="I74" s="7" t="n"/>
       <c r="J74" s="7" t="n"/>
+      <c r="K74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -2456,6 +2635,9 @@
       <c r="J75" s="9" t="n">
         <v>24.07</v>
       </c>
+      <c r="K75" s="9" t="n">
+        <v>25.27</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -2487,6 +2669,9 @@
       </c>
       <c r="J76" s="9" t="n">
         <v>8974.48</v>
+      </c>
+      <c r="K76" s="9" t="n">
+        <v>9056.360000000001</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -2500,6 +2685,7 @@
       <c r="H77" s="7" t="n"/>
       <c r="I77" s="7" t="n"/>
       <c r="J77" s="7" t="n"/>
+      <c r="K77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -2532,6 +2718,9 @@
       <c r="J78" s="9" t="n">
         <v>13.35</v>
       </c>
+      <c r="K78" s="9" t="n">
+        <v>13.57</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -2563,6 +2752,9 @@
       </c>
       <c r="J79" s="9" t="n">
         <v>1311.44</v>
+      </c>
+      <c r="K79" s="9" t="n">
+        <v>1325.88</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -2576,6 +2768,7 @@
       <c r="H80" s="7" t="n"/>
       <c r="I80" s="7" t="n"/>
       <c r="J80" s="7" t="n"/>
+      <c r="K80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -2608,6 +2801,9 @@
       <c r="J81" s="9" t="n">
         <v>54.22</v>
       </c>
+      <c r="K81" s="9" t="n">
+        <v>54.5</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -2639,6 +2835,9 @@
       </c>
       <c r="J82" s="9" t="n">
         <v>2671.07</v>
+      </c>
+      <c r="K82" s="9" t="n">
+        <v>2760.39</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -2652,6 +2851,7 @@
       <c r="H83" s="7" t="n"/>
       <c r="I83" s="7" t="n"/>
       <c r="J83" s="7" t="n"/>
+      <c r="K83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -2684,6 +2884,9 @@
       <c r="J84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="K84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -2715,6 +2918,9 @@
       </c>
       <c r="J85" s="9" t="n">
         <v>2737.09</v>
+      </c>
+      <c r="K85" s="9" t="n">
+        <v>2835.63</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -2728,6 +2934,7 @@
       <c r="H86" s="7" t="n"/>
       <c r="I86" s="7" t="n"/>
       <c r="J86" s="7" t="n"/>
+      <c r="K86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -2760,6 +2967,9 @@
       <c r="J87" s="9" t="n">
         <v>49.61</v>
       </c>
+      <c r="K87" s="9" t="n">
+        <v>49.97</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -2791,6 +3001,9 @@
       </c>
       <c r="J88" s="9" t="n">
         <v>2866.82</v>
+      </c>
+      <c r="K88" s="9" t="n">
+        <v>2877.51</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -2804,6 +3017,7 @@
       <c r="H89" s="7" t="n"/>
       <c r="I89" s="7" t="n"/>
       <c r="J89" s="7" t="n"/>
+      <c r="K89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -2836,6 +3050,9 @@
       <c r="J90" s="9" t="n">
         <v>42.29</v>
       </c>
+      <c r="K90" s="9" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -2867,6 +3084,9 @@
       </c>
       <c r="J91" s="9" t="n">
         <v>1961.39</v>
+      </c>
+      <c r="K91" s="9" t="n">
+        <v>1992.43</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -2880,6 +3100,7 @@
       <c r="H92" s="7" t="n"/>
       <c r="I92" s="7" t="n"/>
       <c r="J92" s="7" t="n"/>
+      <c r="K92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -2912,6 +3133,9 @@
       <c r="J93" s="9" t="n">
         <v>27.15</v>
       </c>
+      <c r="K93" s="9" t="n">
+        <v>27.19</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -2943,6 +3167,9 @@
       </c>
       <c r="J94" s="9" t="n">
         <v>13260.42</v>
+      </c>
+      <c r="K94" s="9" t="n">
+        <v>13513.84</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -2956,6 +3183,7 @@
       <c r="H95" s="7" t="n"/>
       <c r="I95" s="7" t="n"/>
       <c r="J95" s="7" t="n"/>
+      <c r="K95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -2988,6 +3216,9 @@
       <c r="J96" s="9" t="n">
         <v>82.72</v>
       </c>
+      <c r="K96" s="9" t="n">
+        <v>83.98999999999999</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -3019,6 +3250,9 @@
       </c>
       <c r="J97" s="9" t="n">
         <v>8253.1</v>
+      </c>
+      <c r="K97" s="9" t="n">
+        <v>8737.66</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -3032,6 +3266,7 @@
       <c r="H98" s="7" t="n"/>
       <c r="I98" s="7" t="n"/>
       <c r="J98" s="7" t="n"/>
+      <c r="K98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -3064,6 +3299,9 @@
       <c r="J99" s="9" t="n">
         <v>55.43</v>
       </c>
+      <c r="K99" s="9" t="n">
+        <v>55.75</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -3095,6 +3333,9 @@
       </c>
       <c r="J100" s="9" t="n">
         <v>11942.92</v>
+      </c>
+      <c r="K100" s="9" t="n">
+        <v>11835.95</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -3108,6 +3349,7 @@
       <c r="H101" s="7" t="n"/>
       <c r="I101" s="7" t="n"/>
       <c r="J101" s="7" t="n"/>
+      <c r="K101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -3140,6 +3382,9 @@
       <c r="J102" s="9" t="n">
         <v>5.52</v>
       </c>
+      <c r="K102" s="9" t="n">
+        <v>5.62</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -3171,6 +3416,9 @@
       </c>
       <c r="J103" s="9" t="n">
         <v>2211.92</v>
+      </c>
+      <c r="K103" s="9" t="n">
+        <v>2222.72</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -3184,6 +3432,7 @@
       <c r="H104" s="7" t="n"/>
       <c r="I104" s="7" t="n"/>
       <c r="J104" s="7" t="n"/>
+      <c r="K104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -3216,6 +3465,9 @@
       <c r="J105" s="9" t="n">
         <v>25.14</v>
       </c>
+      <c r="K105" s="9" t="n">
+        <v>25.17</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -3247,6 +3499,9 @@
       </c>
       <c r="J106" s="9" t="n">
         <v>825.27</v>
+      </c>
+      <c r="K106" s="9" t="n">
+        <v>828.35</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -3260,6 +3515,7 @@
       <c r="H107" s="7" t="n"/>
       <c r="I107" s="7" t="n"/>
       <c r="J107" s="7" t="n"/>
+      <c r="K107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -3292,6 +3548,9 @@
       <c r="J108" s="9" t="n">
         <v>29.04</v>
       </c>
+      <c r="K108" s="9" t="n">
+        <v>29.26</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -3323,6 +3582,9 @@
       </c>
       <c r="J109" s="9" t="n">
         <v>2602.38</v>
+      </c>
+      <c r="K109" s="9" t="n">
+        <v>2713.49</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -3336,6 +3598,7 @@
       <c r="H110" s="7" t="n"/>
       <c r="I110" s="7" t="n"/>
       <c r="J110" s="7" t="n"/>
+      <c r="K110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -3368,6 +3631,9 @@
       <c r="J111" s="9" t="n">
         <v>19.63</v>
       </c>
+      <c r="K111" s="9" t="n">
+        <v>20.08</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -3399,6 +3665,9 @@
       </c>
       <c r="J112" s="9" t="n">
         <v>3795.3</v>
+      </c>
+      <c r="K112" s="9" t="n">
+        <v>3816.3</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -3412,6 +3681,7 @@
       <c r="H113" s="7" t="n"/>
       <c r="I113" s="7" t="n"/>
       <c r="J113" s="7" t="n"/>
+      <c r="K113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -3444,6 +3714,9 @@
       <c r="J114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="K114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -3475,6 +3748,9 @@
       </c>
       <c r="J115" s="9" t="n">
         <v>3255.03</v>
+      </c>
+      <c r="K115" s="9" t="n">
+        <v>3241.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-01 04:37:35]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:L115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -496,6 +496,7 @@
     <col width="15" customWidth="1" min="9" max="9"/>
     <col width="15" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -554,6 +555,11 @@
           <t>2025/11/27</t>
         </is>
       </c>
+      <c r="L1" s="7" t="inlineStr">
+        <is>
+          <t>2025/12/01</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -611,6 +617,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="L2" s="8" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -646,6 +657,9 @@
       <c r="K3" s="9" t="n">
         <v>60.84</v>
       </c>
+      <c r="L3" s="9" t="n">
+        <v>61.11</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -680,6 +694,9 @@
       </c>
       <c r="K4" s="9" t="n">
         <v>3883.01</v>
+      </c>
+      <c r="L4" s="9" t="n">
+        <v>3904.9</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -694,6 +711,7 @@
       <c r="I5" s="7" t="n"/>
       <c r="J5" s="7" t="n"/>
       <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -729,6 +747,9 @@
       <c r="K6" s="9" t="n">
         <v>47.52</v>
       </c>
+      <c r="L6" s="9" t="n">
+        <v>47.8</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -763,6 +784,9 @@
       </c>
       <c r="K7" s="9" t="n">
         <v>5438.34</v>
+      </c>
+      <c r="L7" s="9" t="n">
+        <v>5487.42</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -777,6 +801,7 @@
       <c r="I8" s="7" t="n"/>
       <c r="J8" s="7" t="n"/>
       <c r="K8" s="7" t="n"/>
+      <c r="L8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -812,6 +837,9 @@
       <c r="K9" s="9" t="n">
         <v>52.69</v>
       </c>
+      <c r="L9" s="9" t="n">
+        <v>52.75</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -846,6 +874,9 @@
       </c>
       <c r="K10" s="9" t="n">
         <v>4531.83</v>
+      </c>
+      <c r="L10" s="9" t="n">
+        <v>4560.67</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -860,6 +891,7 @@
       <c r="I11" s="7" t="n"/>
       <c r="J11" s="7" t="n"/>
       <c r="K11" s="7" t="n"/>
+      <c r="L11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -895,6 +927,9 @@
       <c r="K12" s="9" t="n">
         <v>55.44</v>
       </c>
+      <c r="L12" s="9" t="n">
+        <v>55.87</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -929,6 +964,9 @@
       </c>
       <c r="K13" s="9" t="n">
         <v>6990.32</v>
+      </c>
+      <c r="L13" s="9" t="n">
+        <v>7086.13</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -943,6 +981,7 @@
       <c r="I14" s="7" t="n"/>
       <c r="J14" s="7" t="n"/>
       <c r="K14" s="7" t="n"/>
+      <c r="L14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -978,6 +1017,9 @@
       <c r="K15" s="9" t="n">
         <v>26.21</v>
       </c>
+      <c r="L15" s="9" t="n">
+        <v>26.18</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1012,6 +1054,9 @@
       </c>
       <c r="K16" s="9" t="n">
         <v>2657.21</v>
+      </c>
+      <c r="L16" s="9" t="n">
+        <v>2668.8</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1026,6 +1071,7 @@
       <c r="I17" s="7" t="n"/>
       <c r="J17" s="7" t="n"/>
       <c r="K17" s="7" t="n"/>
+      <c r="L17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1061,6 +1107,9 @@
       <c r="K18" s="9" t="n">
         <v>96.53</v>
       </c>
+      <c r="L18" s="9" t="n">
+        <v>96.8</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1095,6 +1144,9 @@
       </c>
       <c r="K19" s="9" t="n">
         <v>6812.61</v>
+      </c>
+      <c r="L19" s="9" t="n">
+        <v>6849.09</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1109,6 +1161,7 @@
       <c r="I20" s="7" t="n"/>
       <c r="J20" s="7" t="n"/>
       <c r="K20" s="7" t="n"/>
+      <c r="L20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1144,6 +1197,9 @@
       <c r="K21" s="9" t="n">
         <v>69.8</v>
       </c>
+      <c r="L21" s="9" t="n">
+        <v>70.09999999999999</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1178,6 +1234,9 @@
       </c>
       <c r="K22" s="9" t="n">
         <v>85745.05</v>
+      </c>
+      <c r="L22" s="9" t="n">
+        <v>86034.03999999999</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1192,6 +1251,7 @@
       <c r="I23" s="7" t="n"/>
       <c r="J23" s="7" t="n"/>
       <c r="K23" s="7" t="n"/>
+      <c r="L23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1227,6 +1287,9 @@
       <c r="K24" s="9" t="n">
         <v>81.62</v>
       </c>
+      <c r="L24" s="9" t="n">
+        <v>83.29000000000001</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1261,6 +1324,9 @@
       </c>
       <c r="K25" s="9" t="n">
         <v>23695.91</v>
+      </c>
+      <c r="L25" s="9" t="n">
+        <v>23836.79</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1275,6 +1341,7 @@
       <c r="I26" s="7" t="n"/>
       <c r="J26" s="7" t="n"/>
       <c r="K26" s="7" t="n"/>
+      <c r="L26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1310,6 +1377,9 @@
       <c r="K27" s="9" t="n">
         <v>67.17</v>
       </c>
+      <c r="L27" s="9" t="n">
+        <v>70.06999999999999</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1344,6 +1414,9 @@
       </c>
       <c r="K28" s="9" t="n">
         <v>50094.09</v>
+      </c>
+      <c r="L28" s="9" t="n">
+        <v>49371.8</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1358,6 +1431,7 @@
       <c r="I29" s="7" t="n"/>
       <c r="J29" s="7" t="n"/>
       <c r="K29" s="7" t="n"/>
+      <c r="L29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1393,6 +1467,9 @@
       <c r="K30" s="9" t="n">
         <v>47.93</v>
       </c>
+      <c r="L30" s="9" t="n">
+        <v>47.96</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1427,6 +1504,9 @@
       </c>
       <c r="K31" s="9" t="n">
         <v>5543.51</v>
+      </c>
+      <c r="L31" s="9" t="n">
+        <v>5579.25</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1441,6 +1521,7 @@
       <c r="I32" s="7" t="n"/>
       <c r="J32" s="7" t="n"/>
       <c r="K32" s="7" t="n"/>
+      <c r="L32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1476,6 +1557,9 @@
       <c r="K33" s="9" t="n">
         <v>10.13</v>
       </c>
+      <c r="L33" s="9" t="n">
+        <v>9.81</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1510,6 +1594,9 @@
       </c>
       <c r="K34" s="9" t="n">
         <v>31550.46</v>
+      </c>
+      <c r="L34" s="9" t="n">
+        <v>31672.68</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1524,6 +1611,7 @@
       <c r="I35" s="7" t="n"/>
       <c r="J35" s="7" t="n"/>
       <c r="K35" s="7" t="n"/>
+      <c r="L35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1559,6 +1647,9 @@
       <c r="K36" s="9" t="n">
         <v>27.02</v>
       </c>
+      <c r="L36" s="9" t="n">
+        <v>27.05</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1593,6 +1684,9 @@
       </c>
       <c r="K37" s="9" t="n">
         <v>3238.06</v>
+      </c>
+      <c r="L37" s="9" t="n">
+        <v>3253.68</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1607,6 +1701,7 @@
       <c r="I38" s="7" t="n"/>
       <c r="J38" s="7" t="n"/>
       <c r="K38" s="7" t="n"/>
+      <c r="L38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1642,6 +1737,9 @@
       <c r="K39" s="9" t="n">
         <v>41.66</v>
       </c>
+      <c r="L39" s="9" t="n">
+        <v>41.87</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1676,6 +1774,9 @@
       </c>
       <c r="K40" s="9" t="n">
         <v>3061.79</v>
+      </c>
+      <c r="L40" s="9" t="n">
+        <v>3080.16</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1690,6 +1791,7 @@
       <c r="I41" s="7" t="n"/>
       <c r="J41" s="7" t="n"/>
       <c r="K41" s="7" t="n"/>
+      <c r="L41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1725,6 +1827,9 @@
       <c r="K42" s="9" t="n">
         <v>15.05</v>
       </c>
+      <c r="L42" s="9" t="n">
+        <v>15.21</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1759,6 +1864,9 @@
       </c>
       <c r="K43" s="9" t="n">
         <v>6899.6</v>
+      </c>
+      <c r="L43" s="9" t="n">
+        <v>6938.26</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1773,6 +1881,7 @@
       <c r="I44" s="7" t="n"/>
       <c r="J44" s="7" t="n"/>
       <c r="K44" s="7" t="n"/>
+      <c r="L44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1808,6 +1917,9 @@
       <c r="K45" s="9" t="n">
         <v>27.83</v>
       </c>
+      <c r="L45" s="9" t="n">
+        <v>27.4</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1842,6 +1954,9 @@
       </c>
       <c r="K46" s="9" t="n">
         <v>8503.040000000001</v>
+      </c>
+      <c r="L46" s="9" t="n">
+        <v>8493.969999999999</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1856,6 +1971,7 @@
       <c r="I47" s="7" t="n"/>
       <c r="J47" s="7" t="n"/>
       <c r="K47" s="7" t="n"/>
+      <c r="L47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -1891,6 +2007,9 @@
       <c r="K48" s="9" t="n">
         <v>11.52</v>
       </c>
+      <c r="L48" s="9" t="n">
+        <v>11.99</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -1925,6 +2044,9 @@
       </c>
       <c r="K49" s="9" t="n">
         <v>12753.32</v>
+      </c>
+      <c r="L49" s="9" t="n">
+        <v>12878.04</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1939,6 +2061,7 @@
       <c r="I50" s="7" t="n"/>
       <c r="J50" s="7" t="n"/>
       <c r="K50" s="7" t="n"/>
+      <c r="L50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -1974,6 +2097,9 @@
       <c r="K51" s="9" t="n">
         <v>24.41</v>
       </c>
+      <c r="L51" s="9" t="n">
+        <v>24.66</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2008,6 +2134,9 @@
       </c>
       <c r="K52" s="9" t="n">
         <v>12390.6</v>
+      </c>
+      <c r="L52" s="9" t="n">
+        <v>12411.4</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2022,6 +2151,7 @@
       <c r="I53" s="7" t="n"/>
       <c r="J53" s="7" t="n"/>
       <c r="K53" s="7" t="n"/>
+      <c r="L53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2057,6 +2187,9 @@
       <c r="K54" s="9" t="n">
         <v>21.77</v>
       </c>
+      <c r="L54" s="9" t="n">
+        <v>21.94</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2091,6 +2224,9 @@
       </c>
       <c r="K55" s="9" t="n">
         <v>9663.1</v>
+      </c>
+      <c r="L55" s="9" t="n">
+        <v>9682.030000000001</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -2105,6 +2241,7 @@
       <c r="I56" s="7" t="n"/>
       <c r="J56" s="7" t="n"/>
       <c r="K56" s="7" t="n"/>
+      <c r="L56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2140,6 +2277,9 @@
       <c r="K57" s="9" t="n">
         <v>26.61</v>
       </c>
+      <c r="L57" s="9" t="n">
+        <v>26.83</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2174,6 +2314,9 @@
       </c>
       <c r="K58" s="9" t="n">
         <v>15994.54</v>
+      </c>
+      <c r="L58" s="9" t="n">
+        <v>16031.85</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -2188,6 +2331,7 @@
       <c r="I59" s="7" t="n"/>
       <c r="J59" s="7" t="n"/>
       <c r="K59" s="7" t="n"/>
+      <c r="L59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2223,6 +2367,9 @@
       <c r="K60" s="9" t="n">
         <v>31.77</v>
       </c>
+      <c r="L60" s="9" t="n">
+        <v>31.41</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -2256,6 +2403,9 @@
         <v>17526.85</v>
       </c>
       <c r="K61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="L61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -2271,6 +2421,7 @@
       <c r="I62" s="7" t="n"/>
       <c r="J62" s="7" t="n"/>
       <c r="K62" s="7" t="n"/>
+      <c r="L62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -2306,6 +2457,9 @@
       <c r="K63" s="9" t="n">
         <v>19.71</v>
       </c>
+      <c r="L63" s="9" t="n">
+        <v>21.04</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2340,6 +2494,9 @@
       </c>
       <c r="K64" s="9" t="n">
         <v>9719.309999999999</v>
+      </c>
+      <c r="L64" s="9" t="n">
+        <v>9801.49</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -2354,6 +2511,7 @@
       <c r="I65" s="7" t="n"/>
       <c r="J65" s="7" t="n"/>
       <c r="K65" s="7" t="n"/>
+      <c r="L65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -2389,6 +2547,9 @@
       <c r="K66" s="9" t="n">
         <v>15.11</v>
       </c>
+      <c r="L66" s="9" t="n">
+        <v>14.17</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -2423,6 +2584,9 @@
       </c>
       <c r="K67" s="9" t="n">
         <v>9902.99</v>
+      </c>
+      <c r="L67" s="9" t="n">
+        <v>9889.290000000001</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -2437,6 +2601,7 @@
       <c r="I68" s="7" t="n"/>
       <c r="J68" s="7" t="n"/>
       <c r="K68" s="7" t="n"/>
+      <c r="L68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -2472,6 +2637,9 @@
       <c r="K69" s="9" t="n">
         <v>22.23</v>
       </c>
+      <c r="L69" s="9" t="n">
+        <v>23.72</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -2506,6 +2674,9 @@
       </c>
       <c r="K70" s="9" t="n">
         <v>2990.37</v>
+      </c>
+      <c r="L70" s="9" t="n">
+        <v>3020.73</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -2520,6 +2691,7 @@
       <c r="I71" s="7" t="n"/>
       <c r="J71" s="7" t="n"/>
       <c r="K71" s="7" t="n"/>
+      <c r="L71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2555,6 +2727,9 @@
       <c r="K72" s="9" t="n">
         <v>42.23</v>
       </c>
+      <c r="L72" s="9" t="n">
+        <v>41.98</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2589,6 +2764,9 @@
       </c>
       <c r="K73" s="9" t="n">
         <v>5622.48</v>
+      </c>
+      <c r="L73" s="9" t="n">
+        <v>5654.62</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -2603,6 +2781,7 @@
       <c r="I74" s="7" t="n"/>
       <c r="J74" s="7" t="n"/>
       <c r="K74" s="7" t="n"/>
+      <c r="L74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -2638,6 +2817,9 @@
       <c r="K75" s="9" t="n">
         <v>25.27</v>
       </c>
+      <c r="L75" s="9" t="n">
+        <v>25.24</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -2672,6 +2854,9 @@
       </c>
       <c r="K76" s="9" t="n">
         <v>9056.360000000001</v>
+      </c>
+      <c r="L76" s="9" t="n">
+        <v>9059.16</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -2686,6 +2871,7 @@
       <c r="I77" s="7" t="n"/>
       <c r="J77" s="7" t="n"/>
       <c r="K77" s="7" t="n"/>
+      <c r="L77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -2721,6 +2907,9 @@
       <c r="K78" s="9" t="n">
         <v>13.57</v>
       </c>
+      <c r="L78" s="9" t="n">
+        <v>13.37</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -2755,6 +2944,9 @@
       </c>
       <c r="K79" s="9" t="n">
         <v>1325.88</v>
+      </c>
+      <c r="L79" s="9" t="n">
+        <v>1314.12</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -2769,6 +2961,7 @@
       <c r="I80" s="7" t="n"/>
       <c r="J80" s="7" t="n"/>
       <c r="K80" s="7" t="n"/>
+      <c r="L80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -2804,6 +2997,9 @@
       <c r="K81" s="9" t="n">
         <v>54.5</v>
       </c>
+      <c r="L81" s="9" t="n">
+        <v>54.83</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -2838,6 +3034,9 @@
       </c>
       <c r="K82" s="9" t="n">
         <v>2760.39</v>
+      </c>
+      <c r="L82" s="9" t="n">
+        <v>2790.31</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -2852,6 +3051,7 @@
       <c r="I83" s="7" t="n"/>
       <c r="J83" s="7" t="n"/>
       <c r="K83" s="7" t="n"/>
+      <c r="L83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -2887,6 +3087,9 @@
       <c r="K84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="L84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -2921,6 +3124,9 @@
       </c>
       <c r="K85" s="9" t="n">
         <v>2835.63</v>
+      </c>
+      <c r="L85" s="9" t="n">
+        <v>2840.93</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -2935,6 +3141,7 @@
       <c r="I86" s="7" t="n"/>
       <c r="J86" s="7" t="n"/>
       <c r="K86" s="7" t="n"/>
+      <c r="L86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -2970,6 +3177,9 @@
       <c r="K87" s="9" t="n">
         <v>49.97</v>
       </c>
+      <c r="L87" s="9" t="n">
+        <v>50.6</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -3004,6 +3214,9 @@
       </c>
       <c r="K88" s="9" t="n">
         <v>2877.51</v>
+      </c>
+      <c r="L88" s="9" t="n">
+        <v>2928.92</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -3018,6 +3231,7 @@
       <c r="I89" s="7" t="n"/>
       <c r="J89" s="7" t="n"/>
       <c r="K89" s="7" t="n"/>
+      <c r="L89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -3053,6 +3267,9 @@
       <c r="K90" s="9" t="n">
         <v>44</v>
       </c>
+      <c r="L90" s="9" t="n">
+        <v>43.61</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -3087,6 +3304,9 @@
       </c>
       <c r="K91" s="9" t="n">
         <v>1992.43</v>
+      </c>
+      <c r="L91" s="9" t="n">
+        <v>1991.37</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -3101,6 +3321,7 @@
       <c r="I92" s="7" t="n"/>
       <c r="J92" s="7" t="n"/>
       <c r="K92" s="7" t="n"/>
+      <c r="L92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -3136,6 +3357,9 @@
       <c r="K93" s="9" t="n">
         <v>27.19</v>
       </c>
+      <c r="L93" s="9" t="n">
+        <v>27.39</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -3170,6 +3394,9 @@
       </c>
       <c r="K94" s="9" t="n">
         <v>13513.84</v>
+      </c>
+      <c r="L94" s="9" t="n">
+        <v>13621.38</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -3184,6 +3411,7 @@
       <c r="I95" s="7" t="n"/>
       <c r="J95" s="7" t="n"/>
       <c r="K95" s="7" t="n"/>
+      <c r="L95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -3219,6 +3447,9 @@
       <c r="K96" s="9" t="n">
         <v>83.98999999999999</v>
       </c>
+      <c r="L96" s="9" t="n">
+        <v>84.64</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -3253,6 +3484,9 @@
       </c>
       <c r="K97" s="9" t="n">
         <v>8737.66</v>
+      </c>
+      <c r="L97" s="9" t="n">
+        <v>8856.049999999999</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -3267,6 +3501,7 @@
       <c r="I98" s="7" t="n"/>
       <c r="J98" s="7" t="n"/>
       <c r="K98" s="7" t="n"/>
+      <c r="L98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -3302,6 +3537,9 @@
       <c r="K99" s="9" t="n">
         <v>55.75</v>
       </c>
+      <c r="L99" s="9" t="n">
+        <v>56.22</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -3336,6 +3574,9 @@
       </c>
       <c r="K100" s="9" t="n">
         <v>11835.95</v>
+      </c>
+      <c r="L100" s="9" t="n">
+        <v>12114.87</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -3350,6 +3591,7 @@
       <c r="I101" s="7" t="n"/>
       <c r="J101" s="7" t="n"/>
       <c r="K101" s="7" t="n"/>
+      <c r="L101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -3385,6 +3627,9 @@
       <c r="K102" s="9" t="n">
         <v>5.62</v>
       </c>
+      <c r="L102" s="9" t="n">
+        <v>5.82</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -3419,6 +3664,9 @@
       </c>
       <c r="K103" s="9" t="n">
         <v>2222.72</v>
+      </c>
+      <c r="L103" s="9" t="n">
+        <v>2228.44</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -3433,6 +3681,7 @@
       <c r="I104" s="7" t="n"/>
       <c r="J104" s="7" t="n"/>
       <c r="K104" s="7" t="n"/>
+      <c r="L104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -3468,6 +3717,9 @@
       <c r="K105" s="9" t="n">
         <v>25.17</v>
       </c>
+      <c r="L105" s="9" t="n">
+        <v>25.23</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -3502,6 +3754,9 @@
       </c>
       <c r="K106" s="9" t="n">
         <v>828.35</v>
+      </c>
+      <c r="L106" s="9" t="n">
+        <v>831.99</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -3516,6 +3771,7 @@
       <c r="I107" s="7" t="n"/>
       <c r="J107" s="7" t="n"/>
       <c r="K107" s="7" t="n"/>
+      <c r="L107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -3551,6 +3807,9 @@
       <c r="K108" s="9" t="n">
         <v>29.26</v>
       </c>
+      <c r="L108" s="9" t="n">
+        <v>29.4</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -3585,6 +3844,9 @@
       </c>
       <c r="K109" s="9" t="n">
         <v>2713.49</v>
+      </c>
+      <c r="L109" s="9" t="n">
+        <v>2817.43</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -3599,6 +3861,7 @@
       <c r="I110" s="7" t="n"/>
       <c r="J110" s="7" t="n"/>
       <c r="K110" s="7" t="n"/>
+      <c r="L110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -3634,6 +3897,9 @@
       <c r="K111" s="9" t="n">
         <v>20.08</v>
       </c>
+      <c r="L111" s="9" t="n">
+        <v>20.15</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -3668,6 +3934,9 @@
       </c>
       <c r="K112" s="9" t="n">
         <v>3816.3</v>
+      </c>
+      <c r="L112" s="9" t="n">
+        <v>3859.53</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -3682,6 +3951,7 @@
       <c r="I113" s="7" t="n"/>
       <c r="J113" s="7" t="n"/>
       <c r="K113" s="7" t="n"/>
+      <c r="L113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -3717,6 +3987,9 @@
       <c r="K114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="L114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -3751,6 +4024,9 @@
       </c>
       <c r="K115" s="9" t="n">
         <v>3241.08</v>
+      </c>
+      <c r="L115" s="9" t="n">
+        <v>3227.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-04 04:06:33]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -497,6 +497,7 @@
     <col width="15" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -560,6 +561,11 @@
           <t>2025/12/01</t>
         </is>
       </c>
+      <c r="M1" s="7" t="inlineStr">
+        <is>
+          <t>2025/12/04</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -622,6 +628,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="M2" s="8" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -660,6 +671,9 @@
       <c r="L3" s="9" t="n">
         <v>61.11</v>
       </c>
+      <c r="M3" s="9" t="n">
+        <v>60.89</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -697,6 +711,9 @@
       </c>
       <c r="L4" s="9" t="n">
         <v>3904.9</v>
+      </c>
+      <c r="M4" s="9" t="n">
+        <v>3879.52</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -712,6 +729,7 @@
       <c r="J5" s="7" t="n"/>
       <c r="K5" s="7" t="n"/>
       <c r="L5" s="7" t="n"/>
+      <c r="M5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -750,6 +768,9 @@
       <c r="L6" s="9" t="n">
         <v>47.8</v>
       </c>
+      <c r="M6" s="9" t="n">
+        <v>47.64</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -787,6 +808,9 @@
       </c>
       <c r="L7" s="9" t="n">
         <v>5487.42</v>
+      </c>
+      <c r="M7" s="9" t="n">
+        <v>5458.54</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -802,6 +826,7 @@
       <c r="J8" s="7" t="n"/>
       <c r="K8" s="7" t="n"/>
       <c r="L8" s="7" t="n"/>
+      <c r="M8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -840,6 +865,9 @@
       <c r="L9" s="9" t="n">
         <v>52.75</v>
       </c>
+      <c r="M9" s="9" t="n">
+        <v>52.7</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -877,6 +905,9 @@
       </c>
       <c r="L10" s="9" t="n">
         <v>4560.67</v>
+      </c>
+      <c r="M10" s="9" t="n">
+        <v>4543.93</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -892,6 +923,7 @@
       <c r="J11" s="7" t="n"/>
       <c r="K11" s="7" t="n"/>
       <c r="L11" s="7" t="n"/>
+      <c r="M11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -930,6 +962,9 @@
       <c r="L12" s="9" t="n">
         <v>55.87</v>
       </c>
+      <c r="M12" s="9" t="n">
+        <v>55.62</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -967,6 +1002,9 @@
       </c>
       <c r="L13" s="9" t="n">
         <v>7086.13</v>
+      </c>
+      <c r="M13" s="9" t="n">
+        <v>7021.22</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -982,6 +1020,7 @@
       <c r="J14" s="7" t="n"/>
       <c r="K14" s="7" t="n"/>
       <c r="L14" s="7" t="n"/>
+      <c r="M14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1020,6 +1059,9 @@
       <c r="L15" s="9" t="n">
         <v>26.18</v>
       </c>
+      <c r="M15" s="9" t="n">
+        <v>26.32</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1057,6 +1099,9 @@
       </c>
       <c r="L16" s="9" t="n">
         <v>2668.8</v>
+      </c>
+      <c r="M16" s="9" t="n">
+        <v>2650.37</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1072,6 +1117,7 @@
       <c r="J17" s="7" t="n"/>
       <c r="K17" s="7" t="n"/>
       <c r="L17" s="7" t="n"/>
+      <c r="M17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1110,6 +1156,9 @@
       <c r="L18" s="9" t="n">
         <v>96.8</v>
       </c>
+      <c r="M18" s="9" t="n">
+        <v>96.81</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1147,6 +1196,9 @@
       </c>
       <c r="L19" s="9" t="n">
         <v>6849.09</v>
+      </c>
+      <c r="M19" s="9" t="n">
+        <v>6849.72</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1162,6 +1214,7 @@
       <c r="J20" s="7" t="n"/>
       <c r="K20" s="7" t="n"/>
       <c r="L20" s="7" t="n"/>
+      <c r="M20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1200,6 +1253,9 @@
       <c r="L21" s="9" t="n">
         <v>70.09999999999999</v>
       </c>
+      <c r="M21" s="9" t="n">
+        <v>67.97</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1237,6 +1293,9 @@
       </c>
       <c r="L22" s="9" t="n">
         <v>86034.03999999999</v>
+      </c>
+      <c r="M22" s="9" t="n">
+        <v>85013.82000000001</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1252,6 +1311,7 @@
       <c r="J23" s="7" t="n"/>
       <c r="K23" s="7" t="n"/>
       <c r="L23" s="7" t="n"/>
+      <c r="M23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1290,6 +1350,9 @@
       <c r="L24" s="9" t="n">
         <v>83.29000000000001</v>
       </c>
+      <c r="M24" s="9" t="n">
+        <v>83.04000000000001</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1327,6 +1390,9 @@
       </c>
       <c r="L25" s="9" t="n">
         <v>23836.79</v>
+      </c>
+      <c r="M25" s="9" t="n">
+        <v>23690.46</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1342,6 +1408,7 @@
       <c r="J26" s="7" t="n"/>
       <c r="K26" s="7" t="n"/>
       <c r="L26" s="7" t="n"/>
+      <c r="M26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1380,6 +1447,9 @@
       <c r="L27" s="9" t="n">
         <v>70.06999999999999</v>
       </c>
+      <c r="M27" s="9" t="n">
+        <v>68.17</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1417,6 +1487,9 @@
       </c>
       <c r="L28" s="9" t="n">
         <v>49371.8</v>
+      </c>
+      <c r="M28" s="9" t="n">
+        <v>50680.09</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1432,6 +1505,7 @@
       <c r="J29" s="7" t="n"/>
       <c r="K29" s="7" t="n"/>
       <c r="L29" s="7" t="n"/>
+      <c r="M29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1470,6 +1544,9 @@
       <c r="L30" s="9" t="n">
         <v>47.96</v>
       </c>
+      <c r="M30" s="9" t="n">
+        <v>47.41</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1507,6 +1584,9 @@
       </c>
       <c r="L31" s="9" t="n">
         <v>5579.25</v>
+      </c>
+      <c r="M31" s="9" t="n">
+        <v>5565.69</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1522,6 +1602,7 @@
       <c r="J32" s="7" t="n"/>
       <c r="K32" s="7" t="n"/>
       <c r="L32" s="7" t="n"/>
+      <c r="M32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1560,6 +1641,9 @@
       <c r="L33" s="9" t="n">
         <v>9.81</v>
       </c>
+      <c r="M33" s="9" t="n">
+        <v>8.720000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1597,6 +1681,9 @@
       </c>
       <c r="L34" s="9" t="n">
         <v>31672.68</v>
+      </c>
+      <c r="M34" s="9" t="n">
+        <v>31332.8</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1612,6 +1699,7 @@
       <c r="J35" s="7" t="n"/>
       <c r="K35" s="7" t="n"/>
       <c r="L35" s="7" t="n"/>
+      <c r="M35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1650,6 +1738,9 @@
       <c r="L36" s="9" t="n">
         <v>27.05</v>
       </c>
+      <c r="M36" s="9" t="n">
+        <v>26.95</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1687,6 +1778,9 @@
       </c>
       <c r="L37" s="9" t="n">
         <v>3253.68</v>
+      </c>
+      <c r="M37" s="9" t="n">
+        <v>3243.38</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1702,6 +1796,7 @@
       <c r="J38" s="7" t="n"/>
       <c r="K38" s="7" t="n"/>
       <c r="L38" s="7" t="n"/>
+      <c r="M38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1740,6 +1835,9 @@
       <c r="L39" s="9" t="n">
         <v>41.87</v>
       </c>
+      <c r="M39" s="9" t="n">
+        <v>41.57</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1777,6 +1875,9 @@
       </c>
       <c r="L40" s="9" t="n">
         <v>3080.16</v>
+      </c>
+      <c r="M40" s="9" t="n">
+        <v>3059.76</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1792,6 +1893,7 @@
       <c r="J41" s="7" t="n"/>
       <c r="K41" s="7" t="n"/>
       <c r="L41" s="7" t="n"/>
+      <c r="M41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1830,6 +1932,9 @@
       <c r="L42" s="9" t="n">
         <v>15.21</v>
       </c>
+      <c r="M42" s="9" t="n">
+        <v>13.87</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1867,6 +1972,9 @@
       </c>
       <c r="L43" s="9" t="n">
         <v>6938.26</v>
+      </c>
+      <c r="M43" s="9" t="n">
+        <v>6793.08</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1882,6 +1990,7 @@
       <c r="J44" s="7" t="n"/>
       <c r="K44" s="7" t="n"/>
       <c r="L44" s="7" t="n"/>
+      <c r="M44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -1920,6 +2029,9 @@
       <c r="L45" s="9" t="n">
         <v>27.4</v>
       </c>
+      <c r="M45" s="9" t="n">
+        <v>25.75</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -1957,6 +2069,9 @@
       </c>
       <c r="L46" s="9" t="n">
         <v>8493.969999999999</v>
+      </c>
+      <c r="M46" s="9" t="n">
+        <v>8377.370000000001</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1972,6 +2087,7 @@
       <c r="J47" s="7" t="n"/>
       <c r="K47" s="7" t="n"/>
       <c r="L47" s="7" t="n"/>
+      <c r="M47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2010,6 +2126,9 @@
       <c r="L48" s="9" t="n">
         <v>11.99</v>
       </c>
+      <c r="M48" s="9" t="n">
+        <v>11.15</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2047,6 +2166,9 @@
       </c>
       <c r="L49" s="9" t="n">
         <v>12878.04</v>
+      </c>
+      <c r="M49" s="9" t="n">
+        <v>12750.41</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2062,6 +2184,7 @@
       <c r="J50" s="7" t="n"/>
       <c r="K50" s="7" t="n"/>
       <c r="L50" s="7" t="n"/>
+      <c r="M50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2100,6 +2223,9 @@
       <c r="L51" s="9" t="n">
         <v>24.66</v>
       </c>
+      <c r="M51" s="9" t="n">
+        <v>26.15</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2137,6 +2263,9 @@
       </c>
       <c r="L52" s="9" t="n">
         <v>12411.4</v>
+      </c>
+      <c r="M52" s="9" t="n">
+        <v>12535.16</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2152,6 +2281,7 @@
       <c r="J53" s="7" t="n"/>
       <c r="K53" s="7" t="n"/>
       <c r="L53" s="7" t="n"/>
+      <c r="M53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2190,6 +2320,9 @@
       <c r="L54" s="9" t="n">
         <v>21.94</v>
       </c>
+      <c r="M54" s="9" t="n">
+        <v>20.48</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2227,6 +2360,9 @@
       </c>
       <c r="L55" s="9" t="n">
         <v>9682.030000000001</v>
+      </c>
+      <c r="M55" s="9" t="n">
+        <v>9241.42</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -2242,6 +2378,7 @@
       <c r="J56" s="7" t="n"/>
       <c r="K56" s="7" t="n"/>
       <c r="L56" s="7" t="n"/>
+      <c r="M56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2280,6 +2417,9 @@
       <c r="L57" s="9" t="n">
         <v>26.83</v>
       </c>
+      <c r="M57" s="9" t="n">
+        <v>26.14</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2317,6 +2457,9 @@
       </c>
       <c r="L58" s="9" t="n">
         <v>16031.85</v>
+      </c>
+      <c r="M58" s="9" t="n">
+        <v>15665.58</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -2332,6 +2475,7 @@
       <c r="J59" s="7" t="n"/>
       <c r="K59" s="7" t="n"/>
       <c r="L59" s="7" t="n"/>
+      <c r="M59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2370,6 +2514,9 @@
       <c r="L60" s="9" t="n">
         <v>31.41</v>
       </c>
+      <c r="M60" s="9" t="n">
+        <v>30.91</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -2406,6 +2553,9 @@
         <v>17526.85</v>
       </c>
       <c r="L61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="M61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -2422,6 +2572,7 @@
       <c r="J62" s="7" t="n"/>
       <c r="K62" s="7" t="n"/>
       <c r="L62" s="7" t="n"/>
+      <c r="M62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -2460,6 +2611,9 @@
       <c r="L63" s="9" t="n">
         <v>21.04</v>
       </c>
+      <c r="M63" s="9" t="n">
+        <v>20.86</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2497,6 +2651,9 @@
       </c>
       <c r="L64" s="9" t="n">
         <v>9801.49</v>
+      </c>
+      <c r="M64" s="9" t="n">
+        <v>9688.4</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -2512,6 +2669,7 @@
       <c r="J65" s="7" t="n"/>
       <c r="K65" s="7" t="n"/>
       <c r="L65" s="7" t="n"/>
+      <c r="M65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -2550,6 +2708,9 @@
       <c r="L66" s="9" t="n">
         <v>14.17</v>
       </c>
+      <c r="M66" s="9" t="n">
+        <v>15.29</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -2587,6 +2748,9 @@
       </c>
       <c r="L67" s="9" t="n">
         <v>9889.290000000001</v>
+      </c>
+      <c r="M67" s="9" t="n">
+        <v>9913.360000000001</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -2602,6 +2766,7 @@
       <c r="J68" s="7" t="n"/>
       <c r="K68" s="7" t="n"/>
       <c r="L68" s="7" t="n"/>
+      <c r="M68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -2640,6 +2805,9 @@
       <c r="L69" s="9" t="n">
         <v>23.72</v>
       </c>
+      <c r="M69" s="9" t="n">
+        <v>23.61</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -2677,6 +2845,9 @@
       </c>
       <c r="L70" s="9" t="n">
         <v>3020.73</v>
+      </c>
+      <c r="M70" s="9" t="n">
+        <v>2963.64</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -2692,6 +2863,7 @@
       <c r="J71" s="7" t="n"/>
       <c r="K71" s="7" t="n"/>
       <c r="L71" s="7" t="n"/>
+      <c r="M71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2730,6 +2902,9 @@
       <c r="L72" s="9" t="n">
         <v>41.98</v>
       </c>
+      <c r="M72" s="9" t="n">
+        <v>45.64</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2767,6 +2942,9 @@
       </c>
       <c r="L73" s="9" t="n">
         <v>5654.62</v>
+      </c>
+      <c r="M73" s="9" t="n">
+        <v>5567.23</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -2782,6 +2960,7 @@
       <c r="J74" s="7" t="n"/>
       <c r="K74" s="7" t="n"/>
       <c r="L74" s="7" t="n"/>
+      <c r="M74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -2820,6 +2999,9 @@
       <c r="L75" s="9" t="n">
         <v>25.24</v>
       </c>
+      <c r="M75" s="9" t="n">
+        <v>24.15</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -2857,6 +3039,9 @@
       </c>
       <c r="L76" s="9" t="n">
         <v>9059.16</v>
+      </c>
+      <c r="M76" s="9" t="n">
+        <v>8970.639999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -2872,6 +3057,7 @@
       <c r="J77" s="7" t="n"/>
       <c r="K77" s="7" t="n"/>
       <c r="L77" s="7" t="n"/>
+      <c r="M77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -2910,6 +3096,9 @@
       <c r="L78" s="9" t="n">
         <v>13.37</v>
       </c>
+      <c r="M78" s="9" t="n">
+        <v>13.3</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -2947,6 +3136,9 @@
       </c>
       <c r="L79" s="9" t="n">
         <v>1314.12</v>
+      </c>
+      <c r="M79" s="9" t="n">
+        <v>1300.67</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -2962,6 +3154,7 @@
       <c r="J80" s="7" t="n"/>
       <c r="K80" s="7" t="n"/>
       <c r="L80" s="7" t="n"/>
+      <c r="M80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3000,6 +3193,9 @@
       <c r="L81" s="9" t="n">
         <v>54.83</v>
       </c>
+      <c r="M81" s="9" t="n">
+        <v>54.33</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -3037,6 +3233,9 @@
       </c>
       <c r="L82" s="9" t="n">
         <v>2790.31</v>
+      </c>
+      <c r="M82" s="9" t="n">
+        <v>2722.85</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -3052,6 +3251,7 @@
       <c r="J83" s="7" t="n"/>
       <c r="K83" s="7" t="n"/>
       <c r="L83" s="7" t="n"/>
+      <c r="M83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -3090,6 +3290,9 @@
       <c r="L84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="M84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -3127,6 +3330,9 @@
       </c>
       <c r="L85" s="9" t="n">
         <v>2840.93</v>
+      </c>
+      <c r="M85" s="9" t="n">
+        <v>2775.2</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -3142,6 +3348,7 @@
       <c r="J86" s="7" t="n"/>
       <c r="K86" s="7" t="n"/>
       <c r="L86" s="7" t="n"/>
+      <c r="M86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -3180,6 +3387,9 @@
       <c r="L87" s="9" t="n">
         <v>50.6</v>
       </c>
+      <c r="M87" s="9" t="n">
+        <v>49.89</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -3217,6 +3427,9 @@
       </c>
       <c r="L88" s="9" t="n">
         <v>2928.92</v>
+      </c>
+      <c r="M88" s="9" t="n">
+        <v>2848.93</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -3232,6 +3445,7 @@
       <c r="J89" s="7" t="n"/>
       <c r="K89" s="7" t="n"/>
       <c r="L89" s="7" t="n"/>
+      <c r="M89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -3270,6 +3484,9 @@
       <c r="L90" s="9" t="n">
         <v>43.61</v>
       </c>
+      <c r="M90" s="9" t="n">
+        <v>42.21</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -3307,6 +3524,9 @@
       </c>
       <c r="L91" s="9" t="n">
         <v>1991.37</v>
+      </c>
+      <c r="M91" s="9" t="n">
+        <v>1969.04</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -3322,6 +3542,7 @@
       <c r="J92" s="7" t="n"/>
       <c r="K92" s="7" t="n"/>
       <c r="L92" s="7" t="n"/>
+      <c r="M92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -3360,6 +3581,9 @@
       <c r="L93" s="9" t="n">
         <v>27.39</v>
       </c>
+      <c r="M93" s="9" t="n">
+        <v>27.15</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -3397,6 +3621,9 @@
       </c>
       <c r="L94" s="9" t="n">
         <v>13621.38</v>
+      </c>
+      <c r="M94" s="9" t="n">
+        <v>13370.57</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -3412,6 +3639,7 @@
       <c r="J95" s="7" t="n"/>
       <c r="K95" s="7" t="n"/>
       <c r="L95" s="7" t="n"/>
+      <c r="M95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -3450,6 +3678,9 @@
       <c r="L96" s="9" t="n">
         <v>84.64</v>
       </c>
+      <c r="M96" s="9" t="n">
+        <v>84.25</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -3487,6 +3718,9 @@
       </c>
       <c r="L97" s="9" t="n">
         <v>8856.049999999999</v>
+      </c>
+      <c r="M97" s="9" t="n">
+        <v>8816.51</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -3502,6 +3736,7 @@
       <c r="J98" s="7" t="n"/>
       <c r="K98" s="7" t="n"/>
       <c r="L98" s="7" t="n"/>
+      <c r="M98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -3540,6 +3775,9 @@
       <c r="L99" s="9" t="n">
         <v>56.22</v>
       </c>
+      <c r="M99" s="9" t="n">
+        <v>55.75</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -3577,6 +3815,9 @@
       </c>
       <c r="L100" s="9" t="n">
         <v>12114.87</v>
+      </c>
+      <c r="M100" s="9" t="n">
+        <v>12001.13</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -3592,6 +3833,7 @@
       <c r="J101" s="7" t="n"/>
       <c r="K101" s="7" t="n"/>
       <c r="L101" s="7" t="n"/>
+      <c r="M101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -3630,6 +3872,9 @@
       <c r="L102" s="9" t="n">
         <v>5.82</v>
       </c>
+      <c r="M102" s="9" t="n">
+        <v>5.45</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -3667,6 +3912,9 @@
       </c>
       <c r="L103" s="9" t="n">
         <v>2228.44</v>
+      </c>
+      <c r="M103" s="9" t="n">
+        <v>2203.91</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -3682,6 +3930,7 @@
       <c r="J104" s="7" t="n"/>
       <c r="K104" s="7" t="n"/>
       <c r="L104" s="7" t="n"/>
+      <c r="M104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -3720,6 +3969,9 @@
       <c r="L105" s="9" t="n">
         <v>25.23</v>
       </c>
+      <c r="M105" s="9" t="n">
+        <v>25.06</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -3757,6 +4009,9 @@
       </c>
       <c r="L106" s="9" t="n">
         <v>831.99</v>
+      </c>
+      <c r="M106" s="9" t="n">
+        <v>821.28</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -3772,6 +4027,7 @@
       <c r="J107" s="7" t="n"/>
       <c r="K107" s="7" t="n"/>
       <c r="L107" s="7" t="n"/>
+      <c r="M107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -3810,6 +4066,9 @@
       <c r="L108" s="9" t="n">
         <v>29.4</v>
       </c>
+      <c r="M108" s="9" t="n">
+        <v>29.69</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -3847,6 +4106,9 @@
       </c>
       <c r="L109" s="9" t="n">
         <v>2817.43</v>
+      </c>
+      <c r="M109" s="9" t="n">
+        <v>2814.53</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -3862,6 +4124,7 @@
       <c r="J110" s="7" t="n"/>
       <c r="K110" s="7" t="n"/>
       <c r="L110" s="7" t="n"/>
+      <c r="M110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -3900,6 +4163,9 @@
       <c r="L111" s="9" t="n">
         <v>20.15</v>
       </c>
+      <c r="M111" s="9" t="n">
+        <v>20.22</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -3937,6 +4203,9 @@
       </c>
       <c r="L112" s="9" t="n">
         <v>3859.53</v>
+      </c>
+      <c r="M112" s="9" t="n">
+        <v>3853.83</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -3952,6 +4221,7 @@
       <c r="J113" s="7" t="n"/>
       <c r="K113" s="7" t="n"/>
       <c r="L113" s="7" t="n"/>
+      <c r="M113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -3990,6 +4260,9 @@
       <c r="L114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="M114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -4027,6 +4300,9 @@
       </c>
       <c r="L115" s="9" t="n">
         <v>3227.35</v>
+      </c>
+      <c r="M115" s="9" t="n">
+        <v>3174.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-08 04:16:58]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -498,6 +498,7 @@
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
     <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -566,6 +567,7 @@
           <t>2025/12/04</t>
         </is>
       </c>
+      <c r="N1" s="7" t="n"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -633,6 +635,7 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="N2" s="8" t="n"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -674,6 +677,9 @@
       <c r="M3" s="9" t="n">
         <v>60.89</v>
       </c>
+      <c r="N3" s="9" t="n">
+        <v>61.44</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -715,6 +721,7 @@
       <c r="M4" s="9" t="n">
         <v>3879.52</v>
       </c>
+      <c r="N4" s="7" t="n"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="n"/>
@@ -730,6 +737,7 @@
       <c r="K5" s="7" t="n"/>
       <c r="L5" s="7" t="n"/>
       <c r="M5" s="7" t="n"/>
+      <c r="N5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -771,6 +779,9 @@
       <c r="M6" s="9" t="n">
         <v>47.64</v>
       </c>
+      <c r="N6" s="9" t="n">
+        <v>48.52</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -812,6 +823,7 @@
       <c r="M7" s="9" t="n">
         <v>5458.54</v>
       </c>
+      <c r="N7" s="7" t="n"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="n"/>
@@ -827,6 +839,7 @@
       <c r="K8" s="7" t="n"/>
       <c r="L8" s="7" t="n"/>
       <c r="M8" s="7" t="n"/>
+      <c r="N8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -868,6 +881,9 @@
       <c r="M9" s="9" t="n">
         <v>52.7</v>
       </c>
+      <c r="N9" s="9" t="n">
+        <v>53.14</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -909,6 +925,7 @@
       <c r="M10" s="9" t="n">
         <v>4543.93</v>
       </c>
+      <c r="N10" s="7" t="n"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="n"/>
@@ -924,6 +941,7 @@
       <c r="K11" s="7" t="n"/>
       <c r="L11" s="7" t="n"/>
       <c r="M11" s="7" t="n"/>
+      <c r="N11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -965,6 +983,9 @@
       <c r="M12" s="9" t="n">
         <v>55.62</v>
       </c>
+      <c r="N12" s="9" t="n">
+        <v>56.3</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1006,6 +1027,7 @@
       <c r="M13" s="9" t="n">
         <v>7021.22</v>
       </c>
+      <c r="N13" s="7" t="n"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="1" t="n"/>
@@ -1021,6 +1043,7 @@
       <c r="K14" s="7" t="n"/>
       <c r="L14" s="7" t="n"/>
       <c r="M14" s="7" t="n"/>
+      <c r="N14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1062,6 +1085,9 @@
       <c r="M15" s="9" t="n">
         <v>26.32</v>
       </c>
+      <c r="N15" s="9" t="n">
+        <v>27.02</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1102,6 +1128,9 @@
       </c>
       <c r="M16" s="9" t="n">
         <v>2650.37</v>
+      </c>
+      <c r="N16" s="9" t="n">
+        <v>2676.69</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1118,6 +1147,7 @@
       <c r="K17" s="7" t="n"/>
       <c r="L17" s="7" t="n"/>
       <c r="M17" s="7" t="n"/>
+      <c r="N17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1159,6 +1189,9 @@
       <c r="M18" s="9" t="n">
         <v>96.81</v>
       </c>
+      <c r="N18" s="9" t="n">
+        <v>96.93000000000001</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1200,6 +1233,7 @@
       <c r="M19" s="9" t="n">
         <v>6849.72</v>
       </c>
+      <c r="N19" s="7" t="n"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="1" t="n"/>
@@ -1215,6 +1249,7 @@
       <c r="K20" s="7" t="n"/>
       <c r="L20" s="7" t="n"/>
       <c r="M20" s="7" t="n"/>
+      <c r="N20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1256,6 +1291,9 @@
       <c r="M21" s="9" t="n">
         <v>67.97</v>
       </c>
+      <c r="N21" s="9" t="n">
+        <v>70.16</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1296,6 +1334,9 @@
       </c>
       <c r="M22" s="9" t="n">
         <v>85013.82000000001</v>
+      </c>
+      <c r="N22" s="9" t="n">
+        <v>85693.36</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1312,6 +1353,7 @@
       <c r="K23" s="7" t="n"/>
       <c r="L23" s="7" t="n"/>
       <c r="M23" s="7" t="n"/>
+      <c r="N23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1353,6 +1395,9 @@
       <c r="M24" s="9" t="n">
         <v>83.04000000000001</v>
       </c>
+      <c r="N24" s="9" t="n">
+        <v>83.66</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1393,6 +1438,9 @@
       </c>
       <c r="M25" s="9" t="n">
         <v>23690.46</v>
+      </c>
+      <c r="N25" s="9" t="n">
+        <v>24028.14</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1409,6 +1457,7 @@
       <c r="K26" s="7" t="n"/>
       <c r="L26" s="7" t="n"/>
       <c r="M26" s="7" t="n"/>
+      <c r="N26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1450,6 +1499,9 @@
       <c r="M27" s="9" t="n">
         <v>68.17</v>
       </c>
+      <c r="N27" s="9" t="n">
+        <v>71.53</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1490,6 +1542,9 @@
       </c>
       <c r="M28" s="9" t="n">
         <v>50680.09</v>
+      </c>
+      <c r="N28" s="9" t="n">
+        <v>50393.2</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1506,6 +1561,7 @@
       <c r="K29" s="7" t="n"/>
       <c r="L29" s="7" t="n"/>
       <c r="M29" s="7" t="n"/>
+      <c r="N29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1547,6 +1603,9 @@
       <c r="M30" s="9" t="n">
         <v>47.41</v>
       </c>
+      <c r="N30" s="9" t="n">
+        <v>47.6</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1588,6 +1647,7 @@
       <c r="M31" s="9" t="n">
         <v>5565.69</v>
       </c>
+      <c r="N31" s="7" t="n"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="1" t="n"/>
@@ -1603,6 +1663,7 @@
       <c r="K32" s="7" t="n"/>
       <c r="L32" s="7" t="n"/>
       <c r="M32" s="7" t="n"/>
+      <c r="N32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1644,6 +1705,9 @@
       <c r="M33" s="9" t="n">
         <v>8.720000000000001</v>
       </c>
+      <c r="N33" s="9" t="n">
+        <v>8.710000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1684,6 +1748,9 @@
       </c>
       <c r="M34" s="9" t="n">
         <v>31332.8</v>
+      </c>
+      <c r="N34" s="9" t="n">
+        <v>31543.5</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1700,6 +1767,7 @@
       <c r="K35" s="7" t="n"/>
       <c r="L35" s="7" t="n"/>
       <c r="M35" s="7" t="n"/>
+      <c r="N35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1741,6 +1809,9 @@
       <c r="M36" s="9" t="n">
         <v>26.95</v>
       </c>
+      <c r="N36" s="9" t="n">
+        <v>28.09</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1782,6 +1853,7 @@
       <c r="M37" s="9" t="n">
         <v>3243.38</v>
       </c>
+      <c r="N37" s="7" t="n"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="n"/>
@@ -1797,6 +1869,7 @@
       <c r="K38" s="7" t="n"/>
       <c r="L38" s="7" t="n"/>
       <c r="M38" s="7" t="n"/>
+      <c r="N38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1838,6 +1911,9 @@
       <c r="M39" s="9" t="n">
         <v>41.57</v>
       </c>
+      <c r="N39" s="9" t="n">
+        <v>42.67</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1879,6 +1955,7 @@
       <c r="M40" s="9" t="n">
         <v>3059.76</v>
       </c>
+      <c r="N40" s="7" t="n"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1" t="n"/>
@@ -1894,6 +1971,7 @@
       <c r="K41" s="7" t="n"/>
       <c r="L41" s="7" t="n"/>
       <c r="M41" s="7" t="n"/>
+      <c r="N41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -1935,6 +2013,9 @@
       <c r="M42" s="9" t="n">
         <v>13.87</v>
       </c>
+      <c r="N42" s="9" t="n">
+        <v>14.57</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -1976,6 +2057,7 @@
       <c r="M43" s="9" t="n">
         <v>6793.08</v>
       </c>
+      <c r="N43" s="7" t="n"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="n"/>
@@ -1991,6 +2073,7 @@
       <c r="K44" s="7" t="n"/>
       <c r="L44" s="7" t="n"/>
       <c r="M44" s="7" t="n"/>
+      <c r="N44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2032,6 +2115,9 @@
       <c r="M45" s="9" t="n">
         <v>25.75</v>
       </c>
+      <c r="N45" s="9" t="n">
+        <v>26.52</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2073,6 +2159,7 @@
       <c r="M46" s="9" t="n">
         <v>8377.370000000001</v>
       </c>
+      <c r="N46" s="7" t="n"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="1" t="n"/>
@@ -2088,6 +2175,7 @@
       <c r="K47" s="7" t="n"/>
       <c r="L47" s="7" t="n"/>
       <c r="M47" s="7" t="n"/>
+      <c r="N47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2129,6 +2217,9 @@
       <c r="M48" s="9" t="n">
         <v>11.15</v>
       </c>
+      <c r="N48" s="9" t="n">
+        <v>10.82</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2169,6 +2260,9 @@
       </c>
       <c r="M49" s="9" t="n">
         <v>12750.41</v>
+      </c>
+      <c r="N49" s="9" t="n">
+        <v>12705.92</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2185,6 +2279,7 @@
       <c r="K50" s="7" t="n"/>
       <c r="L50" s="7" t="n"/>
       <c r="M50" s="7" t="n"/>
+      <c r="N50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2226,6 +2321,9 @@
       <c r="M51" s="9" t="n">
         <v>26.15</v>
       </c>
+      <c r="N51" s="9" t="n">
+        <v>26.8</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2266,6 +2364,9 @@
       </c>
       <c r="M52" s="9" t="n">
         <v>12535.16</v>
+      </c>
+      <c r="N52" s="9" t="n">
+        <v>12578.17</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2282,6 +2383,7 @@
       <c r="K53" s="7" t="n"/>
       <c r="L53" s="7" t="n"/>
       <c r="M53" s="7" t="n"/>
+      <c r="N53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2323,6 +2425,9 @@
       <c r="M54" s="9" t="n">
         <v>20.48</v>
       </c>
+      <c r="N54" s="9" t="n">
+        <v>20.07</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2364,6 +2469,7 @@
       <c r="M55" s="9" t="n">
         <v>9241.42</v>
       </c>
+      <c r="N55" s="7" t="n"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="n"/>
@@ -2379,6 +2485,7 @@
       <c r="K56" s="7" t="n"/>
       <c r="L56" s="7" t="n"/>
       <c r="M56" s="7" t="n"/>
+      <c r="N56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2420,6 +2527,9 @@
       <c r="M57" s="9" t="n">
         <v>26.14</v>
       </c>
+      <c r="N57" s="9" t="n">
+        <v>25.91</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2461,6 +2571,7 @@
       <c r="M58" s="9" t="n">
         <v>15665.58</v>
       </c>
+      <c r="N58" s="7" t="n"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1" t="n"/>
@@ -2476,6 +2587,7 @@
       <c r="K59" s="7" t="n"/>
       <c r="L59" s="7" t="n"/>
       <c r="M59" s="7" t="n"/>
+      <c r="N59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2517,6 +2629,9 @@
       <c r="M60" s="9" t="n">
         <v>30.91</v>
       </c>
+      <c r="N60" s="9" t="n">
+        <v>31.54</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -2556,6 +2671,9 @@
         <v>17526.85</v>
       </c>
       <c r="M61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="N61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -2573,6 +2691,7 @@
       <c r="K62" s="7" t="n"/>
       <c r="L62" s="7" t="n"/>
       <c r="M62" s="7" t="n"/>
+      <c r="N62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -2614,6 +2733,9 @@
       <c r="M63" s="9" t="n">
         <v>20.86</v>
       </c>
+      <c r="N63" s="9" t="n">
+        <v>21.53</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2654,6 +2776,9 @@
       </c>
       <c r="M64" s="9" t="n">
         <v>9688.4</v>
+      </c>
+      <c r="N64" s="9" t="n">
+        <v>9733</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -2670,6 +2795,7 @@
       <c r="K65" s="7" t="n"/>
       <c r="L65" s="7" t="n"/>
       <c r="M65" s="7" t="n"/>
+      <c r="N65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -2711,6 +2837,9 @@
       <c r="M66" s="9" t="n">
         <v>15.29</v>
       </c>
+      <c r="N66" s="9" t="n">
+        <v>14.56</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -2751,6 +2880,9 @@
       </c>
       <c r="M67" s="9" t="n">
         <v>9913.360000000001</v>
+      </c>
+      <c r="N67" s="9" t="n">
+        <v>9849.84</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -2767,6 +2899,7 @@
       <c r="K68" s="7" t="n"/>
       <c r="L68" s="7" t="n"/>
       <c r="M68" s="7" t="n"/>
+      <c r="N68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -2808,6 +2941,9 @@
       <c r="M69" s="9" t="n">
         <v>23.61</v>
       </c>
+      <c r="N69" s="9" t="n">
+        <v>23.91</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -2848,6 +2984,9 @@
       </c>
       <c r="M70" s="9" t="n">
         <v>2963.64</v>
+      </c>
+      <c r="N70" s="9" t="n">
+        <v>2996.79</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -2864,6 +3003,7 @@
       <c r="K71" s="7" t="n"/>
       <c r="L71" s="7" t="n"/>
       <c r="M71" s="7" t="n"/>
+      <c r="N71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -2905,6 +3045,9 @@
       <c r="M72" s="9" t="n">
         <v>45.64</v>
       </c>
+      <c r="N72" s="9" t="n">
+        <v>46.75</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -2945,6 +3088,9 @@
       </c>
       <c r="M73" s="9" t="n">
         <v>5567.23</v>
+      </c>
+      <c r="N73" s="9" t="n">
+        <v>5649</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -2961,6 +3107,7 @@
       <c r="K74" s="7" t="n"/>
       <c r="L74" s="7" t="n"/>
       <c r="M74" s="7" t="n"/>
+      <c r="N74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3002,6 +3149,9 @@
       <c r="M75" s="9" t="n">
         <v>24.15</v>
       </c>
+      <c r="N75" s="9" t="n">
+        <v>25.12</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3043,6 +3193,7 @@
       <c r="M76" s="9" t="n">
         <v>8970.639999999999</v>
       </c>
+      <c r="N76" s="7" t="n"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="1" t="n"/>
@@ -3058,6 +3209,7 @@
       <c r="K77" s="7" t="n"/>
       <c r="L77" s="7" t="n"/>
       <c r="M77" s="7" t="n"/>
+      <c r="N77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3099,6 +3251,9 @@
       <c r="M78" s="9" t="n">
         <v>13.3</v>
       </c>
+      <c r="N78" s="9" t="n">
+        <v>14.23</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3139,6 +3294,9 @@
       </c>
       <c r="M79" s="9" t="n">
         <v>1300.67</v>
+      </c>
+      <c r="N79" s="9" t="n">
+        <v>1380.92</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -3155,6 +3313,7 @@
       <c r="K80" s="7" t="n"/>
       <c r="L80" s="7" t="n"/>
       <c r="M80" s="7" t="n"/>
+      <c r="N80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3196,6 +3355,9 @@
       <c r="M81" s="9" t="n">
         <v>54.33</v>
       </c>
+      <c r="N81" s="9" t="n">
+        <v>54.87</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -3237,6 +3399,7 @@
       <c r="M82" s="9" t="n">
         <v>2722.85</v>
       </c>
+      <c r="N82" s="7" t="n"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="1" t="n"/>
@@ -3252,6 +3415,7 @@
       <c r="K83" s="7" t="n"/>
       <c r="L83" s="7" t="n"/>
       <c r="M83" s="7" t="n"/>
+      <c r="N83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -3293,6 +3457,9 @@
       <c r="M84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="N84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -3333,6 +3500,9 @@
       </c>
       <c r="M85" s="9" t="n">
         <v>2775.2</v>
+      </c>
+      <c r="N85" s="9" t="n">
+        <v>2878.39</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -3349,6 +3519,7 @@
       <c r="K86" s="7" t="n"/>
       <c r="L86" s="7" t="n"/>
       <c r="M86" s="7" t="n"/>
+      <c r="N86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -3390,6 +3561,9 @@
       <c r="M87" s="9" t="n">
         <v>49.89</v>
       </c>
+      <c r="N87" s="9" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -3430,6 +3604,9 @@
       </c>
       <c r="M88" s="9" t="n">
         <v>2848.93</v>
+      </c>
+      <c r="N88" s="9" t="n">
+        <v>2890.69</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -3446,6 +3623,7 @@
       <c r="K89" s="7" t="n"/>
       <c r="L89" s="7" t="n"/>
       <c r="M89" s="7" t="n"/>
+      <c r="N89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -3487,6 +3665,9 @@
       <c r="M90" s="9" t="n">
         <v>42.21</v>
       </c>
+      <c r="N90" s="9" t="n">
+        <v>43.28</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -3527,6 +3708,9 @@
       </c>
       <c r="M91" s="9" t="n">
         <v>1969.04</v>
+      </c>
+      <c r="N91" s="9" t="n">
+        <v>1978.75</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -3543,6 +3727,7 @@
       <c r="K92" s="7" t="n"/>
       <c r="L92" s="7" t="n"/>
       <c r="M92" s="7" t="n"/>
+      <c r="N92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -3584,6 +3769,9 @@
       <c r="M93" s="9" t="n">
         <v>27.15</v>
       </c>
+      <c r="N93" s="9" t="n">
+        <v>27.25</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -3624,6 +3812,9 @@
       </c>
       <c r="M94" s="9" t="n">
         <v>13370.57</v>
+      </c>
+      <c r="N94" s="9" t="n">
+        <v>13440.18</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -3640,6 +3831,7 @@
       <c r="K95" s="7" t="n"/>
       <c r="L95" s="7" t="n"/>
       <c r="M95" s="7" t="n"/>
+      <c r="N95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -3681,6 +3873,9 @@
       <c r="M96" s="9" t="n">
         <v>84.25</v>
       </c>
+      <c r="N96" s="9" t="n">
+        <v>84.94</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -3721,6 +3916,9 @@
       </c>
       <c r="M97" s="9" t="n">
         <v>8816.51</v>
+      </c>
+      <c r="N97" s="9" t="n">
+        <v>9014.25</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -3737,6 +3935,7 @@
       <c r="K98" s="7" t="n"/>
       <c r="L98" s="7" t="n"/>
       <c r="M98" s="7" t="n"/>
+      <c r="N98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -3778,6 +3977,9 @@
       <c r="M99" s="9" t="n">
         <v>55.75</v>
       </c>
+      <c r="N99" s="9" t="n">
+        <v>56.64</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -3819,6 +4021,7 @@
       <c r="M100" s="9" t="n">
         <v>12001.13</v>
       </c>
+      <c r="N100" s="7" t="n"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="1" t="n"/>
@@ -3834,6 +4037,7 @@
       <c r="K101" s="7" t="n"/>
       <c r="L101" s="7" t="n"/>
       <c r="M101" s="7" t="n"/>
+      <c r="N101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -3875,6 +4079,9 @@
       <c r="M102" s="9" t="n">
         <v>5.45</v>
       </c>
+      <c r="N102" s="9" t="n">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -3915,6 +4122,9 @@
       </c>
       <c r="M103" s="9" t="n">
         <v>2203.91</v>
+      </c>
+      <c r="N103" s="9" t="n">
+        <v>2217.96</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -3931,6 +4141,7 @@
       <c r="K104" s="7" t="n"/>
       <c r="L104" s="7" t="n"/>
       <c r="M104" s="7" t="n"/>
+      <c r="N104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -3972,6 +4183,9 @@
       <c r="M105" s="9" t="n">
         <v>25.06</v>
       </c>
+      <c r="N105" s="9" t="n">
+        <v>25.46</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -4013,6 +4227,7 @@
       <c r="M106" s="9" t="n">
         <v>821.28</v>
       </c>
+      <c r="N106" s="7" t="n"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="1" t="n"/>
@@ -4028,6 +4243,7 @@
       <c r="K107" s="7" t="n"/>
       <c r="L107" s="7" t="n"/>
       <c r="M107" s="7" t="n"/>
+      <c r="N107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -4069,6 +4285,9 @@
       <c r="M108" s="9" t="n">
         <v>29.69</v>
       </c>
+      <c r="N108" s="9" t="n">
+        <v>29.93</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -4109,6 +4328,9 @@
       </c>
       <c r="M109" s="9" t="n">
         <v>2814.53</v>
+      </c>
+      <c r="N109" s="9" t="n">
+        <v>2879.26</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -4125,6 +4347,7 @@
       <c r="K110" s="7" t="n"/>
       <c r="L110" s="7" t="n"/>
       <c r="M110" s="7" t="n"/>
+      <c r="N110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -4166,6 +4389,9 @@
       <c r="M111" s="9" t="n">
         <v>20.22</v>
       </c>
+      <c r="N111" s="9" t="n">
+        <v>20.59</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -4207,6 +4433,7 @@
       <c r="M112" s="9" t="n">
         <v>3853.83</v>
       </c>
+      <c r="N112" s="7" t="n"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="1" t="n"/>
@@ -4222,6 +4449,7 @@
       <c r="K113" s="7" t="n"/>
       <c r="L113" s="7" t="n"/>
       <c r="M113" s="7" t="n"/>
+      <c r="N113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -4263,6 +4491,9 @@
       <c r="M114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="N114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -4304,6 +4535,7 @@
       <c r="M115" s="9" t="n">
         <v>3174.12</v>
       </c>
+      <c r="N115" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-08 04:40:54]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N115"/>
+  <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -499,6 +499,7 @@
     <col width="15" customWidth="1" min="12" max="12"/>
     <col width="15" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="15" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -568,6 +569,11 @@
         </is>
       </c>
       <c r="N1" s="7" t="n"/>
+      <c r="O1" s="7" t="inlineStr">
+        <is>
+          <t>2025/12/08</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -636,6 +642,11 @@
         </is>
       </c>
       <c r="N2" s="8" t="n"/>
+      <c r="O2" s="8" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -680,6 +691,9 @@
       <c r="N3" s="9" t="n">
         <v>61.44</v>
       </c>
+      <c r="O3" s="9" t="n">
+        <v>61.44</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -722,6 +736,9 @@
         <v>3879.52</v>
       </c>
       <c r="N4" s="7" t="n"/>
+      <c r="O4" s="9" t="n">
+        <v>3927.19</v>
+      </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="n"/>
@@ -738,6 +755,7 @@
       <c r="L5" s="7" t="n"/>
       <c r="M5" s="7" t="n"/>
       <c r="N5" s="7" t="n"/>
+      <c r="O5" s="7" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -782,6 +800,9 @@
       <c r="N6" s="9" t="n">
         <v>48.52</v>
       </c>
+      <c r="O6" s="9" t="n">
+        <v>48.52</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -824,6 +845,9 @@
         <v>5458.54</v>
       </c>
       <c r="N7" s="7" t="n"/>
+      <c r="O7" s="9" t="n">
+        <v>5570.34</v>
+      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="n"/>
@@ -840,6 +864,7 @@
       <c r="L8" s="7" t="n"/>
       <c r="M8" s="7" t="n"/>
       <c r="N8" s="7" t="n"/>
+      <c r="O8" s="7" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -884,6 +909,9 @@
       <c r="N9" s="9" t="n">
         <v>53.14</v>
       </c>
+      <c r="O9" s="9" t="n">
+        <v>53.14</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -926,6 +954,9 @@
         <v>4543.93</v>
       </c>
       <c r="N10" s="7" t="n"/>
+      <c r="O10" s="9" t="n">
+        <v>4632.29</v>
+      </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="n"/>
@@ -942,6 +973,7 @@
       <c r="L11" s="7" t="n"/>
       <c r="M11" s="7" t="n"/>
       <c r="N11" s="7" t="n"/>
+      <c r="O11" s="7" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -986,6 +1018,9 @@
       <c r="N12" s="9" t="n">
         <v>56.3</v>
       </c>
+      <c r="O12" s="9" t="n">
+        <v>56.3</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1028,6 +1063,9 @@
         <v>7021.22</v>
       </c>
       <c r="N13" s="7" t="n"/>
+      <c r="O13" s="9" t="n">
+        <v>7168.66</v>
+      </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="1" t="n"/>
@@ -1044,6 +1082,7 @@
       <c r="L14" s="7" t="n"/>
       <c r="M14" s="7" t="n"/>
       <c r="N14" s="7" t="n"/>
+      <c r="O14" s="7" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1088,6 +1127,9 @@
       <c r="N15" s="9" t="n">
         <v>27.02</v>
       </c>
+      <c r="O15" s="9" t="n">
+        <v>27.02</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1130,6 +1172,9 @@
         <v>2650.37</v>
       </c>
       <c r="N16" s="9" t="n">
+        <v>2676.69</v>
+      </c>
+      <c r="O16" s="9" t="n">
         <v>2676.69</v>
       </c>
     </row>
@@ -1148,6 +1193,7 @@
       <c r="L17" s="7" t="n"/>
       <c r="M17" s="7" t="n"/>
       <c r="N17" s="7" t="n"/>
+      <c r="O17" s="7" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1192,6 +1238,9 @@
       <c r="N18" s="9" t="n">
         <v>96.93000000000001</v>
       </c>
+      <c r="O18" s="9" t="n">
+        <v>96.93000000000001</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1234,6 +1283,9 @@
         <v>6849.72</v>
       </c>
       <c r="N19" s="7" t="n"/>
+      <c r="O19" s="9" t="n">
+        <v>6870.4</v>
+      </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="1" t="n"/>
@@ -1250,6 +1302,7 @@
       <c r="L20" s="7" t="n"/>
       <c r="M20" s="7" t="n"/>
       <c r="N20" s="7" t="n"/>
+      <c r="O20" s="7" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1294,6 +1347,9 @@
       <c r="N21" s="9" t="n">
         <v>70.16</v>
       </c>
+      <c r="O21" s="9" t="n">
+        <v>70.16</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1337,6 +1393,9 @@
       </c>
       <c r="N22" s="9" t="n">
         <v>85693.36</v>
+      </c>
+      <c r="O22" s="9" t="n">
+        <v>85430.38</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1354,6 +1413,7 @@
       <c r="L23" s="7" t="n"/>
       <c r="M23" s="7" t="n"/>
       <c r="N23" s="7" t="n"/>
+      <c r="O23" s="7" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1398,6 +1458,9 @@
       <c r="N24" s="9" t="n">
         <v>83.66</v>
       </c>
+      <c r="O24" s="9" t="n">
+        <v>83.66</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1440,6 +1503,9 @@
         <v>23690.46</v>
       </c>
       <c r="N25" s="9" t="n">
+        <v>24028.14</v>
+      </c>
+      <c r="O25" s="9" t="n">
         <v>24028.14</v>
       </c>
     </row>
@@ -1458,6 +1524,7 @@
       <c r="L26" s="7" t="n"/>
       <c r="M26" s="7" t="n"/>
       <c r="N26" s="7" t="n"/>
+      <c r="O26" s="7" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1502,6 +1569,9 @@
       <c r="N27" s="9" t="n">
         <v>71.53</v>
       </c>
+      <c r="O27" s="9" t="n">
+        <v>71.53</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1545,6 +1615,9 @@
       </c>
       <c r="N28" s="9" t="n">
         <v>50393.2</v>
+      </c>
+      <c r="O28" s="9" t="n">
+        <v>50505.55</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1562,6 +1635,7 @@
       <c r="L29" s="7" t="n"/>
       <c r="M29" s="7" t="n"/>
       <c r="N29" s="7" t="n"/>
+      <c r="O29" s="7" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1606,6 +1680,9 @@
       <c r="N30" s="9" t="n">
         <v>47.6</v>
       </c>
+      <c r="O30" s="9" t="n">
+        <v>47.6</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1648,6 +1725,9 @@
         <v>5565.69</v>
       </c>
       <c r="N31" s="7" t="n"/>
+      <c r="O31" s="9" t="n">
+        <v>5531.62</v>
+      </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="1" t="n"/>
@@ -1664,6 +1744,7 @@
       <c r="L32" s="7" t="n"/>
       <c r="M32" s="7" t="n"/>
       <c r="N32" s="7" t="n"/>
+      <c r="O32" s="7" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1708,6 +1789,9 @@
       <c r="N33" s="9" t="n">
         <v>8.710000000000001</v>
       </c>
+      <c r="O33" s="9" t="n">
+        <v>8.710000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1750,6 +1834,9 @@
         <v>31332.8</v>
       </c>
       <c r="N34" s="9" t="n">
+        <v>31543.5</v>
+      </c>
+      <c r="O34" s="9" t="n">
         <v>31543.5</v>
       </c>
     </row>
@@ -1768,6 +1855,7 @@
       <c r="L35" s="7" t="n"/>
       <c r="M35" s="7" t="n"/>
       <c r="N35" s="7" t="n"/>
+      <c r="O35" s="7" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1812,6 +1900,9 @@
       <c r="N36" s="9" t="n">
         <v>28.09</v>
       </c>
+      <c r="O36" s="9" t="n">
+        <v>28.09</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1854,6 +1945,9 @@
         <v>3243.38</v>
       </c>
       <c r="N37" s="7" t="n"/>
+      <c r="O37" s="9" t="n">
+        <v>3416.15</v>
+      </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="n"/>
@@ -1870,6 +1964,7 @@
       <c r="L38" s="7" t="n"/>
       <c r="M38" s="7" t="n"/>
       <c r="N38" s="7" t="n"/>
+      <c r="O38" s="7" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -1914,6 +2009,9 @@
       <c r="N39" s="9" t="n">
         <v>42.67</v>
       </c>
+      <c r="O39" s="9" t="n">
+        <v>42.67</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -1956,6 +2054,9 @@
         <v>3059.76</v>
       </c>
       <c r="N40" s="7" t="n"/>
+      <c r="O40" s="9" t="n">
+        <v>3203.06</v>
+      </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1" t="n"/>
@@ -1972,6 +2073,7 @@
       <c r="L41" s="7" t="n"/>
       <c r="M41" s="7" t="n"/>
       <c r="N41" s="7" t="n"/>
+      <c r="O41" s="7" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2016,6 +2118,9 @@
       <c r="N42" s="9" t="n">
         <v>14.57</v>
       </c>
+      <c r="O42" s="9" t="n">
+        <v>14.57</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2058,6 +2163,9 @@
         <v>6793.08</v>
       </c>
       <c r="N43" s="7" t="n"/>
+      <c r="O43" s="9" t="n">
+        <v>6867.51</v>
+      </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="n"/>
@@ -2074,6 +2182,7 @@
       <c r="L44" s="7" t="n"/>
       <c r="M44" s="7" t="n"/>
       <c r="N44" s="7" t="n"/>
+      <c r="O44" s="7" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2118,6 +2227,9 @@
       <c r="N45" s="9" t="n">
         <v>26.52</v>
       </c>
+      <c r="O45" s="9" t="n">
+        <v>26.52</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2160,6 +2272,9 @@
         <v>8377.370000000001</v>
       </c>
       <c r="N46" s="7" t="n"/>
+      <c r="O46" s="9" t="n">
+        <v>8475.17</v>
+      </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="1" t="n"/>
@@ -2176,6 +2291,7 @@
       <c r="L47" s="7" t="n"/>
       <c r="M47" s="7" t="n"/>
       <c r="N47" s="7" t="n"/>
+      <c r="O47" s="7" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2220,6 +2336,9 @@
       <c r="N48" s="9" t="n">
         <v>10.82</v>
       </c>
+      <c r="O48" s="9" t="n">
+        <v>10.82</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2262,6 +2381,9 @@
         <v>12750.41</v>
       </c>
       <c r="N49" s="9" t="n">
+        <v>12705.92</v>
+      </c>
+      <c r="O49" s="9" t="n">
         <v>12705.92</v>
       </c>
     </row>
@@ -2280,6 +2402,7 @@
       <c r="L50" s="7" t="n"/>
       <c r="M50" s="7" t="n"/>
       <c r="N50" s="7" t="n"/>
+      <c r="O50" s="7" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2324,6 +2447,9 @@
       <c r="N51" s="9" t="n">
         <v>26.8</v>
       </c>
+      <c r="O51" s="9" t="n">
+        <v>26.8</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2366,6 +2492,9 @@
         <v>12535.16</v>
       </c>
       <c r="N52" s="9" t="n">
+        <v>12578.17</v>
+      </c>
+      <c r="O52" s="9" t="n">
         <v>12578.17</v>
       </c>
     </row>
@@ -2384,6 +2513,7 @@
       <c r="L53" s="7" t="n"/>
       <c r="M53" s="7" t="n"/>
       <c r="N53" s="7" t="n"/>
+      <c r="O53" s="7" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2428,6 +2558,9 @@
       <c r="N54" s="9" t="n">
         <v>20.07</v>
       </c>
+      <c r="O54" s="9" t="n">
+        <v>20.07</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2470,6 +2603,9 @@
         <v>9241.42</v>
       </c>
       <c r="N55" s="7" t="n"/>
+      <c r="O55" s="9" t="n">
+        <v>9232.280000000001</v>
+      </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="n"/>
@@ -2486,6 +2622,7 @@
       <c r="L56" s="7" t="n"/>
       <c r="M56" s="7" t="n"/>
       <c r="N56" s="7" t="n"/>
+      <c r="O56" s="7" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2530,6 +2667,9 @@
       <c r="N57" s="9" t="n">
         <v>25.91</v>
       </c>
+      <c r="O57" s="9" t="n">
+        <v>25.91</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2572,6 +2712,9 @@
         <v>15665.58</v>
       </c>
       <c r="N58" s="7" t="n"/>
+      <c r="O58" s="9" t="n">
+        <v>15577.99</v>
+      </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1" t="n"/>
@@ -2588,6 +2731,7 @@
       <c r="L59" s="7" t="n"/>
       <c r="M59" s="7" t="n"/>
       <c r="N59" s="7" t="n"/>
+      <c r="O59" s="7" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2632,6 +2776,9 @@
       <c r="N60" s="9" t="n">
         <v>31.54</v>
       </c>
+      <c r="O60" s="9" t="n">
+        <v>31.54</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -2674,6 +2821,9 @@
         <v>17526.85</v>
       </c>
       <c r="N61" s="9" t="n">
+        <v>17526.85</v>
+      </c>
+      <c r="O61" s="9" t="n">
         <v>17526.85</v>
       </c>
     </row>
@@ -2692,6 +2842,7 @@
       <c r="L62" s="7" t="n"/>
       <c r="M62" s="7" t="n"/>
       <c r="N62" s="7" t="n"/>
+      <c r="O62" s="7" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -2736,6 +2887,9 @@
       <c r="N63" s="9" t="n">
         <v>21.53</v>
       </c>
+      <c r="O63" s="9" t="n">
+        <v>21.53</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2778,6 +2932,9 @@
         <v>9688.4</v>
       </c>
       <c r="N64" s="9" t="n">
+        <v>9733</v>
+      </c>
+      <c r="O64" s="9" t="n">
         <v>9733</v>
       </c>
     </row>
@@ -2796,6 +2953,7 @@
       <c r="L65" s="7" t="n"/>
       <c r="M65" s="7" t="n"/>
       <c r="N65" s="7" t="n"/>
+      <c r="O65" s="7" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -2840,6 +2998,9 @@
       <c r="N66" s="9" t="n">
         <v>14.56</v>
       </c>
+      <c r="O66" s="9" t="n">
+        <v>14.56</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -2882,6 +3043,9 @@
         <v>9913.360000000001</v>
       </c>
       <c r="N67" s="9" t="n">
+        <v>9849.84</v>
+      </c>
+      <c r="O67" s="9" t="n">
         <v>9849.84</v>
       </c>
     </row>
@@ -2900,6 +3064,7 @@
       <c r="L68" s="7" t="n"/>
       <c r="M68" s="7" t="n"/>
       <c r="N68" s="7" t="n"/>
+      <c r="O68" s="7" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -2944,6 +3109,9 @@
       <c r="N69" s="9" t="n">
         <v>23.91</v>
       </c>
+      <c r="O69" s="9" t="n">
+        <v>23.91</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -2986,6 +3154,9 @@
         <v>2963.64</v>
       </c>
       <c r="N70" s="9" t="n">
+        <v>2996.79</v>
+      </c>
+      <c r="O70" s="9" t="n">
         <v>2996.79</v>
       </c>
     </row>
@@ -3004,6 +3175,7 @@
       <c r="L71" s="7" t="n"/>
       <c r="M71" s="7" t="n"/>
       <c r="N71" s="7" t="n"/>
+      <c r="O71" s="7" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3048,6 +3220,9 @@
       <c r="N72" s="9" t="n">
         <v>46.75</v>
       </c>
+      <c r="O72" s="9" t="n">
+        <v>46.75</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3090,6 +3265,9 @@
         <v>5567.23</v>
       </c>
       <c r="N73" s="9" t="n">
+        <v>5649</v>
+      </c>
+      <c r="O73" s="9" t="n">
         <v>5649</v>
       </c>
     </row>
@@ -3108,6 +3286,7 @@
       <c r="L74" s="7" t="n"/>
       <c r="M74" s="7" t="n"/>
       <c r="N74" s="7" t="n"/>
+      <c r="O74" s="7" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3152,6 +3331,9 @@
       <c r="N75" s="9" t="n">
         <v>25.12</v>
       </c>
+      <c r="O75" s="9" t="n">
+        <v>25.12</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3194,6 +3376,9 @@
         <v>8970.639999999999</v>
       </c>
       <c r="N76" s="7" t="n"/>
+      <c r="O76" s="9" t="n">
+        <v>9025.51</v>
+      </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="1" t="n"/>
@@ -3210,6 +3395,7 @@
       <c r="L77" s="7" t="n"/>
       <c r="M77" s="7" t="n"/>
       <c r="N77" s="7" t="n"/>
+      <c r="O77" s="7" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3254,6 +3440,9 @@
       <c r="N78" s="9" t="n">
         <v>14.23</v>
       </c>
+      <c r="O78" s="9" t="n">
+        <v>14.23</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3296,6 +3485,9 @@
         <v>1300.67</v>
       </c>
       <c r="N79" s="9" t="n">
+        <v>1380.92</v>
+      </c>
+      <c r="O79" s="9" t="n">
         <v>1380.92</v>
       </c>
     </row>
@@ -3314,6 +3506,7 @@
       <c r="L80" s="7" t="n"/>
       <c r="M80" s="7" t="n"/>
       <c r="N80" s="7" t="n"/>
+      <c r="O80" s="7" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3358,6 +3551,9 @@
       <c r="N81" s="9" t="n">
         <v>54.87</v>
       </c>
+      <c r="O81" s="9" t="n">
+        <v>54.87</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -3400,6 +3596,9 @@
         <v>2722.85</v>
       </c>
       <c r="N82" s="7" t="n"/>
+      <c r="O82" s="9" t="n">
+        <v>2807.89</v>
+      </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="1" t="n"/>
@@ -3416,6 +3615,7 @@
       <c r="L83" s="7" t="n"/>
       <c r="M83" s="7" t="n"/>
       <c r="N83" s="7" t="n"/>
+      <c r="O83" s="7" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -3460,6 +3660,9 @@
       <c r="N84" s="9" t="n">
         <v>58.79</v>
       </c>
+      <c r="O84" s="9" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -3502,6 +3705,9 @@
         <v>2775.2</v>
       </c>
       <c r="N85" s="9" t="n">
+        <v>2878.39</v>
+      </c>
+      <c r="O85" s="9" t="n">
         <v>2878.39</v>
       </c>
     </row>
@@ -3520,6 +3726,7 @@
       <c r="L86" s="7" t="n"/>
       <c r="M86" s="7" t="n"/>
       <c r="N86" s="7" t="n"/>
+      <c r="O86" s="7" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -3564,6 +3771,9 @@
       <c r="N87" s="9" t="n">
         <v>51</v>
       </c>
+      <c r="O87" s="9" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -3606,6 +3816,9 @@
         <v>2848.93</v>
       </c>
       <c r="N88" s="9" t="n">
+        <v>2890.69</v>
+      </c>
+      <c r="O88" s="9" t="n">
         <v>2890.69</v>
       </c>
     </row>
@@ -3624,6 +3837,7 @@
       <c r="L89" s="7" t="n"/>
       <c r="M89" s="7" t="n"/>
       <c r="N89" s="7" t="n"/>
+      <c r="O89" s="7" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -3668,6 +3882,9 @@
       <c r="N90" s="9" t="n">
         <v>43.28</v>
       </c>
+      <c r="O90" s="9" t="n">
+        <v>43.28</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -3710,6 +3927,9 @@
         <v>1969.04</v>
       </c>
       <c r="N91" s="9" t="n">
+        <v>1978.75</v>
+      </c>
+      <c r="O91" s="9" t="n">
         <v>1978.75</v>
       </c>
     </row>
@@ -3728,6 +3948,7 @@
       <c r="L92" s="7" t="n"/>
       <c r="M92" s="7" t="n"/>
       <c r="N92" s="7" t="n"/>
+      <c r="O92" s="7" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -3772,6 +3993,9 @@
       <c r="N93" s="9" t="n">
         <v>27.25</v>
       </c>
+      <c r="O93" s="9" t="n">
+        <v>27.25</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -3814,6 +4038,9 @@
         <v>13370.57</v>
       </c>
       <c r="N94" s="9" t="n">
+        <v>13440.18</v>
+      </c>
+      <c r="O94" s="9" t="n">
         <v>13440.18</v>
       </c>
     </row>
@@ -3832,6 +4059,7 @@
       <c r="L95" s="7" t="n"/>
       <c r="M95" s="7" t="n"/>
       <c r="N95" s="7" t="n"/>
+      <c r="O95" s="7" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -3876,6 +4104,9 @@
       <c r="N96" s="9" t="n">
         <v>84.94</v>
       </c>
+      <c r="O96" s="9" t="n">
+        <v>84.94</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -3918,6 +4149,9 @@
         <v>8816.51</v>
       </c>
       <c r="N97" s="9" t="n">
+        <v>9014.25</v>
+      </c>
+      <c r="O97" s="9" t="n">
         <v>9014.25</v>
       </c>
     </row>
@@ -3936,6 +4170,7 @@
       <c r="L98" s="7" t="n"/>
       <c r="M98" s="7" t="n"/>
       <c r="N98" s="7" t="n"/>
+      <c r="O98" s="7" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -3980,6 +4215,9 @@
       <c r="N99" s="9" t="n">
         <v>56.64</v>
       </c>
+      <c r="O99" s="9" t="n">
+        <v>56.64</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -4022,6 +4260,9 @@
         <v>12001.13</v>
       </c>
       <c r="N100" s="7" t="n"/>
+      <c r="O100" s="9" t="n">
+        <v>12548.03</v>
+      </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="1" t="n"/>
@@ -4038,6 +4279,7 @@
       <c r="L101" s="7" t="n"/>
       <c r="M101" s="7" t="n"/>
       <c r="N101" s="7" t="n"/>
+      <c r="O101" s="7" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -4082,6 +4324,9 @@
       <c r="N102" s="9" t="n">
         <v>5.5</v>
       </c>
+      <c r="O102" s="9" t="n">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -4124,6 +4369,9 @@
         <v>2203.91</v>
       </c>
       <c r="N103" s="9" t="n">
+        <v>2217.96</v>
+      </c>
+      <c r="O103" s="9" t="n">
         <v>2217.96</v>
       </c>
     </row>
@@ -4142,6 +4390,7 @@
       <c r="L104" s="7" t="n"/>
       <c r="M104" s="7" t="n"/>
       <c r="N104" s="7" t="n"/>
+      <c r="O104" s="7" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -4186,6 +4435,9 @@
       <c r="N105" s="9" t="n">
         <v>25.46</v>
       </c>
+      <c r="O105" s="9" t="n">
+        <v>25.46</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -4228,6 +4480,9 @@
         <v>821.28</v>
       </c>
       <c r="N106" s="7" t="n"/>
+      <c r="O106" s="9" t="n">
+        <v>863.38</v>
+      </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="1" t="n"/>
@@ -4244,6 +4499,7 @@
       <c r="L107" s="7" t="n"/>
       <c r="M107" s="7" t="n"/>
       <c r="N107" s="7" t="n"/>
+      <c r="O107" s="7" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -4288,6 +4544,9 @@
       <c r="N108" s="9" t="n">
         <v>29.93</v>
       </c>
+      <c r="O108" s="9" t="n">
+        <v>29.93</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -4330,6 +4589,9 @@
         <v>2814.53</v>
       </c>
       <c r="N109" s="9" t="n">
+        <v>2879.26</v>
+      </c>
+      <c r="O109" s="9" t="n">
         <v>2879.26</v>
       </c>
     </row>
@@ -4348,6 +4610,7 @@
       <c r="L110" s="7" t="n"/>
       <c r="M110" s="7" t="n"/>
       <c r="N110" s="7" t="n"/>
+      <c r="O110" s="7" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -4392,6 +4655,9 @@
       <c r="N111" s="9" t="n">
         <v>20.59</v>
       </c>
+      <c r="O111" s="9" t="n">
+        <v>20.59</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -4434,6 +4700,9 @@
         <v>3853.83</v>
       </c>
       <c r="N112" s="7" t="n"/>
+      <c r="O112" s="9" t="n">
+        <v>3885.92</v>
+      </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="1" t="n"/>
@@ -4450,6 +4719,7 @@
       <c r="L113" s="7" t="n"/>
       <c r="M113" s="7" t="n"/>
       <c r="N113" s="7" t="n"/>
+      <c r="O113" s="7" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -4494,6 +4764,9 @@
       <c r="N114" s="9" t="n">
         <v>29.02</v>
       </c>
+      <c r="O114" s="9" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -4536,6 +4809,9 @@
         <v>3174.12</v>
       </c>
       <c r="N115" s="7" t="n"/>
+      <c r="O115" s="9" t="n">
+        <v>3177.69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-15 00:49:59]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:P118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
@@ -520,6 +520,7 @@
     <col width="15" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="15" customWidth="1" min="15" max="15"/>
+    <col width="15" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -598,6 +599,11 @@
           <t>2025/12/11</t>
         </is>
       </c>
+      <c r="P1" s="10" t="inlineStr">
+        <is>
+          <t>2025/12/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -675,6 +681,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="P2" s="11" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -722,6 +733,9 @@
       <c r="O3" s="12" t="n">
         <v>61.69</v>
       </c>
+      <c r="P3" s="10" t="n">
+        <v>61.22</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -768,6 +782,9 @@
       </c>
       <c r="O4" s="12" t="n">
         <v>3882.72</v>
+      </c>
+      <c r="P4" s="10" t="n">
+        <v>3889.35</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -786,6 +803,7 @@
       <c r="M5" s="7" t="n"/>
       <c r="N5" s="7" t="n"/>
       <c r="O5" s="10" t="n"/>
+      <c r="P5" s="10" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -833,6 +851,9 @@
       <c r="O6" s="12" t="n">
         <v>48.32</v>
       </c>
+      <c r="P6" s="10" t="n">
+        <v>48.25</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -879,6 +900,9 @@
       </c>
       <c r="O7" s="12" t="n">
         <v>5523.58</v>
+      </c>
+      <c r="P7" s="10" t="n">
+        <v>5530.39</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -897,6 +921,7 @@
       <c r="M8" s="7" t="n"/>
       <c r="N8" s="7" t="n"/>
       <c r="O8" s="10" t="n"/>
+      <c r="P8" s="10" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -944,6 +969,9 @@
       <c r="O9" s="12" t="n">
         <v>52.89</v>
       </c>
+      <c r="P9" s="10" t="n">
+        <v>52.53</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -990,6 +1018,9 @@
       </c>
       <c r="O10" s="12" t="n">
         <v>4582.51</v>
+      </c>
+      <c r="P10" s="10" t="n">
+        <v>4580.95</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1008,6 +1039,7 @@
       <c r="M11" s="7" t="n"/>
       <c r="N11" s="7" t="n"/>
       <c r="O11" s="10" t="n"/>
+      <c r="P11" s="10" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1055,6 +1087,9 @@
       <c r="O12" s="12" t="n">
         <v>56.69</v>
       </c>
+      <c r="P12" s="10" t="n">
+        <v>56.78</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1101,6 +1136,9 @@
       </c>
       <c r="O13" s="12" t="n">
         <v>7129.62</v>
+      </c>
+      <c r="P13" s="10" t="n">
+        <v>7169.79</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1119,6 +1157,7 @@
       <c r="M14" s="7" t="n"/>
       <c r="N14" s="7" t="n"/>
       <c r="O14" s="10" t="n"/>
+      <c r="P14" s="10" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1166,6 +1205,9 @@
       <c r="O15" s="12" t="n">
         <v>26.11</v>
       </c>
+      <c r="P15" s="10" t="n">
+        <v>26.32</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1212,6 +1254,9 @@
       </c>
       <c r="O16" s="12" t="n">
         <v>2653.73</v>
+      </c>
+      <c r="P16" s="10" t="n">
+        <v>2672.5</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1230,6 +1275,7 @@
       <c r="M17" s="7" t="n"/>
       <c r="N17" s="7" t="n"/>
       <c r="O17" s="10" t="n"/>
+      <c r="P17" s="10" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1277,6 +1323,9 @@
       <c r="O18" s="12" t="n">
         <v>96.93000000000001</v>
       </c>
+      <c r="P18" s="10" t="n">
+        <v>96.41</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1323,6 +1372,9 @@
       </c>
       <c r="O19" s="12" t="n">
         <v>6886.68</v>
+      </c>
+      <c r="P19" s="10" t="n">
+        <v>6827.41</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1341,6 +1393,7 @@
       <c r="M20" s="7" t="n"/>
       <c r="N20" s="7" t="n"/>
       <c r="O20" s="10" t="n"/>
+      <c r="P20" s="10" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1388,6 +1441,9 @@
       <c r="O21" s="12" t="n">
         <v>65.18000000000001</v>
       </c>
+      <c r="P21" s="10" t="n">
+        <v>68.42</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1434,6 +1490,9 @@
       </c>
       <c r="O22" s="12" t="n">
         <v>84396.07000000001</v>
+      </c>
+      <c r="P22" s="10" t="n">
+        <v>85267.66</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1452,6 +1511,7 @@
       <c r="M23" s="7" t="n"/>
       <c r="N23" s="7" t="n"/>
       <c r="O23" s="10" t="n"/>
+      <c r="P23" s="10" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1499,6 +1559,9 @@
       <c r="O24" s="12" t="n">
         <v>84.39</v>
       </c>
+      <c r="P24" s="10" t="n">
+        <v>84.69</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1545,6 +1608,9 @@
       </c>
       <c r="O25" s="12" t="n">
         <v>24119.97</v>
+      </c>
+      <c r="P25" s="10" t="n">
+        <v>24186.49</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1563,6 +1629,7 @@
       <c r="M26" s="7" t="n"/>
       <c r="N26" s="7" t="n"/>
       <c r="O26" s="10" t="n"/>
+      <c r="P26" s="10" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1610,6 +1677,9 @@
       <c r="O27" s="12" t="n">
         <v>70.68000000000001</v>
       </c>
+      <c r="P27" s="10" t="n">
+        <v>69.69</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1656,6 +1726,9 @@
       </c>
       <c r="O28" s="12" t="n">
         <v>50103.85</v>
+      </c>
+      <c r="P28" s="10" t="n">
+        <v>50283.56</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1674,6 +1747,7 @@
       <c r="M29" s="7" t="n"/>
       <c r="N29" s="7" t="n"/>
       <c r="O29" s="10" t="n"/>
+      <c r="P29" s="10" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1721,6 +1795,9 @@
       <c r="O30" s="12" t="n">
         <v>48.09</v>
       </c>
+      <c r="P30" s="10" t="n">
+        <v>49.82</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1767,6 +1844,9 @@
       </c>
       <c r="O31" s="12" t="n">
         <v>5454.63</v>
+      </c>
+      <c r="P31" s="10" t="n">
+        <v>5426.72</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1785,6 +1865,7 @@
       <c r="M32" s="7" t="n"/>
       <c r="N32" s="7" t="n"/>
       <c r="O32" s="10" t="n"/>
+      <c r="P32" s="10" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1832,6 +1913,9 @@
       <c r="O33" s="12" t="n">
         <v>7.84</v>
       </c>
+      <c r="P33" s="10" t="n">
+        <v>8.050000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1878,6 +1962,9 @@
       </c>
       <c r="O34" s="12" t="n">
         <v>31307.06</v>
+      </c>
+      <c r="P34" s="10" t="n">
+        <v>31304.53</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1896,6 +1983,7 @@
       <c r="M35" s="7" t="n"/>
       <c r="N35" s="7" t="n"/>
       <c r="O35" s="10" t="n"/>
+      <c r="P35" s="10" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -1943,6 +2031,9 @@
       <c r="O36" s="12" t="n">
         <v>29.27</v>
       </c>
+      <c r="P36" s="10" t="n">
+        <v>29.16</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -1989,6 +2080,9 @@
       </c>
       <c r="O37" s="12" t="n">
         <v>3432.8</v>
+      </c>
+      <c r="P37" s="10" t="n">
+        <v>3397.66</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2007,6 +2101,7 @@
       <c r="M38" s="7" t="n"/>
       <c r="N38" s="7" t="n"/>
       <c r="O38" s="10" t="n"/>
+      <c r="P38" s="10" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2054,6 +2149,9 @@
       <c r="O39" s="12" t="n">
         <v>47.13</v>
       </c>
+      <c r="P39" s="10" t="n">
+        <v>46.99</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2100,6 +2198,9 @@
       </c>
       <c r="O40" s="12" t="n">
         <v>3218.55</v>
+      </c>
+      <c r="P40" s="10" t="n">
+        <v>3194.36</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2118,6 +2219,7 @@
       <c r="M41" s="7" t="n"/>
       <c r="N41" s="7" t="n"/>
       <c r="O41" s="10" t="n"/>
+      <c r="P41" s="10" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2165,6 +2267,9 @@
       <c r="O42" s="12" t="n">
         <v>14.32</v>
       </c>
+      <c r="P42" s="10" t="n">
+        <v>14.46</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2212,6 +2317,7 @@
       <c r="O43" s="12" t="n">
         <v>6812.72</v>
       </c>
+      <c r="P43" s="10" t="inlineStr"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="n"/>
@@ -2229,6 +2335,7 @@
       <c r="M44" s="7" t="n"/>
       <c r="N44" s="7" t="n"/>
       <c r="O44" s="10" t="n"/>
+      <c r="P44" s="10" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2276,6 +2383,9 @@
       <c r="O45" s="12" t="n">
         <v>26.84</v>
       </c>
+      <c r="P45" s="10" t="n">
+        <v>26.61</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2322,6 +2432,9 @@
       </c>
       <c r="O46" s="12" t="n">
         <v>8498.34</v>
+      </c>
+      <c r="P46" s="10" t="n">
+        <v>8478.26</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2340,6 +2453,7 @@
       <c r="M47" s="7" t="n"/>
       <c r="N47" s="7" t="n"/>
       <c r="O47" s="10" t="n"/>
+      <c r="P47" s="10" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2387,6 +2501,9 @@
       <c r="O48" s="12" t="n">
         <v>9.77</v>
       </c>
+      <c r="P48" s="10" t="n">
+        <v>10.31</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2433,6 +2550,9 @@
       </c>
       <c r="O49" s="12" t="n">
         <v>12583.61</v>
+      </c>
+      <c r="P49" s="10" t="n">
+        <v>12651.28</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2451,6 +2571,7 @@
       <c r="M50" s="7" t="n"/>
       <c r="N50" s="7" t="n"/>
       <c r="O50" s="10" t="n"/>
+      <c r="P50" s="10" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2498,6 +2619,9 @@
       <c r="O51" s="12" t="n">
         <v>25.82</v>
       </c>
+      <c r="P51" s="10" t="n">
+        <v>24.88</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2544,6 +2668,9 @@
       </c>
       <c r="O52" s="12" t="n">
         <v>12459.11</v>
+      </c>
+      <c r="P52" s="10" t="n">
+        <v>12418.82</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2562,6 +2689,7 @@
       <c r="M53" s="7" t="n"/>
       <c r="N53" s="7" t="n"/>
       <c r="O53" s="10" t="n"/>
+      <c r="P53" s="10" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2609,6 +2737,9 @@
       <c r="O54" s="12" t="n">
         <v>18.66</v>
       </c>
+      <c r="P54" s="10" t="n">
+        <v>19.1</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2656,6 +2787,7 @@
       <c r="O55" s="12" t="n">
         <v>9087.209999999999</v>
       </c>
+      <c r="P55" s="10" t="inlineStr"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="n"/>
@@ -2673,6 +2805,7 @@
       <c r="M56" s="7" t="n"/>
       <c r="N56" s="7" t="n"/>
       <c r="O56" s="10" t="n"/>
+      <c r="P56" s="10" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2720,6 +2853,9 @@
       <c r="O57" s="12" t="n">
         <v>25.32</v>
       </c>
+      <c r="P57" s="10" t="n">
+        <v>25.44</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2766,6 +2902,9 @@
       </c>
       <c r="O58" s="12" t="n">
         <v>15379.22</v>
+      </c>
+      <c r="P58" s="10" t="n">
+        <v>15417.29</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -2784,6 +2923,7 @@
       <c r="M59" s="7" t="n"/>
       <c r="N59" s="7" t="n"/>
       <c r="O59" s="10" t="n"/>
+      <c r="P59" s="10" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2831,6 +2971,9 @@
       <c r="O60" s="12" t="n">
         <v>31.06</v>
       </c>
+      <c r="P60" s="10" t="n">
+        <v>31.16</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -2878,6 +3021,7 @@
       <c r="O61" s="12" t="n">
         <v>17526.85</v>
       </c>
+      <c r="P61" s="10" t="inlineStr"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="1" t="n"/>
@@ -2895,6 +3039,7 @@
       <c r="M62" s="7" t="n"/>
       <c r="N62" s="7" t="n"/>
       <c r="O62" s="10" t="n"/>
+      <c r="P62" s="10" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -2942,6 +3087,9 @@
       <c r="O63" s="12" t="n">
         <v>20.85</v>
       </c>
+      <c r="P63" s="10" t="n">
+        <v>21.37</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -2988,6 +3136,9 @@
       </c>
       <c r="O64" s="12" t="n">
         <v>9651.24</v>
+      </c>
+      <c r="P64" s="10" t="n">
+        <v>9782.639999999999</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -3006,6 +3157,7 @@
       <c r="M65" s="7" t="n"/>
       <c r="N65" s="7" t="n"/>
       <c r="O65" s="10" t="n"/>
+      <c r="P65" s="10" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3053,6 +3205,9 @@
       <c r="O66" s="12" t="n">
         <v>13.89</v>
       </c>
+      <c r="P66" s="10" t="n">
+        <v>13.51</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3099,6 +3254,9 @@
       </c>
       <c r="O67" s="12" t="n">
         <v>9776.66</v>
+      </c>
+      <c r="P67" s="10" t="n">
+        <v>9711.33</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -3117,6 +3275,7 @@
       <c r="M68" s="7" t="n"/>
       <c r="N68" s="7" t="n"/>
       <c r="O68" s="10" t="n"/>
+      <c r="P68" s="10" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3164,6 +3323,9 @@
       <c r="O69" s="12" t="n">
         <v>23.55</v>
       </c>
+      <c r="P69" s="10" t="n">
+        <v>24.01</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3211,6 +3373,7 @@
       <c r="O70" s="12" t="n">
         <v>2972.4</v>
       </c>
+      <c r="P70" s="10" t="inlineStr"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="1" t="n"/>
@@ -3228,6 +3391,7 @@
       <c r="M71" s="7" t="n"/>
       <c r="N71" s="7" t="n"/>
       <c r="O71" s="10" t="n"/>
+      <c r="P71" s="10" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3275,6 +3439,9 @@
       <c r="O72" s="12" t="n">
         <v>45.95</v>
       </c>
+      <c r="P72" s="10" t="n">
+        <v>47.02</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3322,6 +3489,7 @@
       <c r="O73" s="12" t="n">
         <v>5544.66</v>
       </c>
+      <c r="P73" s="10" t="inlineStr"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="1" t="n"/>
@@ -3339,6 +3507,7 @@
       <c r="M74" s="7" t="n"/>
       <c r="N74" s="7" t="n"/>
       <c r="O74" s="10" t="n"/>
+      <c r="P74" s="10" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3386,6 +3555,9 @@
       <c r="O75" s="12" t="n">
         <v>24.87</v>
       </c>
+      <c r="P75" s="10" t="n">
+        <v>24.59</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3432,6 +3604,9 @@
       </c>
       <c r="O76" s="12" t="n">
         <v>8989.33</v>
+      </c>
+      <c r="P76" s="10" t="n">
+        <v>8973.51</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -3450,6 +3625,7 @@
       <c r="M77" s="7" t="n"/>
       <c r="N77" s="7" t="n"/>
       <c r="O77" s="10" t="n"/>
+      <c r="P77" s="10" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3497,6 +3673,9 @@
       <c r="O78" s="12" t="n">
         <v>14.33</v>
       </c>
+      <c r="P78" s="10" t="n">
+        <v>14.59</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3543,6 +3722,9 @@
       </c>
       <c r="O79" s="12" t="n">
         <v>1390.11</v>
+      </c>
+      <c r="P79" s="10" t="n">
+        <v>1413.51</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -3561,6 +3743,7 @@
       <c r="M80" s="7" t="n"/>
       <c r="N80" s="7" t="n"/>
       <c r="O80" s="10" t="n"/>
+      <c r="P80" s="10" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3608,6 +3791,9 @@
       <c r="O81" s="12" t="n">
         <v>54.86</v>
       </c>
+      <c r="P81" s="10" t="n">
+        <v>18.18</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -3654,6 +3840,9 @@
       </c>
       <c r="O82" s="12" t="n">
         <v>2785.86</v>
+      </c>
+      <c r="P82" s="10" t="n">
+        <v>16511.99</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -3672,6 +3861,7 @@
       <c r="M83" s="7" t="n"/>
       <c r="N83" s="7" t="n"/>
       <c r="O83" s="10" t="n"/>
+      <c r="P83" s="10" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -3719,6 +3909,9 @@
       <c r="O84" s="12" t="n">
         <v>58.79</v>
       </c>
+      <c r="P84" s="10" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -3766,6 +3959,7 @@
       <c r="O85" s="12" t="n">
         <v>2839.34</v>
       </c>
+      <c r="P85" s="10" t="inlineStr"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="1" t="n"/>
@@ -3783,6 +3977,7 @@
       <c r="M86" s="7" t="n"/>
       <c r="N86" s="7" t="n"/>
       <c r="O86" s="10" t="n"/>
+      <c r="P86" s="10" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -3830,6 +4025,9 @@
       <c r="O87" s="12" t="n">
         <v>51.08</v>
       </c>
+      <c r="P87" s="10" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -3876,6 +4074,9 @@
       </c>
       <c r="O88" s="12" t="n">
         <v>2929.31</v>
+      </c>
+      <c r="P88" s="10" t="n">
+        <v>2867.5</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -3894,6 +4095,7 @@
       <c r="M89" s="7" t="n"/>
       <c r="N89" s="7" t="n"/>
       <c r="O89" s="10" t="n"/>
+      <c r="P89" s="10" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -3941,6 +4143,9 @@
       <c r="O90" s="12" t="n">
         <v>43.4</v>
       </c>
+      <c r="P90" s="10" t="n">
+        <v>51.17</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -3987,6 +4192,9 @@
       </c>
       <c r="O91" s="12" t="n">
         <v>1980.68</v>
+      </c>
+      <c r="P91" s="10" t="n">
+        <v>2891.55</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -4005,6 +4213,7 @@
       <c r="M92" s="7" t="n"/>
       <c r="N92" s="7" t="n"/>
       <c r="O92" s="10" t="n"/>
+      <c r="P92" s="10" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4052,6 +4261,9 @@
       <c r="O93" s="12" t="n">
         <v>26.96</v>
       </c>
+      <c r="P93" s="10" t="n">
+        <v>43.2</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -4098,6 +4310,9 @@
       </c>
       <c r="O94" s="12" t="n">
         <v>13120.76</v>
+      </c>
+      <c r="P94" s="10" t="n">
+        <v>1974.54</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -4116,6 +4331,7 @@
       <c r="M95" s="7" t="n"/>
       <c r="N95" s="7" t="n"/>
       <c r="O95" s="10" t="n"/>
+      <c r="P95" s="10" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -4163,6 +4379,9 @@
       <c r="O96" s="12" t="n">
         <v>85.91</v>
       </c>
+      <c r="P96" s="10" t="n">
+        <v>26.88</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -4209,6 +4428,9 @@
       </c>
       <c r="O97" s="12" t="n">
         <v>8969.84</v>
+      </c>
+      <c r="P97" s="10" t="n">
+        <v>9942.059999999999</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -4227,6 +4449,7 @@
       <c r="M98" s="7" t="n"/>
       <c r="N98" s="7" t="n"/>
       <c r="O98" s="10" t="n"/>
+      <c r="P98" s="10" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -4274,6 +4497,9 @@
       <c r="O99" s="12" t="n">
         <v>56.99</v>
       </c>
+      <c r="P99" s="10" t="n">
+        <v>85.97</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -4320,6 +4546,9 @@
       </c>
       <c r="O100" s="12" t="n">
         <v>12533.21</v>
+      </c>
+      <c r="P100" s="10" t="n">
+        <v>9044.780000000001</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -4338,6 +4567,7 @@
       <c r="M101" s="7" t="n"/>
       <c r="N101" s="7" t="n"/>
       <c r="O101" s="10" t="n"/>
+      <c r="P101" s="10" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -4385,6 +4615,9 @@
       <c r="O102" s="12" t="n">
         <v>5.36</v>
       </c>
+      <c r="P102" s="10" t="n">
+        <v>57.07</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -4432,6 +4665,7 @@
       <c r="O103" s="12" t="n">
         <v>2193.69</v>
       </c>
+      <c r="P103" s="10" t="inlineStr"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="n"/>
@@ -4449,6 +4683,7 @@
       <c r="M104" s="7" t="n"/>
       <c r="N104" s="7" t="n"/>
       <c r="O104" s="10" t="n"/>
+      <c r="P104" s="10" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -4496,6 +4731,9 @@
       <c r="O105" s="12" t="n">
         <v>25.56</v>
       </c>
+      <c r="P105" s="10" t="n">
+        <v>5.43</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -4542,6 +4780,9 @@
       </c>
       <c r="O106" s="12" t="n">
         <v>843.17</v>
+      </c>
+      <c r="P106" s="10" t="n">
+        <v>2211.46</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -4560,6 +4801,7 @@
       <c r="M107" s="7" t="n"/>
       <c r="N107" s="7" t="n"/>
       <c r="O107" s="10" t="n"/>
+      <c r="P107" s="10" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -4607,6 +4849,9 @@
       <c r="O108" s="12" t="n">
         <v>29.79</v>
       </c>
+      <c r="P108" s="10" t="n">
+        <v>25.49</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -4654,6 +4899,7 @@
       <c r="O109" s="12" t="n">
         <v>2820.56</v>
       </c>
+      <c r="P109" s="10" t="inlineStr"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="1" t="n"/>
@@ -4671,6 +4917,7 @@
       <c r="M110" s="7" t="n"/>
       <c r="N110" s="7" t="n"/>
       <c r="O110" s="10" t="n"/>
+      <c r="P110" s="10" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -4718,6 +4965,9 @@
       <c r="O111" s="12" t="n">
         <v>20.09</v>
       </c>
+      <c r="P111" s="10" t="n">
+        <v>29.86</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -4764,6 +5014,9 @@
       </c>
       <c r="O112" s="12" t="n">
         <v>3838.51</v>
+      </c>
+      <c r="P112" s="10" t="n">
+        <v>2840.6</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -4782,6 +5035,7 @@
       <c r="M113" s="7" t="n"/>
       <c r="N113" s="7" t="n"/>
       <c r="O113" s="10" t="n"/>
+      <c r="P113" s="10" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -4829,6 +5083,9 @@
       <c r="O114" s="12" t="n">
         <v>29.02</v>
       </c>
+      <c r="P114" s="10" t="n">
+        <v>20.31</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -4875,6 +5132,20 @@
       </c>
       <c r="O115" s="12" t="n">
         <v>3131.36</v>
+      </c>
+      <c r="P115" s="10" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="P116" s="10" t="n"/>
+    </row>
+    <row r="117">
+      <c r="P117" s="10" t="n">
+        <v>29.02</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="P118" s="10" t="n">
+        <v>2959.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-15 00:55:16]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P118"/>
+  <dimension ref="A1:Q118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
@@ -521,6 +521,7 @@
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="15" customWidth="1" min="15" max="15"/>
     <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="15" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -604,6 +605,11 @@
           <t>2025/12/15</t>
         </is>
       </c>
+      <c r="Q1" s="10" t="inlineStr">
+        <is>
+          <t>2025/12/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -686,6 +692,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="Q2" s="11" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -736,6 +747,9 @@
       <c r="P3" s="10" t="n">
         <v>61.22</v>
       </c>
+      <c r="Q3" s="10" t="n">
+        <v>61.22</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -785,6 +799,9 @@
       </c>
       <c r="P4" s="10" t="n">
         <v>3889.35</v>
+      </c>
+      <c r="Q4" s="10" t="n">
+        <v>3884.54</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -804,6 +821,7 @@
       <c r="N5" s="7" t="n"/>
       <c r="O5" s="10" t="n"/>
       <c r="P5" s="10" t="n"/>
+      <c r="Q5" s="10" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -854,6 +872,9 @@
       <c r="P6" s="10" t="n">
         <v>48.25</v>
       </c>
+      <c r="Q6" s="10" t="n">
+        <v>48.25</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -903,6 +924,9 @@
       </c>
       <c r="P7" s="10" t="n">
         <v>5530.39</v>
+      </c>
+      <c r="Q7" s="10" t="n">
+        <v>5528.82</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -922,6 +946,7 @@
       <c r="N8" s="7" t="n"/>
       <c r="O8" s="10" t="n"/>
       <c r="P8" s="10" t="n"/>
+      <c r="Q8" s="10" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -972,6 +997,9 @@
       <c r="P9" s="10" t="n">
         <v>52.53</v>
       </c>
+      <c r="Q9" s="10" t="n">
+        <v>52.53</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1021,6 +1049,9 @@
       </c>
       <c r="P10" s="10" t="n">
         <v>4580.95</v>
+      </c>
+      <c r="Q10" s="10" t="n">
+        <v>4579.49</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1040,6 +1071,7 @@
       <c r="N11" s="7" t="n"/>
       <c r="O11" s="10" t="n"/>
       <c r="P11" s="10" t="n"/>
+      <c r="Q11" s="10" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1090,6 +1122,9 @@
       <c r="P12" s="10" t="n">
         <v>56.78</v>
       </c>
+      <c r="Q12" s="10" t="n">
+        <v>56.78</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1139,6 +1174,9 @@
       </c>
       <c r="P13" s="10" t="n">
         <v>7169.79</v>
+      </c>
+      <c r="Q13" s="10" t="n">
+        <v>7169.64</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1158,6 +1196,7 @@
       <c r="N14" s="7" t="n"/>
       <c r="O14" s="10" t="n"/>
       <c r="P14" s="10" t="n"/>
+      <c r="Q14" s="10" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1208,6 +1247,9 @@
       <c r="P15" s="10" t="n">
         <v>26.32</v>
       </c>
+      <c r="Q15" s="10" t="n">
+        <v>26.32</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1256,6 +1298,9 @@
         <v>2653.73</v>
       </c>
       <c r="P16" s="10" t="n">
+        <v>2672.5</v>
+      </c>
+      <c r="Q16" s="10" t="n">
         <v>2672.5</v>
       </c>
     </row>
@@ -1276,6 +1321,7 @@
       <c r="N17" s="7" t="n"/>
       <c r="O17" s="10" t="n"/>
       <c r="P17" s="10" t="n"/>
+      <c r="Q17" s="10" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1326,6 +1372,9 @@
       <c r="P18" s="10" t="n">
         <v>96.41</v>
       </c>
+      <c r="Q18" s="10" t="n">
+        <v>96.41</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1374,6 +1423,9 @@
         <v>6886.68</v>
       </c>
       <c r="P19" s="10" t="n">
+        <v>6827.41</v>
+      </c>
+      <c r="Q19" s="10" t="n">
         <v>6827.41</v>
       </c>
     </row>
@@ -1394,6 +1446,7 @@
       <c r="N20" s="7" t="n"/>
       <c r="O20" s="10" t="n"/>
       <c r="P20" s="10" t="n"/>
+      <c r="Q20" s="10" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1444,6 +1497,9 @@
       <c r="P21" s="10" t="n">
         <v>68.42</v>
       </c>
+      <c r="Q21" s="10" t="n">
+        <v>68.42</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1492,6 +1548,9 @@
         <v>84396.07000000001</v>
       </c>
       <c r="P22" s="10" t="n">
+        <v>85267.66</v>
+      </c>
+      <c r="Q22" s="10" t="n">
         <v>85267.66</v>
       </c>
     </row>
@@ -1512,6 +1571,7 @@
       <c r="N23" s="7" t="n"/>
       <c r="O23" s="10" t="n"/>
       <c r="P23" s="10" t="n"/>
+      <c r="Q23" s="10" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1562,6 +1622,9 @@
       <c r="P24" s="10" t="n">
         <v>84.69</v>
       </c>
+      <c r="Q24" s="10" t="n">
+        <v>84.69</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1610,6 +1673,9 @@
         <v>24119.97</v>
       </c>
       <c r="P25" s="10" t="n">
+        <v>24186.49</v>
+      </c>
+      <c r="Q25" s="10" t="n">
         <v>24186.49</v>
       </c>
     </row>
@@ -1630,6 +1696,7 @@
       <c r="N26" s="7" t="n"/>
       <c r="O26" s="10" t="n"/>
       <c r="P26" s="10" t="n"/>
+      <c r="Q26" s="10" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1680,6 +1747,9 @@
       <c r="P27" s="10" t="n">
         <v>69.69</v>
       </c>
+      <c r="Q27" s="10" t="n">
+        <v>69.69</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1729,6 +1799,9 @@
       </c>
       <c r="P28" s="10" t="n">
         <v>50283.56</v>
+      </c>
+      <c r="Q28" s="10" t="n">
+        <v>50254.99</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1748,6 +1821,7 @@
       <c r="N29" s="7" t="n"/>
       <c r="O29" s="10" t="n"/>
       <c r="P29" s="10" t="n"/>
+      <c r="Q29" s="10" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1798,6 +1872,9 @@
       <c r="P30" s="10" t="n">
         <v>49.82</v>
       </c>
+      <c r="Q30" s="10" t="n">
+        <v>49.82</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1846,6 +1923,9 @@
         <v>5454.63</v>
       </c>
       <c r="P31" s="10" t="n">
+        <v>5426.72</v>
+      </c>
+      <c r="Q31" s="10" t="n">
         <v>5426.72</v>
       </c>
     </row>
@@ -1866,6 +1946,7 @@
       <c r="N32" s="7" t="n"/>
       <c r="O32" s="10" t="n"/>
       <c r="P32" s="10" t="n"/>
+      <c r="Q32" s="10" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1916,6 +1997,9 @@
       <c r="P33" s="10" t="n">
         <v>8.050000000000001</v>
       </c>
+      <c r="Q33" s="10" t="n">
+        <v>8.050000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1964,6 +2048,9 @@
         <v>31307.06</v>
       </c>
       <c r="P34" s="10" t="n">
+        <v>31304.53</v>
+      </c>
+      <c r="Q34" s="10" t="n">
         <v>31304.53</v>
       </c>
     </row>
@@ -1984,6 +2071,7 @@
       <c r="N35" s="7" t="n"/>
       <c r="O35" s="10" t="n"/>
       <c r="P35" s="10" t="n"/>
+      <c r="Q35" s="10" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2034,6 +2122,9 @@
       <c r="P36" s="10" t="n">
         <v>29.16</v>
       </c>
+      <c r="Q36" s="10" t="n">
+        <v>29.16</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2084,6 +2175,7 @@
       <c r="P37" s="10" t="n">
         <v>3397.66</v>
       </c>
+      <c r="Q37" s="10" t="inlineStr"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="n"/>
@@ -2102,6 +2194,7 @@
       <c r="N38" s="7" t="n"/>
       <c r="O38" s="10" t="n"/>
       <c r="P38" s="10" t="n"/>
+      <c r="Q38" s="10" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2152,6 +2245,9 @@
       <c r="P39" s="10" t="n">
         <v>46.99</v>
       </c>
+      <c r="Q39" s="10" t="n">
+        <v>46.99</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2202,6 +2298,7 @@
       <c r="P40" s="10" t="n">
         <v>3194.36</v>
       </c>
+      <c r="Q40" s="10" t="inlineStr"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1" t="n"/>
@@ -2220,6 +2317,7 @@
       <c r="N41" s="7" t="n"/>
       <c r="O41" s="10" t="n"/>
       <c r="P41" s="10" t="n"/>
+      <c r="Q41" s="10" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2270,6 +2368,9 @@
       <c r="P42" s="10" t="n">
         <v>14.46</v>
       </c>
+      <c r="Q42" s="10" t="n">
+        <v>14.46</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2318,6 +2419,7 @@
         <v>6812.72</v>
       </c>
       <c r="P43" s="10" t="inlineStr"/>
+      <c r="Q43" s="10" t="inlineStr"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="n"/>
@@ -2336,6 +2438,7 @@
       <c r="N44" s="7" t="n"/>
       <c r="O44" s="10" t="n"/>
       <c r="P44" s="10" t="n"/>
+      <c r="Q44" s="10" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2386,6 +2489,9 @@
       <c r="P45" s="10" t="n">
         <v>26.61</v>
       </c>
+      <c r="Q45" s="10" t="n">
+        <v>26.61</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2434,6 +2540,9 @@
         <v>8498.34</v>
       </c>
       <c r="P46" s="10" t="n">
+        <v>8478.26</v>
+      </c>
+      <c r="Q46" s="10" t="n">
         <v>8478.26</v>
       </c>
     </row>
@@ -2454,6 +2563,7 @@
       <c r="N47" s="7" t="n"/>
       <c r="O47" s="10" t="n"/>
       <c r="P47" s="10" t="n"/>
+      <c r="Q47" s="10" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2504,6 +2614,9 @@
       <c r="P48" s="10" t="n">
         <v>10.31</v>
       </c>
+      <c r="Q48" s="10" t="n">
+        <v>10.31</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2552,6 +2665,9 @@
         <v>12583.61</v>
       </c>
       <c r="P49" s="10" t="n">
+        <v>12651.28</v>
+      </c>
+      <c r="Q49" s="10" t="n">
         <v>12651.28</v>
       </c>
     </row>
@@ -2572,6 +2688,7 @@
       <c r="N50" s="7" t="n"/>
       <c r="O50" s="10" t="n"/>
       <c r="P50" s="10" t="n"/>
+      <c r="Q50" s="10" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2622,6 +2739,9 @@
       <c r="P51" s="10" t="n">
         <v>24.88</v>
       </c>
+      <c r="Q51" s="10" t="n">
+        <v>24.88</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2670,6 +2790,9 @@
         <v>12459.11</v>
       </c>
       <c r="P52" s="10" t="n">
+        <v>12418.82</v>
+      </c>
+      <c r="Q52" s="10" t="n">
         <v>12418.82</v>
       </c>
     </row>
@@ -2690,6 +2813,7 @@
       <c r="N53" s="7" t="n"/>
       <c r="O53" s="10" t="n"/>
       <c r="P53" s="10" t="n"/>
+      <c r="Q53" s="10" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2740,6 +2864,9 @@
       <c r="P54" s="10" t="n">
         <v>19.1</v>
       </c>
+      <c r="Q54" s="10" t="n">
+        <v>19.1</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2788,6 +2915,7 @@
         <v>9087.209999999999</v>
       </c>
       <c r="P55" s="10" t="inlineStr"/>
+      <c r="Q55" s="10" t="inlineStr"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="n"/>
@@ -2806,6 +2934,7 @@
       <c r="N56" s="7" t="n"/>
       <c r="O56" s="10" t="n"/>
       <c r="P56" s="10" t="n"/>
+      <c r="Q56" s="10" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2856,6 +2985,9 @@
       <c r="P57" s="10" t="n">
         <v>25.44</v>
       </c>
+      <c r="Q57" s="10" t="n">
+        <v>25.44</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2905,6 +3037,9 @@
       </c>
       <c r="P58" s="10" t="n">
         <v>15417.29</v>
+      </c>
+      <c r="Q58" s="10" t="n">
+        <v>15415.3</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -2924,6 +3059,7 @@
       <c r="N59" s="7" t="n"/>
       <c r="O59" s="10" t="n"/>
       <c r="P59" s="10" t="n"/>
+      <c r="Q59" s="10" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2974,6 +3110,9 @@
       <c r="P60" s="10" t="n">
         <v>31.16</v>
       </c>
+      <c r="Q60" s="10" t="n">
+        <v>31.16</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3022,6 +3161,7 @@
         <v>17526.85</v>
       </c>
       <c r="P61" s="10" t="inlineStr"/>
+      <c r="Q61" s="10" t="inlineStr"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="1" t="n"/>
@@ -3040,6 +3180,7 @@
       <c r="N62" s="7" t="n"/>
       <c r="O62" s="10" t="n"/>
       <c r="P62" s="10" t="n"/>
+      <c r="Q62" s="10" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3090,6 +3231,9 @@
       <c r="P63" s="10" t="n">
         <v>21.37</v>
       </c>
+      <c r="Q63" s="10" t="n">
+        <v>21.37</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3138,6 +3282,9 @@
         <v>9651.24</v>
       </c>
       <c r="P64" s="10" t="n">
+        <v>9782.639999999999</v>
+      </c>
+      <c r="Q64" s="10" t="n">
         <v>9782.639999999999</v>
       </c>
     </row>
@@ -3158,6 +3305,7 @@
       <c r="N65" s="7" t="n"/>
       <c r="O65" s="10" t="n"/>
       <c r="P65" s="10" t="n"/>
+      <c r="Q65" s="10" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3208,6 +3356,9 @@
       <c r="P66" s="10" t="n">
         <v>13.51</v>
       </c>
+      <c r="Q66" s="10" t="n">
+        <v>13.51</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3256,6 +3407,9 @@
         <v>9776.66</v>
       </c>
       <c r="P67" s="10" t="n">
+        <v>9711.33</v>
+      </c>
+      <c r="Q67" s="10" t="n">
         <v>9711.33</v>
       </c>
     </row>
@@ -3276,6 +3430,7 @@
       <c r="N68" s="7" t="n"/>
       <c r="O68" s="10" t="n"/>
       <c r="P68" s="10" t="n"/>
+      <c r="Q68" s="10" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3326,6 +3481,9 @@
       <c r="P69" s="10" t="n">
         <v>24.01</v>
       </c>
+      <c r="Q69" s="10" t="n">
+        <v>24.01</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3374,6 +3532,7 @@
         <v>2972.4</v>
       </c>
       <c r="P70" s="10" t="inlineStr"/>
+      <c r="Q70" s="10" t="inlineStr"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="1" t="n"/>
@@ -3392,6 +3551,7 @@
       <c r="N71" s="7" t="n"/>
       <c r="O71" s="10" t="n"/>
       <c r="P71" s="10" t="n"/>
+      <c r="Q71" s="10" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3442,6 +3602,9 @@
       <c r="P72" s="10" t="n">
         <v>47.02</v>
       </c>
+      <c r="Q72" s="10" t="n">
+        <v>47.02</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3490,6 +3653,7 @@
         <v>5544.66</v>
       </c>
       <c r="P73" s="10" t="inlineStr"/>
+      <c r="Q73" s="10" t="inlineStr"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="1" t="n"/>
@@ -3508,6 +3672,7 @@
       <c r="N74" s="7" t="n"/>
       <c r="O74" s="10" t="n"/>
       <c r="P74" s="10" t="n"/>
+      <c r="Q74" s="10" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3558,6 +3723,9 @@
       <c r="P75" s="10" t="n">
         <v>24.59</v>
       </c>
+      <c r="Q75" s="10" t="n">
+        <v>24.59</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3606,6 +3774,9 @@
         <v>8989.33</v>
       </c>
       <c r="P76" s="10" t="n">
+        <v>8973.51</v>
+      </c>
+      <c r="Q76" s="10" t="n">
         <v>8973.51</v>
       </c>
     </row>
@@ -3626,6 +3797,7 @@
       <c r="N77" s="7" t="n"/>
       <c r="O77" s="10" t="n"/>
       <c r="P77" s="10" t="n"/>
+      <c r="Q77" s="10" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3676,6 +3848,9 @@
       <c r="P78" s="10" t="n">
         <v>14.59</v>
       </c>
+      <c r="Q78" s="10" t="n">
+        <v>14.59</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3724,6 +3899,9 @@
         <v>1390.11</v>
       </c>
       <c r="P79" s="10" t="n">
+        <v>1413.51</v>
+      </c>
+      <c r="Q79" s="10" t="n">
         <v>1413.51</v>
       </c>
     </row>
@@ -3744,6 +3922,7 @@
       <c r="N80" s="7" t="n"/>
       <c r="O80" s="10" t="n"/>
       <c r="P80" s="10" t="n"/>
+      <c r="Q80" s="10" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3794,6 +3973,9 @@
       <c r="P81" s="10" t="n">
         <v>18.18</v>
       </c>
+      <c r="Q81" s="10" t="n">
+        <v>18.18</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -3842,6 +4024,9 @@
         <v>2785.86</v>
       </c>
       <c r="P82" s="10" t="n">
+        <v>16511.99</v>
+      </c>
+      <c r="Q82" s="10" t="n">
         <v>16511.99</v>
       </c>
     </row>
@@ -3862,6 +4047,7 @@
       <c r="N83" s="7" t="n"/>
       <c r="O83" s="10" t="n"/>
       <c r="P83" s="10" t="n"/>
+      <c r="Q83" s="10" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -3912,6 +4098,9 @@
       <c r="P84" s="10" t="n">
         <v>55</v>
       </c>
+      <c r="Q84" s="10" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -3960,6 +4149,7 @@
         <v>2839.34</v>
       </c>
       <c r="P85" s="10" t="inlineStr"/>
+      <c r="Q85" s="10" t="inlineStr"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="1" t="n"/>
@@ -3978,6 +4168,7 @@
       <c r="N86" s="7" t="n"/>
       <c r="O86" s="10" t="n"/>
       <c r="P86" s="10" t="n"/>
+      <c r="Q86" s="10" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4028,6 +4219,9 @@
       <c r="P87" s="10" t="n">
         <v>58.79</v>
       </c>
+      <c r="Q87" s="10" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4076,6 +4270,9 @@
         <v>2929.31</v>
       </c>
       <c r="P88" s="10" t="n">
+        <v>2867.5</v>
+      </c>
+      <c r="Q88" s="10" t="n">
         <v>2867.5</v>
       </c>
     </row>
@@ -4096,6 +4293,7 @@
       <c r="N89" s="7" t="n"/>
       <c r="O89" s="10" t="n"/>
       <c r="P89" s="10" t="n"/>
+      <c r="Q89" s="10" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -4146,6 +4344,9 @@
       <c r="P90" s="10" t="n">
         <v>51.17</v>
       </c>
+      <c r="Q90" s="10" t="n">
+        <v>51.17</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -4194,6 +4395,9 @@
         <v>1980.68</v>
       </c>
       <c r="P91" s="10" t="n">
+        <v>2891.55</v>
+      </c>
+      <c r="Q91" s="10" t="n">
         <v>2891.55</v>
       </c>
     </row>
@@ -4214,6 +4418,7 @@
       <c r="N92" s="7" t="n"/>
       <c r="O92" s="10" t="n"/>
       <c r="P92" s="10" t="n"/>
+      <c r="Q92" s="10" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4264,6 +4469,9 @@
       <c r="P93" s="10" t="n">
         <v>43.2</v>
       </c>
+      <c r="Q93" s="10" t="n">
+        <v>43.2</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -4312,6 +4520,9 @@
         <v>13120.76</v>
       </c>
       <c r="P94" s="10" t="n">
+        <v>1974.54</v>
+      </c>
+      <c r="Q94" s="10" t="n">
         <v>1974.54</v>
       </c>
     </row>
@@ -4332,6 +4543,7 @@
       <c r="N95" s="7" t="n"/>
       <c r="O95" s="10" t="n"/>
       <c r="P95" s="10" t="n"/>
+      <c r="Q95" s="10" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -4382,6 +4594,9 @@
       <c r="P96" s="10" t="n">
         <v>26.88</v>
       </c>
+      <c r="Q96" s="10" t="n">
+        <v>26.88</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -4430,6 +4645,9 @@
         <v>8969.84</v>
       </c>
       <c r="P97" s="10" t="n">
+        <v>9942.059999999999</v>
+      </c>
+      <c r="Q97" s="10" t="n">
         <v>9942.059999999999</v>
       </c>
     </row>
@@ -4450,6 +4668,7 @@
       <c r="N98" s="7" t="n"/>
       <c r="O98" s="10" t="n"/>
       <c r="P98" s="10" t="n"/>
+      <c r="Q98" s="10" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -4500,6 +4719,9 @@
       <c r="P99" s="10" t="n">
         <v>85.97</v>
       </c>
+      <c r="Q99" s="10" t="n">
+        <v>85.97</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -4549,6 +4771,9 @@
       </c>
       <c r="P100" s="10" t="n">
         <v>9044.780000000001</v>
+      </c>
+      <c r="Q100" s="10" t="n">
+        <v>9065.18</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -4568,6 +4793,7 @@
       <c r="N101" s="7" t="n"/>
       <c r="O101" s="10" t="n"/>
       <c r="P101" s="10" t="n"/>
+      <c r="Q101" s="10" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -4618,6 +4844,9 @@
       <c r="P102" s="10" t="n">
         <v>57.07</v>
       </c>
+      <c r="Q102" s="10" t="n">
+        <v>57.07</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -4666,6 +4895,7 @@
         <v>2193.69</v>
       </c>
       <c r="P103" s="10" t="inlineStr"/>
+      <c r="Q103" s="10" t="inlineStr"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="n"/>
@@ -4684,6 +4914,7 @@
       <c r="N104" s="7" t="n"/>
       <c r="O104" s="10" t="n"/>
       <c r="P104" s="10" t="n"/>
+      <c r="Q104" s="10" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -4734,6 +4965,9 @@
       <c r="P105" s="10" t="n">
         <v>5.43</v>
       </c>
+      <c r="Q105" s="10" t="n">
+        <v>5.43</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -4782,6 +5016,9 @@
         <v>843.17</v>
       </c>
       <c r="P106" s="10" t="n">
+        <v>2211.46</v>
+      </c>
+      <c r="Q106" s="10" t="n">
         <v>2211.46</v>
       </c>
     </row>
@@ -4802,6 +5039,7 @@
       <c r="N107" s="7" t="n"/>
       <c r="O107" s="10" t="n"/>
       <c r="P107" s="10" t="n"/>
+      <c r="Q107" s="10" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -4852,6 +5090,9 @@
       <c r="P108" s="10" t="n">
         <v>25.49</v>
       </c>
+      <c r="Q108" s="10" t="n">
+        <v>25.49</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -4900,6 +5141,7 @@
         <v>2820.56</v>
       </c>
       <c r="P109" s="10" t="inlineStr"/>
+      <c r="Q109" s="10" t="inlineStr"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="1" t="n"/>
@@ -4918,6 +5160,7 @@
       <c r="N110" s="7" t="n"/>
       <c r="O110" s="10" t="n"/>
       <c r="P110" s="10" t="n"/>
+      <c r="Q110" s="10" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -4968,6 +5211,9 @@
       <c r="P111" s="10" t="n">
         <v>29.86</v>
       </c>
+      <c r="Q111" s="10" t="n">
+        <v>29.86</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -5016,6 +5262,9 @@
         <v>3838.51</v>
       </c>
       <c r="P112" s="10" t="n">
+        <v>2840.6</v>
+      </c>
+      <c r="Q112" s="10" t="n">
         <v>2840.6</v>
       </c>
     </row>
@@ -5036,6 +5285,7 @@
       <c r="N113" s="7" t="n"/>
       <c r="O113" s="10" t="n"/>
       <c r="P113" s="10" t="n"/>
+      <c r="Q113" s="10" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -5086,6 +5336,9 @@
       <c r="P114" s="10" t="n">
         <v>20.31</v>
       </c>
+      <c r="Q114" s="10" t="n">
+        <v>20.31</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -5134,18 +5387,26 @@
         <v>3131.36</v>
       </c>
       <c r="P115" s="10" t="inlineStr"/>
+      <c r="Q115" s="10" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="P116" s="10" t="n"/>
+      <c r="Q116" s="10" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="10" t="n">
         <v>29.02</v>
       </c>
+      <c r="Q117" s="10" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="10" t="n">
         <v>2959.6</v>
+      </c>
+      <c r="Q118" s="10" t="n">
+        <v>2958.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-15 01:42:17]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -497,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q118"/>
+  <dimension ref="A1:R118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
@@ -522,6 +522,7 @@
     <col width="15" customWidth="1" min="15" max="15"/>
     <col width="15" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -610,6 +611,11 @@
           <t>2025/12/15</t>
         </is>
       </c>
+      <c r="R1" s="10" t="inlineStr">
+        <is>
+          <t>2025/12/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -697,6 +703,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="R2" s="11" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -750,6 +761,9 @@
       <c r="Q3" s="10" t="n">
         <v>61.22</v>
       </c>
+      <c r="R3" s="10" t="n">
+        <v>61.22</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -802,6 +816,9 @@
       </c>
       <c r="Q4" s="10" t="n">
         <v>3884.54</v>
+      </c>
+      <c r="R4" s="10" t="n">
+        <v>3873.31</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -822,6 +839,7 @@
       <c r="O5" s="10" t="n"/>
       <c r="P5" s="10" t="n"/>
       <c r="Q5" s="10" t="n"/>
+      <c r="R5" s="10" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -875,6 +893,9 @@
       <c r="Q6" s="10" t="n">
         <v>48.25</v>
       </c>
+      <c r="R6" s="10" t="n">
+        <v>48.25</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -927,6 +948,9 @@
       </c>
       <c r="Q7" s="10" t="n">
         <v>5528.82</v>
+      </c>
+      <c r="R7" s="10" t="n">
+        <v>5518.58</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -947,6 +971,7 @@
       <c r="O8" s="10" t="n"/>
       <c r="P8" s="10" t="n"/>
       <c r="Q8" s="10" t="n"/>
+      <c r="R8" s="10" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1000,6 +1025,9 @@
       <c r="Q9" s="10" t="n">
         <v>52.53</v>
       </c>
+      <c r="R9" s="10" t="n">
+        <v>52.53</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1052,6 +1080,9 @@
       </c>
       <c r="Q10" s="10" t="n">
         <v>4579.49</v>
+      </c>
+      <c r="R10" s="10" t="n">
+        <v>4575.61</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1072,6 +1103,7 @@
       <c r="O11" s="10" t="n"/>
       <c r="P11" s="10" t="n"/>
       <c r="Q11" s="10" t="n"/>
+      <c r="R11" s="10" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1125,6 +1157,9 @@
       <c r="Q12" s="10" t="n">
         <v>56.78</v>
       </c>
+      <c r="R12" s="10" t="n">
+        <v>56.78</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1177,6 +1212,9 @@
       </c>
       <c r="Q13" s="10" t="n">
         <v>7169.64</v>
+      </c>
+      <c r="R13" s="10" t="n">
+        <v>7131.63</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1197,6 +1235,7 @@
       <c r="O14" s="10" t="n"/>
       <c r="P14" s="10" t="n"/>
       <c r="Q14" s="10" t="n"/>
+      <c r="R14" s="10" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1250,6 +1289,9 @@
       <c r="Q15" s="10" t="n">
         <v>26.32</v>
       </c>
+      <c r="R15" s="10" t="n">
+        <v>26.32</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1301,6 +1343,9 @@
         <v>2672.5</v>
       </c>
       <c r="Q16" s="10" t="n">
+        <v>2672.5</v>
+      </c>
+      <c r="R16" s="10" t="n">
         <v>2672.5</v>
       </c>
     </row>
@@ -1322,6 +1367,7 @@
       <c r="O17" s="10" t="n"/>
       <c r="P17" s="10" t="n"/>
       <c r="Q17" s="10" t="n"/>
+      <c r="R17" s="10" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1375,6 +1421,9 @@
       <c r="Q18" s="10" t="n">
         <v>96.41</v>
       </c>
+      <c r="R18" s="10" t="n">
+        <v>96.41</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1426,6 +1475,9 @@
         <v>6827.41</v>
       </c>
       <c r="Q19" s="10" t="n">
+        <v>6827.41</v>
+      </c>
+      <c r="R19" s="10" t="n">
         <v>6827.41</v>
       </c>
     </row>
@@ -1447,6 +1499,7 @@
       <c r="O20" s="10" t="n"/>
       <c r="P20" s="10" t="n"/>
       <c r="Q20" s="10" t="n"/>
+      <c r="R20" s="10" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1500,6 +1553,9 @@
       <c r="Q21" s="10" t="n">
         <v>68.42</v>
       </c>
+      <c r="R21" s="10" t="n">
+        <v>68.42</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1551,6 +1607,9 @@
         <v>85267.66</v>
       </c>
       <c r="Q22" s="10" t="n">
+        <v>85267.66</v>
+      </c>
+      <c r="R22" s="10" t="n">
         <v>85267.66</v>
       </c>
     </row>
@@ -1572,6 +1631,7 @@
       <c r="O23" s="10" t="n"/>
       <c r="P23" s="10" t="n"/>
       <c r="Q23" s="10" t="n"/>
+      <c r="R23" s="10" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1625,6 +1685,9 @@
       <c r="Q24" s="10" t="n">
         <v>84.69</v>
       </c>
+      <c r="R24" s="10" t="n">
+        <v>84.69</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1676,6 +1739,9 @@
         <v>24186.49</v>
       </c>
       <c r="Q25" s="10" t="n">
+        <v>24186.49</v>
+      </c>
+      <c r="R25" s="10" t="n">
         <v>24186.49</v>
       </c>
     </row>
@@ -1697,6 +1763,7 @@
       <c r="O26" s="10" t="n"/>
       <c r="P26" s="10" t="n"/>
       <c r="Q26" s="10" t="n"/>
+      <c r="R26" s="10" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1750,6 +1817,9 @@
       <c r="Q27" s="10" t="n">
         <v>69.69</v>
       </c>
+      <c r="R27" s="10" t="n">
+        <v>69.69</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1802,6 +1872,9 @@
       </c>
       <c r="Q28" s="10" t="n">
         <v>50254.99</v>
+      </c>
+      <c r="R28" s="10" t="n">
+        <v>50176.2</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1822,6 +1895,7 @@
       <c r="O29" s="10" t="n"/>
       <c r="P29" s="10" t="n"/>
       <c r="Q29" s="10" t="n"/>
+      <c r="R29" s="10" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1875,6 +1949,9 @@
       <c r="Q30" s="10" t="n">
         <v>49.82</v>
       </c>
+      <c r="R30" s="10" t="n">
+        <v>49.82</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1927,6 +2004,9 @@
       </c>
       <c r="Q31" s="10" t="n">
         <v>5426.72</v>
+      </c>
+      <c r="R31" s="10" t="n">
+        <v>5438.27</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1947,6 +2027,7 @@
       <c r="O32" s="10" t="n"/>
       <c r="P32" s="10" t="n"/>
       <c r="Q32" s="10" t="n"/>
+      <c r="R32" s="10" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2000,6 +2081,9 @@
       <c r="Q33" s="10" t="n">
         <v>8.050000000000001</v>
       </c>
+      <c r="R33" s="10" t="n">
+        <v>8.050000000000001</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2051,6 +2135,9 @@
         <v>31304.53</v>
       </c>
       <c r="Q34" s="10" t="n">
+        <v>31304.53</v>
+      </c>
+      <c r="R34" s="10" t="n">
         <v>31304.53</v>
       </c>
     </row>
@@ -2072,6 +2159,7 @@
       <c r="O35" s="10" t="n"/>
       <c r="P35" s="10" t="n"/>
       <c r="Q35" s="10" t="n"/>
+      <c r="R35" s="10" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2125,6 +2213,9 @@
       <c r="Q36" s="10" t="n">
         <v>29.16</v>
       </c>
+      <c r="R36" s="10" t="n">
+        <v>29.16</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2176,6 +2267,9 @@
         <v>3397.66</v>
       </c>
       <c r="Q37" s="10" t="inlineStr"/>
+      <c r="R37" s="10" t="n">
+        <v>3380.35</v>
+      </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="n"/>
@@ -2195,6 +2289,7 @@
       <c r="O38" s="10" t="n"/>
       <c r="P38" s="10" t="n"/>
       <c r="Q38" s="10" t="n"/>
+      <c r="R38" s="10" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2248,6 +2343,9 @@
       <c r="Q39" s="10" t="n">
         <v>46.99</v>
       </c>
+      <c r="R39" s="10" t="n">
+        <v>46.99</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2299,6 +2397,9 @@
         <v>3194.36</v>
       </c>
       <c r="Q40" s="10" t="inlineStr"/>
+      <c r="R40" s="10" t="n">
+        <v>3176.43</v>
+      </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1" t="n"/>
@@ -2318,6 +2419,7 @@
       <c r="O41" s="10" t="n"/>
       <c r="P41" s="10" t="n"/>
       <c r="Q41" s="10" t="n"/>
+      <c r="R41" s="10" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2371,6 +2473,9 @@
       <c r="Q42" s="10" t="n">
         <v>14.46</v>
       </c>
+      <c r="R42" s="10" t="n">
+        <v>14.46</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2420,6 +2525,9 @@
       </c>
       <c r="P43" s="10" t="inlineStr"/>
       <c r="Q43" s="10" t="inlineStr"/>
+      <c r="R43" s="10" t="n">
+        <v>6827.49</v>
+      </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="n"/>
@@ -2439,6 +2547,7 @@
       <c r="O44" s="10" t="n"/>
       <c r="P44" s="10" t="n"/>
       <c r="Q44" s="10" t="n"/>
+      <c r="R44" s="10" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2492,6 +2601,9 @@
       <c r="Q45" s="10" t="n">
         <v>26.61</v>
       </c>
+      <c r="R45" s="10" t="n">
+        <v>26.61</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2544,6 +2656,9 @@
       </c>
       <c r="Q46" s="10" t="n">
         <v>8478.26</v>
+      </c>
+      <c r="R46" s="10" t="n">
+        <v>8407.51</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2564,6 +2679,7 @@
       <c r="O47" s="10" t="n"/>
       <c r="P47" s="10" t="n"/>
       <c r="Q47" s="10" t="n"/>
+      <c r="R47" s="10" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2617,6 +2733,9 @@
       <c r="Q48" s="10" t="n">
         <v>10.31</v>
       </c>
+      <c r="R48" s="10" t="n">
+        <v>10.31</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2668,6 +2787,9 @@
         <v>12651.28</v>
       </c>
       <c r="Q49" s="10" t="n">
+        <v>12651.28</v>
+      </c>
+      <c r="R49" s="10" t="n">
         <v>12651.28</v>
       </c>
     </row>
@@ -2689,6 +2811,7 @@
       <c r="O50" s="10" t="n"/>
       <c r="P50" s="10" t="n"/>
       <c r="Q50" s="10" t="n"/>
+      <c r="R50" s="10" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2742,6 +2865,9 @@
       <c r="Q51" s="10" t="n">
         <v>24.88</v>
       </c>
+      <c r="R51" s="10" t="n">
+        <v>24.88</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2794,6 +2920,9 @@
       </c>
       <c r="Q52" s="10" t="n">
         <v>12418.82</v>
+      </c>
+      <c r="R52" s="10" t="n">
+        <v>12385.61</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2814,6 +2943,7 @@
       <c r="O53" s="10" t="n"/>
       <c r="P53" s="10" t="n"/>
       <c r="Q53" s="10" t="n"/>
+      <c r="R53" s="10" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2867,6 +2997,9 @@
       <c r="Q54" s="10" t="n">
         <v>19.1</v>
       </c>
+      <c r="R54" s="10" t="n">
+        <v>19.1</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2916,6 +3049,9 @@
       </c>
       <c r="P55" s="10" t="inlineStr"/>
       <c r="Q55" s="10" t="inlineStr"/>
+      <c r="R55" s="10" t="n">
+        <v>9203.370000000001</v>
+      </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="n"/>
@@ -2935,6 +3071,7 @@
       <c r="O56" s="10" t="n"/>
       <c r="P56" s="10" t="n"/>
       <c r="Q56" s="10" t="n"/>
+      <c r="R56" s="10" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2988,6 +3125,9 @@
       <c r="Q57" s="10" t="n">
         <v>25.44</v>
       </c>
+      <c r="R57" s="10" t="n">
+        <v>25.44</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3040,6 +3180,9 @@
       </c>
       <c r="Q58" s="10" t="n">
         <v>15415.3</v>
+      </c>
+      <c r="R58" s="10" t="n">
+        <v>15538.31</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3060,6 +3203,7 @@
       <c r="O59" s="10" t="n"/>
       <c r="P59" s="10" t="n"/>
       <c r="Q59" s="10" t="n"/>
+      <c r="R59" s="10" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3113,6 +3257,9 @@
       <c r="Q60" s="10" t="n">
         <v>31.16</v>
       </c>
+      <c r="R60" s="10" t="n">
+        <v>31.16</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3162,6 +3309,9 @@
       </c>
       <c r="P61" s="10" t="inlineStr"/>
       <c r="Q61" s="10" t="inlineStr"/>
+      <c r="R61" s="10" t="n">
+        <v>15098.39</v>
+      </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="1" t="n"/>
@@ -3181,6 +3331,7 @@
       <c r="O62" s="10" t="n"/>
       <c r="P62" s="10" t="n"/>
       <c r="Q62" s="10" t="n"/>
+      <c r="R62" s="10" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3234,6 +3385,9 @@
       <c r="Q63" s="10" t="n">
         <v>21.37</v>
       </c>
+      <c r="R63" s="10" t="n">
+        <v>21.37</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3285,6 +3439,9 @@
         <v>9782.639999999999</v>
       </c>
       <c r="Q64" s="10" t="n">
+        <v>9782.639999999999</v>
+      </c>
+      <c r="R64" s="10" t="n">
         <v>9782.639999999999</v>
       </c>
     </row>
@@ -3306,6 +3463,7 @@
       <c r="O65" s="10" t="n"/>
       <c r="P65" s="10" t="n"/>
       <c r="Q65" s="10" t="n"/>
+      <c r="R65" s="10" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3359,6 +3517,9 @@
       <c r="Q66" s="10" t="n">
         <v>13.51</v>
       </c>
+      <c r="R66" s="10" t="n">
+        <v>13.51</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3410,6 +3571,9 @@
         <v>9711.33</v>
       </c>
       <c r="Q67" s="10" t="n">
+        <v>9711.33</v>
+      </c>
+      <c r="R67" s="10" t="n">
         <v>9711.33</v>
       </c>
     </row>
@@ -3431,6 +3595,7 @@
       <c r="O68" s="10" t="n"/>
       <c r="P68" s="10" t="n"/>
       <c r="Q68" s="10" t="n"/>
+      <c r="R68" s="10" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3484,6 +3649,9 @@
       <c r="Q69" s="10" t="n">
         <v>24.01</v>
       </c>
+      <c r="R69" s="10" t="n">
+        <v>24.01</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3533,6 +3701,9 @@
       </c>
       <c r="P70" s="10" t="inlineStr"/>
       <c r="Q70" s="10" t="inlineStr"/>
+      <c r="R70" s="10" t="n">
+        <v>2986.6</v>
+      </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="1" t="n"/>
@@ -3552,6 +3723,7 @@
       <c r="O71" s="10" t="n"/>
       <c r="P71" s="10" t="n"/>
       <c r="Q71" s="10" t="n"/>
+      <c r="R71" s="10" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3605,6 +3777,9 @@
       <c r="Q72" s="10" t="n">
         <v>47.02</v>
       </c>
+      <c r="R72" s="10" t="n">
+        <v>47.02</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3654,6 +3829,9 @@
       </c>
       <c r="P73" s="10" t="inlineStr"/>
       <c r="Q73" s="10" t="inlineStr"/>
+      <c r="R73" s="10" t="n">
+        <v>5562.67</v>
+      </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="1" t="n"/>
@@ -3673,6 +3851,7 @@
       <c r="O74" s="10" t="n"/>
       <c r="P74" s="10" t="n"/>
       <c r="Q74" s="10" t="n"/>
+      <c r="R74" s="10" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3726,6 +3905,9 @@
       <c r="Q75" s="10" t="n">
         <v>24.59</v>
       </c>
+      <c r="R75" s="10" t="n">
+        <v>24.59</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3778,6 +3960,9 @@
       </c>
       <c r="Q76" s="10" t="n">
         <v>8973.51</v>
+      </c>
+      <c r="R76" s="10" t="n">
+        <v>8916.23</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -3798,6 +3983,7 @@
       <c r="O77" s="10" t="n"/>
       <c r="P77" s="10" t="n"/>
       <c r="Q77" s="10" t="n"/>
+      <c r="R77" s="10" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3851,6 +4037,9 @@
       <c r="Q78" s="10" t="n">
         <v>14.59</v>
       </c>
+      <c r="R78" s="10" t="n">
+        <v>14.59</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3902,6 +4091,9 @@
         <v>1413.51</v>
       </c>
       <c r="Q79" s="10" t="n">
+        <v>1413.51</v>
+      </c>
+      <c r="R79" s="10" t="n">
         <v>1413.51</v>
       </c>
     </row>
@@ -3923,6 +4115,7 @@
       <c r="O80" s="10" t="n"/>
       <c r="P80" s="10" t="n"/>
       <c r="Q80" s="10" t="n"/>
+      <c r="R80" s="10" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3976,6 +4169,9 @@
       <c r="Q81" s="10" t="n">
         <v>18.18</v>
       </c>
+      <c r="R81" s="10" t="n">
+        <v>18.18</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -4027,6 +4223,9 @@
         <v>16511.99</v>
       </c>
       <c r="Q82" s="10" t="n">
+        <v>16511.99</v>
+      </c>
+      <c r="R82" s="10" t="n">
         <v>16511.99</v>
       </c>
     </row>
@@ -4048,6 +4247,7 @@
       <c r="O83" s="10" t="n"/>
       <c r="P83" s="10" t="n"/>
       <c r="Q83" s="10" t="n"/>
+      <c r="R83" s="10" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -4101,6 +4301,9 @@
       <c r="Q84" s="10" t="n">
         <v>55</v>
       </c>
+      <c r="R84" s="10" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -4150,6 +4353,9 @@
       </c>
       <c r="P85" s="10" t="inlineStr"/>
       <c r="Q85" s="10" t="inlineStr"/>
+      <c r="R85" s="10" t="n">
+        <v>2770.6</v>
+      </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="1" t="n"/>
@@ -4169,6 +4375,7 @@
       <c r="O86" s="10" t="n"/>
       <c r="P86" s="10" t="n"/>
       <c r="Q86" s="10" t="n"/>
+      <c r="R86" s="10" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4222,6 +4429,9 @@
       <c r="Q87" s="10" t="n">
         <v>58.79</v>
       </c>
+      <c r="R87" s="10" t="n">
+        <v>58.79</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4273,6 +4483,9 @@
         <v>2867.5</v>
       </c>
       <c r="Q88" s="10" t="n">
+        <v>2867.5</v>
+      </c>
+      <c r="R88" s="10" t="n">
         <v>2867.5</v>
       </c>
     </row>
@@ -4294,6 +4507,7 @@
       <c r="O89" s="10" t="n"/>
       <c r="P89" s="10" t="n"/>
       <c r="Q89" s="10" t="n"/>
+      <c r="R89" s="10" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -4347,6 +4561,9 @@
       <c r="Q90" s="10" t="n">
         <v>51.17</v>
       </c>
+      <c r="R90" s="10" t="n">
+        <v>51.17</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -4398,6 +4615,9 @@
         <v>2891.55</v>
       </c>
       <c r="Q91" s="10" t="n">
+        <v>2891.55</v>
+      </c>
+      <c r="R91" s="10" t="n">
         <v>2891.55</v>
       </c>
     </row>
@@ -4419,6 +4639,7 @@
       <c r="O92" s="10" t="n"/>
       <c r="P92" s="10" t="n"/>
       <c r="Q92" s="10" t="n"/>
+      <c r="R92" s="10" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4472,6 +4693,9 @@
       <c r="Q93" s="10" t="n">
         <v>43.2</v>
       </c>
+      <c r="R93" s="10" t="n">
+        <v>43.2</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -4523,6 +4747,9 @@
         <v>1974.54</v>
       </c>
       <c r="Q94" s="10" t="n">
+        <v>1974.54</v>
+      </c>
+      <c r="R94" s="10" t="n">
         <v>1974.54</v>
       </c>
     </row>
@@ -4544,6 +4771,7 @@
       <c r="O95" s="10" t="n"/>
       <c r="P95" s="10" t="n"/>
       <c r="Q95" s="10" t="n"/>
+      <c r="R95" s="10" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -4597,6 +4825,9 @@
       <c r="Q96" s="10" t="n">
         <v>26.88</v>
       </c>
+      <c r="R96" s="10" t="n">
+        <v>26.88</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -4648,6 +4879,9 @@
         <v>9942.059999999999</v>
       </c>
       <c r="Q97" s="10" t="n">
+        <v>9942.059999999999</v>
+      </c>
+      <c r="R97" s="10" t="n">
         <v>9942.059999999999</v>
       </c>
     </row>
@@ -4669,6 +4903,7 @@
       <c r="O98" s="10" t="n"/>
       <c r="P98" s="10" t="n"/>
       <c r="Q98" s="10" t="n"/>
+      <c r="R98" s="10" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -4722,6 +4957,9 @@
       <c r="Q99" s="10" t="n">
         <v>85.97</v>
       </c>
+      <c r="R99" s="10" t="n">
+        <v>85.97</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -4774,6 +5012,9 @@
       </c>
       <c r="Q100" s="10" t="n">
         <v>9065.18</v>
+      </c>
+      <c r="R100" s="10" t="n">
+        <v>9044.780000000001</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -4794,6 +5035,7 @@
       <c r="O101" s="10" t="n"/>
       <c r="P101" s="10" t="n"/>
       <c r="Q101" s="10" t="n"/>
+      <c r="R101" s="10" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -4847,6 +5089,9 @@
       <c r="Q102" s="10" t="n">
         <v>57.07</v>
       </c>
+      <c r="R102" s="10" t="n">
+        <v>57.07</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -4896,6 +5141,9 @@
       </c>
       <c r="P103" s="10" t="inlineStr"/>
       <c r="Q103" s="10" t="inlineStr"/>
+      <c r="R103" s="10" t="n">
+        <v>12521.82</v>
+      </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="n"/>
@@ -4915,6 +5163,7 @@
       <c r="O104" s="10" t="n"/>
       <c r="P104" s="10" t="n"/>
       <c r="Q104" s="10" t="n"/>
+      <c r="R104" s="10" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -4968,6 +5217,9 @@
       <c r="Q105" s="10" t="n">
         <v>5.43</v>
       </c>
+      <c r="R105" s="10" t="n">
+        <v>5.43</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -5019,6 +5271,9 @@
         <v>2211.46</v>
       </c>
       <c r="Q106" s="10" t="n">
+        <v>2211.46</v>
+      </c>
+      <c r="R106" s="10" t="n">
         <v>2211.46</v>
       </c>
     </row>
@@ -5040,6 +5295,7 @@
       <c r="O107" s="10" t="n"/>
       <c r="P107" s="10" t="n"/>
       <c r="Q107" s="10" t="n"/>
+      <c r="R107" s="10" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -5093,6 +5349,9 @@
       <c r="Q108" s="10" t="n">
         <v>25.49</v>
       </c>
+      <c r="R108" s="10" t="n">
+        <v>25.49</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -5142,6 +5401,9 @@
       </c>
       <c r="P109" s="10" t="inlineStr"/>
       <c r="Q109" s="10" t="inlineStr"/>
+      <c r="R109" s="10" t="n">
+        <v>841.09</v>
+      </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="1" t="n"/>
@@ -5161,6 +5423,7 @@
       <c r="O110" s="10" t="n"/>
       <c r="P110" s="10" t="n"/>
       <c r="Q110" s="10" t="n"/>
+      <c r="R110" s="10" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -5214,6 +5477,9 @@
       <c r="Q111" s="10" t="n">
         <v>29.86</v>
       </c>
+      <c r="R111" s="10" t="n">
+        <v>29.86</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -5265,6 +5531,9 @@
         <v>2840.6</v>
       </c>
       <c r="Q112" s="10" t="n">
+        <v>2840.6</v>
+      </c>
+      <c r="R112" s="10" t="n">
         <v>2840.6</v>
       </c>
     </row>
@@ -5286,6 +5555,7 @@
       <c r="O113" s="10" t="n"/>
       <c r="P113" s="10" t="n"/>
       <c r="Q113" s="10" t="n"/>
+      <c r="R113" s="10" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -5339,6 +5609,9 @@
       <c r="Q114" s="10" t="n">
         <v>20.31</v>
       </c>
+      <c r="R114" s="10" t="n">
+        <v>20.31</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -5388,10 +5661,14 @@
       </c>
       <c r="P115" s="10" t="inlineStr"/>
       <c r="Q115" s="10" t="inlineStr"/>
+      <c r="R115" s="10" t="n">
+        <v>3840.85</v>
+      </c>
     </row>
     <row r="116">
       <c r="P116" s="10" t="n"/>
       <c r="Q116" s="10" t="n"/>
+      <c r="R116" s="10" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="10" t="n">
@@ -5400,6 +5677,9 @@
       <c r="Q117" s="10" t="n">
         <v>29.02</v>
       </c>
+      <c r="R117" s="10" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="10" t="n">
@@ -5407,6 +5687,9 @@
       </c>
       <c r="Q118" s="10" t="n">
         <v>2958.04</v>
+      </c>
+      <c r="R118" s="10" t="n">
+        <v>2932.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-18 04:10:00]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P118"/>
+  <dimension ref="A1:Q118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -538,6 +538,7 @@
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="15" customWidth="1" min="15" max="15"/>
     <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="15" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -621,6 +622,11 @@
           <t>2025/12/15</t>
         </is>
       </c>
+      <c r="Q1" s="13" t="inlineStr">
+        <is>
+          <t>2025/12/18</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -703,6 +709,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="Q2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -753,6 +764,9 @@
       <c r="P3" s="13" t="n">
         <v>61.22</v>
       </c>
+      <c r="Q3" s="13" t="n">
+        <v>60.92</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -802,6 +816,9 @@
       </c>
       <c r="P4" s="13" t="n">
         <v>3884.93</v>
+      </c>
+      <c r="Q4" s="13" t="n">
+        <v>3876.4</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -821,6 +838,7 @@
       <c r="N5" s="7" t="n"/>
       <c r="O5" s="10" t="n"/>
       <c r="P5" s="13" t="n"/>
+      <c r="Q5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -871,6 +889,9 @@
       <c r="P6" s="13" t="n">
         <v>48.25</v>
       </c>
+      <c r="Q6" s="13" t="n">
+        <v>48.98</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -920,6 +941,9 @@
       </c>
       <c r="P7" s="13" t="n">
         <v>5512.48</v>
+      </c>
+      <c r="Q7" s="13" t="n">
+        <v>5496.6</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -939,6 +963,7 @@
       <c r="N8" s="7" t="n"/>
       <c r="O8" s="10" t="n"/>
       <c r="P8" s="13" t="n"/>
+      <c r="Q8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -989,6 +1014,9 @@
       <c r="P9" s="13" t="n">
         <v>52.53</v>
       </c>
+      <c r="Q9" s="13" t="n">
+        <v>52.75</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1038,6 +1066,9 @@
       </c>
       <c r="P10" s="13" t="n">
         <v>4573.3</v>
+      </c>
+      <c r="Q10" s="13" t="n">
+        <v>4554.12</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1057,6 +1088,7 @@
       <c r="N11" s="7" t="n"/>
       <c r="O11" s="10" t="n"/>
       <c r="P11" s="13" t="n"/>
+      <c r="Q11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1107,6 +1139,9 @@
       <c r="P12" s="13" t="n">
         <v>56.78</v>
       </c>
+      <c r="Q12" s="13" t="n">
+        <v>56.44</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1156,6 +1191,9 @@
       </c>
       <c r="P13" s="13" t="n">
         <v>7137.42</v>
+      </c>
+      <c r="Q13" s="13" t="n">
+        <v>7139.53</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1175,6 +1213,7 @@
       <c r="N14" s="7" t="n"/>
       <c r="O14" s="10" t="n"/>
       <c r="P14" s="13" t="n"/>
+      <c r="Q14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1225,6 +1264,9 @@
       <c r="P15" s="13" t="n">
         <v>26.32</v>
       </c>
+      <c r="Q15" s="13" t="n">
+        <v>26.97</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1273,6 +1315,9 @@
         <v>2653.73</v>
       </c>
       <c r="P16" s="13" t="n">
+        <v>2672.5</v>
+      </c>
+      <c r="Q16" s="13" t="n">
         <v>2672.5</v>
       </c>
     </row>
@@ -1293,6 +1338,7 @@
       <c r="N17" s="7" t="n"/>
       <c r="O17" s="10" t="n"/>
       <c r="P17" s="13" t="n"/>
+      <c r="Q17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1343,6 +1389,9 @@
       <c r="P18" s="13" t="n">
         <v>96.41</v>
       </c>
+      <c r="Q18" s="13" t="n">
+        <v>95.75</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1392,6 +1441,9 @@
       </c>
       <c r="P19" s="13" t="n">
         <v>6827.41</v>
+      </c>
+      <c r="Q19" s="13" t="n">
+        <v>6721.43</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1411,6 +1463,7 @@
       <c r="N20" s="7" t="n"/>
       <c r="O20" s="10" t="n"/>
       <c r="P20" s="13" t="n"/>
+      <c r="Q20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1461,6 +1514,9 @@
       <c r="P21" s="13" t="n">
         <v>68.42</v>
       </c>
+      <c r="Q21" s="13" t="n">
+        <v>66.36</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1510,6 +1566,9 @@
       </c>
       <c r="P22" s="13" t="n">
         <v>84933.39999999999</v>
+      </c>
+      <c r="Q22" s="13" t="n">
+        <v>84420.08</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1529,6 +1588,7 @@
       <c r="N23" s="7" t="n"/>
       <c r="O23" s="10" t="n"/>
       <c r="P23" s="13" t="n"/>
+      <c r="Q23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1579,6 +1639,9 @@
       <c r="P24" s="13" t="n">
         <v>84.69</v>
       </c>
+      <c r="Q24" s="13" t="n">
+        <v>84.11</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1628,6 +1691,9 @@
       </c>
       <c r="P25" s="13" t="n">
         <v>24186.49</v>
+      </c>
+      <c r="Q25" s="13" t="n">
+        <v>23960.59</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1647,6 +1713,7 @@
       <c r="N26" s="7" t="n"/>
       <c r="O26" s="10" t="n"/>
       <c r="P26" s="13" t="n"/>
+      <c r="Q26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1697,6 +1764,9 @@
       <c r="P27" s="13" t="n">
         <v>69.69</v>
       </c>
+      <c r="Q27" s="13" t="n">
+        <v>68.27</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1746,6 +1816,9 @@
       </c>
       <c r="P28" s="13" t="n">
         <v>50070.95</v>
+      </c>
+      <c r="Q28" s="13" t="n">
+        <v>48886.03</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1765,6 +1838,7 @@
       <c r="N29" s="7" t="n"/>
       <c r="O29" s="10" t="n"/>
       <c r="P29" s="13" t="n"/>
+      <c r="Q29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1815,6 +1889,9 @@
       <c r="P30" s="13" t="n">
         <v>49.82</v>
       </c>
+      <c r="Q30" s="13" t="n">
+        <v>55.22</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1864,6 +1941,9 @@
       </c>
       <c r="P31" s="13" t="n">
         <v>5473.89</v>
+      </c>
+      <c r="Q31" s="13" t="n">
+        <v>5457.05</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1883,6 +1963,7 @@
       <c r="N32" s="7" t="n"/>
       <c r="O32" s="10" t="n"/>
       <c r="P32" s="13" t="n"/>
+      <c r="Q32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -1933,6 +2014,9 @@
       <c r="P33" s="13" t="n">
         <v>8.050000000000001</v>
       </c>
+      <c r="Q33" s="13" t="n">
+        <v>0.98</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -1982,6 +2066,9 @@
       </c>
       <c r="P34" s="13" t="n">
         <v>31304.53</v>
+      </c>
+      <c r="Q34" s="13" t="n">
+        <v>30886.41</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2001,6 +2088,7 @@
       <c r="N35" s="7" t="n"/>
       <c r="O35" s="10" t="n"/>
       <c r="P35" s="13" t="n"/>
+      <c r="Q35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2051,6 +2139,9 @@
       <c r="P36" s="13" t="n">
         <v>29.16</v>
       </c>
+      <c r="Q36" s="13" t="n">
+        <v>30.1</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2100,6 +2191,9 @@
       </c>
       <c r="P37" s="13" t="n">
         <v>3350.52</v>
+      </c>
+      <c r="Q37" s="13" t="n">
+        <v>3304.59</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2119,6 +2213,7 @@
       <c r="N38" s="7" t="n"/>
       <c r="O38" s="10" t="n"/>
       <c r="P38" s="13" t="n"/>
+      <c r="Q38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2169,6 +2264,9 @@
       <c r="P39" s="13" t="n">
         <v>46.99</v>
       </c>
+      <c r="Q39" s="13" t="n">
+        <v>46.57</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2218,6 +2316,9 @@
       </c>
       <c r="P40" s="13" t="n">
         <v>3153.07</v>
+      </c>
+      <c r="Q40" s="13" t="n">
+        <v>3118.3</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2237,6 +2338,7 @@
       <c r="N41" s="7" t="n"/>
       <c r="O41" s="10" t="n"/>
       <c r="P41" s="13" t="n"/>
+      <c r="Q41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2287,6 +2389,9 @@
       <c r="P42" s="13" t="n">
         <v>14.46</v>
       </c>
+      <c r="Q42" s="13" t="n">
+        <v>16.74</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2336,6 +2441,9 @@
       </c>
       <c r="P43" s="13" t="n">
         <v>6797.23</v>
+      </c>
+      <c r="Q43" s="13" t="n">
+        <v>6880.35</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -2355,6 +2463,7 @@
       <c r="N44" s="7" t="n"/>
       <c r="O44" s="10" t="n"/>
       <c r="P44" s="13" t="n"/>
+      <c r="Q44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2405,6 +2514,9 @@
       <c r="P45" s="13" t="n">
         <v>26.61</v>
       </c>
+      <c r="Q45" s="13" t="n">
+        <v>26.75</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2454,6 +2566,9 @@
       </c>
       <c r="P46" s="13" t="n">
         <v>8371.290000000001</v>
+      </c>
+      <c r="Q46" s="13" t="n">
+        <v>8310.389999999999</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2473,6 +2588,7 @@
       <c r="N47" s="7" t="n"/>
       <c r="O47" s="10" t="n"/>
       <c r="P47" s="13" t="n"/>
+      <c r="Q47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2523,6 +2639,9 @@
       <c r="P48" s="13" t="n">
         <v>10.31</v>
       </c>
+      <c r="Q48" s="13" t="n">
+        <v>7.74</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2572,6 +2691,9 @@
       </c>
       <c r="P49" s="13" t="n">
         <v>12725.66</v>
+      </c>
+      <c r="Q49" s="13" t="n">
+        <v>12652.6</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2591,6 +2713,7 @@
       <c r="N50" s="7" t="n"/>
       <c r="O50" s="10" t="n"/>
       <c r="P50" s="13" t="n"/>
+      <c r="Q50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2641,6 +2764,9 @@
       <c r="P51" s="13" t="n">
         <v>24.88</v>
       </c>
+      <c r="Q51" s="13" t="n">
+        <v>26.35</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2690,6 +2816,9 @@
       </c>
       <c r="P52" s="13" t="n">
         <v>12418.82</v>
+      </c>
+      <c r="Q52" s="13" t="n">
+        <v>12419.7</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2709,6 +2838,7 @@
       <c r="N53" s="7" t="n"/>
       <c r="O53" s="10" t="n"/>
       <c r="P53" s="13" t="n"/>
+      <c r="Q53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2759,6 +2889,9 @@
       <c r="P54" s="13" t="n">
         <v>19.1</v>
       </c>
+      <c r="Q54" s="13" t="n">
+        <v>19.5</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2808,6 +2941,9 @@
       </c>
       <c r="P55" s="13" t="n">
         <v>9177.540000000001</v>
+      </c>
+      <c r="Q55" s="13" t="n">
+        <v>9066.379999999999</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -2827,6 +2963,7 @@
       <c r="N56" s="7" t="n"/>
       <c r="O56" s="10" t="n"/>
       <c r="P56" s="13" t="n"/>
+      <c r="Q56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -2877,6 +3014,9 @@
       <c r="P57" s="13" t="n">
         <v>25.44</v>
       </c>
+      <c r="Q57" s="13" t="n">
+        <v>25.73</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -2926,6 +3066,9 @@
       </c>
       <c r="P58" s="13" t="n">
         <v>15561.4</v>
+      </c>
+      <c r="Q58" s="13" t="n">
+        <v>15498.89</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -2945,6 +3088,7 @@
       <c r="N59" s="7" t="n"/>
       <c r="O59" s="10" t="n"/>
       <c r="P59" s="13" t="n"/>
+      <c r="Q59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -2995,6 +3139,9 @@
       <c r="P60" s="13" t="n">
         <v>31.16</v>
       </c>
+      <c r="Q60" s="13" t="n">
+        <v>30.38</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3044,6 +3191,9 @@
       </c>
       <c r="P61" s="13" t="n">
         <v>14664.43</v>
+      </c>
+      <c r="Q61" s="13" t="n">
+        <v>14701.15</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3063,6 +3213,7 @@
       <c r="N62" s="7" t="n"/>
       <c r="O62" s="10" t="n"/>
       <c r="P62" s="13" t="n"/>
+      <c r="Q62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3113,6 +3264,9 @@
       <c r="P63" s="13" t="n">
         <v>21.37</v>
       </c>
+      <c r="Q63" s="13" t="n">
+        <v>20.2</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3161,6 +3315,9 @@
         <v>9651.24</v>
       </c>
       <c r="P64" s="13" t="n">
+        <v>9782.639999999999</v>
+      </c>
+      <c r="Q64" s="13" t="n">
         <v>9782.639999999999</v>
       </c>
     </row>
@@ -3181,6 +3338,7 @@
       <c r="N65" s="7" t="n"/>
       <c r="O65" s="10" t="n"/>
       <c r="P65" s="13" t="n"/>
+      <c r="Q65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3231,6 +3389,9 @@
       <c r="P66" s="13" t="n">
         <v>13.51</v>
       </c>
+      <c r="Q66" s="13" t="n">
+        <v>12.64</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3280,6 +3441,9 @@
       </c>
       <c r="P67" s="13" t="n">
         <v>9711.33</v>
+      </c>
+      <c r="Q67" s="13" t="n">
+        <v>9623.42</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -3299,6 +3463,7 @@
       <c r="N68" s="7" t="n"/>
       <c r="O68" s="10" t="n"/>
       <c r="P68" s="13" t="n"/>
+      <c r="Q68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3349,6 +3514,9 @@
       <c r="P69" s="13" t="n">
         <v>24.01</v>
       </c>
+      <c r="Q69" s="13" t="n">
+        <v>23.13</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3398,6 +3566,9 @@
       </c>
       <c r="P70" s="13" t="n">
         <v>2970.64</v>
+      </c>
+      <c r="Q70" s="13" t="n">
+        <v>2887.88</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -3417,6 +3588,7 @@
       <c r="N71" s="7" t="n"/>
       <c r="O71" s="10" t="n"/>
       <c r="P71" s="13" t="n"/>
+      <c r="Q71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3467,6 +3639,9 @@
       <c r="P72" s="13" t="n">
         <v>47.02</v>
       </c>
+      <c r="Q72" s="13" t="n">
+        <v>44.62</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3516,6 +3691,9 @@
       </c>
       <c r="P73" s="13" t="n">
         <v>5537.11</v>
+      </c>
+      <c r="Q73" s="13" t="n">
+        <v>5389.42</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -3535,6 +3713,7 @@
       <c r="N74" s="7" t="n"/>
       <c r="O74" s="10" t="n"/>
       <c r="P74" s="13" t="n"/>
+      <c r="Q74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3585,6 +3764,9 @@
       <c r="P75" s="13" t="n">
         <v>24.59</v>
       </c>
+      <c r="Q75" s="13" t="n">
+        <v>24.43</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3634,6 +3816,9 @@
       </c>
       <c r="P76" s="13" t="n">
         <v>8888.92</v>
+      </c>
+      <c r="Q76" s="13" t="n">
+        <v>8847.959999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -3653,6 +3838,7 @@
       <c r="N77" s="7" t="n"/>
       <c r="O77" s="10" t="n"/>
       <c r="P77" s="13" t="n"/>
+      <c r="Q77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3703,6 +3889,9 @@
       <c r="P78" s="13" t="n">
         <v>14.59</v>
       </c>
+      <c r="Q78" s="13" t="n">
+        <v>16.95</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3752,6 +3941,9 @@
       </c>
       <c r="P79" s="13" t="n">
         <v>1413.51</v>
+      </c>
+      <c r="Q79" s="13" t="n">
+        <v>1498.69</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -3771,6 +3963,7 @@
       <c r="N80" s="7" t="n"/>
       <c r="O80" s="10" t="n"/>
       <c r="P80" s="13" t="n"/>
+      <c r="Q80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -3821,6 +4014,9 @@
       <c r="P81" s="13" t="n">
         <v>18.18</v>
       </c>
+      <c r="Q81" s="13" t="n">
+        <v>18.71</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -3870,6 +4066,9 @@
       </c>
       <c r="P82" s="13" t="n">
         <v>16511.99</v>
+      </c>
+      <c r="Q82" s="13" t="n">
+        <v>16696.11</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -3889,6 +4088,7 @@
       <c r="N83" s="7" t="n"/>
       <c r="O83" s="10" t="n"/>
       <c r="P83" s="13" t="n"/>
+      <c r="Q83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -3939,6 +4139,9 @@
       <c r="P84" s="13" t="n">
         <v>55</v>
       </c>
+      <c r="Q84" s="13" t="n">
+        <v>52.42</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -3988,6 +4191,9 @@
       </c>
       <c r="P85" s="13" t="n">
         <v>2731.63</v>
+      </c>
+      <c r="Q85" s="13" t="n">
+        <v>2706.96</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -4007,6 +4213,7 @@
       <c r="N86" s="7" t="n"/>
       <c r="O86" s="10" t="n"/>
       <c r="P86" s="13" t="n"/>
+      <c r="Q86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4057,6 +4264,9 @@
       <c r="P87" s="13" t="n">
         <v>58.79</v>
       </c>
+      <c r="Q87" s="13" t="n">
+        <v>58.66</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4106,6 +4316,9 @@
       </c>
       <c r="P88" s="13" t="n">
         <v>2867.5</v>
+      </c>
+      <c r="Q88" s="13" t="n">
+        <v>2775.73</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -4125,6 +4338,7 @@
       <c r="N89" s="7" t="n"/>
       <c r="O89" s="10" t="n"/>
       <c r="P89" s="13" t="n"/>
+      <c r="Q89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -4175,6 +4389,9 @@
       <c r="P90" s="13" t="n">
         <v>51.17</v>
       </c>
+      <c r="Q90" s="13" t="n">
+        <v>50.01</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -4224,6 +4441,9 @@
       </c>
       <c r="P91" s="13" t="n">
         <v>2891.55</v>
+      </c>
+      <c r="Q91" s="13" t="n">
+        <v>2873.72</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -4243,6 +4463,7 @@
       <c r="N92" s="7" t="n"/>
       <c r="O92" s="10" t="n"/>
       <c r="P92" s="13" t="n"/>
+      <c r="Q92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4293,6 +4514,9 @@
       <c r="P93" s="13" t="n">
         <v>43.2</v>
       </c>
+      <c r="Q93" s="13" t="n">
+        <v>44.19</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -4341,6 +4565,9 @@
         <v>13120.76</v>
       </c>
       <c r="P94" s="13" t="n">
+        <v>1974.54</v>
+      </c>
+      <c r="Q94" s="13" t="n">
         <v>1974.54</v>
       </c>
     </row>
@@ -4361,6 +4588,7 @@
       <c r="N95" s="7" t="n"/>
       <c r="O95" s="10" t="n"/>
       <c r="P95" s="13" t="n"/>
+      <c r="Q95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -4411,6 +4639,9 @@
       <c r="P96" s="13" t="n">
         <v>26.88</v>
       </c>
+      <c r="Q96" s="13" t="n">
+        <v>26.56</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -4460,6 +4691,9 @@
       </c>
       <c r="P97" s="13" t="n">
         <v>9945.110000000001</v>
+      </c>
+      <c r="Q97" s="13" t="n">
+        <v>9997.530000000001</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -4479,6 +4713,7 @@
       <c r="N98" s="7" t="n"/>
       <c r="O98" s="10" t="n"/>
       <c r="P98" s="13" t="n"/>
+      <c r="Q98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -4529,6 +4764,9 @@
       <c r="P99" s="13" t="n">
         <v>85.97</v>
       </c>
+      <c r="Q99" s="13" t="n">
+        <v>84.42</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -4578,6 +4816,9 @@
       </c>
       <c r="P100" s="13" t="n">
         <v>8932.200000000001</v>
+      </c>
+      <c r="Q100" s="13" t="n">
+        <v>8832.940000000001</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -4597,6 +4838,7 @@
       <c r="N101" s="7" t="n"/>
       <c r="O101" s="10" t="n"/>
       <c r="P101" s="13" t="n"/>
+      <c r="Q101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -4647,6 +4889,9 @@
       <c r="P102" s="13" t="n">
         <v>57.07</v>
       </c>
+      <c r="Q102" s="13" t="n">
+        <v>57.1</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -4696,6 +4941,9 @@
       </c>
       <c r="P103" s="13" t="n">
         <v>12727.21</v>
+      </c>
+      <c r="Q103" s="13" t="n">
+        <v>12751.03</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -4715,6 +4963,7 @@
       <c r="N104" s="7" t="n"/>
       <c r="O104" s="10" t="n"/>
       <c r="P104" s="13" t="n"/>
+      <c r="Q104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -4765,6 +5014,9 @@
       <c r="P105" s="13" t="n">
         <v>5.43</v>
       </c>
+      <c r="Q105" s="13" t="n">
+        <v>5.98</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -4813,6 +5065,9 @@
         <v>843.17</v>
       </c>
       <c r="P106" s="13" t="n">
+        <v>2211.46</v>
+      </c>
+      <c r="Q106" s="13" t="n">
         <v>2211.46</v>
       </c>
     </row>
@@ -4833,6 +5088,7 @@
       <c r="N107" s="7" t="n"/>
       <c r="O107" s="10" t="n"/>
       <c r="P107" s="13" t="n"/>
+      <c r="Q107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -4883,6 +5139,9 @@
       <c r="P108" s="13" t="n">
         <v>25.49</v>
       </c>
+      <c r="Q108" s="13" t="n">
+        <v>25.77</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -4932,6 +5191,9 @@
       </c>
       <c r="P109" s="13" t="n">
         <v>850.95</v>
+      </c>
+      <c r="Q109" s="13" t="n">
+        <v>849.5</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -4951,6 +5213,7 @@
       <c r="N110" s="7" t="n"/>
       <c r="O110" s="10" t="n"/>
       <c r="P110" s="13" t="n"/>
+      <c r="Q110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -5001,6 +5264,9 @@
       <c r="P111" s="13" t="n">
         <v>29.86</v>
       </c>
+      <c r="Q111" s="13" t="n">
+        <v>29.84</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -5050,6 +5316,9 @@
       </c>
       <c r="P112" s="13" t="n">
         <v>2840.6</v>
+      </c>
+      <c r="Q112" s="13" t="n">
+        <v>2834.31</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -5069,6 +5338,7 @@
       <c r="N113" s="7" t="n"/>
       <c r="O113" s="10" t="n"/>
       <c r="P113" s="13" t="n"/>
+      <c r="Q113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -5119,6 +5389,9 @@
       <c r="P114" s="13" t="n">
         <v>20.31</v>
       </c>
+      <c r="Q114" s="13" t="n">
+        <v>20.2</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -5169,18 +5442,28 @@
       <c r="P115" s="13" t="n">
         <v>3858.77</v>
       </c>
+      <c r="Q115" s="13" t="n">
+        <v>3830.75</v>
+      </c>
     </row>
     <row r="116">
       <c r="P116" s="13" t="n"/>
+      <c r="Q116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="Q117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
         <v>2932.32</v>
+      </c>
+      <c r="Q118" s="13" t="n">
+        <v>2880.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-22 04:29:53]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q118"/>
+  <dimension ref="A1:R118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -539,6 +539,7 @@
     <col width="15" customWidth="1" min="15" max="15"/>
     <col width="15" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -627,6 +628,11 @@
           <t>2025/12/18</t>
         </is>
       </c>
+      <c r="R1" s="13" t="inlineStr">
+        <is>
+          <t>2025/12/22</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -714,6 +720,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="R2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -767,6 +778,9 @@
       <c r="Q3" s="13" t="n">
         <v>60.92</v>
       </c>
+      <c r="R3" s="13" t="n">
+        <v>61.5</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -819,6 +833,9 @@
       </c>
       <c r="Q4" s="13" t="n">
         <v>3876.4</v>
+      </c>
+      <c r="R4" s="13" t="n">
+        <v>3915.2</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -839,6 +856,7 @@
       <c r="O5" s="10" t="n"/>
       <c r="P5" s="13" t="n"/>
       <c r="Q5" s="13" t="n"/>
+      <c r="R5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -892,6 +910,9 @@
       <c r="Q6" s="13" t="n">
         <v>48.98</v>
       </c>
+      <c r="R6" s="13" t="n">
+        <v>49.01</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -944,6 +965,9 @@
       </c>
       <c r="Q7" s="13" t="n">
         <v>5496.6</v>
+      </c>
+      <c r="R7" s="13" t="n">
+        <v>5574.74</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -964,6 +988,7 @@
       <c r="O8" s="10" t="n"/>
       <c r="P8" s="13" t="n"/>
       <c r="Q8" s="13" t="n"/>
+      <c r="R8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1017,6 +1042,9 @@
       <c r="Q9" s="13" t="n">
         <v>52.75</v>
       </c>
+      <c r="R9" s="13" t="n">
+        <v>52.81</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1069,6 +1097,9 @@
       </c>
       <c r="Q10" s="13" t="n">
         <v>4554.12</v>
+      </c>
+      <c r="R10" s="13" t="n">
+        <v>4604.43</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1089,6 +1120,7 @@
       <c r="O11" s="10" t="n"/>
       <c r="P11" s="13" t="n"/>
       <c r="Q11" s="13" t="n"/>
+      <c r="R11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1142,6 +1174,9 @@
       <c r="Q12" s="13" t="n">
         <v>56.44</v>
       </c>
+      <c r="R12" s="13" t="n">
+        <v>56.7</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1194,6 +1229,9 @@
       </c>
       <c r="Q13" s="13" t="n">
         <v>7139.53</v>
+      </c>
+      <c r="R13" s="13" t="n">
+        <v>7265.85</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1214,6 +1252,7 @@
       <c r="O14" s="10" t="n"/>
       <c r="P14" s="13" t="n"/>
       <c r="Q14" s="13" t="n"/>
+      <c r="R14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1267,6 +1306,9 @@
       <c r="Q15" s="13" t="n">
         <v>26.97</v>
       </c>
+      <c r="R15" s="13" t="n">
+        <v>27.39</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1319,6 +1361,9 @@
       </c>
       <c r="Q16" s="13" t="n">
         <v>2672.5</v>
+      </c>
+      <c r="R16" s="13" t="n">
+        <v>2665.99</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1339,6 +1384,7 @@
       <c r="O17" s="10" t="n"/>
       <c r="P17" s="13" t="n"/>
       <c r="Q17" s="13" t="n"/>
+      <c r="R17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1392,6 +1438,9 @@
       <c r="Q18" s="13" t="n">
         <v>95.75</v>
       </c>
+      <c r="R18" s="13" t="n">
+        <v>96.44</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1444,6 +1493,9 @@
       </c>
       <c r="Q19" s="13" t="n">
         <v>6721.43</v>
+      </c>
+      <c r="R19" s="13" t="n">
+        <v>6834.5</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1464,6 +1516,7 @@
       <c r="O20" s="10" t="n"/>
       <c r="P20" s="13" t="n"/>
       <c r="Q20" s="13" t="n"/>
+      <c r="R20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1517,6 +1570,9 @@
       <c r="Q21" s="13" t="n">
         <v>66.36</v>
       </c>
+      <c r="R21" s="13" t="n">
+        <v>67.09999999999999</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1569,6 +1625,9 @@
       </c>
       <c r="Q22" s="13" t="n">
         <v>84420.08</v>
+      </c>
+      <c r="R22" s="13" t="n">
+        <v>85370.8</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1589,6 +1648,7 @@
       <c r="O23" s="10" t="n"/>
       <c r="P23" s="13" t="n"/>
       <c r="Q23" s="13" t="n"/>
+      <c r="R23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1642,6 +1702,9 @@
       <c r="Q24" s="13" t="n">
         <v>84.11</v>
       </c>
+      <c r="R24" s="13" t="n">
+        <v>84.48</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1694,6 +1757,9 @@
       </c>
       <c r="Q25" s="13" t="n">
         <v>23960.59</v>
+      </c>
+      <c r="R25" s="13" t="n">
+        <v>24288.4</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1714,6 +1780,7 @@
       <c r="O26" s="10" t="n"/>
       <c r="P26" s="13" t="n"/>
       <c r="Q26" s="13" t="n"/>
+      <c r="R26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1767,6 +1834,9 @@
       <c r="Q27" s="13" t="n">
         <v>68.27</v>
       </c>
+      <c r="R27" s="13" t="n">
+        <v>67.42</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1819,6 +1889,9 @@
       </c>
       <c r="Q28" s="13" t="n">
         <v>48886.03</v>
+      </c>
+      <c r="R28" s="13" t="n">
+        <v>50427.56</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1839,6 +1912,7 @@
       <c r="O29" s="10" t="n"/>
       <c r="P29" s="13" t="n"/>
       <c r="Q29" s="13" t="n"/>
+      <c r="R29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1892,6 +1966,9 @@
       <c r="Q30" s="13" t="n">
         <v>55.22</v>
       </c>
+      <c r="R30" s="13" t="n">
+        <v>55.21</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -1944,6 +2021,9 @@
       </c>
       <c r="Q31" s="13" t="n">
         <v>5457.05</v>
+      </c>
+      <c r="R31" s="13" t="n">
+        <v>5465.41</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1964,6 +2044,7 @@
       <c r="O32" s="10" t="n"/>
       <c r="P32" s="13" t="n"/>
       <c r="Q32" s="13" t="n"/>
+      <c r="R32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2017,6 +2098,9 @@
       <c r="Q33" s="13" t="n">
         <v>0.98</v>
       </c>
+      <c r="R33" s="13" t="n">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2068,6 +2152,9 @@
         <v>31304.53</v>
       </c>
       <c r="Q34" s="13" t="n">
+        <v>30886.41</v>
+      </c>
+      <c r="R34" s="13" t="n">
         <v>30886.41</v>
       </c>
     </row>
@@ -2089,6 +2176,7 @@
       <c r="O35" s="10" t="n"/>
       <c r="P35" s="13" t="n"/>
       <c r="Q35" s="13" t="n"/>
+      <c r="R35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2142,6 +2230,9 @@
       <c r="Q36" s="13" t="n">
         <v>30.1</v>
       </c>
+      <c r="R36" s="13" t="n">
+        <v>29.21</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2194,6 +2285,9 @@
       </c>
       <c r="Q37" s="13" t="n">
         <v>3304.59</v>
+      </c>
+      <c r="R37" s="13" t="n">
+        <v>3371.14</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2214,6 +2308,7 @@
       <c r="O38" s="10" t="n"/>
       <c r="P38" s="13" t="n"/>
       <c r="Q38" s="13" t="n"/>
+      <c r="R38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2267,6 +2362,9 @@
       <c r="Q39" s="13" t="n">
         <v>46.57</v>
       </c>
+      <c r="R39" s="13" t="n">
+        <v>45.72</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2319,6 +2417,9 @@
       </c>
       <c r="Q40" s="13" t="n">
         <v>3118.3</v>
+      </c>
+      <c r="R40" s="13" t="n">
+        <v>3178.51</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2339,6 +2440,7 @@
       <c r="O41" s="10" t="n"/>
       <c r="P41" s="13" t="n"/>
       <c r="Q41" s="13" t="n"/>
+      <c r="R41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2392,6 +2494,9 @@
       <c r="Q42" s="13" t="n">
         <v>16.74</v>
       </c>
+      <c r="R42" s="13" t="n">
+        <v>17.69</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2444,6 +2549,9 @@
       </c>
       <c r="Q43" s="13" t="n">
         <v>6880.35</v>
+      </c>
+      <c r="R43" s="13" t="n">
+        <v>6912.21</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -2464,6 +2572,7 @@
       <c r="O44" s="10" t="n"/>
       <c r="P44" s="13" t="n"/>
       <c r="Q44" s="13" t="n"/>
+      <c r="R44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2517,6 +2626,9 @@
       <c r="Q45" s="13" t="n">
         <v>26.75</v>
       </c>
+      <c r="R45" s="13" t="n">
+        <v>27.94</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2569,6 +2681,9 @@
       </c>
       <c r="Q46" s="13" t="n">
         <v>8310.389999999999</v>
+      </c>
+      <c r="R46" s="13" t="n">
+        <v>8390.75</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2589,6 +2704,7 @@
       <c r="O47" s="10" t="n"/>
       <c r="P47" s="13" t="n"/>
       <c r="Q47" s="13" t="n"/>
+      <c r="R47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2642,6 +2758,9 @@
       <c r="Q48" s="13" t="n">
         <v>7.74</v>
       </c>
+      <c r="R48" s="13" t="n">
+        <v>7.59</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2694,6 +2813,9 @@
       </c>
       <c r="Q49" s="13" t="n">
         <v>12652.6</v>
+      </c>
+      <c r="R49" s="13" t="n">
+        <v>12771.22</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2714,6 +2836,7 @@
       <c r="O50" s="10" t="n"/>
       <c r="P50" s="13" t="n"/>
       <c r="Q50" s="13" t="n"/>
+      <c r="R50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2767,6 +2890,9 @@
       <c r="Q51" s="13" t="n">
         <v>26.35</v>
       </c>
+      <c r="R51" s="13" t="n">
+        <v>26.04</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2819,6 +2945,9 @@
       </c>
       <c r="Q52" s="13" t="n">
         <v>12419.7</v>
+      </c>
+      <c r="R52" s="13" t="n">
+        <v>12457.91</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2839,6 +2968,7 @@
       <c r="O53" s="10" t="n"/>
       <c r="P53" s="13" t="n"/>
       <c r="Q53" s="13" t="n"/>
+      <c r="R53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -2892,6 +3022,9 @@
       <c r="Q54" s="13" t="n">
         <v>19.5</v>
       </c>
+      <c r="R54" s="13" t="n">
+        <v>18.52</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -2944,6 +3077,9 @@
       </c>
       <c r="Q55" s="13" t="n">
         <v>9066.379999999999</v>
+      </c>
+      <c r="R55" s="13" t="n">
+        <v>9089.52</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -2964,6 +3100,7 @@
       <c r="O56" s="10" t="n"/>
       <c r="P56" s="13" t="n"/>
       <c r="Q56" s="13" t="n"/>
+      <c r="R56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3017,6 +3154,9 @@
       <c r="Q57" s="13" t="n">
         <v>25.73</v>
       </c>
+      <c r="R57" s="13" t="n">
+        <v>25.54</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3069,6 +3209,9 @@
       </c>
       <c r="Q58" s="13" t="n">
         <v>15498.89</v>
+      </c>
+      <c r="R58" s="13" t="n">
+        <v>15544.96</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3089,6 +3232,7 @@
       <c r="O59" s="10" t="n"/>
       <c r="P59" s="13" t="n"/>
       <c r="Q59" s="13" t="n"/>
+      <c r="R59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3142,6 +3286,9 @@
       <c r="Q60" s="13" t="n">
         <v>30.38</v>
       </c>
+      <c r="R60" s="13" t="n">
+        <v>30.75</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3194,6 +3341,9 @@
       </c>
       <c r="Q61" s="13" t="n">
         <v>14701.15</v>
+      </c>
+      <c r="R61" s="13" t="n">
+        <v>14813.29</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3214,6 +3364,7 @@
       <c r="O62" s="10" t="n"/>
       <c r="P62" s="13" t="n"/>
       <c r="Q62" s="13" t="n"/>
+      <c r="R62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3267,6 +3418,9 @@
       <c r="Q63" s="13" t="n">
         <v>20.2</v>
       </c>
+      <c r="R63" s="13" t="n">
+        <v>20.44</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3319,6 +3473,9 @@
       </c>
       <c r="Q64" s="13" t="n">
         <v>9782.639999999999</v>
+      </c>
+      <c r="R64" s="13" t="n">
+        <v>9525.889999999999</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -3339,6 +3496,7 @@
       <c r="O65" s="10" t="n"/>
       <c r="P65" s="13" t="n"/>
       <c r="Q65" s="13" t="n"/>
+      <c r="R65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3392,6 +3550,9 @@
       <c r="Q66" s="13" t="n">
         <v>12.64</v>
       </c>
+      <c r="R66" s="13" t="n">
+        <v>13.41</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3444,6 +3605,9 @@
       </c>
       <c r="Q67" s="13" t="n">
         <v>9623.42</v>
+      </c>
+      <c r="R67" s="13" t="n">
+        <v>9701.17</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -3464,6 +3628,7 @@
       <c r="O68" s="10" t="n"/>
       <c r="P68" s="13" t="n"/>
       <c r="Q68" s="13" t="n"/>
+      <c r="R68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3517,6 +3682,9 @@
       <c r="Q69" s="13" t="n">
         <v>23.13</v>
       </c>
+      <c r="R69" s="13" t="n">
+        <v>23.32</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3569,6 +3737,9 @@
       </c>
       <c r="Q70" s="13" t="n">
         <v>2887.88</v>
+      </c>
+      <c r="R70" s="13" t="n">
+        <v>2952.44</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -3589,6 +3760,7 @@
       <c r="O71" s="10" t="n"/>
       <c r="P71" s="13" t="n"/>
       <c r="Q71" s="13" t="n"/>
+      <c r="R71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3642,6 +3814,9 @@
       <c r="Q72" s="13" t="n">
         <v>44.62</v>
       </c>
+      <c r="R72" s="13" t="n">
+        <v>45.05</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3694,6 +3869,9 @@
       </c>
       <c r="Q73" s="13" t="n">
         <v>5389.42</v>
+      </c>
+      <c r="R73" s="13" t="n">
+        <v>5528.05</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -3714,6 +3892,7 @@
       <c r="O74" s="10" t="n"/>
       <c r="P74" s="13" t="n"/>
       <c r="Q74" s="13" t="n"/>
+      <c r="R74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3767,6 +3946,9 @@
       <c r="Q75" s="13" t="n">
         <v>24.43</v>
       </c>
+      <c r="R75" s="13" t="n">
+        <v>25.29</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -3819,6 +4001,9 @@
       </c>
       <c r="Q76" s="13" t="n">
         <v>8847.959999999999</v>
+      </c>
+      <c r="R76" s="13" t="n">
+        <v>8935.959999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -3839,6 +4024,7 @@
       <c r="O77" s="10" t="n"/>
       <c r="P77" s="13" t="n"/>
       <c r="Q77" s="13" t="n"/>
+      <c r="R77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -3892,6 +4078,9 @@
       <c r="Q78" s="13" t="n">
         <v>16.95</v>
       </c>
+      <c r="R78" s="13" t="n">
+        <v>17.3</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -3944,6 +4133,9 @@
       </c>
       <c r="Q79" s="13" t="n">
         <v>1498.69</v>
+      </c>
+      <c r="R79" s="13" t="n">
+        <v>1512.82</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -3964,6 +4156,7 @@
       <c r="O80" s="10" t="n"/>
       <c r="P80" s="13" t="n"/>
       <c r="Q80" s="13" t="n"/>
+      <c r="R80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -4017,6 +4210,9 @@
       <c r="Q81" s="13" t="n">
         <v>18.71</v>
       </c>
+      <c r="R81" s="13" t="n">
+        <v>18.7</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -4069,6 +4265,9 @@
       </c>
       <c r="Q82" s="13" t="n">
         <v>16696.11</v>
+      </c>
+      <c r="R82" s="13" t="n">
+        <v>16685.08</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -4089,6 +4288,7 @@
       <c r="O83" s="10" t="n"/>
       <c r="P83" s="13" t="n"/>
       <c r="Q83" s="13" t="n"/>
+      <c r="R83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -4142,6 +4342,9 @@
       <c r="Q84" s="13" t="n">
         <v>52.42</v>
       </c>
+      <c r="R84" s="13" t="n">
+        <v>51.81</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -4194,6 +4397,9 @@
       </c>
       <c r="Q85" s="13" t="n">
         <v>2706.96</v>
+      </c>
+      <c r="R85" s="13" t="n">
+        <v>2745.66</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -4214,6 +4420,7 @@
       <c r="O86" s="10" t="n"/>
       <c r="P86" s="13" t="n"/>
       <c r="Q86" s="13" t="n"/>
+      <c r="R86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4267,6 +4474,9 @@
       <c r="Q87" s="13" t="n">
         <v>58.66</v>
       </c>
+      <c r="R87" s="13" t="n">
+        <v>58.62</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4319,6 +4529,9 @@
       </c>
       <c r="Q88" s="13" t="n">
         <v>2775.73</v>
+      </c>
+      <c r="R88" s="13" t="n">
+        <v>2814.43</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -4339,6 +4552,7 @@
       <c r="O89" s="10" t="n"/>
       <c r="P89" s="13" t="n"/>
       <c r="Q89" s="13" t="n"/>
+      <c r="R89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -4392,6 +4606,9 @@
       <c r="Q90" s="13" t="n">
         <v>50.01</v>
       </c>
+      <c r="R90" s="13" t="n">
+        <v>49.38</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -4444,6 +4661,9 @@
       </c>
       <c r="Q91" s="13" t="n">
         <v>2873.72</v>
+      </c>
+      <c r="R91" s="13" t="n">
+        <v>2898.18</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -4464,6 +4684,7 @@
       <c r="O92" s="10" t="n"/>
       <c r="P92" s="13" t="n"/>
       <c r="Q92" s="13" t="n"/>
+      <c r="R92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4517,6 +4738,9 @@
       <c r="Q93" s="13" t="n">
         <v>44.19</v>
       </c>
+      <c r="R93" s="13" t="n">
+        <v>45.01</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -4568,6 +4792,9 @@
         <v>1974.54</v>
       </c>
       <c r="Q94" s="13" t="n">
+        <v>1974.54</v>
+      </c>
+      <c r="R94" s="13" t="n">
         <v>1974.54</v>
       </c>
     </row>
@@ -4589,6 +4816,7 @@
       <c r="O95" s="10" t="n"/>
       <c r="P95" s="13" t="n"/>
       <c r="Q95" s="13" t="n"/>
+      <c r="R95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -4642,6 +4870,9 @@
       <c r="Q96" s="13" t="n">
         <v>26.56</v>
       </c>
+      <c r="R96" s="13" t="n">
+        <v>26.82</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -4694,6 +4925,9 @@
       </c>
       <c r="Q97" s="13" t="n">
         <v>9997.530000000001</v>
+      </c>
+      <c r="R97" s="13" t="n">
+        <v>10055.11</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -4714,6 +4948,7 @@
       <c r="O98" s="10" t="n"/>
       <c r="P98" s="13" t="n"/>
       <c r="Q98" s="13" t="n"/>
+      <c r="R98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -4767,6 +5002,9 @@
       <c r="Q99" s="13" t="n">
         <v>84.42</v>
       </c>
+      <c r="R99" s="13" t="n">
+        <v>83.89</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -4819,6 +5057,9 @@
       </c>
       <c r="Q100" s="13" t="n">
         <v>8832.940000000001</v>
+      </c>
+      <c r="R100" s="13" t="n">
+        <v>9065.18</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -4839,6 +5080,7 @@
       <c r="O101" s="10" t="n"/>
       <c r="P101" s="13" t="n"/>
       <c r="Q101" s="13" t="n"/>
+      <c r="R101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -4892,6 +5134,9 @@
       <c r="Q102" s="13" t="n">
         <v>57.1</v>
       </c>
+      <c r="R102" s="13" t="n">
+        <v>57.22</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -4944,6 +5189,9 @@
       </c>
       <c r="Q103" s="13" t="n">
         <v>12751.03</v>
+      </c>
+      <c r="R103" s="13" t="n">
+        <v>12935.41</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -4964,6 +5212,7 @@
       <c r="O104" s="10" t="n"/>
       <c r="P104" s="13" t="n"/>
       <c r="Q104" s="13" t="n"/>
+      <c r="R104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -5017,6 +5266,9 @@
       <c r="Q105" s="13" t="n">
         <v>5.98</v>
       </c>
+      <c r="R105" s="13" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -5069,6 +5321,9 @@
       </c>
       <c r="Q106" s="13" t="n">
         <v>2211.46</v>
+      </c>
+      <c r="R106" s="13" t="n">
+        <v>2199.83</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -5089,6 +5344,7 @@
       <c r="O107" s="10" t="n"/>
       <c r="P107" s="13" t="n"/>
       <c r="Q107" s="13" t="n"/>
+      <c r="R107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -5142,6 +5398,9 @@
       <c r="Q108" s="13" t="n">
         <v>25.77</v>
       </c>
+      <c r="R108" s="13" t="n">
+        <v>25.69</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -5194,6 +5453,9 @@
       </c>
       <c r="Q109" s="13" t="n">
         <v>849.5</v>
+      </c>
+      <c r="R109" s="13" t="n">
+        <v>851.8200000000001</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -5214,6 +5476,7 @@
       <c r="O110" s="10" t="n"/>
       <c r="P110" s="13" t="n"/>
       <c r="Q110" s="13" t="n"/>
+      <c r="R110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -5267,6 +5530,9 @@
       <c r="Q111" s="13" t="n">
         <v>29.84</v>
       </c>
+      <c r="R111" s="13" t="n">
+        <v>30.08</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -5319,6 +5585,9 @@
       </c>
       <c r="Q112" s="13" t="n">
         <v>2834.31</v>
+      </c>
+      <c r="R112" s="13" t="n">
+        <v>2860.49</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -5339,6 +5608,7 @@
       <c r="O113" s="10" t="n"/>
       <c r="P113" s="13" t="n"/>
       <c r="Q113" s="13" t="n"/>
+      <c r="R113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -5392,6 +5662,9 @@
       <c r="Q114" s="13" t="n">
         <v>20.2</v>
       </c>
+      <c r="R114" s="13" t="n">
+        <v>20.61</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -5445,10 +5718,14 @@
       <c r="Q115" s="13" t="n">
         <v>3830.75</v>
       </c>
+      <c r="R115" s="13" t="n">
+        <v>3877.72</v>
+      </c>
     </row>
     <row r="116">
       <c r="P116" s="13" t="n"/>
       <c r="Q116" s="13" t="n"/>
+      <c r="R116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -5457,12 +5734,18 @@
       <c r="Q117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="R117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
         <v>2932.32</v>
       </c>
       <c r="Q118" s="13" t="n">
+        <v>2880.27</v>
+      </c>
+      <c r="R118" s="13" t="n">
         <v>2880.27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-25 04:14:36]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R118"/>
+  <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -540,6 +540,7 @@
     <col width="15" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="15" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -633,6 +634,11 @@
           <t>2025/12/22</t>
         </is>
       </c>
+      <c r="S1" s="13" t="inlineStr">
+        <is>
+          <t>2025/12/25</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -725,6 +731,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="S2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -781,6 +792,9 @@
       <c r="R3" s="13" t="n">
         <v>61.5</v>
       </c>
+      <c r="S3" s="13" t="n">
+        <v>62.67</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -836,6 +850,9 @@
       </c>
       <c r="R4" s="13" t="n">
         <v>3915.2</v>
+      </c>
+      <c r="S4" s="13" t="n">
+        <v>3952.5</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -857,6 +874,7 @@
       <c r="P5" s="13" t="n"/>
       <c r="Q5" s="13" t="n"/>
       <c r="R5" s="13" t="n"/>
+      <c r="S5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -913,6 +931,9 @@
       <c r="R6" s="13" t="n">
         <v>49.01</v>
       </c>
+      <c r="S6" s="13" t="n">
+        <v>50.08</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -968,6 +989,9 @@
       </c>
       <c r="R7" s="13" t="n">
         <v>5574.74</v>
+      </c>
+      <c r="S7" s="13" t="n">
+        <v>5618.23</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -989,6 +1013,7 @@
       <c r="P8" s="13" t="n"/>
       <c r="Q8" s="13" t="n"/>
       <c r="R8" s="13" t="n"/>
+      <c r="S8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1045,6 +1070,9 @@
       <c r="R9" s="13" t="n">
         <v>52.81</v>
       </c>
+      <c r="S9" s="13" t="n">
+        <v>53.84</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1100,6 +1128,9 @@
       </c>
       <c r="R10" s="13" t="n">
         <v>4604.43</v>
+      </c>
+      <c r="S10" s="13" t="n">
+        <v>4631</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1121,6 +1152,7 @@
       <c r="P11" s="13" t="n"/>
       <c r="Q11" s="13" t="n"/>
       <c r="R11" s="13" t="n"/>
+      <c r="S11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1177,6 +1209,9 @@
       <c r="R12" s="13" t="n">
         <v>56.7</v>
       </c>
+      <c r="S12" s="13" t="n">
+        <v>57.63</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1232,6 +1267,9 @@
       </c>
       <c r="R13" s="13" t="n">
         <v>7265.85</v>
+      </c>
+      <c r="S13" s="13" t="n">
+        <v>7375.81</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1253,6 +1291,7 @@
       <c r="P14" s="13" t="n"/>
       <c r="Q14" s="13" t="n"/>
       <c r="R14" s="13" t="n"/>
+      <c r="S14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1309,6 +1348,9 @@
       <c r="R15" s="13" t="n">
         <v>27.39</v>
       </c>
+      <c r="S15" s="13" t="n">
+        <v>28.16</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1364,6 +1406,9 @@
       </c>
       <c r="R16" s="13" t="n">
         <v>2665.99</v>
+      </c>
+      <c r="S16" s="13" t="n">
+        <v>2672.5</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1385,6 +1430,7 @@
       <c r="P17" s="13" t="n"/>
       <c r="Q17" s="13" t="n"/>
       <c r="R17" s="13" t="n"/>
+      <c r="S17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1441,6 +1487,9 @@
       <c r="R18" s="13" t="n">
         <v>96.44</v>
       </c>
+      <c r="S18" s="13" t="n">
+        <v>97.03</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1496,6 +1545,9 @@
       </c>
       <c r="R19" s="13" t="n">
         <v>6834.5</v>
+      </c>
+      <c r="S19" s="13" t="n">
+        <v>6932.05</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1517,6 +1569,7 @@
       <c r="P20" s="13" t="n"/>
       <c r="Q20" s="13" t="n"/>
       <c r="R20" s="13" t="n"/>
+      <c r="S20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1573,6 +1626,9 @@
       <c r="R21" s="13" t="n">
         <v>67.09999999999999</v>
       </c>
+      <c r="S21" s="13" t="n">
+        <v>71.94</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1628,6 +1684,9 @@
       </c>
       <c r="R22" s="13" t="n">
         <v>85370.8</v>
+      </c>
+      <c r="S22" s="13" t="n">
+        <v>85408.7</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1649,6 +1708,7 @@
       <c r="P23" s="13" t="n"/>
       <c r="Q23" s="13" t="n"/>
       <c r="R23" s="13" t="n"/>
+      <c r="S23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1705,6 +1765,9 @@
       <c r="R24" s="13" t="n">
         <v>84.48</v>
       </c>
+      <c r="S24" s="13" t="n">
+        <v>85.70999999999999</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1760,6 +1823,9 @@
       </c>
       <c r="R25" s="13" t="n">
         <v>24288.4</v>
+      </c>
+      <c r="S25" s="13" t="n">
+        <v>24340.06</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1781,6 +1847,7 @@
       <c r="P26" s="13" t="n"/>
       <c r="Q26" s="13" t="n"/>
       <c r="R26" s="13" t="n"/>
+      <c r="S26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1837,6 +1904,9 @@
       <c r="R27" s="13" t="n">
         <v>67.42</v>
       </c>
+      <c r="S27" s="13" t="n">
+        <v>70.29000000000001</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1892,6 +1962,9 @@
       </c>
       <c r="R28" s="13" t="n">
         <v>50427.56</v>
+      </c>
+      <c r="S28" s="13" t="n">
+        <v>50347.18</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1913,6 +1986,7 @@
       <c r="P29" s="13" t="n"/>
       <c r="Q29" s="13" t="n"/>
       <c r="R29" s="13" t="n"/>
+      <c r="S29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -1969,6 +2043,9 @@
       <c r="R30" s="13" t="n">
         <v>55.21</v>
       </c>
+      <c r="S30" s="13" t="n">
+        <v>55.16</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2024,6 +2101,9 @@
       </c>
       <c r="R31" s="13" t="n">
         <v>5465.41</v>
+      </c>
+      <c r="S31" s="13" t="n">
+        <v>5485.9</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2045,6 +2125,7 @@
       <c r="P32" s="13" t="n"/>
       <c r="Q32" s="13" t="n"/>
       <c r="R32" s="13" t="n"/>
+      <c r="S32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2101,6 +2182,9 @@
       <c r="R33" s="13" t="n">
         <v>0.95</v>
       </c>
+      <c r="S33" s="13" t="n">
+        <v>1.09</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2156,6 +2240,9 @@
       </c>
       <c r="R34" s="13" t="n">
         <v>30886.41</v>
+      </c>
+      <c r="S34" s="13" t="n">
+        <v>31244.23</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2177,6 +2264,7 @@
       <c r="P35" s="13" t="n"/>
       <c r="Q35" s="13" t="n"/>
       <c r="R35" s="13" t="n"/>
+      <c r="S35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2233,6 +2321,9 @@
       <c r="R36" s="13" t="n">
         <v>29.21</v>
       </c>
+      <c r="S36" s="13" t="n">
+        <v>30.44</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2288,6 +2379,9 @@
       </c>
       <c r="R37" s="13" t="n">
         <v>3371.14</v>
+      </c>
+      <c r="S37" s="13" t="n">
+        <v>3411.53</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2309,6 +2403,7 @@
       <c r="P38" s="13" t="n"/>
       <c r="Q38" s="13" t="n"/>
       <c r="R38" s="13" t="n"/>
+      <c r="S38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2365,6 +2460,9 @@
       <c r="R39" s="13" t="n">
         <v>45.72</v>
       </c>
+      <c r="S39" s="13" t="n">
+        <v>47.56</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2420,6 +2518,9 @@
       </c>
       <c r="R40" s="13" t="n">
         <v>3178.51</v>
+      </c>
+      <c r="S40" s="13" t="n">
+        <v>3217.47</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2441,6 +2542,7 @@
       <c r="P41" s="13" t="n"/>
       <c r="Q41" s="13" t="n"/>
       <c r="R41" s="13" t="n"/>
+      <c r="S41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2497,6 +2599,9 @@
       <c r="R42" s="13" t="n">
         <v>17.69</v>
       </c>
+      <c r="S42" s="13" t="n">
+        <v>16.86</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2552,6 +2657,9 @@
       </c>
       <c r="R43" s="13" t="n">
         <v>6912.21</v>
+      </c>
+      <c r="S43" s="13" t="n">
+        <v>6894.99</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -2573,6 +2681,7 @@
       <c r="P44" s="13" t="n"/>
       <c r="Q44" s="13" t="n"/>
       <c r="R44" s="13" t="n"/>
+      <c r="S44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2629,6 +2738,9 @@
       <c r="R45" s="13" t="n">
         <v>27.94</v>
       </c>
+      <c r="S45" s="13" t="n">
+        <v>27.04</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2684,6 +2796,9 @@
       </c>
       <c r="R46" s="13" t="n">
         <v>8390.75</v>
+      </c>
+      <c r="S46" s="13" t="n">
+        <v>8341.719999999999</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2705,6 +2820,7 @@
       <c r="P47" s="13" t="n"/>
       <c r="Q47" s="13" t="n"/>
       <c r="R47" s="13" t="n"/>
+      <c r="S47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2761,6 +2877,9 @@
       <c r="R48" s="13" t="n">
         <v>7.59</v>
       </c>
+      <c r="S48" s="13" t="n">
+        <v>7.15</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2816,6 +2935,9 @@
       </c>
       <c r="R49" s="13" t="n">
         <v>12771.22</v>
+      </c>
+      <c r="S49" s="13" t="n">
+        <v>12716.79</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2837,6 +2959,7 @@
       <c r="P50" s="13" t="n"/>
       <c r="Q50" s="13" t="n"/>
       <c r="R50" s="13" t="n"/>
+      <c r="S50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -2893,6 +3016,9 @@
       <c r="R51" s="13" t="n">
         <v>26.04</v>
       </c>
+      <c r="S51" s="13" t="n">
+        <v>26.04</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -2948,6 +3074,9 @@
       </c>
       <c r="R52" s="13" t="n">
         <v>12457.91</v>
+      </c>
+      <c r="S52" s="13" t="n">
+        <v>12530.66</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -2969,6 +3098,7 @@
       <c r="P53" s="13" t="n"/>
       <c r="Q53" s="13" t="n"/>
       <c r="R53" s="13" t="n"/>
+      <c r="S53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3025,6 +3155,9 @@
       <c r="R54" s="13" t="n">
         <v>18.52</v>
       </c>
+      <c r="S54" s="13" t="n">
+        <v>17.91</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3080,6 +3213,9 @@
       </c>
       <c r="R55" s="13" t="n">
         <v>9089.52</v>
+      </c>
+      <c r="S55" s="13" t="n">
+        <v>8997.59</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3101,6 +3237,7 @@
       <c r="P56" s="13" t="n"/>
       <c r="Q56" s="13" t="n"/>
       <c r="R56" s="13" t="n"/>
+      <c r="S56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3157,6 +3294,9 @@
       <c r="R57" s="13" t="n">
         <v>25.54</v>
       </c>
+      <c r="S57" s="13" t="n">
+        <v>24.84</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3212,6 +3352,9 @@
       </c>
       <c r="R58" s="13" t="n">
         <v>15544.96</v>
+      </c>
+      <c r="S58" s="13" t="n">
+        <v>15421.39</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3233,6 +3376,7 @@
       <c r="P59" s="13" t="n"/>
       <c r="Q59" s="13" t="n"/>
       <c r="R59" s="13" t="n"/>
+      <c r="S59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3289,6 +3433,9 @@
       <c r="R60" s="13" t="n">
         <v>30.75</v>
       </c>
+      <c r="S60" s="13" t="n">
+        <v>30.34</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3344,6 +3491,9 @@
       </c>
       <c r="R61" s="13" t="n">
         <v>14813.29</v>
+      </c>
+      <c r="S61" s="13" t="n">
+        <v>14658.44</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3365,6 +3515,7 @@
       <c r="P62" s="13" t="n"/>
       <c r="Q62" s="13" t="n"/>
       <c r="R62" s="13" t="n"/>
+      <c r="S62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3421,6 +3572,9 @@
       <c r="R63" s="13" t="n">
         <v>20.44</v>
       </c>
+      <c r="S63" s="13" t="n">
+        <v>20.32</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3476,6 +3630,9 @@
       </c>
       <c r="R64" s="13" t="n">
         <v>9525.889999999999</v>
+      </c>
+      <c r="S64" s="13" t="n">
+        <v>9782.639999999999</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -3497,6 +3654,7 @@
       <c r="P65" s="13" t="n"/>
       <c r="Q65" s="13" t="n"/>
       <c r="R65" s="13" t="n"/>
+      <c r="S65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3553,6 +3711,9 @@
       <c r="R66" s="13" t="n">
         <v>13.41</v>
       </c>
+      <c r="S66" s="13" t="n">
+        <v>12.75</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3608,6 +3769,9 @@
       </c>
       <c r="R67" s="13" t="n">
         <v>9701.17</v>
+      </c>
+      <c r="S67" s="13" t="n">
+        <v>9637.16</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -3629,6 +3793,7 @@
       <c r="P68" s="13" t="n"/>
       <c r="Q68" s="13" t="n"/>
       <c r="R68" s="13" t="n"/>
+      <c r="S68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3685,6 +3850,9 @@
       <c r="R69" s="13" t="n">
         <v>23.32</v>
       </c>
+      <c r="S69" s="13" t="n">
+        <v>23.06</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3740,6 +3908,9 @@
       </c>
       <c r="R70" s="13" t="n">
         <v>2952.44</v>
+      </c>
+      <c r="S70" s="13" t="n">
+        <v>2927.75</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -3761,6 +3932,7 @@
       <c r="P71" s="13" t="n"/>
       <c r="Q71" s="13" t="n"/>
       <c r="R71" s="13" t="n"/>
+      <c r="S71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3817,6 +3989,9 @@
       <c r="R72" s="13" t="n">
         <v>45.05</v>
       </c>
+      <c r="S72" s="13" t="n">
+        <v>44.49</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -3872,6 +4047,9 @@
       </c>
       <c r="R73" s="13" t="n">
         <v>5528.05</v>
+      </c>
+      <c r="S73" s="13" t="n">
+        <v>5499.3</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -3893,6 +4071,7 @@
       <c r="P74" s="13" t="n"/>
       <c r="Q74" s="13" t="n"/>
       <c r="R74" s="13" t="n"/>
+      <c r="S74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -3949,6 +4128,9 @@
       <c r="R75" s="13" t="n">
         <v>25.29</v>
       </c>
+      <c r="S75" s="13" t="n">
+        <v>24.98</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -4004,6 +4186,9 @@
       </c>
       <c r="R76" s="13" t="n">
         <v>8935.959999999999</v>
+      </c>
+      <c r="S76" s="13" t="n">
+        <v>8892.59</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -4025,6 +4210,7 @@
       <c r="P77" s="13" t="n"/>
       <c r="Q77" s="13" t="n"/>
       <c r="R77" s="13" t="n"/>
+      <c r="S77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -4081,6 +4267,9 @@
       <c r="R78" s="13" t="n">
         <v>17.3</v>
       </c>
+      <c r="S78" s="13" t="n">
+        <v>17.41</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -4136,6 +4325,9 @@
       </c>
       <c r="R79" s="13" t="n">
         <v>1512.82</v>
+      </c>
+      <c r="S79" s="13" t="n">
+        <v>1518.56</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -4157,6 +4349,7 @@
       <c r="P80" s="13" t="n"/>
       <c r="Q80" s="13" t="n"/>
       <c r="R80" s="13" t="n"/>
+      <c r="S80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -4213,6 +4406,9 @@
       <c r="R81" s="13" t="n">
         <v>18.7</v>
       </c>
+      <c r="S81" s="13" t="n">
+        <v>18.22</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -4268,6 +4464,9 @@
       </c>
       <c r="R82" s="13" t="n">
         <v>16685.08</v>
+      </c>
+      <c r="S82" s="13" t="n">
+        <v>16521.46</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -4289,6 +4488,7 @@
       <c r="P83" s="13" t="n"/>
       <c r="Q83" s="13" t="n"/>
       <c r="R83" s="13" t="n"/>
+      <c r="S83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -4345,6 +4545,9 @@
       <c r="R84" s="13" t="n">
         <v>51.81</v>
       </c>
+      <c r="S84" s="13" t="n">
+        <v>52.91</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -4400,6 +4603,9 @@
       </c>
       <c r="R85" s="13" t="n">
         <v>2745.66</v>
+      </c>
+      <c r="S85" s="13" t="n">
+        <v>2793.37</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -4421,6 +4627,7 @@
       <c r="P86" s="13" t="n"/>
       <c r="Q86" s="13" t="n"/>
       <c r="R86" s="13" t="n"/>
+      <c r="S86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4477,6 +4684,9 @@
       <c r="R87" s="13" t="n">
         <v>58.62</v>
       </c>
+      <c r="S87" s="13" t="n">
+        <v>58.66</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4532,6 +4742,9 @@
       </c>
       <c r="R88" s="13" t="n">
         <v>2814.43</v>
+      </c>
+      <c r="S88" s="13" t="n">
+        <v>2861.77</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -4553,6 +4766,7 @@
       <c r="P89" s="13" t="n"/>
       <c r="Q89" s="13" t="n"/>
       <c r="R89" s="13" t="n"/>
+      <c r="S89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -4609,6 +4823,9 @@
       <c r="R90" s="13" t="n">
         <v>49.38</v>
       </c>
+      <c r="S90" s="13" t="n">
+        <v>50.8</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -4664,6 +4881,9 @@
       </c>
       <c r="R91" s="13" t="n">
         <v>2898.18</v>
+      </c>
+      <c r="S91" s="13" t="n">
+        <v>2961.73</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -4685,6 +4905,7 @@
       <c r="P92" s="13" t="n"/>
       <c r="Q92" s="13" t="n"/>
       <c r="R92" s="13" t="n"/>
+      <c r="S92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4741,6 +4962,9 @@
       <c r="R93" s="13" t="n">
         <v>45.01</v>
       </c>
+      <c r="S93" s="13" t="n">
+        <v>44.84</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -4796,6 +5020,9 @@
       </c>
       <c r="R94" s="13" t="n">
         <v>1974.54</v>
+      </c>
+      <c r="S94" s="13" t="n">
+        <v>1936.43</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -4817,6 +5044,7 @@
       <c r="P95" s="13" t="n"/>
       <c r="Q95" s="13" t="n"/>
       <c r="R95" s="13" t="n"/>
+      <c r="S95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -4873,6 +5101,9 @@
       <c r="R96" s="13" t="n">
         <v>26.82</v>
       </c>
+      <c r="S96" s="13" t="n">
+        <v>26.65</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -4928,6 +5159,9 @@
       </c>
       <c r="R97" s="13" t="n">
         <v>10055.11</v>
+      </c>
+      <c r="S97" s="13" t="n">
+        <v>9948.450000000001</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -4949,6 +5183,7 @@
       <c r="P98" s="13" t="n"/>
       <c r="Q98" s="13" t="n"/>
       <c r="R98" s="13" t="n"/>
+      <c r="S98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -5005,6 +5240,9 @@
       <c r="R99" s="13" t="n">
         <v>83.89</v>
       </c>
+      <c r="S99" s="13" t="n">
+        <v>86.27</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -5060,6 +5298,9 @@
       </c>
       <c r="R100" s="13" t="n">
         <v>9065.18</v>
+      </c>
+      <c r="S100" s="13" t="n">
+        <v>9206.59</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -5081,6 +5322,7 @@
       <c r="P101" s="13" t="n"/>
       <c r="Q101" s="13" t="n"/>
       <c r="R101" s="13" t="n"/>
+      <c r="S101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -5137,6 +5379,9 @@
       <c r="R102" s="13" t="n">
         <v>57.22</v>
       </c>
+      <c r="S102" s="13" t="n">
+        <v>57.37</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -5192,6 +5437,9 @@
       </c>
       <c r="R103" s="13" t="n">
         <v>12935.41</v>
+      </c>
+      <c r="S103" s="13" t="n">
+        <v>13352.12</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -5213,6 +5461,7 @@
       <c r="P104" s="13" t="n"/>
       <c r="Q104" s="13" t="n"/>
       <c r="R104" s="13" t="n"/>
+      <c r="S104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -5269,6 +5518,9 @@
       <c r="R105" s="13" t="n">
         <v>6</v>
       </c>
+      <c r="S105" s="13" t="n">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -5324,6 +5576,9 @@
       </c>
       <c r="R106" s="13" t="n">
         <v>2199.83</v>
+      </c>
+      <c r="S106" s="13" t="n">
+        <v>2210.5</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -5345,6 +5600,7 @@
       <c r="P107" s="13" t="n"/>
       <c r="Q107" s="13" t="n"/>
       <c r="R107" s="13" t="n"/>
+      <c r="S107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -5401,6 +5657,9 @@
       <c r="R108" s="13" t="n">
         <v>25.69</v>
       </c>
+      <c r="S108" s="13" t="n">
+        <v>25.75</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -5456,6 +5715,9 @@
       </c>
       <c r="R109" s="13" t="n">
         <v>851.8200000000001</v>
+      </c>
+      <c r="S109" s="13" t="n">
+        <v>857.6</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -5477,6 +5739,7 @@
       <c r="P110" s="13" t="n"/>
       <c r="Q110" s="13" t="n"/>
       <c r="R110" s="13" t="n"/>
+      <c r="S110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -5533,6 +5796,9 @@
       <c r="R111" s="13" t="n">
         <v>30.08</v>
       </c>
+      <c r="S111" s="13" t="n">
+        <v>30.66</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -5588,6 +5854,9 @@
       </c>
       <c r="R112" s="13" t="n">
         <v>2860.49</v>
+      </c>
+      <c r="S112" s="13" t="n">
+        <v>2987.21</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -5609,6 +5878,7 @@
       <c r="P113" s="13" t="n"/>
       <c r="Q113" s="13" t="n"/>
       <c r="R113" s="13" t="n"/>
+      <c r="S113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -5665,6 +5935,9 @@
       <c r="R114" s="13" t="n">
         <v>20.61</v>
       </c>
+      <c r="S114" s="13" t="n">
+        <v>21.04</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -5720,12 +5993,16 @@
       </c>
       <c r="R115" s="13" t="n">
         <v>3877.72</v>
+      </c>
+      <c r="S115" s="13" t="n">
+        <v>3922.81</v>
       </c>
     </row>
     <row r="116">
       <c r="P116" s="13" t="n"/>
       <c r="Q116" s="13" t="n"/>
       <c r="R116" s="13" t="n"/>
+      <c r="S116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -5737,6 +6014,9 @@
       <c r="R117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="S117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -5746,6 +6026,9 @@
         <v>2880.27</v>
       </c>
       <c r="R118" s="13" t="n">
+        <v>2880.27</v>
+      </c>
+      <c r="S118" s="13" t="n">
         <v>2880.27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2025-12-29 04:37:38]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S118"/>
+  <dimension ref="A1:T118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -541,6 +541,7 @@
     <col width="15" customWidth="1" min="17" max="17"/>
     <col width="15" customWidth="1" min="18" max="18"/>
     <col width="15" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -639,6 +640,11 @@
           <t>2025/12/25</t>
         </is>
       </c>
+      <c r="T1" s="13" t="inlineStr">
+        <is>
+          <t>2025/12/29</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -736,6 +742,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="T2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -795,6 +806,9 @@
       <c r="S3" s="13" t="n">
         <v>62.67</v>
       </c>
+      <c r="T3" s="13" t="n">
+        <v>63.55</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -853,6 +867,9 @@
       </c>
       <c r="S4" s="13" t="n">
         <v>3952.5</v>
+      </c>
+      <c r="T4" s="13" t="n">
+        <v>3975.92</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -875,6 +892,7 @@
       <c r="Q5" s="13" t="n"/>
       <c r="R5" s="13" t="n"/>
       <c r="S5" s="13" t="n"/>
+      <c r="T5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -934,6 +952,9 @@
       <c r="S6" s="13" t="n">
         <v>50.08</v>
       </c>
+      <c r="T6" s="13" t="n">
+        <v>50.31</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -992,6 +1013,9 @@
       </c>
       <c r="S7" s="13" t="n">
         <v>5618.23</v>
+      </c>
+      <c r="T7" s="13" t="n">
+        <v>5672.26</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1014,6 +1038,7 @@
       <c r="Q8" s="13" t="n"/>
       <c r="R8" s="13" t="n"/>
       <c r="S8" s="13" t="n"/>
+      <c r="T8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1073,6 +1098,9 @@
       <c r="S9" s="13" t="n">
         <v>53.84</v>
       </c>
+      <c r="T9" s="13" t="n">
+        <v>54.24</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1131,6 +1159,9 @@
       </c>
       <c r="S10" s="13" t="n">
         <v>4631</v>
+      </c>
+      <c r="T10" s="13" t="n">
+        <v>4660.9</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1153,6 +1184,7 @@
       <c r="Q11" s="13" t="n"/>
       <c r="R11" s="13" t="n"/>
       <c r="S11" s="13" t="n"/>
+      <c r="T11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1212,6 +1244,9 @@
       <c r="S12" s="13" t="n">
         <v>57.63</v>
       </c>
+      <c r="T12" s="13" t="n">
+        <v>58.41</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1270,6 +1305,9 @@
       </c>
       <c r="S13" s="13" t="n">
         <v>7375.81</v>
+      </c>
+      <c r="T13" s="13" t="n">
+        <v>7473.69</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1292,6 +1330,7 @@
       <c r="Q14" s="13" t="n"/>
       <c r="R14" s="13" t="n"/>
       <c r="S14" s="13" t="n"/>
+      <c r="T14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1351,6 +1390,9 @@
       <c r="S15" s="13" t="n">
         <v>28.16</v>
       </c>
+      <c r="T15" s="13" t="n">
+        <v>28.22</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1409,6 +1451,9 @@
       </c>
       <c r="S16" s="13" t="n">
         <v>2672.5</v>
+      </c>
+      <c r="T16" s="13" t="n">
+        <v>2684.67</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1431,6 +1476,7 @@
       <c r="Q17" s="13" t="n"/>
       <c r="R17" s="13" t="n"/>
       <c r="S17" s="13" t="n"/>
+      <c r="T17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1490,6 +1536,9 @@
       <c r="S18" s="13" t="n">
         <v>97.03</v>
       </c>
+      <c r="T18" s="13" t="n">
+        <v>97.02</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1548,6 +1597,9 @@
       </c>
       <c r="S19" s="13" t="n">
         <v>6932.05</v>
+      </c>
+      <c r="T19" s="13" t="n">
+        <v>6929.94</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1570,6 +1622,7 @@
       <c r="Q20" s="13" t="n"/>
       <c r="R20" s="13" t="n"/>
       <c r="S20" s="13" t="n"/>
+      <c r="T20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1629,6 +1682,9 @@
       <c r="S21" s="13" t="n">
         <v>71.94</v>
       </c>
+      <c r="T21" s="13" t="n">
+        <v>70.98</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1687,6 +1743,9 @@
       </c>
       <c r="S22" s="13" t="n">
         <v>85408.7</v>
+      </c>
+      <c r="T22" s="13" t="n">
+        <v>85137.92999999999</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1709,6 +1768,7 @@
       <c r="Q23" s="13" t="n"/>
       <c r="R23" s="13" t="n"/>
       <c r="S23" s="13" t="n"/>
+      <c r="T23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1768,6 +1828,9 @@
       <c r="S24" s="13" t="n">
         <v>85.70999999999999</v>
       </c>
+      <c r="T24" s="13" t="n">
+        <v>85.77</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1825,6 +1888,9 @@
         <v>24288.4</v>
       </c>
       <c r="S25" s="13" t="n">
+        <v>24340.06</v>
+      </c>
+      <c r="T25" s="13" t="n">
         <v>24340.06</v>
       </c>
     </row>
@@ -1848,6 +1914,7 @@
       <c r="Q26" s="13" t="n"/>
       <c r="R26" s="13" t="n"/>
       <c r="S26" s="13" t="n"/>
+      <c r="T26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1907,6 +1974,9 @@
       <c r="S27" s="13" t="n">
         <v>70.29000000000001</v>
       </c>
+      <c r="T27" s="13" t="n">
+        <v>70.23999999999999</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -1965,6 +2035,9 @@
       </c>
       <c r="S28" s="13" t="n">
         <v>50347.18</v>
+      </c>
+      <c r="T28" s="13" t="n">
+        <v>50644.66</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1987,6 +2060,7 @@
       <c r="Q29" s="13" t="n"/>
       <c r="R29" s="13" t="n"/>
       <c r="S29" s="13" t="n"/>
+      <c r="T29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2046,6 +2120,9 @@
       <c r="S30" s="13" t="n">
         <v>55.16</v>
       </c>
+      <c r="T30" s="13" t="n">
+        <v>55.74</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2104,6 +2181,9 @@
       </c>
       <c r="S31" s="13" t="n">
         <v>5485.9</v>
+      </c>
+      <c r="T31" s="13" t="n">
+        <v>5514.62</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2126,6 +2206,7 @@
       <c r="Q32" s="13" t="n"/>
       <c r="R32" s="13" t="n"/>
       <c r="S32" s="13" t="n"/>
+      <c r="T32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2185,6 +2266,9 @@
       <c r="S33" s="13" t="n">
         <v>1.09</v>
       </c>
+      <c r="T33" s="13" t="n">
+        <v>1.24</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2243,6 +2327,9 @@
       </c>
       <c r="S34" s="13" t="n">
         <v>31244.23</v>
+      </c>
+      <c r="T34" s="13" t="n">
+        <v>31691.42</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2265,6 +2352,7 @@
       <c r="Q35" s="13" t="n"/>
       <c r="R35" s="13" t="n"/>
       <c r="S35" s="13" t="n"/>
+      <c r="T35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2324,6 +2412,9 @@
       <c r="S36" s="13" t="n">
         <v>30.44</v>
       </c>
+      <c r="T36" s="13" t="n">
+        <v>30.62</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2382,6 +2473,9 @@
       </c>
       <c r="S37" s="13" t="n">
         <v>3411.53</v>
+      </c>
+      <c r="T37" s="13" t="n">
+        <v>3426.06</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2404,6 +2498,7 @@
       <c r="Q38" s="13" t="n"/>
       <c r="R38" s="13" t="n"/>
       <c r="S38" s="13" t="n"/>
+      <c r="T38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2463,6 +2558,9 @@
       <c r="S39" s="13" t="n">
         <v>47.56</v>
       </c>
+      <c r="T39" s="13" t="n">
+        <v>50.3</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2521,6 +2619,9 @@
       </c>
       <c r="S40" s="13" t="n">
         <v>3217.47</v>
+      </c>
+      <c r="T40" s="13" t="n">
+        <v>3233.53</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2543,6 +2644,7 @@
       <c r="Q41" s="13" t="n"/>
       <c r="R41" s="13" t="n"/>
       <c r="S41" s="13" t="n"/>
+      <c r="T41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2602,6 +2704,9 @@
       <c r="S42" s="13" t="n">
         <v>16.86</v>
       </c>
+      <c r="T42" s="13" t="n">
+        <v>17.62</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2660,6 +2765,9 @@
       </c>
       <c r="S43" s="13" t="n">
         <v>6894.99</v>
+      </c>
+      <c r="T43" s="13" t="n">
+        <v>6870.64</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -2682,6 +2790,7 @@
       <c r="Q44" s="13" t="n"/>
       <c r="R44" s="13" t="n"/>
       <c r="S44" s="13" t="n"/>
+      <c r="T44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2741,6 +2850,9 @@
       <c r="S45" s="13" t="n">
         <v>27.04</v>
       </c>
+      <c r="T45" s="13" t="n">
+        <v>27.62</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2799,6 +2911,9 @@
       </c>
       <c r="S46" s="13" t="n">
         <v>8341.719999999999</v>
+      </c>
+      <c r="T46" s="13" t="n">
+        <v>8338.93</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2821,6 +2936,7 @@
       <c r="Q47" s="13" t="n"/>
       <c r="R47" s="13" t="n"/>
       <c r="S47" s="13" t="n"/>
+      <c r="T47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2880,6 +2996,9 @@
       <c r="S48" s="13" t="n">
         <v>7.15</v>
       </c>
+      <c r="T48" s="13" t="n">
+        <v>7.56</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -2938,6 +3057,9 @@
       </c>
       <c r="S49" s="13" t="n">
         <v>12716.79</v>
+      </c>
+      <c r="T49" s="13" t="n">
+        <v>12734.37</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -2960,6 +3082,7 @@
       <c r="Q50" s="13" t="n"/>
       <c r="R50" s="13" t="n"/>
       <c r="S50" s="13" t="n"/>
+      <c r="T50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3019,6 +3142,9 @@
       <c r="S51" s="13" t="n">
         <v>26.04</v>
       </c>
+      <c r="T51" s="13" t="n">
+        <v>26.81</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3077,6 +3203,9 @@
       </c>
       <c r="S52" s="13" t="n">
         <v>12530.66</v>
+      </c>
+      <c r="T52" s="13" t="n">
+        <v>12672.18</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -3099,6 +3228,7 @@
       <c r="Q53" s="13" t="n"/>
       <c r="R53" s="13" t="n"/>
       <c r="S53" s="13" t="n"/>
+      <c r="T53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3158,6 +3288,9 @@
       <c r="S54" s="13" t="n">
         <v>17.91</v>
       </c>
+      <c r="T54" s="13" t="n">
+        <v>18.49</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3216,6 +3349,9 @@
       </c>
       <c r="S55" s="13" t="n">
         <v>8997.59</v>
+      </c>
+      <c r="T55" s="13" t="n">
+        <v>8926.58</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3238,6 +3374,7 @@
       <c r="Q56" s="13" t="n"/>
       <c r="R56" s="13" t="n"/>
       <c r="S56" s="13" t="n"/>
+      <c r="T56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3297,6 +3434,9 @@
       <c r="S57" s="13" t="n">
         <v>24.84</v>
       </c>
+      <c r="T57" s="13" t="n">
+        <v>25.26</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3355,6 +3495,9 @@
       </c>
       <c r="S58" s="13" t="n">
         <v>15421.39</v>
+      </c>
+      <c r="T58" s="13" t="n">
+        <v>15384.09</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3377,6 +3520,7 @@
       <c r="Q59" s="13" t="n"/>
       <c r="R59" s="13" t="n"/>
       <c r="S59" s="13" t="n"/>
+      <c r="T59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3436,6 +3580,9 @@
       <c r="S60" s="13" t="n">
         <v>30.34</v>
       </c>
+      <c r="T60" s="13" t="n">
+        <v>30.35</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3494,6 +3641,9 @@
       </c>
       <c r="S61" s="13" t="n">
         <v>14658.44</v>
+      </c>
+      <c r="T61" s="13" t="n">
+        <v>14617.56</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3516,6 +3666,7 @@
       <c r="Q62" s="13" t="n"/>
       <c r="R62" s="13" t="n"/>
       <c r="S62" s="13" t="n"/>
+      <c r="T62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3575,6 +3726,9 @@
       <c r="S63" s="13" t="n">
         <v>20.32</v>
       </c>
+      <c r="T63" s="13" t="n">
+        <v>20.37</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3632,6 +3786,9 @@
         <v>9525.889999999999</v>
       </c>
       <c r="S64" s="13" t="n">
+        <v>9782.639999999999</v>
+      </c>
+      <c r="T64" s="13" t="n">
         <v>9782.639999999999</v>
       </c>
     </row>
@@ -3655,6 +3812,7 @@
       <c r="Q65" s="13" t="n"/>
       <c r="R65" s="13" t="n"/>
       <c r="S65" s="13" t="n"/>
+      <c r="T65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3714,6 +3872,9 @@
       <c r="S66" s="13" t="n">
         <v>12.75</v>
       </c>
+      <c r="T66" s="13" t="n">
+        <v>13.11</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3772,6 +3933,9 @@
       </c>
       <c r="S67" s="13" t="n">
         <v>9637.16</v>
+      </c>
+      <c r="T67" s="13" t="n">
+        <v>9580.24</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -3794,6 +3958,7 @@
       <c r="Q68" s="13" t="n"/>
       <c r="R68" s="13" t="n"/>
       <c r="S68" s="13" t="n"/>
+      <c r="T68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -3853,6 +4018,9 @@
       <c r="S69" s="13" t="n">
         <v>23.06</v>
       </c>
+      <c r="T69" s="13" t="n">
+        <v>23.05</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -3911,6 +4079,9 @@
       </c>
       <c r="S70" s="13" t="n">
         <v>2927.75</v>
+      </c>
+      <c r="T70" s="13" t="n">
+        <v>2959</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -3933,6 +4104,7 @@
       <c r="Q71" s="13" t="n"/>
       <c r="R71" s="13" t="n"/>
       <c r="S71" s="13" t="n"/>
+      <c r="T71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -3992,6 +4164,9 @@
       <c r="S72" s="13" t="n">
         <v>44.49</v>
       </c>
+      <c r="T72" s="13" t="n">
+        <v>44.55</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -4050,6 +4225,9 @@
       </c>
       <c r="S73" s="13" t="n">
         <v>5499.3</v>
+      </c>
+      <c r="T73" s="13" t="n">
+        <v>5587.46</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -4072,6 +4250,7 @@
       <c r="Q74" s="13" t="n"/>
       <c r="R74" s="13" t="n"/>
       <c r="S74" s="13" t="n"/>
+      <c r="T74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -4131,6 +4310,9 @@
       <c r="S75" s="13" t="n">
         <v>24.98</v>
       </c>
+      <c r="T75" s="13" t="n">
+        <v>25.12</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -4189,6 +4371,9 @@
       </c>
       <c r="S76" s="13" t="n">
         <v>8892.59</v>
+      </c>
+      <c r="T76" s="13" t="n">
+        <v>8858.379999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -4211,6 +4396,7 @@
       <c r="Q77" s="13" t="n"/>
       <c r="R77" s="13" t="n"/>
       <c r="S77" s="13" t="n"/>
+      <c r="T77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -4270,6 +4456,9 @@
       <c r="S78" s="13" t="n">
         <v>17.41</v>
       </c>
+      <c r="T78" s="13" t="n">
+        <v>18.64</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -4328,6 +4517,9 @@
       </c>
       <c r="S79" s="13" t="n">
         <v>1518.56</v>
+      </c>
+      <c r="T79" s="13" t="n">
+        <v>1557.81</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -4350,6 +4542,7 @@
       <c r="Q80" s="13" t="n"/>
       <c r="R80" s="13" t="n"/>
       <c r="S80" s="13" t="n"/>
+      <c r="T80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -4409,6 +4602,9 @@
       <c r="S81" s="13" t="n">
         <v>18.22</v>
       </c>
+      <c r="T81" s="13" t="n">
+        <v>18.5</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -4467,6 +4663,9 @@
       </c>
       <c r="S82" s="13" t="n">
         <v>16521.46</v>
+      </c>
+      <c r="T82" s="13" t="n">
+        <v>16592.03</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -4489,6 +4688,7 @@
       <c r="Q83" s="13" t="n"/>
       <c r="R83" s="13" t="n"/>
       <c r="S83" s="13" t="n"/>
+      <c r="T83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -4548,6 +4748,9 @@
       <c r="S84" s="13" t="n">
         <v>52.91</v>
       </c>
+      <c r="T84" s="13" t="n">
+        <v>53.64</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -4606,6 +4809,9 @@
       </c>
       <c r="S85" s="13" t="n">
         <v>2793.37</v>
+      </c>
+      <c r="T85" s="13" t="n">
+        <v>2867.44</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -4628,6 +4834,7 @@
       <c r="Q86" s="13" t="n"/>
       <c r="R86" s="13" t="n"/>
       <c r="S86" s="13" t="n"/>
+      <c r="T86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4687,6 +4894,9 @@
       <c r="S87" s="13" t="n">
         <v>58.66</v>
       </c>
+      <c r="T87" s="13" t="n">
+        <v>58.72</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4745,6 +4955,9 @@
       </c>
       <c r="S88" s="13" t="n">
         <v>2861.77</v>
+      </c>
+      <c r="T88" s="13" t="n">
+        <v>2867.5</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -4767,6 +4980,7 @@
       <c r="Q89" s="13" t="n"/>
       <c r="R89" s="13" t="n"/>
       <c r="S89" s="13" t="n"/>
+      <c r="T89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -4826,6 +5040,9 @@
       <c r="S90" s="13" t="n">
         <v>50.8</v>
       </c>
+      <c r="T90" s="13" t="n">
+        <v>51.89</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -4884,6 +5101,9 @@
       </c>
       <c r="S91" s="13" t="n">
         <v>2961.73</v>
+      </c>
+      <c r="T91" s="13" t="n">
+        <v>3029.12</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -4906,6 +5126,7 @@
       <c r="Q92" s="13" t="n"/>
       <c r="R92" s="13" t="n"/>
       <c r="S92" s="13" t="n"/>
+      <c r="T92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -4965,6 +5186,9 @@
       <c r="S93" s="13" t="n">
         <v>44.84</v>
       </c>
+      <c r="T93" s="13" t="n">
+        <v>44.86</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -5023,6 +5247,9 @@
       </c>
       <c r="S94" s="13" t="n">
         <v>1936.43</v>
+      </c>
+      <c r="T94" s="13" t="n">
+        <v>1944.41</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -5045,6 +5272,7 @@
       <c r="Q95" s="13" t="n"/>
       <c r="R95" s="13" t="n"/>
       <c r="S95" s="13" t="n"/>
+      <c r="T95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -5104,6 +5332,9 @@
       <c r="S96" s="13" t="n">
         <v>26.65</v>
       </c>
+      <c r="T96" s="13" t="n">
+        <v>26.88</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -5162,6 +5393,9 @@
       </c>
       <c r="S97" s="13" t="n">
         <v>9948.450000000001</v>
+      </c>
+      <c r="T97" s="13" t="n">
+        <v>10003.13</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -5184,6 +5418,7 @@
       <c r="Q98" s="13" t="n"/>
       <c r="R98" s="13" t="n"/>
       <c r="S98" s="13" t="n"/>
+      <c r="T98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -5243,6 +5478,9 @@
       <c r="S99" s="13" t="n">
         <v>86.27</v>
       </c>
+      <c r="T99" s="13" t="n">
+        <v>86.09</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -5301,6 +5539,9 @@
       </c>
       <c r="S100" s="13" t="n">
         <v>9206.59</v>
+      </c>
+      <c r="T100" s="13" t="n">
+        <v>9117.9</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -5323,6 +5564,7 @@
       <c r="Q101" s="13" t="n"/>
       <c r="R101" s="13" t="n"/>
       <c r="S101" s="13" t="n"/>
+      <c r="T101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -5382,6 +5624,9 @@
       <c r="S102" s="13" t="n">
         <v>57.37</v>
       </c>
+      <c r="T102" s="13" t="n">
+        <v>57.62</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -5440,6 +5685,9 @@
       </c>
       <c r="S103" s="13" t="n">
         <v>13352.12</v>
+      </c>
+      <c r="T103" s="13" t="n">
+        <v>13768.05</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -5462,6 +5710,7 @@
       <c r="Q104" s="13" t="n"/>
       <c r="R104" s="13" t="n"/>
       <c r="S104" s="13" t="n"/>
+      <c r="T104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -5521,6 +5770,9 @@
       <c r="S105" s="13" t="n">
         <v>5.7</v>
       </c>
+      <c r="T105" s="13" t="n">
+        <v>5.82</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -5579,6 +5831,9 @@
       </c>
       <c r="S106" s="13" t="n">
         <v>2210.5</v>
+      </c>
+      <c r="T106" s="13" t="n">
+        <v>2215.71</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -5601,6 +5856,7 @@
       <c r="Q107" s="13" t="n"/>
       <c r="R107" s="13" t="n"/>
       <c r="S107" s="13" t="n"/>
+      <c r="T107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -5660,6 +5916,9 @@
       <c r="S108" s="13" t="n">
         <v>25.75</v>
       </c>
+      <c r="T108" s="13" t="n">
+        <v>25.94</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -5718,6 +5977,9 @@
       </c>
       <c r="S109" s="13" t="n">
         <v>857.6</v>
+      </c>
+      <c r="T109" s="13" t="n">
+        <v>859.49</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -5740,6 +6002,7 @@
       <c r="Q110" s="13" t="n"/>
       <c r="R110" s="13" t="n"/>
       <c r="S110" s="13" t="n"/>
+      <c r="T110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -5799,6 +6062,9 @@
       <c r="S111" s="13" t="n">
         <v>30.66</v>
       </c>
+      <c r="T111" s="13" t="n">
+        <v>31.32</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -5857,6 +6123,9 @@
       </c>
       <c r="S112" s="13" t="n">
         <v>2987.21</v>
+      </c>
+      <c r="T112" s="13" t="n">
+        <v>3067.2</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -5879,6 +6148,7 @@
       <c r="Q113" s="13" t="n"/>
       <c r="R113" s="13" t="n"/>
       <c r="S113" s="13" t="n"/>
+      <c r="T113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -5938,6 +6208,9 @@
       <c r="S114" s="13" t="n">
         <v>21.04</v>
       </c>
+      <c r="T114" s="13" t="n">
+        <v>21.14</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -5996,6 +6269,9 @@
       </c>
       <c r="S115" s="13" t="n">
         <v>3922.81</v>
+      </c>
+      <c r="T115" s="13" t="n">
+        <v>3950.58</v>
       </c>
     </row>
     <row r="116">
@@ -6003,6 +6279,7 @@
       <c r="Q116" s="13" t="n"/>
       <c r="R116" s="13" t="n"/>
       <c r="S116" s="13" t="n"/>
+      <c r="T116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -6017,6 +6294,9 @@
       <c r="S117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="T117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -6030,6 +6310,9 @@
       </c>
       <c r="S118" s="13" t="n">
         <v>2880.27</v>
+      </c>
+      <c r="T118" s="13" t="n">
+        <v>2947.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-01 04:35:57]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T118"/>
+  <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -542,6 +542,7 @@
     <col width="15" customWidth="1" min="18" max="18"/>
     <col width="15" customWidth="1" min="19" max="19"/>
     <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -645,6 +646,11 @@
           <t>2025/12/29</t>
         </is>
       </c>
+      <c r="U1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/01</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -747,6 +753,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="U2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -809,6 +820,9 @@
       <c r="T3" s="13" t="n">
         <v>63.55</v>
       </c>
+      <c r="U3" s="13" t="n">
+        <v>63.73</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -870,6 +884,9 @@
       </c>
       <c r="T4" s="13" t="n">
         <v>3975.92</v>
+      </c>
+      <c r="U4" s="13" t="n">
+        <v>3968.84</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -893,6 +910,7 @@
       <c r="R5" s="13" t="n"/>
       <c r="S5" s="13" t="n"/>
       <c r="T5" s="13" t="n"/>
+      <c r="U5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -955,6 +973,9 @@
       <c r="T6" s="13" t="n">
         <v>50.31</v>
       </c>
+      <c r="U6" s="13" t="n">
+        <v>50.5</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1016,6 +1037,9 @@
       </c>
       <c r="T7" s="13" t="n">
         <v>5672.26</v>
+      </c>
+      <c r="U7" s="13" t="n">
+        <v>5642.82</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1039,6 +1063,7 @@
       <c r="R8" s="13" t="n"/>
       <c r="S8" s="13" t="n"/>
       <c r="T8" s="13" t="n"/>
+      <c r="U8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1101,6 +1126,9 @@
       <c r="T9" s="13" t="n">
         <v>54.24</v>
       </c>
+      <c r="U9" s="13" t="n">
+        <v>54.51</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1162,6 +1190,9 @@
       </c>
       <c r="T10" s="13" t="n">
         <v>4660.9</v>
+      </c>
+      <c r="U10" s="13" t="n">
+        <v>4629.94</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1185,6 +1216,7 @@
       <c r="R11" s="13" t="n"/>
       <c r="S11" s="13" t="n"/>
       <c r="T11" s="13" t="n"/>
+      <c r="U11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1247,6 +1279,9 @@
       <c r="T12" s="13" t="n">
         <v>58.41</v>
       </c>
+      <c r="U12" s="13" t="n">
+        <v>58.37</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1308,6 +1343,9 @@
       </c>
       <c r="T13" s="13" t="n">
         <v>7473.69</v>
+      </c>
+      <c r="U13" s="13" t="n">
+        <v>7465.57</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1331,6 +1369,7 @@
       <c r="R14" s="13" t="n"/>
       <c r="S14" s="13" t="n"/>
       <c r="T14" s="13" t="n"/>
+      <c r="U14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1393,6 +1432,9 @@
       <c r="T15" s="13" t="n">
         <v>28.22</v>
       </c>
+      <c r="U15" s="13" t="n">
+        <v>28.09</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1454,6 +1496,9 @@
       </c>
       <c r="T16" s="13" t="n">
         <v>2684.67</v>
+      </c>
+      <c r="U16" s="13" t="n">
+        <v>2674.72</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1477,6 +1522,7 @@
       <c r="R17" s="13" t="n"/>
       <c r="S17" s="13" t="n"/>
       <c r="T17" s="13" t="n"/>
+      <c r="U17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1539,6 +1585,9 @@
       <c r="T18" s="13" t="n">
         <v>97.02</v>
       </c>
+      <c r="U18" s="13" t="n">
+        <v>96.52</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1600,6 +1649,9 @@
       </c>
       <c r="T19" s="13" t="n">
         <v>6929.94</v>
+      </c>
+      <c r="U19" s="13" t="n">
+        <v>6845.5</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1623,6 +1675,7 @@
       <c r="R20" s="13" t="n"/>
       <c r="S20" s="13" t="n"/>
       <c r="T20" s="13" t="n"/>
+      <c r="U20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1685,6 +1738,9 @@
       <c r="T21" s="13" t="n">
         <v>70.98</v>
       </c>
+      <c r="U21" s="13" t="n">
+        <v>71.59999999999999</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1746,6 +1802,9 @@
       </c>
       <c r="T22" s="13" t="n">
         <v>85137.92999999999</v>
+      </c>
+      <c r="U22" s="13" t="n">
+        <v>85376.88</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1769,6 +1828,7 @@
       <c r="R23" s="13" t="n"/>
       <c r="S23" s="13" t="n"/>
       <c r="T23" s="13" t="n"/>
+      <c r="U23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1831,6 +1891,9 @@
       <c r="T24" s="13" t="n">
         <v>85.77</v>
       </c>
+      <c r="U24" s="13" t="n">
+        <v>86.12</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1892,6 +1955,9 @@
       </c>
       <c r="T25" s="13" t="n">
         <v>24340.06</v>
+      </c>
+      <c r="U25" s="13" t="n">
+        <v>24490.41</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1915,6 +1981,7 @@
       <c r="R26" s="13" t="n"/>
       <c r="S26" s="13" t="n"/>
       <c r="T26" s="13" t="n"/>
+      <c r="U26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -1977,6 +2044,9 @@
       <c r="T27" s="13" t="n">
         <v>70.23999999999999</v>
       </c>
+      <c r="U27" s="13" t="n">
+        <v>70.19</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2038,6 +2108,9 @@
       </c>
       <c r="T28" s="13" t="n">
         <v>50644.66</v>
+      </c>
+      <c r="U28" s="13" t="n">
+        <v>50339.48</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2061,6 +2134,7 @@
       <c r="R29" s="13" t="n"/>
       <c r="S29" s="13" t="n"/>
       <c r="T29" s="13" t="n"/>
+      <c r="U29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2123,6 +2197,9 @@
       <c r="T30" s="13" t="n">
         <v>55.74</v>
       </c>
+      <c r="U30" s="13" t="n">
+        <v>55.58</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2184,6 +2261,9 @@
       </c>
       <c r="T31" s="13" t="n">
         <v>5514.62</v>
+      </c>
+      <c r="U31" s="13" t="n">
+        <v>5503.98</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2207,6 +2287,7 @@
       <c r="R32" s="13" t="n"/>
       <c r="S32" s="13" t="n"/>
       <c r="T32" s="13" t="n"/>
+      <c r="U32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2269,6 +2350,9 @@
       <c r="T33" s="13" t="n">
         <v>1.24</v>
       </c>
+      <c r="U33" s="13" t="n">
+        <v>1.28</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2330,6 +2414,9 @@
       </c>
       <c r="T34" s="13" t="n">
         <v>31691.42</v>
+      </c>
+      <c r="U34" s="13" t="n">
+        <v>31751.49</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2353,6 +2440,7 @@
       <c r="R35" s="13" t="n"/>
       <c r="S35" s="13" t="n"/>
       <c r="T35" s="13" t="n"/>
+      <c r="U35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2415,6 +2503,9 @@
       <c r="T36" s="13" t="n">
         <v>30.62</v>
       </c>
+      <c r="U36" s="13" t="n">
+        <v>30.09</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2476,6 +2567,9 @@
       </c>
       <c r="T37" s="13" t="n">
         <v>3426.06</v>
+      </c>
+      <c r="U37" s="13" t="n">
+        <v>3390.24</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2499,6 +2593,7 @@
       <c r="R38" s="13" t="n"/>
       <c r="S38" s="13" t="n"/>
       <c r="T38" s="13" t="n"/>
+      <c r="U38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2561,6 +2656,9 @@
       <c r="T39" s="13" t="n">
         <v>50.3</v>
       </c>
+      <c r="U39" s="13" t="n">
+        <v>49.05</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2622,6 +2720,9 @@
       </c>
       <c r="T40" s="13" t="n">
         <v>3233.53</v>
+      </c>
+      <c r="U40" s="13" t="n">
+        <v>3203.17</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2645,6 +2746,7 @@
       <c r="R41" s="13" t="n"/>
       <c r="S41" s="13" t="n"/>
       <c r="T41" s="13" t="n"/>
+      <c r="U41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2707,6 +2809,9 @@
       <c r="T42" s="13" t="n">
         <v>17.62</v>
       </c>
+      <c r="U42" s="13" t="n">
+        <v>15.89</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2768,6 +2873,9 @@
       </c>
       <c r="T43" s="13" t="n">
         <v>6870.64</v>
+      </c>
+      <c r="U43" s="13" t="n">
+        <v>6760.06</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -2791,6 +2899,7 @@
       <c r="R44" s="13" t="n"/>
       <c r="S44" s="13" t="n"/>
       <c r="T44" s="13" t="n"/>
+      <c r="U44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2853,6 +2962,9 @@
       <c r="T45" s="13" t="n">
         <v>27.62</v>
       </c>
+      <c r="U45" s="13" t="n">
+        <v>25.21</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -2914,6 +3026,9 @@
       </c>
       <c r="T46" s="13" t="n">
         <v>8338.93</v>
+      </c>
+      <c r="U46" s="13" t="n">
+        <v>8210.309999999999</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -2937,6 +3052,7 @@
       <c r="R47" s="13" t="n"/>
       <c r="S47" s="13" t="n"/>
       <c r="T47" s="13" t="n"/>
+      <c r="U47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -2999,6 +3115,9 @@
       <c r="T48" s="13" t="n">
         <v>7.56</v>
       </c>
+      <c r="U48" s="13" t="n">
+        <v>7.12</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3059,6 +3178,9 @@
         <v>12716.79</v>
       </c>
       <c r="T49" s="13" t="n">
+        <v>12734.37</v>
+      </c>
+      <c r="U49" s="13" t="n">
         <v>12734.37</v>
       </c>
     </row>
@@ -3083,6 +3205,7 @@
       <c r="R50" s="13" t="n"/>
       <c r="S50" s="13" t="n"/>
       <c r="T50" s="13" t="n"/>
+      <c r="U50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3145,6 +3268,9 @@
       <c r="T51" s="13" t="n">
         <v>26.81</v>
       </c>
+      <c r="U51" s="13" t="n">
+        <v>28.2</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3205,6 +3331,9 @@
         <v>12530.66</v>
       </c>
       <c r="T52" s="13" t="n">
+        <v>12672.18</v>
+      </c>
+      <c r="U52" s="13" t="n">
         <v>12672.18</v>
       </c>
     </row>
@@ -3229,6 +3358,7 @@
       <c r="R53" s="13" t="n"/>
       <c r="S53" s="13" t="n"/>
       <c r="T53" s="13" t="n"/>
+      <c r="U53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3291,6 +3421,9 @@
       <c r="T54" s="13" t="n">
         <v>18.49</v>
       </c>
+      <c r="U54" s="13" t="n">
+        <v>16.84</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3352,6 +3485,9 @@
       </c>
       <c r="T55" s="13" t="n">
         <v>8926.58</v>
+      </c>
+      <c r="U55" s="13" t="n">
+        <v>8763.030000000001</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3375,6 +3511,7 @@
       <c r="R56" s="13" t="n"/>
       <c r="S56" s="13" t="n"/>
       <c r="T56" s="13" t="n"/>
+      <c r="U56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3437,6 +3574,9 @@
       <c r="T57" s="13" t="n">
         <v>25.26</v>
       </c>
+      <c r="U57" s="13" t="n">
+        <v>24.16</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3498,6 +3638,9 @@
       </c>
       <c r="T58" s="13" t="n">
         <v>15384.09</v>
+      </c>
+      <c r="U58" s="13" t="n">
+        <v>15248.57</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3521,6 +3664,7 @@
       <c r="R59" s="13" t="n"/>
       <c r="S59" s="13" t="n"/>
       <c r="T59" s="13" t="n"/>
+      <c r="U59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3583,6 +3727,9 @@
       <c r="T60" s="13" t="n">
         <v>30.35</v>
       </c>
+      <c r="U60" s="13" t="n">
+        <v>30.06</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3644,6 +3791,9 @@
       </c>
       <c r="T61" s="13" t="n">
         <v>14617.56</v>
+      </c>
+      <c r="U61" s="13" t="n">
+        <v>14178.48</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3667,6 +3817,7 @@
       <c r="R62" s="13" t="n"/>
       <c r="S62" s="13" t="n"/>
       <c r="T62" s="13" t="n"/>
+      <c r="U62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3729,6 +3880,9 @@
       <c r="T63" s="13" t="n">
         <v>20.37</v>
       </c>
+      <c r="U63" s="13" t="n">
+        <v>20.02</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3789,6 +3943,9 @@
         <v>9782.639999999999</v>
       </c>
       <c r="T64" s="13" t="n">
+        <v>9782.639999999999</v>
+      </c>
+      <c r="U64" s="13" t="n">
         <v>9782.639999999999</v>
       </c>
     </row>
@@ -3813,6 +3970,7 @@
       <c r="R65" s="13" t="n"/>
       <c r="S65" s="13" t="n"/>
       <c r="T65" s="13" t="n"/>
+      <c r="U65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -3875,6 +4033,9 @@
       <c r="T66" s="13" t="n">
         <v>13.11</v>
       </c>
+      <c r="U66" s="13" t="n">
+        <v>11.53</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -3936,6 +4097,9 @@
       </c>
       <c r="T67" s="13" t="n">
         <v>9580.24</v>
+      </c>
+      <c r="U67" s="13" t="n">
+        <v>9531.52</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -3959,6 +4123,7 @@
       <c r="R68" s="13" t="n"/>
       <c r="S68" s="13" t="n"/>
       <c r="T68" s="13" t="n"/>
+      <c r="U68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -4021,6 +4186,9 @@
       <c r="T69" s="13" t="n">
         <v>23.05</v>
       </c>
+      <c r="U69" s="13" t="n">
+        <v>22.96</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -4082,6 +4250,9 @@
       </c>
       <c r="T70" s="13" t="n">
         <v>2959</v>
+      </c>
+      <c r="U70" s="13" t="n">
+        <v>2936.46</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -4105,6 +4276,7 @@
       <c r="R71" s="13" t="n"/>
       <c r="S71" s="13" t="n"/>
       <c r="T71" s="13" t="n"/>
+      <c r="U71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -4167,6 +4339,9 @@
       <c r="T72" s="13" t="n">
         <v>44.55</v>
       </c>
+      <c r="U72" s="13" t="n">
+        <v>43.99</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -4228,6 +4403,9 @@
       </c>
       <c r="T73" s="13" t="n">
         <v>5587.46</v>
+      </c>
+      <c r="U73" s="13" t="n">
+        <v>5515.98</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -4251,6 +4429,7 @@
       <c r="R74" s="13" t="n"/>
       <c r="S74" s="13" t="n"/>
       <c r="T74" s="13" t="n"/>
+      <c r="U74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -4313,6 +4492,9 @@
       <c r="T75" s="13" t="n">
         <v>25.12</v>
       </c>
+      <c r="U75" s="13" t="n">
+        <v>23.36</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -4374,6 +4556,9 @@
       </c>
       <c r="T76" s="13" t="n">
         <v>8858.379999999999</v>
+      </c>
+      <c r="U76" s="13" t="n">
+        <v>8718.139999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -4397,6 +4582,7 @@
       <c r="R77" s="13" t="n"/>
       <c r="S77" s="13" t="n"/>
       <c r="T77" s="13" t="n"/>
+      <c r="U77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -4459,6 +4645,9 @@
       <c r="T78" s="13" t="n">
         <v>18.64</v>
       </c>
+      <c r="U78" s="13" t="n">
+        <v>17.02</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -4520,6 +4709,9 @@
       </c>
       <c r="T79" s="13" t="n">
         <v>1557.81</v>
+      </c>
+      <c r="U79" s="13" t="n">
+        <v>1505.88</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -4543,6 +4735,7 @@
       <c r="R80" s="13" t="n"/>
       <c r="S80" s="13" t="n"/>
       <c r="T80" s="13" t="n"/>
+      <c r="U80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -4605,6 +4798,9 @@
       <c r="T81" s="13" t="n">
         <v>18.5</v>
       </c>
+      <c r="U81" s="13" t="n">
+        <v>16.97</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -4666,6 +4862,9 @@
       </c>
       <c r="T82" s="13" t="n">
         <v>16592.03</v>
+      </c>
+      <c r="U82" s="13" t="n">
+        <v>16217.81</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -4689,6 +4888,7 @@
       <c r="R83" s="13" t="n"/>
       <c r="S83" s="13" t="n"/>
       <c r="T83" s="13" t="n"/>
+      <c r="U83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -4751,6 +4951,9 @@
       <c r="T84" s="13" t="n">
         <v>53.64</v>
       </c>
+      <c r="U84" s="13" t="n">
+        <v>52.62</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -4812,6 +5015,9 @@
       </c>
       <c r="T85" s="13" t="n">
         <v>2867.44</v>
+      </c>
+      <c r="U85" s="13" t="n">
+        <v>2814.99</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -4835,6 +5041,7 @@
       <c r="R86" s="13" t="n"/>
       <c r="S86" s="13" t="n"/>
       <c r="T86" s="13" t="n"/>
+      <c r="U86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -4897,6 +5104,9 @@
       <c r="T87" s="13" t="n">
         <v>58.72</v>
       </c>
+      <c r="U87" s="13" t="n">
+        <v>58.48</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -4957,6 +5167,9 @@
         <v>2861.77</v>
       </c>
       <c r="T88" s="13" t="n">
+        <v>2867.5</v>
+      </c>
+      <c r="U88" s="13" t="n">
         <v>2867.5</v>
       </c>
     </row>
@@ -4981,6 +5194,7 @@
       <c r="R89" s="13" t="n"/>
       <c r="S89" s="13" t="n"/>
       <c r="T89" s="13" t="n"/>
+      <c r="U89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -5043,6 +5257,9 @@
       <c r="T90" s="13" t="n">
         <v>51.89</v>
       </c>
+      <c r="U90" s="13" t="n">
+        <v>51.27</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -5104,6 +5321,9 @@
       </c>
       <c r="T91" s="13" t="n">
         <v>3029.12</v>
+      </c>
+      <c r="U91" s="13" t="n">
+        <v>3025.68</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -5127,6 +5347,7 @@
       <c r="R92" s="13" t="n"/>
       <c r="S92" s="13" t="n"/>
       <c r="T92" s="13" t="n"/>
+      <c r="U92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -5189,6 +5410,9 @@
       <c r="T93" s="13" t="n">
         <v>44.86</v>
       </c>
+      <c r="U93" s="13" t="n">
+        <v>42.48</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -5249,6 +5473,9 @@
         <v>1936.43</v>
       </c>
       <c r="T94" s="13" t="n">
+        <v>1944.41</v>
+      </c>
+      <c r="U94" s="13" t="n">
         <v>1944.41</v>
       </c>
     </row>
@@ -5273,6 +5500,7 @@
       <c r="R95" s="13" t="n"/>
       <c r="S95" s="13" t="n"/>
       <c r="T95" s="13" t="n"/>
+      <c r="U95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -5335,6 +5563,9 @@
       <c r="T96" s="13" t="n">
         <v>26.88</v>
       </c>
+      <c r="U96" s="13" t="n">
+        <v>25.96</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -5396,6 +5627,9 @@
       </c>
       <c r="T97" s="13" t="n">
         <v>10003.13</v>
+      </c>
+      <c r="U97" s="13" t="n">
+        <v>9997.530000000001</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -5419,6 +5653,7 @@
       <c r="R98" s="13" t="n"/>
       <c r="S98" s="13" t="n"/>
       <c r="T98" s="13" t="n"/>
+      <c r="U98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -5481,6 +5716,9 @@
       <c r="T99" s="13" t="n">
         <v>86.09</v>
       </c>
+      <c r="U99" s="13" t="n">
+        <v>86.15000000000001</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -5542,6 +5780,9 @@
       </c>
       <c r="T100" s="13" t="n">
         <v>9117.9</v>
+      </c>
+      <c r="U100" s="13" t="n">
+        <v>9065.18</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -5565,6 +5806,7 @@
       <c r="R101" s="13" t="n"/>
       <c r="S101" s="13" t="n"/>
       <c r="T101" s="13" t="n"/>
+      <c r="U101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -5627,6 +5869,9 @@
       <c r="T102" s="13" t="n">
         <v>57.62</v>
       </c>
+      <c r="U102" s="13" t="n">
+        <v>58.2</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -5688,6 +5933,9 @@
       </c>
       <c r="T103" s="13" t="n">
         <v>13768.05</v>
+      </c>
+      <c r="U103" s="13" t="n">
+        <v>14011.14</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -5711,6 +5959,7 @@
       <c r="R104" s="13" t="n"/>
       <c r="S104" s="13" t="n"/>
       <c r="T104" s="13" t="n"/>
+      <c r="U104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -5773,6 +6022,9 @@
       <c r="T105" s="13" t="n">
         <v>5.82</v>
       </c>
+      <c r="U105" s="13" t="n">
+        <v>6.36</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -5834,6 +6086,9 @@
       </c>
       <c r="T106" s="13" t="n">
         <v>2215.71</v>
+      </c>
+      <c r="U106" s="13" t="n">
+        <v>2218.47</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -5857,6 +6112,7 @@
       <c r="R107" s="13" t="n"/>
       <c r="S107" s="13" t="n"/>
       <c r="T107" s="13" t="n"/>
+      <c r="U107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -5919,6 +6175,9 @@
       <c r="T108" s="13" t="n">
         <v>25.94</v>
       </c>
+      <c r="U108" s="13" t="n">
+        <v>25.71</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -5980,6 +6239,9 @@
       </c>
       <c r="T109" s="13" t="n">
         <v>859.49</v>
+      </c>
+      <c r="U109" s="13" t="n">
+        <v>852.64</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -6003,6 +6265,7 @@
       <c r="R110" s="13" t="n"/>
       <c r="S110" s="13" t="n"/>
       <c r="T110" s="13" t="n"/>
+      <c r="U110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -6065,6 +6328,9 @@
       <c r="T111" s="13" t="n">
         <v>31.32</v>
       </c>
+      <c r="U111" s="13" t="n">
+        <v>31.51</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -6125,6 +6391,9 @@
         <v>2987.21</v>
       </c>
       <c r="T112" s="13" t="n">
+        <v>3067.2</v>
+      </c>
+      <c r="U112" s="13" t="n">
         <v>3067.2</v>
       </c>
     </row>
@@ -6149,6 +6418,7 @@
       <c r="R113" s="13" t="n"/>
       <c r="S113" s="13" t="n"/>
       <c r="T113" s="13" t="n"/>
+      <c r="U113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -6211,6 +6481,9 @@
       <c r="T114" s="13" t="n">
         <v>21.14</v>
       </c>
+      <c r="U114" s="13" t="n">
+        <v>20.84</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -6272,6 +6545,9 @@
       </c>
       <c r="T115" s="13" t="n">
         <v>3950.58</v>
+      </c>
+      <c r="U115" s="13" t="n">
+        <v>3906.46</v>
       </c>
     </row>
     <row r="116">
@@ -6280,6 +6556,7 @@
       <c r="R116" s="13" t="n"/>
       <c r="S116" s="13" t="n"/>
       <c r="T116" s="13" t="n"/>
+      <c r="U116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -6297,6 +6574,9 @@
       <c r="T117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="U117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -6313,6 +6593,9 @@
       </c>
       <c r="T118" s="13" t="n">
         <v>2947.02</v>
+      </c>
+      <c r="U118" s="13" t="n">
+        <v>2943.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-05 04:44:32]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U118"/>
+  <dimension ref="A1:V118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -543,6 +543,7 @@
     <col width="15" customWidth="1" min="19" max="19"/>
     <col width="15" customWidth="1" min="20" max="20"/>
     <col width="15" customWidth="1" min="21" max="21"/>
+    <col width="15" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -651,6 +652,11 @@
           <t>2026/01/01</t>
         </is>
       </c>
+      <c r="V1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/05</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -758,6 +764,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="V2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -823,6 +834,9 @@
       <c r="U3" s="13" t="n">
         <v>63.73</v>
       </c>
+      <c r="V3" s="13" t="n">
+        <v>63.73</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -887,6 +901,9 @@
       </c>
       <c r="U4" s="13" t="n">
         <v>3968.84</v>
+      </c>
+      <c r="V4" s="13" t="n">
+        <v>4011.45</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -911,6 +928,7 @@
       <c r="S5" s="13" t="n"/>
       <c r="T5" s="13" t="n"/>
       <c r="U5" s="13" t="n"/>
+      <c r="V5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -976,6 +994,9 @@
       <c r="U6" s="13" t="n">
         <v>50.5</v>
       </c>
+      <c r="V6" s="13" t="n">
+        <v>50.5</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1040,6 +1061,9 @@
       </c>
       <c r="U7" s="13" t="n">
         <v>5642.82</v>
+      </c>
+      <c r="V7" s="13" t="n">
+        <v>5745.04</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1064,6 +1088,7 @@
       <c r="S8" s="13" t="n"/>
       <c r="T8" s="13" t="n"/>
       <c r="U8" s="13" t="n"/>
+      <c r="V8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1129,6 +1154,9 @@
       <c r="U9" s="13" t="n">
         <v>54.51</v>
       </c>
+      <c r="V9" s="13" t="n">
+        <v>54.51</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1193,6 +1221,9 @@
       </c>
       <c r="U10" s="13" t="n">
         <v>4629.94</v>
+      </c>
+      <c r="V10" s="13" t="n">
+        <v>4703.41</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1217,6 +1248,7 @@
       <c r="S11" s="13" t="n"/>
       <c r="T11" s="13" t="n"/>
       <c r="U11" s="13" t="n"/>
+      <c r="V11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1282,6 +1314,9 @@
       <c r="U12" s="13" t="n">
         <v>58.37</v>
       </c>
+      <c r="V12" s="13" t="n">
+        <v>58.37</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1346,6 +1381,9 @@
       </c>
       <c r="U13" s="13" t="n">
         <v>7465.57</v>
+      </c>
+      <c r="V13" s="13" t="n">
+        <v>7626.72</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1370,6 +1408,7 @@
       <c r="S14" s="13" t="n"/>
       <c r="T14" s="13" t="n"/>
       <c r="U14" s="13" t="n"/>
+      <c r="V14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1435,6 +1474,9 @@
       <c r="U15" s="13" t="n">
         <v>28.09</v>
       </c>
+      <c r="V15" s="13" t="n">
+        <v>28.09</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1499,6 +1541,9 @@
       </c>
       <c r="U16" s="13" t="n">
         <v>2674.72</v>
+      </c>
+      <c r="V16" s="13" t="n">
+        <v>2713.89</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1523,6 +1568,7 @@
       <c r="S17" s="13" t="n"/>
       <c r="T17" s="13" t="n"/>
       <c r="U17" s="13" t="n"/>
+      <c r="V17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1588,6 +1634,9 @@
       <c r="U18" s="13" t="n">
         <v>96.52</v>
       </c>
+      <c r="V18" s="13" t="n">
+        <v>96.52</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1652,6 +1701,9 @@
       </c>
       <c r="U19" s="13" t="n">
         <v>6845.5</v>
+      </c>
+      <c r="V19" s="13" t="n">
+        <v>6858.47</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1676,6 +1728,7 @@
       <c r="S20" s="13" t="n"/>
       <c r="T20" s="13" t="n"/>
       <c r="U20" s="13" t="n"/>
+      <c r="V20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1741,6 +1794,9 @@
       <c r="U21" s="13" t="n">
         <v>71.59999999999999</v>
       </c>
+      <c r="V21" s="13" t="n">
+        <v>71.59999999999999</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1805,6 +1861,9 @@
       </c>
       <c r="U22" s="13" t="n">
         <v>85376.88</v>
+      </c>
+      <c r="V22" s="13" t="n">
+        <v>85700.96000000001</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1829,6 +1888,7 @@
       <c r="S23" s="13" t="n"/>
       <c r="T23" s="13" t="n"/>
       <c r="U23" s="13" t="n"/>
+      <c r="V23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1894,6 +1954,9 @@
       <c r="U24" s="13" t="n">
         <v>86.12</v>
       </c>
+      <c r="V24" s="13" t="n">
+        <v>86.12</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -1958,6 +2021,9 @@
       </c>
       <c r="U25" s="13" t="n">
         <v>24490.41</v>
+      </c>
+      <c r="V25" s="13" t="n">
+        <v>24539.34</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1982,6 +2048,7 @@
       <c r="S26" s="13" t="n"/>
       <c r="T26" s="13" t="n"/>
       <c r="U26" s="13" t="n"/>
+      <c r="V26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2047,6 +2114,9 @@
       <c r="U27" s="13" t="n">
         <v>70.19</v>
       </c>
+      <c r="V27" s="13" t="n">
+        <v>70.19</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2111,6 +2181,9 @@
       </c>
       <c r="U28" s="13" t="n">
         <v>50339.48</v>
+      </c>
+      <c r="V28" s="13" t="n">
+        <v>51850.54</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2135,6 +2208,7 @@
       <c r="S29" s="13" t="n"/>
       <c r="T29" s="13" t="n"/>
       <c r="U29" s="13" t="n"/>
+      <c r="V29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2200,6 +2274,9 @@
       <c r="U30" s="13" t="n">
         <v>55.58</v>
       </c>
+      <c r="V30" s="13" t="n">
+        <v>55.58</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2264,6 +2341,9 @@
       </c>
       <c r="U31" s="13" t="n">
         <v>5503.98</v>
+      </c>
+      <c r="V31" s="13" t="n">
+        <v>5520.95</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2288,6 +2368,7 @@
       <c r="S32" s="13" t="n"/>
       <c r="T32" s="13" t="n"/>
       <c r="U32" s="13" t="n"/>
+      <c r="V32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2353,6 +2434,9 @@
       <c r="U33" s="13" t="n">
         <v>1.28</v>
       </c>
+      <c r="V33" s="13" t="n">
+        <v>1.28</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2417,6 +2501,9 @@
       </c>
       <c r="U34" s="13" t="n">
         <v>31751.49</v>
+      </c>
+      <c r="V34" s="13" t="n">
+        <v>32269.26</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2441,6 +2528,7 @@
       <c r="S35" s="13" t="n"/>
       <c r="T35" s="13" t="n"/>
       <c r="U35" s="13" t="n"/>
+      <c r="V35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2506,6 +2594,9 @@
       <c r="U36" s="13" t="n">
         <v>30.09</v>
       </c>
+      <c r="V36" s="13" t="n">
+        <v>30.09</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2570,6 +2661,9 @@
       </c>
       <c r="U37" s="13" t="n">
         <v>3390.24</v>
+      </c>
+      <c r="V37" s="13" t="n">
+        <v>3462</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2594,6 +2688,7 @@
       <c r="S38" s="13" t="n"/>
       <c r="T38" s="13" t="n"/>
       <c r="U38" s="13" t="n"/>
+      <c r="V38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2659,6 +2754,9 @@
       <c r="U39" s="13" t="n">
         <v>49.05</v>
       </c>
+      <c r="V39" s="13" t="n">
+        <v>49.05</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2723,6 +2821,9 @@
       </c>
       <c r="U40" s="13" t="n">
         <v>3203.17</v>
+      </c>
+      <c r="V40" s="13" t="n">
+        <v>3272.07</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2747,6 +2848,7 @@
       <c r="S41" s="13" t="n"/>
       <c r="T41" s="13" t="n"/>
       <c r="U41" s="13" t="n"/>
+      <c r="V41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2812,6 +2914,9 @@
       <c r="U42" s="13" t="n">
         <v>15.89</v>
       </c>
+      <c r="V42" s="13" t="n">
+        <v>15.89</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2876,6 +2981,9 @@
       </c>
       <c r="U43" s="13" t="n">
         <v>6760.06</v>
+      </c>
+      <c r="V43" s="13" t="n">
+        <v>7067.29</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -2900,6 +3008,7 @@
       <c r="S44" s="13" t="n"/>
       <c r="T44" s="13" t="n"/>
       <c r="U44" s="13" t="n"/>
+      <c r="V44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -2965,6 +3074,9 @@
       <c r="U45" s="13" t="n">
         <v>25.21</v>
       </c>
+      <c r="V45" s="13" t="n">
+        <v>25.21</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3029,6 +3141,9 @@
       </c>
       <c r="U46" s="13" t="n">
         <v>8210.309999999999</v>
+      </c>
+      <c r="V46" s="13" t="n">
+        <v>8515.639999999999</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3053,6 +3168,7 @@
       <c r="S47" s="13" t="n"/>
       <c r="T47" s="13" t="n"/>
       <c r="U47" s="13" t="n"/>
+      <c r="V47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3118,6 +3234,9 @@
       <c r="U48" s="13" t="n">
         <v>7.12</v>
       </c>
+      <c r="V48" s="13" t="n">
+        <v>7.12</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3182,6 +3301,9 @@
       </c>
       <c r="U49" s="13" t="n">
         <v>12734.37</v>
+      </c>
+      <c r="V49" s="13" t="n">
+        <v>12740.56</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3206,6 +3328,7 @@
       <c r="S50" s="13" t="n"/>
       <c r="T50" s="13" t="n"/>
       <c r="U50" s="13" t="n"/>
+      <c r="V50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3271,6 +3394,9 @@
       <c r="U51" s="13" t="n">
         <v>28.2</v>
       </c>
+      <c r="V51" s="13" t="n">
+        <v>28.2</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3335,6 +3461,9 @@
       </c>
       <c r="U52" s="13" t="n">
         <v>12672.18</v>
+      </c>
+      <c r="V52" s="13" t="n">
+        <v>12426.73</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -3359,6 +3488,7 @@
       <c r="S53" s="13" t="n"/>
       <c r="T53" s="13" t="n"/>
       <c r="U53" s="13" t="n"/>
+      <c r="V53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3424,6 +3554,9 @@
       <c r="U54" s="13" t="n">
         <v>16.84</v>
       </c>
+      <c r="V54" s="13" t="n">
+        <v>16.84</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3488,6 +3621,9 @@
       </c>
       <c r="U55" s="13" t="n">
         <v>8763.030000000001</v>
+      </c>
+      <c r="V55" s="13" t="n">
+        <v>8914.65</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3512,6 +3648,7 @@
       <c r="S56" s="13" t="n"/>
       <c r="T56" s="13" t="n"/>
       <c r="U56" s="13" t="n"/>
+      <c r="V56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3577,6 +3714,9 @@
       <c r="U57" s="13" t="n">
         <v>24.16</v>
       </c>
+      <c r="V57" s="13" t="n">
+        <v>24.16</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3641,6 +3781,9 @@
       </c>
       <c r="U58" s="13" t="n">
         <v>15248.57</v>
+      </c>
+      <c r="V58" s="13" t="n">
+        <v>15403.84</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3665,6 +3808,7 @@
       <c r="S59" s="13" t="n"/>
       <c r="T59" s="13" t="n"/>
       <c r="U59" s="13" t="n"/>
+      <c r="V59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3730,6 +3874,9 @@
       <c r="U60" s="13" t="n">
         <v>30.06</v>
       </c>
+      <c r="V60" s="13" t="n">
+        <v>30.06</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3794,6 +3941,9 @@
       </c>
       <c r="U61" s="13" t="n">
         <v>14178.48</v>
+      </c>
+      <c r="V61" s="13" t="n">
+        <v>15054.07</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3818,6 +3968,7 @@
       <c r="S62" s="13" t="n"/>
       <c r="T62" s="13" t="n"/>
       <c r="U62" s="13" t="n"/>
+      <c r="V62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -3883,6 +4034,9 @@
       <c r="U63" s="13" t="n">
         <v>20.02</v>
       </c>
+      <c r="V63" s="13" t="n">
+        <v>20.02</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -3947,6 +4101,9 @@
       </c>
       <c r="U64" s="13" t="n">
         <v>9782.639999999999</v>
+      </c>
+      <c r="V64" s="13" t="n">
+        <v>9765.02</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -3971,6 +4128,7 @@
       <c r="S65" s="13" t="n"/>
       <c r="T65" s="13" t="n"/>
       <c r="U65" s="13" t="n"/>
+      <c r="V65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4036,6 +4194,9 @@
       <c r="U66" s="13" t="n">
         <v>11.53</v>
       </c>
+      <c r="V66" s="13" t="n">
+        <v>11.53</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -4100,6 +4261,9 @@
       </c>
       <c r="U67" s="13" t="n">
         <v>9531.52</v>
+      </c>
+      <c r="V67" s="13" t="n">
+        <v>9661.379999999999</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -4124,6 +4288,7 @@
       <c r="S68" s="13" t="n"/>
       <c r="T68" s="13" t="n"/>
       <c r="U68" s="13" t="n"/>
+      <c r="V68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -4189,6 +4354,9 @@
       <c r="U69" s="13" t="n">
         <v>22.96</v>
       </c>
+      <c r="V69" s="13" t="n">
+        <v>22.96</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -4253,6 +4421,9 @@
       </c>
       <c r="U70" s="13" t="n">
         <v>2936.46</v>
+      </c>
+      <c r="V70" s="13" t="n">
+        <v>3065.3</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -4277,6 +4448,7 @@
       <c r="S71" s="13" t="n"/>
       <c r="T71" s="13" t="n"/>
       <c r="U71" s="13" t="n"/>
+      <c r="V71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -4342,6 +4514,9 @@
       <c r="U72" s="13" t="n">
         <v>43.99</v>
       </c>
+      <c r="V72" s="13" t="n">
+        <v>43.99</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -4406,6 +4581,9 @@
       </c>
       <c r="U73" s="13" t="n">
         <v>5515.98</v>
+      </c>
+      <c r="V73" s="13" t="n">
+        <v>5726.11</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -4430,6 +4608,7 @@
       <c r="S74" s="13" t="n"/>
       <c r="T74" s="13" t="n"/>
       <c r="U74" s="13" t="n"/>
+      <c r="V74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -4495,6 +4674,9 @@
       <c r="U75" s="13" t="n">
         <v>23.36</v>
       </c>
+      <c r="V75" s="13" t="n">
+        <v>23.36</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -4559,6 +4741,9 @@
       </c>
       <c r="U76" s="13" t="n">
         <v>8718.139999999999</v>
+      </c>
+      <c r="V76" s="13" t="n">
+        <v>9037.35</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -4583,6 +4768,7 @@
       <c r="S77" s="13" t="n"/>
       <c r="T77" s="13" t="n"/>
       <c r="U77" s="13" t="n"/>
+      <c r="V77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -4648,6 +4834,9 @@
       <c r="U78" s="13" t="n">
         <v>17.02</v>
       </c>
+      <c r="V78" s="13" t="n">
+        <v>17.02</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -4711,6 +4900,9 @@
         <v>1557.81</v>
       </c>
       <c r="U79" s="13" t="n">
+        <v>1505.88</v>
+      </c>
+      <c r="V79" s="13" t="n">
         <v>1505.88</v>
       </c>
     </row>
@@ -4736,6 +4928,7 @@
       <c r="S80" s="13" t="n"/>
       <c r="T80" s="13" t="n"/>
       <c r="U80" s="13" t="n"/>
+      <c r="V80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -4801,6 +4994,9 @@
       <c r="U81" s="13" t="n">
         <v>16.97</v>
       </c>
+      <c r="V81" s="13" t="n">
+        <v>16.97</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -4864,6 +5060,9 @@
         <v>16592.03</v>
       </c>
       <c r="U82" s="13" t="n">
+        <v>16217.81</v>
+      </c>
+      <c r="V82" s="13" t="n">
         <v>16217.81</v>
       </c>
     </row>
@@ -4889,6 +5088,7 @@
       <c r="S83" s="13" t="n"/>
       <c r="T83" s="13" t="n"/>
       <c r="U83" s="13" t="n"/>
+      <c r="V83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -4954,6 +5154,9 @@
       <c r="U84" s="13" t="n">
         <v>52.62</v>
       </c>
+      <c r="V84" s="13" t="n">
+        <v>52.62</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -5018,6 +5221,9 @@
       </c>
       <c r="U85" s="13" t="n">
         <v>2814.99</v>
+      </c>
+      <c r="V85" s="13" t="n">
+        <v>2865.99</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -5042,6 +5248,7 @@
       <c r="S86" s="13" t="n"/>
       <c r="T86" s="13" t="n"/>
       <c r="U86" s="13" t="n"/>
+      <c r="V86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -5107,6 +5314,9 @@
       <c r="U87" s="13" t="n">
         <v>58.48</v>
       </c>
+      <c r="V87" s="13" t="n">
+        <v>58.48</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -5171,6 +5381,9 @@
       </c>
       <c r="U88" s="13" t="n">
         <v>2867.5</v>
+      </c>
+      <c r="V88" s="13" t="n">
+        <v>2903.95</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -5195,6 +5408,7 @@
       <c r="S89" s="13" t="n"/>
       <c r="T89" s="13" t="n"/>
       <c r="U89" s="13" t="n"/>
+      <c r="V89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -5260,6 +5474,9 @@
       <c r="U90" s="13" t="n">
         <v>51.27</v>
       </c>
+      <c r="V90" s="13" t="n">
+        <v>51.27</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -5324,6 +5541,9 @@
       </c>
       <c r="U91" s="13" t="n">
         <v>3025.68</v>
+      </c>
+      <c r="V91" s="13" t="n">
+        <v>3103.22</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -5348,6 +5568,7 @@
       <c r="S92" s="13" t="n"/>
       <c r="T92" s="13" t="n"/>
       <c r="U92" s="13" t="n"/>
+      <c r="V92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -5413,6 +5634,9 @@
       <c r="U93" s="13" t="n">
         <v>42.48</v>
       </c>
+      <c r="V93" s="13" t="n">
+        <v>42.48</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -5477,6 +5701,9 @@
       </c>
       <c r="U94" s="13" t="n">
         <v>1944.41</v>
+      </c>
+      <c r="V94" s="13" t="n">
+        <v>1970.07</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -5501,6 +5728,7 @@
       <c r="S95" s="13" t="n"/>
       <c r="T95" s="13" t="n"/>
       <c r="U95" s="13" t="n"/>
+      <c r="V95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -5566,6 +5794,9 @@
       <c r="U96" s="13" t="n">
         <v>25.96</v>
       </c>
+      <c r="V96" s="13" t="n">
+        <v>25.96</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -5630,6 +5861,9 @@
       </c>
       <c r="U97" s="13" t="n">
         <v>9997.530000000001</v>
+      </c>
+      <c r="V97" s="13" t="n">
+        <v>10292.69</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -5654,6 +5888,7 @@
       <c r="S98" s="13" t="n"/>
       <c r="T98" s="13" t="n"/>
       <c r="U98" s="13" t="n"/>
+      <c r="V98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -5719,6 +5954,9 @@
       <c r="U99" s="13" t="n">
         <v>86.15000000000001</v>
       </c>
+      <c r="V99" s="13" t="n">
+        <v>86.15000000000001</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -5783,6 +6021,9 @@
       </c>
       <c r="U100" s="13" t="n">
         <v>9065.18</v>
+      </c>
+      <c r="V100" s="13" t="n">
+        <v>9572.860000000001</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -5807,6 +6048,7 @@
       <c r="S101" s="13" t="n"/>
       <c r="T101" s="13" t="n"/>
       <c r="U101" s="13" t="n"/>
+      <c r="V101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -5872,6 +6114,9 @@
       <c r="U102" s="13" t="n">
         <v>58.2</v>
       </c>
+      <c r="V102" s="13" t="n">
+        <v>58.2</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -5936,6 +6181,9 @@
       </c>
       <c r="U103" s="13" t="n">
         <v>14011.14</v>
+      </c>
+      <c r="V103" s="13" t="n">
+        <v>14411.79</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -5960,6 +6208,7 @@
       <c r="S104" s="13" t="n"/>
       <c r="T104" s="13" t="n"/>
       <c r="U104" s="13" t="n"/>
+      <c r="V104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -6025,6 +6274,9 @@
       <c r="U105" s="13" t="n">
         <v>6.36</v>
       </c>
+      <c r="V105" s="13" t="n">
+        <v>6.36</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -6089,6 +6341,9 @@
       </c>
       <c r="U106" s="13" t="n">
         <v>2218.47</v>
+      </c>
+      <c r="V106" s="13" t="n">
+        <v>2215.71</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -6113,6 +6368,7 @@
       <c r="S107" s="13" t="n"/>
       <c r="T107" s="13" t="n"/>
       <c r="U107" s="13" t="n"/>
+      <c r="V107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -6178,6 +6434,9 @@
       <c r="U108" s="13" t="n">
         <v>25.71</v>
       </c>
+      <c r="V108" s="13" t="n">
+        <v>25.71</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -6242,6 +6501,9 @@
       </c>
       <c r="U109" s="13" t="n">
         <v>852.64</v>
+      </c>
+      <c r="V109" s="13" t="n">
+        <v>865.83</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -6266,6 +6528,7 @@
       <c r="S110" s="13" t="n"/>
       <c r="T110" s="13" t="n"/>
       <c r="U110" s="13" t="n"/>
+      <c r="V110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -6331,6 +6594,9 @@
       <c r="U111" s="13" t="n">
         <v>31.51</v>
       </c>
+      <c r="V111" s="13" t="n">
+        <v>31.51</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -6395,6 +6661,9 @@
       </c>
       <c r="U112" s="13" t="n">
         <v>3067.2</v>
+      </c>
+      <c r="V112" s="13" t="n">
+        <v>3058.48</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -6419,6 +6688,7 @@
       <c r="S113" s="13" t="n"/>
       <c r="T113" s="13" t="n"/>
       <c r="U113" s="13" t="n"/>
+      <c r="V113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -6484,6 +6754,9 @@
       <c r="U114" s="13" t="n">
         <v>20.84</v>
       </c>
+      <c r="V114" s="13" t="n">
+        <v>20.84</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -6548,6 +6821,9 @@
       </c>
       <c r="U115" s="13" t="n">
         <v>3906.46</v>
+      </c>
+      <c r="V115" s="13" t="n">
+        <v>3920.55</v>
       </c>
     </row>
     <row r="116">
@@ -6557,6 +6833,7 @@
       <c r="S116" s="13" t="n"/>
       <c r="T116" s="13" t="n"/>
       <c r="U116" s="13" t="n"/>
+      <c r="V116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -6577,6 +6854,9 @@
       <c r="U117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="V117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -6596,6 +6876,9 @@
       </c>
       <c r="U118" s="13" t="n">
         <v>2943.17</v>
+      </c>
+      <c r="V118" s="13" t="n">
+        <v>2947.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-15 04:29:33]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V118"/>
+  <dimension ref="A1:W118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -544,6 +544,7 @@
     <col width="15" customWidth="1" min="20" max="20"/>
     <col width="15" customWidth="1" min="21" max="21"/>
     <col width="15" customWidth="1" min="22" max="22"/>
+    <col width="15" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -657,6 +658,11 @@
           <t>2026/01/05</t>
         </is>
       </c>
+      <c r="W1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -769,6 +775,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="W2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -837,6 +848,9 @@
       <c r="V3" s="13" t="n">
         <v>63.73</v>
       </c>
+      <c r="W3" s="13" t="n">
+        <v>65.97</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -904,6 +918,9 @@
       </c>
       <c r="V4" s="13" t="n">
         <v>4011.45</v>
+      </c>
+      <c r="W4" s="13" t="n">
+        <v>4101.52</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -929,6 +946,7 @@
       <c r="T5" s="13" t="n"/>
       <c r="U5" s="13" t="n"/>
       <c r="V5" s="13" t="n"/>
+      <c r="W5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -997,6 +1015,9 @@
       <c r="V6" s="13" t="n">
         <v>50.5</v>
       </c>
+      <c r="W6" s="13" t="n">
+        <v>51.45</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1064,6 +1085,9 @@
       </c>
       <c r="V7" s="13" t="n">
         <v>5745.04</v>
+      </c>
+      <c r="W7" s="13" t="n">
+        <v>5884.61</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1089,6 +1113,7 @@
       <c r="T8" s="13" t="n"/>
       <c r="U8" s="13" t="n"/>
       <c r="V8" s="13" t="n"/>
+      <c r="W8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1157,6 +1182,9 @@
       <c r="V9" s="13" t="n">
         <v>54.51</v>
       </c>
+      <c r="W9" s="13" t="n">
+        <v>55.55</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1224,6 +1252,9 @@
       </c>
       <c r="V10" s="13" t="n">
         <v>4703.41</v>
+      </c>
+      <c r="W10" s="13" t="n">
+        <v>4731.15</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1249,6 +1280,7 @@
       <c r="T11" s="13" t="n"/>
       <c r="U11" s="13" t="n"/>
       <c r="V11" s="13" t="n"/>
+      <c r="W11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1317,6 +1349,9 @@
       <c r="V12" s="13" t="n">
         <v>58.37</v>
       </c>
+      <c r="W12" s="13" t="n">
+        <v>61.12</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1384,6 +1419,9 @@
       </c>
       <c r="V13" s="13" t="n">
         <v>7626.72</v>
+      </c>
+      <c r="W13" s="13" t="n">
+        <v>8166.87</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1409,6 +1447,7 @@
       <c r="T14" s="13" t="n"/>
       <c r="U14" s="13" t="n"/>
       <c r="V14" s="13" t="n"/>
+      <c r="W14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1477,6 +1516,9 @@
       <c r="V15" s="13" t="n">
         <v>28.09</v>
       </c>
+      <c r="W15" s="13" t="n">
+        <v>30.91</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1544,6 +1586,9 @@
       </c>
       <c r="V16" s="13" t="n">
         <v>2713.89</v>
+      </c>
+      <c r="W16" s="13" t="n">
+        <v>2754.84</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1569,6 +1614,7 @@
       <c r="T17" s="13" t="n"/>
       <c r="U17" s="13" t="n"/>
       <c r="V17" s="13" t="n"/>
+      <c r="W17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1637,6 +1683,9 @@
       <c r="V18" s="13" t="n">
         <v>96.52</v>
       </c>
+      <c r="W18" s="13" t="n">
+        <v>97.15000000000001</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1704,6 +1753,9 @@
       </c>
       <c r="V19" s="13" t="n">
         <v>6858.47</v>
+      </c>
+      <c r="W19" s="13" t="n">
+        <v>6926.6</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1729,6 +1781,7 @@
       <c r="T20" s="13" t="n"/>
       <c r="U20" s="13" t="n"/>
       <c r="V20" s="13" t="n"/>
+      <c r="W20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1797,6 +1850,9 @@
       <c r="V21" s="13" t="n">
         <v>71.59999999999999</v>
       </c>
+      <c r="W21" s="13" t="n">
+        <v>65.05</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1865,6 +1921,7 @@
       <c r="V22" s="13" t="n">
         <v>85700.96000000001</v>
       </c>
+      <c r="W22" s="13" t="inlineStr"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="1" t="n"/>
@@ -1889,6 +1946,7 @@
       <c r="T23" s="13" t="n"/>
       <c r="U23" s="13" t="n"/>
       <c r="V23" s="13" t="n"/>
+      <c r="W23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -1957,6 +2015,9 @@
       <c r="V24" s="13" t="n">
         <v>86.12</v>
       </c>
+      <c r="W24" s="13" t="n">
+        <v>88.31999999999999</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2024,6 +2085,9 @@
       </c>
       <c r="V25" s="13" t="n">
         <v>24539.34</v>
+      </c>
+      <c r="W25" s="13" t="n">
+        <v>25286.24</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2049,6 +2113,7 @@
       <c r="T26" s="13" t="n"/>
       <c r="U26" s="13" t="n"/>
       <c r="V26" s="13" t="n"/>
+      <c r="W26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2117,6 +2182,9 @@
       <c r="V27" s="13" t="n">
         <v>70.19</v>
       </c>
+      <c r="W27" s="13" t="n">
+        <v>76.04000000000001</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2184,6 +2252,9 @@
       </c>
       <c r="V28" s="13" t="n">
         <v>51850.54</v>
+      </c>
+      <c r="W28" s="13" t="n">
+        <v>53856.42</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2209,6 +2280,7 @@
       <c r="T29" s="13" t="n"/>
       <c r="U29" s="13" t="n"/>
       <c r="V29" s="13" t="n"/>
+      <c r="W29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2277,6 +2349,9 @@
       <c r="V30" s="13" t="n">
         <v>55.58</v>
       </c>
+      <c r="W30" s="13" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2344,6 +2419,9 @@
       </c>
       <c r="V31" s="13" t="n">
         <v>5520.95</v>
+      </c>
+      <c r="W31" s="13" t="n">
+        <v>5546.98</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2369,6 +2447,7 @@
       <c r="T32" s="13" t="n"/>
       <c r="U32" s="13" t="n"/>
       <c r="V32" s="13" t="n"/>
+      <c r="W32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2437,6 +2516,9 @@
       <c r="V33" s="13" t="n">
         <v>1.28</v>
       </c>
+      <c r="W33" s="13" t="n">
+        <v>1.42</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2504,6 +2586,9 @@
       </c>
       <c r="V34" s="13" t="n">
         <v>32269.26</v>
+      </c>
+      <c r="W34" s="13" t="n">
+        <v>32943.67</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2529,6 +2614,7 @@
       <c r="T35" s="13" t="n"/>
       <c r="U35" s="13" t="n"/>
       <c r="V35" s="13" t="n"/>
+      <c r="W35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2597,6 +2683,9 @@
       <c r="V36" s="13" t="n">
         <v>30.09</v>
       </c>
+      <c r="W36" s="13" t="n">
+        <v>31.61</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2664,6 +2753,9 @@
       </c>
       <c r="V37" s="13" t="n">
         <v>3462</v>
+      </c>
+      <c r="W37" s="13" t="n">
+        <v>3463.87</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2689,6 +2781,7 @@
       <c r="T38" s="13" t="n"/>
       <c r="U38" s="13" t="n"/>
       <c r="V38" s="13" t="n"/>
+      <c r="W38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2757,6 +2850,9 @@
       <c r="V39" s="13" t="n">
         <v>49.05</v>
       </c>
+      <c r="W39" s="13" t="n">
+        <v>54.16</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2824,6 +2920,9 @@
       </c>
       <c r="V40" s="13" t="n">
         <v>3272.07</v>
+      </c>
+      <c r="W40" s="13" t="n">
+        <v>3314.88</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2849,6 +2948,7 @@
       <c r="T41" s="13" t="n"/>
       <c r="U41" s="13" t="n"/>
       <c r="V41" s="13" t="n"/>
+      <c r="W41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -2917,6 +3017,9 @@
       <c r="V42" s="13" t="n">
         <v>15.89</v>
       </c>
+      <c r="W42" s="13" t="n">
+        <v>21.44</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -2984,6 +3087,9 @@
       </c>
       <c r="V43" s="13" t="n">
         <v>7067.29</v>
+      </c>
+      <c r="W43" s="13" t="n">
+        <v>7671.11</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3009,6 +3115,7 @@
       <c r="T44" s="13" t="n"/>
       <c r="U44" s="13" t="n"/>
       <c r="V44" s="13" t="n"/>
+      <c r="W44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3077,6 +3184,9 @@
       <c r="V45" s="13" t="n">
         <v>25.21</v>
       </c>
+      <c r="W45" s="13" t="n">
+        <v>32.52</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3144,6 +3254,9 @@
       </c>
       <c r="V46" s="13" t="n">
         <v>8515.639999999999</v>
+      </c>
+      <c r="W46" s="13" t="n">
+        <v>8758.370000000001</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3169,6 +3282,7 @@
       <c r="T47" s="13" t="n"/>
       <c r="U47" s="13" t="n"/>
       <c r="V47" s="13" t="n"/>
+      <c r="W47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3237,6 +3351,9 @@
       <c r="V48" s="13" t="n">
         <v>7.12</v>
       </c>
+      <c r="W48" s="13" t="n">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3304,6 +3421,9 @@
       </c>
       <c r="V49" s="13" t="n">
         <v>12740.56</v>
+      </c>
+      <c r="W49" s="13" t="n">
+        <v>12731.65</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3329,6 +3449,7 @@
       <c r="T50" s="13" t="n"/>
       <c r="U50" s="13" t="n"/>
       <c r="V50" s="13" t="n"/>
+      <c r="W50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3397,6 +3518,9 @@
       <c r="V51" s="13" t="n">
         <v>28.2</v>
       </c>
+      <c r="W51" s="13" t="n">
+        <v>31.21</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3464,6 +3588,9 @@
       </c>
       <c r="V52" s="13" t="n">
         <v>12426.73</v>
+      </c>
+      <c r="W52" s="13" t="n">
+        <v>13090.7</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -3489,6 +3616,7 @@
       <c r="T53" s="13" t="n"/>
       <c r="U53" s="13" t="n"/>
       <c r="V53" s="13" t="n"/>
+      <c r="W53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3557,6 +3685,9 @@
       <c r="V54" s="13" t="n">
         <v>16.84</v>
       </c>
+      <c r="W54" s="13" t="n">
+        <v>17.58</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3624,6 +3755,9 @@
       </c>
       <c r="V55" s="13" t="n">
         <v>8914.65</v>
+      </c>
+      <c r="W55" s="13" t="n">
+        <v>8816.1</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3649,6 +3783,7 @@
       <c r="T56" s="13" t="n"/>
       <c r="U56" s="13" t="n"/>
       <c r="V56" s="13" t="n"/>
+      <c r="W56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3717,6 +3852,9 @@
       <c r="V57" s="13" t="n">
         <v>24.16</v>
       </c>
+      <c r="W57" s="13" t="n">
+        <v>24.7</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3784,6 +3922,9 @@
       </c>
       <c r="V58" s="13" t="n">
         <v>15403.84</v>
+      </c>
+      <c r="W58" s="13" t="n">
+        <v>15246.63</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3809,6 +3950,7 @@
       <c r="T59" s="13" t="n"/>
       <c r="U59" s="13" t="n"/>
       <c r="V59" s="13" t="n"/>
+      <c r="W59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -3877,6 +4019,9 @@
       <c r="V60" s="13" t="n">
         <v>30.06</v>
       </c>
+      <c r="W60" s="13" t="n">
+        <v>34.26</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -3944,6 +4089,9 @@
       </c>
       <c r="V61" s="13" t="n">
         <v>15054.07</v>
+      </c>
+      <c r="W61" s="13" t="n">
+        <v>16456.67</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -3969,6 +4117,7 @@
       <c r="T62" s="13" t="n"/>
       <c r="U62" s="13" t="n"/>
       <c r="V62" s="13" t="n"/>
+      <c r="W62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4037,6 +4186,9 @@
       <c r="V63" s="13" t="n">
         <v>20.02</v>
       </c>
+      <c r="W63" s="13" t="n">
+        <v>22.94</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -4104,6 +4256,9 @@
       </c>
       <c r="V64" s="13" t="n">
         <v>9765.02</v>
+      </c>
+      <c r="W64" s="13" t="n">
+        <v>9525.889999999999</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -4129,6 +4284,7 @@
       <c r="T65" s="13" t="n"/>
       <c r="U65" s="13" t="n"/>
       <c r="V65" s="13" t="n"/>
+      <c r="W65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4197,6 +4353,9 @@
       <c r="V66" s="13" t="n">
         <v>11.53</v>
       </c>
+      <c r="W66" s="13" t="n">
+        <v>13.3</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -4264,6 +4423,9 @@
       </c>
       <c r="V67" s="13" t="n">
         <v>9661.379999999999</v>
+      </c>
+      <c r="W67" s="13" t="n">
+        <v>9691.440000000001</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -4289,6 +4451,7 @@
       <c r="T68" s="13" t="n"/>
       <c r="U68" s="13" t="n"/>
       <c r="V68" s="13" t="n"/>
+      <c r="W68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -4357,6 +4520,9 @@
       <c r="V69" s="13" t="n">
         <v>22.96</v>
       </c>
+      <c r="W69" s="13" t="n">
+        <v>25.39</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -4424,6 +4590,9 @@
       </c>
       <c r="V70" s="13" t="n">
         <v>3065.3</v>
+      </c>
+      <c r="W70" s="13" t="n">
+        <v>3161.56</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -4449,6 +4618,7 @@
       <c r="T71" s="13" t="n"/>
       <c r="U71" s="13" t="n"/>
       <c r="V71" s="13" t="n"/>
+      <c r="W71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -4517,6 +4687,9 @@
       <c r="V72" s="13" t="n">
         <v>43.99</v>
       </c>
+      <c r="W72" s="13" t="n">
+        <v>49.18</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -4584,6 +4757,9 @@
       </c>
       <c r="V73" s="13" t="n">
         <v>5726.11</v>
+      </c>
+      <c r="W73" s="13" t="n">
+        <v>5800.32</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -4609,6 +4785,7 @@
       <c r="T74" s="13" t="n"/>
       <c r="U74" s="13" t="n"/>
       <c r="V74" s="13" t="n"/>
+      <c r="W74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -4677,6 +4854,9 @@
       <c r="V75" s="13" t="n">
         <v>23.36</v>
       </c>
+      <c r="W75" s="13" t="n">
+        <v>29.66</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -4744,6 +4924,9 @@
       </c>
       <c r="V76" s="13" t="n">
         <v>9037.35</v>
+      </c>
+      <c r="W76" s="13" t="n">
+        <v>9346.059999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -4769,6 +4952,7 @@
       <c r="T77" s="13" t="n"/>
       <c r="U77" s="13" t="n"/>
       <c r="V77" s="13" t="n"/>
+      <c r="W77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -4837,6 +5021,9 @@
       <c r="V78" s="13" t="n">
         <v>17.02</v>
       </c>
+      <c r="W78" s="13" t="n">
+        <v>17.64</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -4904,6 +5091,9 @@
       </c>
       <c r="V79" s="13" t="n">
         <v>1505.88</v>
+      </c>
+      <c r="W79" s="13" t="n">
+        <v>1526.45</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -4929,6 +5119,7 @@
       <c r="T80" s="13" t="n"/>
       <c r="U80" s="13" t="n"/>
       <c r="V80" s="13" t="n"/>
+      <c r="W80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -4997,6 +5188,9 @@
       <c r="V81" s="13" t="n">
         <v>16.97</v>
       </c>
+      <c r="W81" s="13" t="n">
+        <v>17.82</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -5064,6 +5258,9 @@
       </c>
       <c r="V82" s="13" t="n">
         <v>16217.81</v>
+      </c>
+      <c r="W82" s="13" t="n">
+        <v>16412.83</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -5089,6 +5286,7 @@
       <c r="T83" s="13" t="n"/>
       <c r="U83" s="13" t="n"/>
       <c r="V83" s="13" t="n"/>
+      <c r="W83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -5157,6 +5355,9 @@
       <c r="V84" s="13" t="n">
         <v>52.62</v>
       </c>
+      <c r="W84" s="13" t="n">
+        <v>53.73</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -5224,6 +5425,9 @@
       </c>
       <c r="V85" s="13" t="n">
         <v>2865.99</v>
+      </c>
+      <c r="W85" s="13" t="n">
+        <v>2977.45</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -5249,6 +5453,7 @@
       <c r="T86" s="13" t="n"/>
       <c r="U86" s="13" t="n"/>
       <c r="V86" s="13" t="n"/>
+      <c r="W86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -5317,6 +5522,9 @@
       <c r="V87" s="13" t="n">
         <v>58.48</v>
       </c>
+      <c r="W87" s="13" t="n">
+        <v>58.69</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -5384,6 +5592,9 @@
       </c>
       <c r="V88" s="13" t="n">
         <v>2903.95</v>
+      </c>
+      <c r="W88" s="13" t="n">
+        <v>3069.18</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -5409,6 +5620,7 @@
       <c r="T89" s="13" t="n"/>
       <c r="U89" s="13" t="n"/>
       <c r="V89" s="13" t="n"/>
+      <c r="W89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -5477,6 +5689,9 @@
       <c r="V90" s="13" t="n">
         <v>51.27</v>
       </c>
+      <c r="W90" s="13" t="n">
+        <v>51.18</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -5544,6 +5759,9 @@
       </c>
       <c r="V91" s="13" t="n">
         <v>3103.22</v>
+      </c>
+      <c r="W91" s="13" t="n">
+        <v>3159.03</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -5569,6 +5787,7 @@
       <c r="T92" s="13" t="n"/>
       <c r="U92" s="13" t="n"/>
       <c r="V92" s="13" t="n"/>
+      <c r="W92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -5637,6 +5856,9 @@
       <c r="V93" s="13" t="n">
         <v>42.48</v>
       </c>
+      <c r="W93" s="13" t="n">
+        <v>48.64</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -5704,6 +5926,9 @@
       </c>
       <c r="V94" s="13" t="n">
         <v>1970.07</v>
+      </c>
+      <c r="W94" s="13" t="n">
+        <v>2027.75</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -5729,6 +5954,7 @@
       <c r="T95" s="13" t="n"/>
       <c r="U95" s="13" t="n"/>
       <c r="V95" s="13" t="n"/>
+      <c r="W95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -5797,6 +6023,9 @@
       <c r="V96" s="13" t="n">
         <v>25.96</v>
       </c>
+      <c r="W96" s="13" t="n">
+        <v>28.84</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -5864,6 +6093,9 @@
       </c>
       <c r="V97" s="13" t="n">
         <v>10292.69</v>
+      </c>
+      <c r="W97" s="13" t="n">
+        <v>9948.450000000001</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -5889,6 +6121,7 @@
       <c r="T98" s="13" t="n"/>
       <c r="U98" s="13" t="n"/>
       <c r="V98" s="13" t="n"/>
+      <c r="W98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -5957,6 +6190,9 @@
       <c r="V99" s="13" t="n">
         <v>86.15000000000001</v>
       </c>
+      <c r="W99" s="13" t="n">
+        <v>87.62</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -6024,6 +6260,9 @@
       </c>
       <c r="V100" s="13" t="n">
         <v>9572.860000000001</v>
+      </c>
+      <c r="W100" s="13" t="n">
+        <v>10081.28</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -6049,6 +6288,7 @@
       <c r="T101" s="13" t="n"/>
       <c r="U101" s="13" t="n"/>
       <c r="V101" s="13" t="n"/>
+      <c r="W101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -6117,6 +6357,9 @@
       <c r="V102" s="13" t="n">
         <v>58.2</v>
       </c>
+      <c r="W102" s="13" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -6184,6 +6427,9 @@
       </c>
       <c r="V103" s="13" t="n">
         <v>14411.79</v>
+      </c>
+      <c r="W103" s="13" t="n">
+        <v>15399.22</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -6209,6 +6455,7 @@
       <c r="T104" s="13" t="n"/>
       <c r="U104" s="13" t="n"/>
       <c r="V104" s="13" t="n"/>
+      <c r="W104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -6277,6 +6524,9 @@
       <c r="V105" s="13" t="n">
         <v>6.36</v>
       </c>
+      <c r="W105" s="13" t="n">
+        <v>5.92</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -6344,6 +6594,9 @@
       </c>
       <c r="V106" s="13" t="n">
         <v>2215.71</v>
+      </c>
+      <c r="W106" s="13" t="n">
+        <v>2231.08</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -6369,6 +6622,7 @@
       <c r="T107" s="13" t="n"/>
       <c r="U107" s="13" t="n"/>
       <c r="V107" s="13" t="n"/>
+      <c r="W107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -6437,6 +6691,9 @@
       <c r="V108" s="13" t="n">
         <v>25.71</v>
       </c>
+      <c r="W108" s="13" t="n">
+        <v>26.13</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -6504,6 +6761,9 @@
       </c>
       <c r="V109" s="13" t="n">
         <v>865.83</v>
+      </c>
+      <c r="W109" s="13" t="n">
+        <v>857</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -6529,6 +6789,7 @@
       <c r="T110" s="13" t="n"/>
       <c r="U110" s="13" t="n"/>
       <c r="V110" s="13" t="n"/>
+      <c r="W110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -6597,6 +6858,9 @@
       <c r="V111" s="13" t="n">
         <v>31.51</v>
       </c>
+      <c r="W111" s="13" t="n">
+        <v>32.94</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -6664,6 +6928,9 @@
       </c>
       <c r="V112" s="13" t="n">
         <v>3058.48</v>
+      </c>
+      <c r="W112" s="13" t="n">
+        <v>3582.4</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -6689,6 +6956,7 @@
       <c r="T113" s="13" t="n"/>
       <c r="U113" s="13" t="n"/>
       <c r="V113" s="13" t="n"/>
+      <c r="W113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -6757,6 +7025,9 @@
       <c r="V114" s="13" t="n">
         <v>20.84</v>
       </c>
+      <c r="W114" s="13" t="n">
+        <v>22.07</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -6824,6 +7095,9 @@
       </c>
       <c r="V115" s="13" t="n">
         <v>3920.55</v>
+      </c>
+      <c r="W115" s="13" t="n">
+        <v>4062.45</v>
       </c>
     </row>
     <row r="116">
@@ -6834,6 +7108,7 @@
       <c r="T116" s="13" t="n"/>
       <c r="U116" s="13" t="n"/>
       <c r="V116" s="13" t="n"/>
+      <c r="W116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -6857,6 +7132,9 @@
       <c r="V117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="W117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -6879,6 +7157,9 @@
       </c>
       <c r="V118" s="13" t="n">
         <v>2947.02</v>
+      </c>
+      <c r="W118" s="13" t="n">
+        <v>3013.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-19 04:40:07]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W118"/>
+  <dimension ref="A1:X118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -545,6 +545,7 @@
     <col width="15" customWidth="1" min="21" max="21"/>
     <col width="15" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
+    <col width="15" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -663,6 +664,11 @@
           <t>2026/01/15</t>
         </is>
       </c>
+      <c r="X1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/19</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -780,6 +786,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="X2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -851,6 +862,9 @@
       <c r="W3" s="13" t="n">
         <v>65.97</v>
       </c>
+      <c r="X3" s="13" t="n">
+        <v>65.83</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -921,6 +935,9 @@
       </c>
       <c r="W4" s="13" t="n">
         <v>4101.52</v>
+      </c>
+      <c r="X4" s="13" t="n">
+        <v>4107.18</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -947,6 +964,7 @@
       <c r="U5" s="13" t="n"/>
       <c r="V5" s="13" t="n"/>
       <c r="W5" s="13" t="n"/>
+      <c r="X5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1018,6 +1036,9 @@
       <c r="W6" s="13" t="n">
         <v>51.45</v>
       </c>
+      <c r="X6" s="13" t="n">
+        <v>51.1</v>
+      </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1088,6 +1109,9 @@
       </c>
       <c r="W7" s="13" t="n">
         <v>5884.61</v>
+      </c>
+      <c r="X7" s="13" t="n">
+        <v>5892.9</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1114,6 +1138,7 @@
       <c r="U8" s="13" t="n"/>
       <c r="V8" s="13" t="n"/>
       <c r="W8" s="13" t="n"/>
+      <c r="X8" s="13" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1185,6 +1210,9 @@
       <c r="W9" s="13" t="n">
         <v>55.55</v>
       </c>
+      <c r="X9" s="13" t="n">
+        <v>54.81</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1255,6 +1283,9 @@
       </c>
       <c r="W10" s="13" t="n">
         <v>4731.15</v>
+      </c>
+      <c r="X10" s="13" t="n">
+        <v>4721.07</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1281,6 +1312,7 @@
       <c r="U11" s="13" t="n"/>
       <c r="V11" s="13" t="n"/>
       <c r="W11" s="13" t="n"/>
+      <c r="X11" s="13" t="n"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1352,6 +1384,9 @@
       <c r="W12" s="13" t="n">
         <v>61.12</v>
       </c>
+      <c r="X12" s="13" t="n">
+        <v>61.12</v>
+      </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1422,6 +1457,9 @@
       </c>
       <c r="W13" s="13" t="n">
         <v>8166.87</v>
+      </c>
+      <c r="X13" s="13" t="n">
+        <v>8289.58</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1448,6 +1486,7 @@
       <c r="U14" s="13" t="n"/>
       <c r="V14" s="13" t="n"/>
       <c r="W14" s="13" t="n"/>
+      <c r="X14" s="13" t="n"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1519,6 +1558,9 @@
       <c r="W15" s="13" t="n">
         <v>30.91</v>
       </c>
+      <c r="X15" s="13" t="n">
+        <v>30.34</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1589,6 +1631,9 @@
       </c>
       <c r="W16" s="13" t="n">
         <v>2754.84</v>
+      </c>
+      <c r="X16" s="13" t="n">
+        <v>2738.68</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1615,6 +1660,7 @@
       <c r="U17" s="13" t="n"/>
       <c r="V17" s="13" t="n"/>
       <c r="W17" s="13" t="n"/>
+      <c r="X17" s="13" t="n"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1686,6 +1732,9 @@
       <c r="W18" s="13" t="n">
         <v>97.15000000000001</v>
       </c>
+      <c r="X18" s="13" t="n">
+        <v>97.05</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1756,6 +1805,9 @@
       </c>
       <c r="W19" s="13" t="n">
         <v>6926.6</v>
+      </c>
+      <c r="X19" s="13" t="n">
+        <v>6940.01</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1782,6 +1834,7 @@
       <c r="U20" s="13" t="n"/>
       <c r="V20" s="13" t="n"/>
       <c r="W20" s="13" t="n"/>
+      <c r="X20" s="13" t="n"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1853,6 +1906,9 @@
       <c r="W21" s="13" t="n">
         <v>65.05</v>
       </c>
+      <c r="X21" s="13" t="n">
+        <v>65.92</v>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1922,6 +1978,9 @@
         <v>85700.96000000001</v>
       </c>
       <c r="W22" s="13" t="inlineStr"/>
+      <c r="X22" s="13" t="n">
+        <v>83171.28</v>
+      </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="1" t="n"/>
@@ -1947,6 +2006,7 @@
       <c r="U23" s="13" t="n"/>
       <c r="V23" s="13" t="n"/>
       <c r="W23" s="13" t="n"/>
+      <c r="X23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2018,6 +2078,9 @@
       <c r="W24" s="13" t="n">
         <v>88.31999999999999</v>
       </c>
+      <c r="X24" s="13" t="n">
+        <v>82.66</v>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2088,6 +2151,9 @@
       </c>
       <c r="W25" s="13" t="n">
         <v>25286.24</v>
+      </c>
+      <c r="X25" s="13" t="n">
+        <v>25297.13</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2114,6 +2180,7 @@
       <c r="U26" s="13" t="n"/>
       <c r="V26" s="13" t="n"/>
       <c r="W26" s="13" t="n"/>
+      <c r="X26" s="13" t="n"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2185,6 +2252,9 @@
       <c r="W27" s="13" t="n">
         <v>76.04000000000001</v>
       </c>
+      <c r="X27" s="13" t="n">
+        <v>76.81</v>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2255,6 +2325,9 @@
       </c>
       <c r="W28" s="13" t="n">
         <v>53856.42</v>
+      </c>
+      <c r="X28" s="13" t="n">
+        <v>53467.27</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2281,6 +2354,7 @@
       <c r="U29" s="13" t="n"/>
       <c r="V29" s="13" t="n"/>
       <c r="W29" s="13" t="n"/>
+      <c r="X29" s="13" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2352,6 +2426,9 @@
       <c r="W30" s="13" t="n">
         <v>51</v>
       </c>
+      <c r="X30" s="13" t="n">
+        <v>51.71</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2422,6 +2499,9 @@
       </c>
       <c r="W31" s="13" t="n">
         <v>5546.98</v>
+      </c>
+      <c r="X31" s="13" t="n">
+        <v>5512.31</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2448,6 +2528,7 @@
       <c r="U32" s="13" t="n"/>
       <c r="V32" s="13" t="n"/>
       <c r="W32" s="13" t="n"/>
+      <c r="X32" s="13" t="n"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2519,6 +2600,9 @@
       <c r="W33" s="13" t="n">
         <v>1.42</v>
       </c>
+      <c r="X33" s="13" t="n">
+        <v>1.39</v>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2589,6 +2673,9 @@
       </c>
       <c r="W34" s="13" t="n">
         <v>32943.67</v>
+      </c>
+      <c r="X34" s="13" t="n">
+        <v>33771.52</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2615,6 +2702,7 @@
       <c r="U35" s="13" t="n"/>
       <c r="V35" s="13" t="n"/>
       <c r="W35" s="13" t="n"/>
+      <c r="X35" s="13" t="n"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2686,6 +2774,9 @@
       <c r="W36" s="13" t="n">
         <v>31.61</v>
       </c>
+      <c r="X36" s="13" t="n">
+        <v>31.83</v>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2756,6 +2847,9 @@
       </c>
       <c r="W37" s="13" t="n">
         <v>3463.87</v>
+      </c>
+      <c r="X37" s="13" t="n">
+        <v>3489.83</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2782,6 +2876,7 @@
       <c r="U38" s="13" t="n"/>
       <c r="V38" s="13" t="n"/>
       <c r="W38" s="13" t="n"/>
+      <c r="X38" s="13" t="n"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2853,6 +2948,9 @@
       <c r="W39" s="13" t="n">
         <v>54.16</v>
       </c>
+      <c r="X39" s="13" t="n">
+        <v>54.85</v>
+      </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -2923,6 +3021,9 @@
       </c>
       <c r="W40" s="13" t="n">
         <v>3314.88</v>
+      </c>
+      <c r="X40" s="13" t="n">
+        <v>3339.56</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -2949,6 +3050,7 @@
       <c r="U41" s="13" t="n"/>
       <c r="V41" s="13" t="n"/>
       <c r="W41" s="13" t="n"/>
+      <c r="X41" s="13" t="n"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3020,6 +3122,9 @@
       <c r="W42" s="13" t="n">
         <v>21.44</v>
       </c>
+      <c r="X42" s="13" t="n">
+        <v>20.69</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3090,6 +3195,9 @@
       </c>
       <c r="W43" s="13" t="n">
         <v>7671.11</v>
+      </c>
+      <c r="X43" s="13" t="n">
+        <v>7420.84</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3116,6 +3224,7 @@
       <c r="U44" s="13" t="n"/>
       <c r="V44" s="13" t="n"/>
       <c r="W44" s="13" t="n"/>
+      <c r="X44" s="13" t="n"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3187,6 +3296,9 @@
       <c r="W45" s="13" t="n">
         <v>32.52</v>
       </c>
+      <c r="X45" s="13" t="n">
+        <v>30.05</v>
+      </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3257,6 +3369,9 @@
       </c>
       <c r="W46" s="13" t="n">
         <v>8758.370000000001</v>
+      </c>
+      <c r="X46" s="13" t="n">
+        <v>8564.43</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3283,6 +3398,7 @@
       <c r="U47" s="13" t="n"/>
       <c r="V47" s="13" t="n"/>
       <c r="W47" s="13" t="n"/>
+      <c r="X47" s="13" t="n"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3354,6 +3470,9 @@
       <c r="W48" s="13" t="n">
         <v>7.2</v>
       </c>
+      <c r="X48" s="13" t="n">
+        <v>6.88</v>
+      </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3424,6 +3543,9 @@
       </c>
       <c r="W49" s="13" t="n">
         <v>12731.65</v>
+      </c>
+      <c r="X49" s="13" t="n">
+        <v>12578.05</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3450,6 +3572,7 @@
       <c r="U50" s="13" t="n"/>
       <c r="V50" s="13" t="n"/>
       <c r="W50" s="13" t="n"/>
+      <c r="X50" s="13" t="n"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3521,6 +3644,9 @@
       <c r="W51" s="13" t="n">
         <v>31.21</v>
       </c>
+      <c r="X51" s="13" t="n">
+        <v>31.55</v>
+      </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3591,6 +3717,9 @@
       </c>
       <c r="W52" s="13" t="n">
         <v>13090.7</v>
+      </c>
+      <c r="X52" s="13" t="n">
+        <v>13344.13</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -3617,6 +3746,7 @@
       <c r="U53" s="13" t="n"/>
       <c r="V53" s="13" t="n"/>
       <c r="W53" s="13" t="n"/>
+      <c r="X53" s="13" t="n"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3688,6 +3818,9 @@
       <c r="W54" s="13" t="n">
         <v>17.58</v>
       </c>
+      <c r="X54" s="13" t="n">
+        <v>16.91</v>
+      </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3758,6 +3891,9 @@
       </c>
       <c r="W55" s="13" t="n">
         <v>8816.1</v>
+      </c>
+      <c r="X55" s="13" t="n">
+        <v>8718.83</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3784,6 +3920,7 @@
       <c r="U56" s="13" t="n"/>
       <c r="V56" s="13" t="n"/>
       <c r="W56" s="13" t="n"/>
+      <c r="X56" s="13" t="n"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3855,6 +3992,9 @@
       <c r="W57" s="13" t="n">
         <v>24.7</v>
       </c>
+      <c r="X57" s="13" t="n">
+        <v>23.82</v>
+      </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -3925,6 +4065,9 @@
       </c>
       <c r="W58" s="13" t="n">
         <v>15246.63</v>
+      </c>
+      <c r="X58" s="13" t="n">
+        <v>15061.91</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -3951,6 +4094,7 @@
       <c r="U59" s="13" t="n"/>
       <c r="V59" s="13" t="n"/>
       <c r="W59" s="13" t="n"/>
+      <c r="X59" s="13" t="n"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4022,6 +4166,9 @@
       <c r="W60" s="13" t="n">
         <v>34.26</v>
       </c>
+      <c r="X60" s="13" t="n">
+        <v>33.52</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4092,6 +4239,9 @@
       </c>
       <c r="W61" s="13" t="n">
         <v>16456.67</v>
+      </c>
+      <c r="X61" s="13" t="n">
+        <v>15812.7</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -4118,6 +4268,7 @@
       <c r="U62" s="13" t="n"/>
       <c r="V62" s="13" t="n"/>
       <c r="W62" s="13" t="n"/>
+      <c r="X62" s="13" t="n"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4189,6 +4340,9 @@
       <c r="W63" s="13" t="n">
         <v>22.94</v>
       </c>
+      <c r="X63" s="13" t="n">
+        <v>21.86</v>
+      </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -4259,6 +4413,9 @@
       </c>
       <c r="W64" s="13" t="n">
         <v>9525.889999999999</v>
+      </c>
+      <c r="X64" s="13" t="n">
+        <v>9802.43</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -4285,6 +4442,7 @@
       <c r="U65" s="13" t="n"/>
       <c r="V65" s="13" t="n"/>
       <c r="W65" s="13" t="n"/>
+      <c r="X65" s="13" t="n"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4356,6 +4514,9 @@
       <c r="W66" s="13" t="n">
         <v>13.3</v>
       </c>
+      <c r="X66" s="13" t="n">
+        <v>12.46</v>
+      </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -4426,6 +4587,9 @@
       </c>
       <c r="W67" s="13" t="n">
         <v>9691.440000000001</v>
+      </c>
+      <c r="X67" s="13" t="n">
+        <v>9639.700000000001</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -4452,6 +4616,7 @@
       <c r="U68" s="13" t="n"/>
       <c r="V68" s="13" t="n"/>
       <c r="W68" s="13" t="n"/>
+      <c r="X68" s="13" t="n"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -4523,6 +4688,9 @@
       <c r="W69" s="13" t="n">
         <v>25.39</v>
       </c>
+      <c r="X69" s="13" t="n">
+        <v>24.92</v>
+      </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -4593,6 +4761,9 @@
       </c>
       <c r="W70" s="13" t="n">
         <v>3161.56</v>
+      </c>
+      <c r="X70" s="13" t="n">
+        <v>3112.96</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -4619,6 +4790,7 @@
       <c r="U71" s="13" t="n"/>
       <c r="V71" s="13" t="n"/>
       <c r="W71" s="13" t="n"/>
+      <c r="X71" s="13" t="n"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -4690,6 +4862,9 @@
       <c r="W72" s="13" t="n">
         <v>49.18</v>
       </c>
+      <c r="X72" s="13" t="n">
+        <v>48.12</v>
+      </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -4760,6 +4935,9 @@
       </c>
       <c r="W73" s="13" t="n">
         <v>5800.32</v>
+      </c>
+      <c r="X73" s="13" t="n">
+        <v>5755.35</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -4786,6 +4964,7 @@
       <c r="U74" s="13" t="n"/>
       <c r="V74" s="13" t="n"/>
       <c r="W74" s="13" t="n"/>
+      <c r="X74" s="13" t="n"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -4857,6 +5036,9 @@
       <c r="W75" s="13" t="n">
         <v>29.66</v>
       </c>
+      <c r="X75" s="13" t="n">
+        <v>28.1</v>
+      </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -4927,6 +5109,9 @@
       </c>
       <c r="W76" s="13" t="n">
         <v>9346.059999999999</v>
+      </c>
+      <c r="X76" s="13" t="n">
+        <v>9164.23</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -4953,6 +5138,7 @@
       <c r="U77" s="13" t="n"/>
       <c r="V77" s="13" t="n"/>
       <c r="W77" s="13" t="n"/>
+      <c r="X77" s="13" t="n"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -5024,6 +5210,9 @@
       <c r="W78" s="13" t="n">
         <v>17.64</v>
       </c>
+      <c r="X78" s="13" t="n">
+        <v>17.07</v>
+      </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -5094,6 +5283,9 @@
       </c>
       <c r="W79" s="13" t="n">
         <v>1526.45</v>
+      </c>
+      <c r="X79" s="13" t="n">
+        <v>1503.78</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -5120,6 +5312,7 @@
       <c r="U80" s="13" t="n"/>
       <c r="V80" s="13" t="n"/>
       <c r="W80" s="13" t="n"/>
+      <c r="X80" s="13" t="n"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -5191,6 +5384,9 @@
       <c r="W81" s="13" t="n">
         <v>17.82</v>
       </c>
+      <c r="X81" s="13" t="n">
+        <v>16.94</v>
+      </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -5261,6 +5457,9 @@
       </c>
       <c r="W82" s="13" t="n">
         <v>16412.83</v>
+      </c>
+      <c r="X82" s="13" t="n">
+        <v>16214.18</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -5287,6 +5486,7 @@
       <c r="U83" s="13" t="n"/>
       <c r="V83" s="13" t="n"/>
       <c r="W83" s="13" t="n"/>
+      <c r="X83" s="13" t="n"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -5358,6 +5558,9 @@
       <c r="W84" s="13" t="n">
         <v>53.73</v>
       </c>
+      <c r="X84" s="13" t="n">
+        <v>53.89</v>
+      </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -5428,6 +5631,9 @@
       </c>
       <c r="W85" s="13" t="n">
         <v>2977.45</v>
+      </c>
+      <c r="X85" s="13" t="n">
+        <v>3003.31</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -5454,6 +5660,7 @@
       <c r="U86" s="13" t="n"/>
       <c r="V86" s="13" t="n"/>
       <c r="W86" s="13" t="n"/>
+      <c r="X86" s="13" t="n"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -5525,6 +5732,9 @@
       <c r="W87" s="13" t="n">
         <v>58.69</v>
       </c>
+      <c r="X87" s="13" t="n">
+        <v>58.73</v>
+      </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -5595,6 +5805,9 @@
       </c>
       <c r="W88" s="13" t="n">
         <v>3069.18</v>
+      </c>
+      <c r="X88" s="13" t="n">
+        <v>3141.27</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -5621,6 +5834,7 @@
       <c r="U89" s="13" t="n"/>
       <c r="V89" s="13" t="n"/>
       <c r="W89" s="13" t="n"/>
+      <c r="X89" s="13" t="n"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -5692,6 +5906,9 @@
       <c r="W90" s="13" t="n">
         <v>51.18</v>
       </c>
+      <c r="X90" s="13" t="n">
+        <v>51.62</v>
+      </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -5762,6 +5979,9 @@
       </c>
       <c r="W91" s="13" t="n">
         <v>3159.03</v>
+      </c>
+      <c r="X91" s="13" t="n">
+        <v>3165.74</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -5788,6 +6008,7 @@
       <c r="U92" s="13" t="n"/>
       <c r="V92" s="13" t="n"/>
       <c r="W92" s="13" t="n"/>
+      <c r="X92" s="13" t="n"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -5859,6 +6080,9 @@
       <c r="W93" s="13" t="n">
         <v>48.64</v>
       </c>
+      <c r="X93" s="13" t="n">
+        <v>47.65</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -5929,6 +6153,9 @@
       </c>
       <c r="W94" s="13" t="n">
         <v>2027.75</v>
+      </c>
+      <c r="X94" s="13" t="n">
+        <v>2009.24</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -5955,6 +6182,7 @@
       <c r="U95" s="13" t="n"/>
       <c r="V95" s="13" t="n"/>
       <c r="W95" s="13" t="n"/>
+      <c r="X95" s="13" t="n"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -6026,6 +6254,9 @@
       <c r="W96" s="13" t="n">
         <v>28.84</v>
       </c>
+      <c r="X96" s="13" t="n">
+        <v>27.88</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -6096,6 +6327,9 @@
       </c>
       <c r="W97" s="13" t="n">
         <v>9948.450000000001</v>
+      </c>
+      <c r="X97" s="13" t="n">
+        <v>10691.64</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -6122,6 +6356,7 @@
       <c r="U98" s="13" t="n"/>
       <c r="V98" s="13" t="n"/>
       <c r="W98" s="13" t="n"/>
+      <c r="X98" s="13" t="n"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -6193,6 +6428,9 @@
       <c r="W99" s="13" t="n">
         <v>87.62</v>
       </c>
+      <c r="X99" s="13" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -6263,6 +6501,9 @@
       </c>
       <c r="W100" s="13" t="n">
         <v>10081.28</v>
+      </c>
+      <c r="X100" s="13" t="n">
+        <v>10734.32</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -6289,6 +6530,7 @@
       <c r="U101" s="13" t="n"/>
       <c r="V101" s="13" t="n"/>
       <c r="W101" s="13" t="n"/>
+      <c r="X101" s="13" t="n"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -6360,6 +6602,9 @@
       <c r="W102" s="13" t="n">
         <v>60</v>
       </c>
+      <c r="X102" s="13" t="n">
+        <v>59.67</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -6430,6 +6675,9 @@
       </c>
       <c r="W103" s="13" t="n">
         <v>15399.22</v>
+      </c>
+      <c r="X103" s="13" t="n">
+        <v>15526.61</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -6456,6 +6704,7 @@
       <c r="U104" s="13" t="n"/>
       <c r="V104" s="13" t="n"/>
       <c r="W104" s="13" t="n"/>
+      <c r="X104" s="13" t="n"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -6527,6 +6776,9 @@
       <c r="W105" s="13" t="n">
         <v>5.92</v>
       </c>
+      <c r="X105" s="13" t="n">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -6597,6 +6849,9 @@
       </c>
       <c r="W106" s="13" t="n">
         <v>2231.08</v>
+      </c>
+      <c r="X106" s="13" t="n">
+        <v>2217.44</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -6623,6 +6878,7 @@
       <c r="U107" s="13" t="n"/>
       <c r="V107" s="13" t="n"/>
       <c r="W107" s="13" t="n"/>
+      <c r="X107" s="13" t="n"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -6694,6 +6950,9 @@
       <c r="W108" s="13" t="n">
         <v>26.13</v>
       </c>
+      <c r="X108" s="13" t="n">
+        <v>25.43</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -6764,6 +7023,9 @@
       </c>
       <c r="W109" s="13" t="n">
         <v>857</v>
+      </c>
+      <c r="X109" s="13" t="n">
+        <v>843.23</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -6790,6 +7052,7 @@
       <c r="U110" s="13" t="n"/>
       <c r="V110" s="13" t="n"/>
       <c r="W110" s="13" t="n"/>
+      <c r="X110" s="13" t="n"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -6861,6 +7124,9 @@
       <c r="W111" s="13" t="n">
         <v>32.94</v>
       </c>
+      <c r="X111" s="13" t="n">
+        <v>32.94</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -6931,6 +7197,9 @@
       </c>
       <c r="W112" s="13" t="n">
         <v>3582.4</v>
+      </c>
+      <c r="X112" s="13" t="n">
+        <v>3473.84</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -6957,6 +7226,7 @@
       <c r="U113" s="13" t="n"/>
       <c r="V113" s="13" t="n"/>
       <c r="W113" s="13" t="n"/>
+      <c r="X113" s="13" t="n"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -7028,6 +7298,9 @@
       <c r="W114" s="13" t="n">
         <v>22.07</v>
       </c>
+      <c r="X114" s="13" t="n">
+        <v>22.19</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -7098,6 +7371,9 @@
       </c>
       <c r="W115" s="13" t="n">
         <v>4062.45</v>
+      </c>
+      <c r="X115" s="13" t="n">
+        <v>4078.21</v>
       </c>
     </row>
     <row r="116">
@@ -7109,6 +7385,7 @@
       <c r="U116" s="13" t="n"/>
       <c r="V116" s="13" t="n"/>
       <c r="W116" s="13" t="n"/>
+      <c r="X116" s="13" t="n"/>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -7135,6 +7412,9 @@
       <c r="W117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="X117" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -7160,6 +7440,9 @@
       </c>
       <c r="W118" s="13" t="n">
         <v>3013.79</v>
+      </c>
+      <c r="X118" s="13" t="n">
+        <v>3041.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-22 04:36:24]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X118"/>
+  <dimension ref="A1:Y119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -546,6 +546,7 @@
     <col width="15" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
     <col width="15" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -669,6 +670,11 @@
           <t>2026/01/19</t>
         </is>
       </c>
+      <c r="Y1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/22</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -791,6 +797,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="Y2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -865,6 +876,9 @@
       <c r="X3" s="13" t="n">
         <v>65.83</v>
       </c>
+      <c r="Y3" s="13" t="n">
+        <v>65.88</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -938,6 +952,9 @@
       </c>
       <c r="X4" s="13" t="n">
         <v>4107.18</v>
+      </c>
+      <c r="Y4" s="13" t="n">
+        <v>4110.86</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -965,6 +982,7 @@
       <c r="V5" s="13" t="n"/>
       <c r="W5" s="13" t="n"/>
       <c r="X5" s="13" t="n"/>
+      <c r="Y5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1039,6 +1057,7 @@
       <c r="X6" s="13" t="n">
         <v>51.1</v>
       </c>
+      <c r="Y6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1112,6 +1131,9 @@
       </c>
       <c r="X7" s="13" t="n">
         <v>5892.9</v>
+      </c>
+      <c r="Y7" s="13" t="n">
+        <v>51.13</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1139,6 +1161,9 @@
       <c r="V8" s="13" t="n"/>
       <c r="W8" s="13" t="n"/>
       <c r="X8" s="13" t="n"/>
+      <c r="Y8" s="13" t="n">
+        <v>5881.72</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1213,6 +1238,7 @@
       <c r="X9" s="13" t="n">
         <v>54.81</v>
       </c>
+      <c r="Y9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1286,6 +1312,9 @@
       </c>
       <c r="X10" s="13" t="n">
         <v>4721.07</v>
+      </c>
+      <c r="Y10" s="13" t="n">
+        <v>54.42</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1313,6 +1342,9 @@
       <c r="V11" s="13" t="n"/>
       <c r="W11" s="13" t="n"/>
       <c r="X11" s="13" t="n"/>
+      <c r="Y11" s="13" t="n">
+        <v>4701.22</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1387,6 +1419,7 @@
       <c r="X12" s="13" t="n">
         <v>61.12</v>
       </c>
+      <c r="Y12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1460,6 +1493,9 @@
       </c>
       <c r="X13" s="13" t="n">
         <v>8289.58</v>
+      </c>
+      <c r="Y13" s="13" t="n">
+        <v>61.34</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1487,6 +1523,9 @@
       <c r="V14" s="13" t="n"/>
       <c r="W14" s="13" t="n"/>
       <c r="X14" s="13" t="n"/>
+      <c r="Y14" s="13" t="n">
+        <v>8349.83</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1561,6 +1600,7 @@
       <c r="X15" s="13" t="n">
         <v>30.34</v>
       </c>
+      <c r="Y15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1634,6 +1674,9 @@
       </c>
       <c r="X16" s="13" t="n">
         <v>2738.68</v>
+      </c>
+      <c r="Y16" s="13" t="n">
+        <v>29.57</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1661,6 +1704,9 @@
       <c r="V17" s="13" t="n"/>
       <c r="W17" s="13" t="n"/>
       <c r="X17" s="13" t="n"/>
+      <c r="Y17" s="13" t="n">
+        <v>2743.09</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1735,6 +1781,7 @@
       <c r="X18" s="13" t="n">
         <v>97.05</v>
       </c>
+      <c r="Y18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1808,6 +1855,9 @@
       </c>
       <c r="X19" s="13" t="n">
         <v>6940.01</v>
+      </c>
+      <c r="Y19" s="13" t="n">
+        <v>96.06</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1835,6 +1885,9 @@
       <c r="V20" s="13" t="n"/>
       <c r="W20" s="13" t="n"/>
       <c r="X20" s="13" t="n"/>
+      <c r="Y20" s="13" t="n">
+        <v>6875.62</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1909,6 +1962,7 @@
       <c r="X21" s="13" t="n">
         <v>65.92</v>
       </c>
+      <c r="Y21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -1980,6 +2034,9 @@
       <c r="W22" s="13" t="inlineStr"/>
       <c r="X22" s="13" t="n">
         <v>83171.28</v>
+      </c>
+      <c r="Y22" s="13" t="n">
+        <v>59.46</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2007,6 +2064,9 @@
       <c r="V23" s="13" t="n"/>
       <c r="W23" s="13" t="n"/>
       <c r="X23" s="13" t="n"/>
+      <c r="Y23" s="13" t="n">
+        <v>82749.64</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2081,6 +2141,7 @@
       <c r="X24" s="13" t="n">
         <v>82.66</v>
       </c>
+      <c r="Y24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2154,6 +2215,9 @@
       </c>
       <c r="X25" s="13" t="n">
         <v>25297.13</v>
+      </c>
+      <c r="Y25" s="13" t="n">
+        <v>85.44</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2181,6 +2245,9 @@
       <c r="V26" s="13" t="n"/>
       <c r="W26" s="13" t="n"/>
       <c r="X26" s="13" t="n"/>
+      <c r="Y26" s="13" t="n">
+        <v>24560.98</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2255,6 +2322,7 @@
       <c r="X27" s="13" t="n">
         <v>76.81</v>
       </c>
+      <c r="Y27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2328,6 +2396,9 @@
       </c>
       <c r="X28" s="13" t="n">
         <v>53467.27</v>
+      </c>
+      <c r="Y28" s="13" t="n">
+        <v>74.48999999999999</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2355,6 +2426,9 @@
       <c r="V29" s="13" t="n"/>
       <c r="W29" s="13" t="n"/>
       <c r="X29" s="13" t="n"/>
+      <c r="Y29" s="13" t="n">
+        <v>53827.48</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2429,6 +2503,7 @@
       <c r="X30" s="13" t="n">
         <v>51.71</v>
       </c>
+      <c r="Y30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2502,6 +2577,9 @@
       </c>
       <c r="X31" s="13" t="n">
         <v>5512.31</v>
+      </c>
+      <c r="Y31" s="13" t="n">
+        <v>51.54</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2529,6 +2607,9 @@
       <c r="V32" s="13" t="n"/>
       <c r="W32" s="13" t="n"/>
       <c r="X32" s="13" t="n"/>
+      <c r="Y32" s="13" t="n">
+        <v>5610.43</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2603,6 +2684,7 @@
       <c r="X33" s="13" t="n">
         <v>1.39</v>
       </c>
+      <c r="Y33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2676,6 +2758,9 @@
       </c>
       <c r="X34" s="13" t="n">
         <v>33771.52</v>
+      </c>
+      <c r="Y34" s="13" t="n">
+        <v>1.49</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2703,6 +2788,9 @@
       <c r="V35" s="13" t="n"/>
       <c r="W35" s="13" t="n"/>
       <c r="X35" s="13" t="n"/>
+      <c r="Y35" s="13" t="n">
+        <v>33870.82</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2777,6 +2865,7 @@
       <c r="X36" s="13" t="n">
         <v>31.83</v>
       </c>
+      <c r="Y36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2850,6 +2939,9 @@
       </c>
       <c r="X37" s="13" t="n">
         <v>3489.83</v>
+      </c>
+      <c r="Y37" s="13" t="n">
+        <v>30.78</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2877,6 +2969,9 @@
       <c r="V38" s="13" t="n"/>
       <c r="W38" s="13" t="n"/>
       <c r="X38" s="13" t="n"/>
+      <c r="Y38" s="13" t="n">
+        <v>3419.01</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -2951,6 +3046,7 @@
       <c r="X39" s="13" t="n">
         <v>54.85</v>
       </c>
+      <c r="Y39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3024,6 +3120,9 @@
       </c>
       <c r="X40" s="13" t="n">
         <v>3339.56</v>
+      </c>
+      <c r="Y40" s="13" t="n">
+        <v>53.63</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3051,6 +3150,9 @@
       <c r="V41" s="13" t="n"/>
       <c r="W41" s="13" t="n"/>
       <c r="X41" s="13" t="n"/>
+      <c r="Y41" s="13" t="n">
+        <v>3282.48</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3125,6 +3227,7 @@
       <c r="X42" s="13" t="n">
         <v>20.69</v>
       </c>
+      <c r="Y42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3198,6 +3301,9 @@
       </c>
       <c r="X43" s="13" t="n">
         <v>7420.84</v>
+      </c>
+      <c r="Y43" s="13" t="n">
+        <v>20.12</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3225,6 +3331,9 @@
       <c r="V44" s="13" t="n"/>
       <c r="W44" s="13" t="n"/>
       <c r="X44" s="13" t="n"/>
+      <c r="Y44" s="13" t="n">
+        <v>7266.86</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3299,6 +3408,7 @@
       <c r="X45" s="13" t="n">
         <v>30.05</v>
       </c>
+      <c r="Y45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3372,6 +3482,9 @@
       </c>
       <c r="X46" s="13" t="n">
         <v>8564.43</v>
+      </c>
+      <c r="Y46" s="13" t="n">
+        <v>27.34</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3399,6 +3512,9 @@
       <c r="V47" s="13" t="n"/>
       <c r="W47" s="13" t="n"/>
       <c r="X47" s="13" t="n"/>
+      <c r="Y47" s="13" t="n">
+        <v>8372.07</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3473,6 +3589,7 @@
       <c r="X48" s="13" t="n">
         <v>6.88</v>
       </c>
+      <c r="Y48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3546,6 +3663,9 @@
       </c>
       <c r="X49" s="13" t="n">
         <v>12578.05</v>
+      </c>
+      <c r="Y49" s="13" t="n">
+        <v>6.71</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3573,6 +3693,9 @@
       <c r="V50" s="13" t="n"/>
       <c r="W50" s="13" t="n"/>
       <c r="X50" s="13" t="n"/>
+      <c r="Y50" s="13" t="n">
+        <v>12585.89</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3647,6 +3770,7 @@
       <c r="X51" s="13" t="n">
         <v>31.55</v>
       </c>
+      <c r="Y51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3720,6 +3844,9 @@
       </c>
       <c r="X52" s="13" t="n">
         <v>13344.13</v>
+      </c>
+      <c r="Y52" s="13" t="n">
+        <v>32.86</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -3747,6 +3874,9 @@
       <c r="V53" s="13" t="n"/>
       <c r="W53" s="13" t="n"/>
       <c r="X53" s="13" t="n"/>
+      <c r="Y53" s="13" t="n">
+        <v>13442.13</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3821,6 +3951,7 @@
       <c r="X54" s="13" t="n">
         <v>16.91</v>
       </c>
+      <c r="Y54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -3894,6 +4025,9 @@
       </c>
       <c r="X55" s="13" t="n">
         <v>8718.83</v>
+      </c>
+      <c r="Y55" s="13" t="n">
+        <v>15.68</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -3921,6 +4055,9 @@
       <c r="V56" s="13" t="n"/>
       <c r="W56" s="13" t="n"/>
       <c r="X56" s="13" t="n"/>
+      <c r="Y56" s="13" t="n">
+        <v>8598.309999999999</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -3995,6 +4132,7 @@
       <c r="X57" s="13" t="n">
         <v>23.82</v>
       </c>
+      <c r="Y57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4068,6 +4206,9 @@
       </c>
       <c r="X58" s="13" t="n">
         <v>15061.91</v>
+      </c>
+      <c r="Y58" s="13" t="n">
+        <v>22.93</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4095,6 +4236,9 @@
       <c r="V59" s="13" t="n"/>
       <c r="W59" s="13" t="n"/>
       <c r="X59" s="13" t="n"/>
+      <c r="Y59" s="13" t="n">
+        <v>14878.7</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4169,6 +4313,7 @@
       <c r="X60" s="13" t="n">
         <v>33.52</v>
       </c>
+      <c r="Y60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4242,6 +4387,9 @@
       </c>
       <c r="X61" s="13" t="n">
         <v>15812.7</v>
+      </c>
+      <c r="Y61" s="13" t="n">
+        <v>32.1</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -4269,6 +4417,9 @@
       <c r="V62" s="13" t="n"/>
       <c r="W62" s="13" t="n"/>
       <c r="X62" s="13" t="n"/>
+      <c r="Y62" s="13" t="n">
+        <v>15732.81</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4343,6 +4494,7 @@
       <c r="X63" s="13" t="n">
         <v>21.86</v>
       </c>
+      <c r="Y63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -4416,6 +4568,9 @@
       </c>
       <c r="X64" s="13" t="n">
         <v>9802.43</v>
+      </c>
+      <c r="Y64" s="13" t="n">
+        <v>20.76</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -4443,6 +4598,9 @@
       <c r="V65" s="13" t="n"/>
       <c r="W65" s="13" t="n"/>
       <c r="X65" s="13" t="n"/>
+      <c r="Y65" s="13" t="n">
+        <v>9629.93</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4517,6 +4675,7 @@
       <c r="X66" s="13" t="n">
         <v>12.46</v>
       </c>
+      <c r="Y66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -4590,6 +4749,9 @@
       </c>
       <c r="X67" s="13" t="n">
         <v>9639.700000000001</v>
+      </c>
+      <c r="Y67" s="13" t="n">
+        <v>12.73</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -4617,6 +4779,9 @@
       <c r="V68" s="13" t="n"/>
       <c r="W68" s="13" t="n"/>
       <c r="X68" s="13" t="n"/>
+      <c r="Y68" s="13" t="n">
+        <v>9654.24</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -4691,6 +4856,7 @@
       <c r="X69" s="13" t="n">
         <v>24.92</v>
       </c>
+      <c r="Y69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -4764,6 +4930,9 @@
       </c>
       <c r="X70" s="13" t="n">
         <v>3112.96</v>
+      </c>
+      <c r="Y70" s="13" t="n">
+        <v>24.24</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -4791,6 +4960,9 @@
       <c r="V71" s="13" t="n"/>
       <c r="W71" s="13" t="n"/>
       <c r="X71" s="13" t="n"/>
+      <c r="Y71" s="13" t="n">
+        <v>3100.66</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -4865,6 +5037,7 @@
       <c r="X72" s="13" t="n">
         <v>48.12</v>
       </c>
+      <c r="Y72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -4938,6 +5111,9 @@
       </c>
       <c r="X73" s="13" t="n">
         <v>5755.35</v>
+      </c>
+      <c r="Y73" s="13" t="n">
+        <v>47.42</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -4965,6 +5141,9 @@
       <c r="V74" s="13" t="n"/>
       <c r="W74" s="13" t="n"/>
       <c r="X74" s="13" t="n"/>
+      <c r="Y74" s="13" t="n">
+        <v>5722.87</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -5039,6 +5218,7 @@
       <c r="X75" s="13" t="n">
         <v>28.1</v>
       </c>
+      <c r="Y75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -5112,6 +5292,9 @@
       </c>
       <c r="X76" s="13" t="n">
         <v>9164.23</v>
+      </c>
+      <c r="Y76" s="13" t="n">
+        <v>26.57</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -5139,6 +5322,9 @@
       <c r="V77" s="13" t="n"/>
       <c r="W77" s="13" t="n"/>
       <c r="X77" s="13" t="n"/>
+      <c r="Y77" s="13" t="n">
+        <v>9010.57</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -5213,6 +5399,7 @@
       <c r="X78" s="13" t="n">
         <v>17.07</v>
       </c>
+      <c r="Y78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -5286,6 +5473,9 @@
       </c>
       <c r="X79" s="13" t="n">
         <v>1503.78</v>
+      </c>
+      <c r="Y79" s="13" t="n">
+        <v>16.66</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -5313,6 +5503,9 @@
       <c r="V80" s="13" t="n"/>
       <c r="W80" s="13" t="n"/>
       <c r="X80" s="13" t="n"/>
+      <c r="Y80" s="13" t="n">
+        <v>1492.61</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -5387,6 +5580,7 @@
       <c r="X81" s="13" t="n">
         <v>16.94</v>
       </c>
+      <c r="Y81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -5460,6 +5654,9 @@
       </c>
       <c r="X82" s="13" t="n">
         <v>16214.18</v>
+      </c>
+      <c r="Y82" s="13" t="n">
+        <v>16.42</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -5487,6 +5684,9 @@
       <c r="V83" s="13" t="n"/>
       <c r="W83" s="13" t="n"/>
       <c r="X83" s="13" t="n"/>
+      <c r="Y83" s="13" t="n">
+        <v>16043.32</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -5561,6 +5761,7 @@
       <c r="X84" s="13" t="n">
         <v>53.89</v>
       </c>
+      <c r="Y84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -5634,6 +5835,9 @@
       </c>
       <c r="X85" s="13" t="n">
         <v>3003.31</v>
+      </c>
+      <c r="Y85" s="13" t="n">
+        <v>53.66</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -5661,6 +5865,9 @@
       <c r="V86" s="13" t="n"/>
       <c r="W86" s="13" t="n"/>
       <c r="X86" s="13" t="n"/>
+      <c r="Y86" s="13" t="n">
+        <v>2966.75</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -5735,6 +5942,7 @@
       <c r="X87" s="13" t="n">
         <v>58.73</v>
       </c>
+      <c r="Y87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -5808,6 +6016,9 @@
       </c>
       <c r="X88" s="13" t="n">
         <v>3141.27</v>
+      </c>
+      <c r="Y88" s="13" t="n">
+        <v>58.55</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -5835,6 +6046,9 @@
       <c r="V89" s="13" t="n"/>
       <c r="W89" s="13" t="n"/>
       <c r="X89" s="13" t="n"/>
+      <c r="Y89" s="13" t="n">
+        <v>3141.27</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -5909,6 +6123,7 @@
       <c r="X90" s="13" t="n">
         <v>51.62</v>
       </c>
+      <c r="Y90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -5982,6 +6197,9 @@
       </c>
       <c r="X91" s="13" t="n">
         <v>3165.74</v>
+      </c>
+      <c r="Y91" s="13" t="n">
+        <v>51.41</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -6009,6 +6227,9 @@
       <c r="V92" s="13" t="n"/>
       <c r="W92" s="13" t="n"/>
       <c r="X92" s="13" t="n"/>
+      <c r="Y92" s="13" t="n">
+        <v>3160.49</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -6083,6 +6304,7 @@
       <c r="X93" s="13" t="n">
         <v>47.65</v>
       </c>
+      <c r="Y93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -6156,6 +6378,9 @@
       </c>
       <c r="X94" s="13" t="n">
         <v>2009.24</v>
+      </c>
+      <c r="Y94" s="13" t="n">
+        <v>46.14</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -6183,6 +6408,9 @@
       <c r="V95" s="13" t="n"/>
       <c r="W95" s="13" t="n"/>
       <c r="X95" s="13" t="n"/>
+      <c r="Y95" s="13" t="n">
+        <v>1979.81</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -6257,6 +6485,7 @@
       <c r="X96" s="13" t="n">
         <v>27.88</v>
       </c>
+      <c r="Y96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -6330,6 +6559,9 @@
       </c>
       <c r="X97" s="13" t="n">
         <v>10691.64</v>
+      </c>
+      <c r="Y97" s="13" t="n">
+        <v>27.62</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -6357,6 +6589,9 @@
       <c r="V98" s="13" t="n"/>
       <c r="W98" s="13" t="n"/>
       <c r="X98" s="13" t="n"/>
+      <c r="Y98" s="13" t="n">
+        <v>10593.43</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -6431,6 +6666,7 @@
       <c r="X99" s="13" t="n">
         <v>88</v>
       </c>
+      <c r="Y99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -6504,6 +6740,9 @@
       </c>
       <c r="X100" s="13" t="n">
         <v>10734.32</v>
+      </c>
+      <c r="Y100" s="13" t="n">
+        <v>88.17</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -6531,6 +6770,9 @@
       <c r="V101" s="13" t="n"/>
       <c r="W101" s="13" t="n"/>
       <c r="X101" s="13" t="n"/>
+      <c r="Y101" s="13" t="n">
+        <v>10831.45</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -6605,6 +6847,7 @@
       <c r="X102" s="13" t="n">
         <v>59.67</v>
       </c>
+      <c r="Y102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -6678,6 +6921,9 @@
       </c>
       <c r="X103" s="13" t="n">
         <v>15526.61</v>
+      </c>
+      <c r="Y103" s="13" t="n">
+        <v>59.41</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -6705,6 +6951,9 @@
       <c r="V104" s="13" t="n"/>
       <c r="W104" s="13" t="n"/>
       <c r="X104" s="13" t="n"/>
+      <c r="Y104" s="13" t="n">
+        <v>15472.74</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -6779,6 +7028,7 @@
       <c r="X105" s="13" t="n">
         <v>5.6</v>
       </c>
+      <c r="Y105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -6852,6 +7102,9 @@
       </c>
       <c r="X106" s="13" t="n">
         <v>2217.44</v>
+      </c>
+      <c r="Y106" s="13" t="n">
+        <v>5.45</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -6879,6 +7132,9 @@
       <c r="V107" s="13" t="n"/>
       <c r="W107" s="13" t="n"/>
       <c r="X107" s="13" t="n"/>
+      <c r="Y107" s="13" t="n">
+        <v>2199.48</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -6953,6 +7209,7 @@
       <c r="X108" s="13" t="n">
         <v>25.43</v>
       </c>
+      <c r="Y108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -7026,6 +7283,9 @@
       </c>
       <c r="X109" s="13" t="n">
         <v>843.23</v>
+      </c>
+      <c r="Y109" s="13" t="n">
+        <v>25.31</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -7053,6 +7313,9 @@
       <c r="V110" s="13" t="n"/>
       <c r="W110" s="13" t="n"/>
       <c r="X110" s="13" t="n"/>
+      <c r="Y110" s="13" t="n">
+        <v>844.78</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -7127,6 +7390,7 @@
       <c r="X111" s="13" t="n">
         <v>32.94</v>
       </c>
+      <c r="Y111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -7200,6 +7464,9 @@
       </c>
       <c r="X112" s="13" t="n">
         <v>3473.84</v>
+      </c>
+      <c r="Y112" s="13" t="n">
+        <v>33.36</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -7227,6 +7494,9 @@
       <c r="V113" s="13" t="n"/>
       <c r="W113" s="13" t="n"/>
       <c r="X113" s="13" t="n"/>
+      <c r="Y113" s="13" t="n">
+        <v>3561.41</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -7301,6 +7571,7 @@
       <c r="X114" s="13" t="n">
         <v>22.19</v>
       </c>
+      <c r="Y114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -7374,6 +7645,9 @@
       </c>
       <c r="X115" s="13" t="n">
         <v>4078.21</v>
+      </c>
+      <c r="Y115" s="13" t="n">
+        <v>22.53</v>
       </c>
     </row>
     <row r="116">
@@ -7386,6 +7660,9 @@
       <c r="V116" s="13" t="n"/>
       <c r="W116" s="13" t="n"/>
       <c r="X116" s="13" t="n"/>
+      <c r="Y116" s="13" t="n">
+        <v>4141.75</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -7415,6 +7692,7 @@
       <c r="X117" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="Y117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -7443,6 +7721,14 @@
       </c>
       <c r="X118" s="13" t="n">
         <v>3041.64</v>
+      </c>
+      <c r="Y118" s="13" t="n">
+        <v>29.02</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="Y119" s="13" t="n">
+        <v>3126.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-26 04:43:27]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y119"/>
+  <dimension ref="A1:Z119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -547,6 +547,7 @@
     <col width="15" customWidth="1" min="23" max="23"/>
     <col width="15" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -675,6 +676,11 @@
           <t>2026/01/22</t>
         </is>
       </c>
+      <c r="Z1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/26</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -802,6 +808,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="Z2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -879,6 +890,9 @@
       <c r="Y3" s="13" t="n">
         <v>65.88</v>
       </c>
+      <c r="Z3" s="13" t="n">
+        <v>66.14</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -955,6 +969,9 @@
       </c>
       <c r="Y4" s="13" t="n">
         <v>4110.86</v>
+      </c>
+      <c r="Z4" s="13" t="n">
+        <v>4141.01</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -983,6 +1000,7 @@
       <c r="W5" s="13" t="n"/>
       <c r="X5" s="13" t="n"/>
       <c r="Y5" s="13" t="n"/>
+      <c r="Z5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1058,6 +1076,7 @@
         <v>51.1</v>
       </c>
       <c r="Y6" s="13" t="n"/>
+      <c r="Z6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1133,6 +1152,9 @@
         <v>5892.9</v>
       </c>
       <c r="Y7" s="13" t="n">
+        <v>51.13</v>
+      </c>
+      <c r="Z7" s="13" t="n">
         <v>51.13</v>
       </c>
     </row>
@@ -1164,6 +1186,9 @@
       <c r="Y8" s="13" t="n">
         <v>5881.72</v>
       </c>
+      <c r="Z8" s="13" t="n">
+        <v>5936.21</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1239,6 +1264,7 @@
         <v>54.81</v>
       </c>
       <c r="Y9" s="13" t="n"/>
+      <c r="Z9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1315,6 +1341,9 @@
       </c>
       <c r="Y10" s="13" t="n">
         <v>54.42</v>
+      </c>
+      <c r="Z10" s="13" t="n">
+        <v>53.34</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1345,6 +1374,9 @@
       <c r="Y11" s="13" t="n">
         <v>4701.22</v>
       </c>
+      <c r="Z11" s="13" t="n">
+        <v>4715.12</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1420,6 +1452,7 @@
         <v>61.12</v>
       </c>
       <c r="Y12" s="13" t="n"/>
+      <c r="Z12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1496,6 +1529,9 @@
       </c>
       <c r="Y13" s="13" t="n">
         <v>61.34</v>
+      </c>
+      <c r="Z13" s="13" t="n">
+        <v>61.84</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1526,6 +1562,9 @@
       <c r="Y14" s="13" t="n">
         <v>8349.83</v>
       </c>
+      <c r="Z14" s="13" t="n">
+        <v>8522.32</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1601,6 +1640,7 @@
         <v>30.34</v>
       </c>
       <c r="Y15" s="13" t="n"/>
+      <c r="Z15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1677,6 +1717,9 @@
       </c>
       <c r="Y16" s="13" t="n">
         <v>29.57</v>
+      </c>
+      <c r="Z16" s="13" t="n">
+        <v>29.21</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1707,6 +1750,9 @@
       <c r="Y17" s="13" t="n">
         <v>2743.09</v>
       </c>
+      <c r="Z17" s="13" t="n">
+        <v>2748.51</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1782,6 +1828,7 @@
         <v>97.05</v>
       </c>
       <c r="Y18" s="13" t="n"/>
+      <c r="Z18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1858,6 +1905,9 @@
       </c>
       <c r="Y19" s="13" t="n">
         <v>96.06</v>
+      </c>
+      <c r="Z19" s="13" t="n">
+        <v>96.88</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1888,6 +1938,9 @@
       <c r="Y20" s="13" t="n">
         <v>6875.62</v>
       </c>
+      <c r="Z20" s="13" t="n">
+        <v>6915.61</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -1963,6 +2016,7 @@
         <v>65.92</v>
       </c>
       <c r="Y21" s="13" t="n"/>
+      <c r="Z21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2037,6 +2091,9 @@
       </c>
       <c r="Y22" s="13" t="n">
         <v>59.46</v>
+      </c>
+      <c r="Z22" s="13" t="n">
+        <v>59.07</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2067,6 +2124,9 @@
       <c r="Y23" s="13" t="n">
         <v>82749.64</v>
       </c>
+      <c r="Z23" s="13" t="n">
+        <v>81537.7</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2142,6 +2202,7 @@
         <v>82.66</v>
       </c>
       <c r="Y24" s="13" t="n"/>
+      <c r="Z24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2218,6 +2279,9 @@
       </c>
       <c r="Y25" s="13" t="n">
         <v>85.44</v>
+      </c>
+      <c r="Z25" s="13" t="n">
+        <v>80.97</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2248,6 +2312,9 @@
       <c r="Y26" s="13" t="n">
         <v>24560.98</v>
       </c>
+      <c r="Z26" s="13" t="n">
+        <v>24900.71</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2323,6 +2390,7 @@
         <v>76.81</v>
       </c>
       <c r="Y27" s="13" t="n"/>
+      <c r="Z27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2399,6 +2467,9 @@
       </c>
       <c r="Y28" s="13" t="n">
         <v>74.48999999999999</v>
+      </c>
+      <c r="Z28" s="13" t="n">
+        <v>76.06</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2429,6 +2500,9 @@
       <c r="Y29" s="13" t="n">
         <v>53827.48</v>
       </c>
+      <c r="Z29" s="13" t="n">
+        <v>52800.06</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2504,6 +2578,7 @@
         <v>51.71</v>
       </c>
       <c r="Y30" s="13" t="n"/>
+      <c r="Z30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2580,6 +2655,9 @@
       </c>
       <c r="Y31" s="13" t="n">
         <v>51.54</v>
+      </c>
+      <c r="Z31" s="13" t="n">
+        <v>51.89</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2610,6 +2688,9 @@
       <c r="Y32" s="13" t="n">
         <v>5610.43</v>
       </c>
+      <c r="Z32" s="13" t="n">
+        <v>5654.38</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2685,6 +2766,7 @@
         <v>1.39</v>
       </c>
       <c r="Y33" s="13" t="n"/>
+      <c r="Z33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2761,6 +2843,9 @@
       </c>
       <c r="Y34" s="13" t="n">
         <v>1.49</v>
+      </c>
+      <c r="Z34" s="13" t="n">
+        <v>1.46</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2791,6 +2876,9 @@
       <c r="Y35" s="13" t="n">
         <v>33870.82</v>
       </c>
+      <c r="Z35" s="13" t="n">
+        <v>34321.84</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2866,6 +2954,7 @@
         <v>31.83</v>
       </c>
       <c r="Y36" s="13" t="n"/>
+      <c r="Z36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -2942,6 +3031,9 @@
       </c>
       <c r="Y37" s="13" t="n">
         <v>30.78</v>
+      </c>
+      <c r="Z37" s="13" t="n">
+        <v>31.34</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -2972,6 +3064,9 @@
       <c r="Y38" s="13" t="n">
         <v>3419.01</v>
       </c>
+      <c r="Z38" s="13" t="n">
+        <v>3453.07</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3047,6 +3142,7 @@
         <v>54.85</v>
       </c>
       <c r="Y39" s="13" t="n"/>
+      <c r="Z39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3123,6 +3219,9 @@
       </c>
       <c r="Y40" s="13" t="n">
         <v>53.63</v>
+      </c>
+      <c r="Z40" s="13" t="n">
+        <v>54.84</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3153,6 +3252,9 @@
       <c r="Y41" s="13" t="n">
         <v>3282.48</v>
       </c>
+      <c r="Z41" s="13" t="n">
+        <v>3320.81</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3228,6 +3330,7 @@
         <v>20.69</v>
       </c>
       <c r="Y42" s="13" t="n"/>
+      <c r="Z42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3304,6 +3407,9 @@
       </c>
       <c r="Y43" s="13" t="n">
         <v>20.12</v>
+      </c>
+      <c r="Z43" s="13" t="n">
+        <v>20.35</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3334,6 +3440,9 @@
       <c r="Y44" s="13" t="n">
         <v>7266.86</v>
       </c>
+      <c r="Z44" s="13" t="n">
+        <v>7259.36</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3409,6 +3518,7 @@
         <v>30.05</v>
       </c>
       <c r="Y45" s="13" t="n"/>
+      <c r="Z45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3485,6 +3595,9 @@
       </c>
       <c r="Y46" s="13" t="n">
         <v>27.34</v>
+      </c>
+      <c r="Z46" s="13" t="n">
+        <v>26.64</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3515,6 +3628,9 @@
       <c r="Y47" s="13" t="n">
         <v>8372.07</v>
       </c>
+      <c r="Z47" s="13" t="n">
+        <v>8344.1</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3590,6 +3706,7 @@
         <v>6.88</v>
       </c>
       <c r="Y48" s="13" t="n"/>
+      <c r="Z48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3666,6 +3783,9 @@
       </c>
       <c r="Y49" s="13" t="n">
         <v>6.71</v>
+      </c>
+      <c r="Z49" s="13" t="n">
+        <v>6.62</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3696,6 +3816,9 @@
       <c r="Y50" s="13" t="n">
         <v>12585.89</v>
       </c>
+      <c r="Z50" s="13" t="n">
+        <v>12336.44</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3771,6 +3894,7 @@
         <v>31.55</v>
       </c>
       <c r="Y51" s="13" t="n"/>
+      <c r="Z51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3847,6 +3971,9 @@
       </c>
       <c r="Y52" s="13" t="n">
         <v>32.86</v>
+      </c>
+      <c r="Z52" s="13" t="n">
+        <v>31.98</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -3877,6 +4004,9 @@
       <c r="Y53" s="13" t="n">
         <v>13442.13</v>
       </c>
+      <c r="Z53" s="13" t="n">
+        <v>13181.48</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -3952,6 +4082,7 @@
         <v>16.91</v>
       </c>
       <c r="Y54" s="13" t="n"/>
+      <c r="Z54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4028,6 +4159,9 @@
       </c>
       <c r="Y55" s="13" t="n">
         <v>15.68</v>
+      </c>
+      <c r="Z55" s="13" t="n">
+        <v>15.37</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4058,6 +4192,9 @@
       <c r="Y56" s="13" t="n">
         <v>8598.309999999999</v>
       </c>
+      <c r="Z56" s="13" t="n">
+        <v>8399.9</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4133,6 +4270,7 @@
         <v>23.82</v>
       </c>
       <c r="Y57" s="13" t="n"/>
+      <c r="Z57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4209,6 +4347,9 @@
       </c>
       <c r="Y58" s="13" t="n">
         <v>22.93</v>
+      </c>
+      <c r="Z58" s="13" t="n">
+        <v>22.71</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4239,6 +4380,9 @@
       <c r="Y59" s="13" t="n">
         <v>14878.7</v>
       </c>
+      <c r="Z59" s="13" t="n">
+        <v>14741.85</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4314,6 +4458,7 @@
         <v>33.52</v>
       </c>
       <c r="Y60" s="13" t="n"/>
+      <c r="Z60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4390,6 +4535,9 @@
       </c>
       <c r="Y61" s="13" t="n">
         <v>32.1</v>
+      </c>
+      <c r="Z61" s="13" t="n">
+        <v>32.02</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -4420,6 +4568,9 @@
       <c r="Y62" s="13" t="n">
         <v>15732.81</v>
       </c>
+      <c r="Z62" s="13" t="n">
+        <v>15529.62</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4495,6 +4646,7 @@
         <v>21.86</v>
       </c>
       <c r="Y63" s="13" t="n"/>
+      <c r="Z63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -4571,6 +4723,9 @@
       </c>
       <c r="Y64" s="13" t="n">
         <v>20.76</v>
+      </c>
+      <c r="Z64" s="13" t="n">
+        <v>21.07</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -4601,6 +4756,9 @@
       <c r="Y65" s="13" t="n">
         <v>9629.93</v>
       </c>
+      <c r="Z65" s="13" t="n">
+        <v>9668.809999999999</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4676,6 +4834,7 @@
         <v>12.46</v>
       </c>
       <c r="Y66" s="13" t="n"/>
+      <c r="Z66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -4752,6 +4911,9 @@
       </c>
       <c r="Y67" s="13" t="n">
         <v>12.73</v>
+      </c>
+      <c r="Z67" s="13" t="n">
+        <v>12.84</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -4782,6 +4944,9 @@
       <c r="Y68" s="13" t="n">
         <v>9654.24</v>
       </c>
+      <c r="Z68" s="13" t="n">
+        <v>9712.48</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -4857,6 +5022,7 @@
         <v>24.92</v>
       </c>
       <c r="Y69" s="13" t="n"/>
+      <c r="Z69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -4933,6 +5099,9 @@
       </c>
       <c r="Y70" s="13" t="n">
         <v>24.24</v>
+      </c>
+      <c r="Z70" s="13" t="n">
+        <v>24.61</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -4963,6 +5132,9 @@
       <c r="Y71" s="13" t="n">
         <v>3100.66</v>
       </c>
+      <c r="Z71" s="13" t="n">
+        <v>3112.04</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -5038,6 +5210,7 @@
         <v>48.12</v>
       </c>
       <c r="Y72" s="13" t="n"/>
+      <c r="Z72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -5114,6 +5287,9 @@
       </c>
       <c r="Y73" s="13" t="n">
         <v>47.42</v>
+      </c>
+      <c r="Z73" s="13" t="n">
+        <v>47.87</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -5144,6 +5320,9 @@
       <c r="Y74" s="13" t="n">
         <v>5722.87</v>
       </c>
+      <c r="Z74" s="13" t="n">
+        <v>5722.24</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -5219,6 +5398,7 @@
         <v>28.1</v>
       </c>
       <c r="Y75" s="13" t="n"/>
+      <c r="Z75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -5295,6 +5475,9 @@
       </c>
       <c r="Y76" s="13" t="n">
         <v>26.57</v>
+      </c>
+      <c r="Z76" s="13" t="n">
+        <v>26.68</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -5325,6 +5508,9 @@
       <c r="Y77" s="13" t="n">
         <v>9010.57</v>
       </c>
+      <c r="Z77" s="13" t="n">
+        <v>9031.110000000001</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -5400,6 +5586,7 @@
         <v>17.07</v>
       </c>
       <c r="Y78" s="13" t="n"/>
+      <c r="Z78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -5476,6 +5663,9 @@
       </c>
       <c r="Y79" s="13" t="n">
         <v>16.66</v>
+      </c>
+      <c r="Z79" s="13" t="n">
+        <v>14.92</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -5506,6 +5696,9 @@
       <c r="Y80" s="13" t="n">
         <v>1492.61</v>
       </c>
+      <c r="Z80" s="13" t="n">
+        <v>1443.29</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -5581,6 +5774,7 @@
         <v>16.94</v>
       </c>
       <c r="Y81" s="13" t="n"/>
+      <c r="Z81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -5657,6 +5851,9 @@
       </c>
       <c r="Y82" s="13" t="n">
         <v>16.42</v>
+      </c>
+      <c r="Z82" s="13" t="n">
+        <v>16.25</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -5687,6 +5884,9 @@
       <c r="Y83" s="13" t="n">
         <v>16043.32</v>
       </c>
+      <c r="Z83" s="13" t="n">
+        <v>15985</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -5762,6 +5962,7 @@
         <v>53.89</v>
       </c>
       <c r="Y84" s="13" t="n"/>
+      <c r="Z84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -5838,6 +6039,9 @@
       </c>
       <c r="Y85" s="13" t="n">
         <v>53.66</v>
+      </c>
+      <c r="Z85" s="13" t="n">
+        <v>55.05</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -5868,6 +6072,9 @@
       <c r="Y86" s="13" t="n">
         <v>2966.75</v>
       </c>
+      <c r="Z86" s="13" t="n">
+        <v>3097.65</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -5943,6 +6150,7 @@
         <v>58.73</v>
       </c>
       <c r="Y87" s="13" t="n"/>
+      <c r="Z87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -6019,6 +6227,9 @@
       </c>
       <c r="Y88" s="13" t="n">
         <v>58.55</v>
+      </c>
+      <c r="Z88" s="13" t="n">
+        <v>58.73</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -6049,6 +6260,9 @@
       <c r="Y89" s="13" t="n">
         <v>3141.27</v>
       </c>
+      <c r="Z89" s="13" t="n">
+        <v>3354.76</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -6124,6 +6338,7 @@
         <v>51.62</v>
       </c>
       <c r="Y90" s="13" t="n"/>
+      <c r="Z90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -6200,6 +6415,9 @@
       </c>
       <c r="Y91" s="13" t="n">
         <v>51.41</v>
+      </c>
+      <c r="Z91" s="13" t="n">
+        <v>51.86</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -6230,6 +6448,9 @@
       <c r="Y92" s="13" t="n">
         <v>3160.49</v>
       </c>
+      <c r="Z92" s="13" t="n">
+        <v>3209.69</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -6305,6 +6526,7 @@
         <v>47.65</v>
       </c>
       <c r="Y93" s="13" t="n"/>
+      <c r="Z93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -6381,6 +6603,9 @@
       </c>
       <c r="Y94" s="13" t="n">
         <v>46.14</v>
+      </c>
+      <c r="Z94" s="13" t="n">
+        <v>45.76</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -6411,6 +6636,9 @@
       <c r="Y95" s="13" t="n">
         <v>1979.81</v>
       </c>
+      <c r="Z95" s="13" t="n">
+        <v>1947.38</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -6486,6 +6714,7 @@
         <v>27.88</v>
       </c>
       <c r="Y96" s="13" t="n"/>
+      <c r="Z96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -6562,6 +6791,9 @@
       </c>
       <c r="Y97" s="13" t="n">
         <v>27.62</v>
+      </c>
+      <c r="Z97" s="13" t="n">
+        <v>27.88</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -6592,6 +6824,9 @@
       <c r="Y98" s="13" t="n">
         <v>10593.43</v>
       </c>
+      <c r="Z98" s="13" t="n">
+        <v>10602.82</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -6667,6 +6902,7 @@
         <v>88</v>
       </c>
       <c r="Y99" s="13" t="n"/>
+      <c r="Z99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -6743,6 +6979,9 @@
       </c>
       <c r="Y100" s="13" t="n">
         <v>88.17</v>
+      </c>
+      <c r="Z100" s="13" t="n">
+        <v>88.05</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -6773,6 +7012,9 @@
       <c r="Y101" s="13" t="n">
         <v>10831.45</v>
       </c>
+      <c r="Z101" s="13" t="n">
+        <v>10704.68</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -6848,6 +7090,7 @@
         <v>59.67</v>
       </c>
       <c r="Y102" s="13" t="n"/>
+      <c r="Z102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -6924,6 +7167,9 @@
       </c>
       <c r="Y103" s="13" t="n">
         <v>59.41</v>
+      </c>
+      <c r="Z103" s="13" t="n">
+        <v>60.03</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -6954,6 +7200,9 @@
       <c r="Y104" s="13" t="n">
         <v>15472.74</v>
       </c>
+      <c r="Z104" s="13" t="n">
+        <v>15500.32</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -7029,6 +7278,7 @@
         <v>5.6</v>
       </c>
       <c r="Y105" s="13" t="n"/>
+      <c r="Z105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -7105,6 +7355,9 @@
       </c>
       <c r="Y106" s="13" t="n">
         <v>5.45</v>
+      </c>
+      <c r="Z106" s="13" t="n">
+        <v>5.46</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -7135,6 +7388,9 @@
       <c r="Y107" s="13" t="n">
         <v>2199.48</v>
       </c>
+      <c r="Z107" s="13" t="n">
+        <v>2199.54</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -7210,6 +7466,7 @@
         <v>25.43</v>
       </c>
       <c r="Y108" s="13" t="n"/>
+      <c r="Z108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -7285,6 +7542,9 @@
         <v>843.23</v>
       </c>
       <c r="Y109" s="13" t="n">
+        <v>25.31</v>
+      </c>
+      <c r="Z109" s="13" t="n">
         <v>25.31</v>
       </c>
     </row>
@@ -7316,6 +7576,9 @@
       <c r="Y110" s="13" t="n">
         <v>844.78</v>
       </c>
+      <c r="Z110" s="13" t="n">
+        <v>853.6799999999999</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -7391,6 +7654,7 @@
         <v>32.94</v>
       </c>
       <c r="Y111" s="13" t="n"/>
+      <c r="Z111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -7467,6 +7731,9 @@
       </c>
       <c r="Y112" s="13" t="n">
         <v>33.36</v>
+      </c>
+      <c r="Z112" s="13" t="n">
+        <v>33.59</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -7497,6 +7764,9 @@
       <c r="Y113" s="13" t="n">
         <v>3561.41</v>
       </c>
+      <c r="Z113" s="13" t="n">
+        <v>3855.83</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -7572,6 +7842,7 @@
         <v>22.19</v>
       </c>
       <c r="Y114" s="13" t="n"/>
+      <c r="Z114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -7648,6 +7919,9 @@
       </c>
       <c r="Y115" s="13" t="n">
         <v>22.53</v>
+      </c>
+      <c r="Z115" s="13" t="n">
+        <v>22.52</v>
       </c>
     </row>
     <row r="116">
@@ -7663,6 +7937,9 @@
       <c r="Y116" s="13" t="n">
         <v>4141.75</v>
       </c>
+      <c r="Z116" s="13" t="n">
+        <v>4168.32</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -7693,6 +7970,7 @@
         <v>29.02</v>
       </c>
       <c r="Y117" s="13" t="n"/>
+      <c r="Z117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -7725,10 +8003,16 @@
       <c r="Y118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="Z118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
         <v>3126.1</v>
+      </c>
+      <c r="Z119" s="13" t="n">
+        <v>3104.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-01-29 04:56:02]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z119"/>
+  <dimension ref="A1:AA119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -548,6 +548,7 @@
     <col width="15" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="15" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -681,6 +682,11 @@
           <t>2026/01/26</t>
         </is>
       </c>
+      <c r="AA1" s="13" t="inlineStr">
+        <is>
+          <t>2026/01/29</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -813,6 +819,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AA2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -893,6 +904,9 @@
       <c r="Z3" s="13" t="n">
         <v>66.14</v>
       </c>
+      <c r="AA3" s="13" t="n">
+        <v>66.16</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -972,6 +986,9 @@
       </c>
       <c r="Z4" s="13" t="n">
         <v>4141.01</v>
+      </c>
+      <c r="AA4" s="13" t="n">
+        <v>4147.15</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1001,6 +1018,7 @@
       <c r="X5" s="13" t="n"/>
       <c r="Y5" s="13" t="n"/>
       <c r="Z5" s="13" t="n"/>
+      <c r="AA5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1077,6 +1095,7 @@
       </c>
       <c r="Y6" s="13" t="n"/>
       <c r="Z6" s="13" t="n"/>
+      <c r="AA6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1156,6 +1175,9 @@
       </c>
       <c r="Z7" s="13" t="n">
         <v>51.13</v>
+      </c>
+      <c r="AA7" s="13" t="n">
+        <v>51.43</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1189,6 +1211,9 @@
       <c r="Z8" s="13" t="n">
         <v>5936.21</v>
       </c>
+      <c r="AA8" s="13" t="n">
+        <v>5950.84</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1265,6 +1290,7 @@
       </c>
       <c r="Y9" s="13" t="n"/>
       <c r="Z9" s="13" t="n"/>
+      <c r="AA9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1344,6 +1370,9 @@
       </c>
       <c r="Z10" s="13" t="n">
         <v>53.34</v>
+      </c>
+      <c r="AA10" s="13" t="n">
+        <v>54.62</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1377,6 +1406,9 @@
       <c r="Z11" s="13" t="n">
         <v>4715.12</v>
       </c>
+      <c r="AA11" s="13" t="n">
+        <v>4713.5</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1453,6 +1485,7 @@
       </c>
       <c r="Y12" s="13" t="n"/>
       <c r="Z12" s="13" t="n"/>
+      <c r="AA12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1532,6 +1565,9 @@
       </c>
       <c r="Z13" s="13" t="n">
         <v>61.84</v>
+      </c>
+      <c r="AA13" s="13" t="n">
+        <v>61.88</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1565,6 +1601,9 @@
       <c r="Z14" s="13" t="n">
         <v>8522.32</v>
       </c>
+      <c r="AA14" s="13" t="n">
+        <v>8605.49</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1641,6 +1680,7 @@
       </c>
       <c r="Y15" s="13" t="n"/>
       <c r="Z15" s="13" t="n"/>
+      <c r="AA15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1720,6 +1760,9 @@
       </c>
       <c r="Z16" s="13" t="n">
         <v>29.21</v>
+      </c>
+      <c r="AA16" s="13" t="n">
+        <v>31.7</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1753,6 +1796,9 @@
       <c r="Z17" s="13" t="n">
         <v>2748.51</v>
       </c>
+      <c r="AA17" s="13" t="n">
+        <v>2740.51</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1829,6 +1875,7 @@
       </c>
       <c r="Y18" s="13" t="n"/>
       <c r="Z18" s="13" t="n"/>
+      <c r="AA18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1908,6 +1955,9 @@
       </c>
       <c r="Z19" s="13" t="n">
         <v>96.88</v>
+      </c>
+      <c r="AA19" s="13" t="n">
+        <v>96.72</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1941,6 +1991,9 @@
       <c r="Z20" s="13" t="n">
         <v>6915.61</v>
       </c>
+      <c r="AA20" s="13" t="n">
+        <v>6978.03</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2017,6 +2070,7 @@
       </c>
       <c r="Y21" s="13" t="n"/>
       <c r="Z21" s="13" t="n"/>
+      <c r="AA21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2094,6 +2148,9 @@
       </c>
       <c r="Z22" s="13" t="n">
         <v>59.07</v>
+      </c>
+      <c r="AA22" s="13" t="n">
+        <v>60.87</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2127,6 +2184,9 @@
       <c r="Z23" s="13" t="n">
         <v>81537.7</v>
       </c>
+      <c r="AA23" s="13" t="n">
+        <v>81785.89999999999</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2203,6 +2263,7 @@
       </c>
       <c r="Y24" s="13" t="n"/>
       <c r="Z24" s="13" t="n"/>
+      <c r="AA24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2282,6 +2343,9 @@
       </c>
       <c r="Z25" s="13" t="n">
         <v>80.97</v>
+      </c>
+      <c r="AA25" s="13" t="n">
+        <v>80.98999999999999</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2315,6 +2379,9 @@
       <c r="Z26" s="13" t="n">
         <v>24900.71</v>
       </c>
+      <c r="AA26" s="13" t="n">
+        <v>24822.79</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2391,6 +2458,7 @@
       </c>
       <c r="Y27" s="13" t="n"/>
       <c r="Z27" s="13" t="n"/>
+      <c r="AA27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2470,6 +2538,9 @@
       </c>
       <c r="Z28" s="13" t="n">
         <v>76.06</v>
+      </c>
+      <c r="AA28" s="13" t="n">
+        <v>75.38</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2503,6 +2574,9 @@
       <c r="Z29" s="13" t="n">
         <v>52800.06</v>
       </c>
+      <c r="AA29" s="13" t="n">
+        <v>53403.15</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2579,6 +2653,7 @@
       </c>
       <c r="Y30" s="13" t="n"/>
       <c r="Z30" s="13" t="n"/>
+      <c r="AA30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2658,6 +2733,9 @@
       </c>
       <c r="Z31" s="13" t="n">
         <v>51.89</v>
+      </c>
+      <c r="AA31" s="13" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2691,6 +2769,9 @@
       <c r="Z32" s="13" t="n">
         <v>5654.38</v>
       </c>
+      <c r="AA32" s="13" t="n">
+        <v>5726.73</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2767,6 +2848,7 @@
       </c>
       <c r="Y33" s="13" t="n"/>
       <c r="Z33" s="13" t="n"/>
+      <c r="AA33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2846,6 +2928,9 @@
       </c>
       <c r="Z34" s="13" t="n">
         <v>1.46</v>
+      </c>
+      <c r="AA34" s="13" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2879,6 +2964,9 @@
       <c r="Z35" s="13" t="n">
         <v>34321.84</v>
       </c>
+      <c r="AA35" s="13" t="n">
+        <v>34653.62</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -2955,6 +3043,7 @@
       </c>
       <c r="Y36" s="13" t="n"/>
       <c r="Z36" s="13" t="n"/>
+      <c r="AA36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3034,6 +3123,9 @@
       </c>
       <c r="Z37" s="13" t="n">
         <v>31.34</v>
+      </c>
+      <c r="AA37" s="13" t="n">
+        <v>30.94</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3067,6 +3159,9 @@
       <c r="Z38" s="13" t="n">
         <v>3453.07</v>
       </c>
+      <c r="AA38" s="13" t="n">
+        <v>3464.91</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3143,6 +3238,7 @@
       </c>
       <c r="Y39" s="13" t="n"/>
       <c r="Z39" s="13" t="n"/>
+      <c r="AA39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3222,6 +3318,9 @@
       </c>
       <c r="Z40" s="13" t="n">
         <v>54.84</v>
+      </c>
+      <c r="AA40" s="13" t="n">
+        <v>54.22</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3255,6 +3354,9 @@
       <c r="Z41" s="13" t="n">
         <v>3320.81</v>
       </c>
+      <c r="AA41" s="13" t="n">
+        <v>3322</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3331,6 +3433,7 @@
       </c>
       <c r="Y42" s="13" t="n"/>
       <c r="Z42" s="13" t="n"/>
+      <c r="AA42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3410,6 +3513,9 @@
       </c>
       <c r="Z43" s="13" t="n">
         <v>20.35</v>
+      </c>
+      <c r="AA43" s="13" t="n">
+        <v>18.92</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3443,6 +3549,9 @@
       <c r="Z44" s="13" t="n">
         <v>7259.36</v>
       </c>
+      <c r="AA44" s="13" t="n">
+        <v>7151.29</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3519,6 +3628,7 @@
       </c>
       <c r="Y45" s="13" t="n"/>
       <c r="Z45" s="13" t="n"/>
+      <c r="AA45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3598,6 +3708,9 @@
       </c>
       <c r="Z46" s="13" t="n">
         <v>26.64</v>
+      </c>
+      <c r="AA46" s="13" t="n">
+        <v>23.61</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3631,6 +3744,9 @@
       <c r="Z47" s="13" t="n">
         <v>8344.1</v>
       </c>
+      <c r="AA47" s="13" t="n">
+        <v>8179.11</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3707,6 +3823,7 @@
       </c>
       <c r="Y48" s="13" t="n"/>
       <c r="Z48" s="13" t="n"/>
+      <c r="AA48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3786,6 +3903,9 @@
       </c>
       <c r="Z49" s="13" t="n">
         <v>6.62</v>
+      </c>
+      <c r="AA49" s="13" t="n">
+        <v>6.12</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3819,6 +3939,9 @@
       <c r="Z50" s="13" t="n">
         <v>12336.44</v>
       </c>
+      <c r="AA50" s="13" t="n">
+        <v>12220.92</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -3895,6 +4018,7 @@
       </c>
       <c r="Y51" s="13" t="n"/>
       <c r="Z51" s="13" t="n"/>
+      <c r="AA51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -3974,6 +4098,9 @@
       </c>
       <c r="Z52" s="13" t="n">
         <v>31.98</v>
+      </c>
+      <c r="AA52" s="13" t="n">
+        <v>27.32</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4007,6 +4134,9 @@
       <c r="Z53" s="13" t="n">
         <v>13181.48</v>
       </c>
+      <c r="AA53" s="13" t="n">
+        <v>12936.65</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4083,6 +4213,7 @@
       </c>
       <c r="Y54" s="13" t="n"/>
       <c r="Z54" s="13" t="n"/>
+      <c r="AA54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4162,6 +4293,9 @@
       </c>
       <c r="Z55" s="13" t="n">
         <v>15.37</v>
+      </c>
+      <c r="AA55" s="13" t="n">
+        <v>14.99</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4195,6 +4329,9 @@
       <c r="Z56" s="13" t="n">
         <v>8399.9</v>
       </c>
+      <c r="AA56" s="13" t="n">
+        <v>8557.110000000001</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4271,6 +4408,7 @@
       </c>
       <c r="Y57" s="13" t="n"/>
       <c r="Z57" s="13" t="n"/>
+      <c r="AA57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4350,6 +4488,9 @@
       </c>
       <c r="Z58" s="13" t="n">
         <v>22.71</v>
+      </c>
+      <c r="AA58" s="13" t="n">
+        <v>21.84</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4383,6 +4524,9 @@
       <c r="Z59" s="13" t="n">
         <v>14741.85</v>
       </c>
+      <c r="AA59" s="13" t="n">
+        <v>14790.28</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4459,6 +4603,7 @@
       </c>
       <c r="Y60" s="13" t="n"/>
       <c r="Z60" s="13" t="n"/>
+      <c r="AA60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4538,6 +4683,9 @@
       </c>
       <c r="Z61" s="13" t="n">
         <v>32.02</v>
+      </c>
+      <c r="AA61" s="13" t="n">
+        <v>31.8</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -4571,6 +4719,9 @@
       <c r="Z62" s="13" t="n">
         <v>15529.62</v>
       </c>
+      <c r="AA62" s="13" t="n">
+        <v>15842.76</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4647,6 +4798,7 @@
       </c>
       <c r="Y63" s="13" t="n"/>
       <c r="Z63" s="13" t="n"/>
+      <c r="AA63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -4726,6 +4878,9 @@
       </c>
       <c r="Z64" s="13" t="n">
         <v>21.07</v>
+      </c>
+      <c r="AA64" s="13" t="n">
+        <v>22.25</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -4759,6 +4914,9 @@
       <c r="Z65" s="13" t="n">
         <v>9668.809999999999</v>
       </c>
+      <c r="AA65" s="13" t="n">
+        <v>9648.25</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4835,6 +4993,7 @@
       </c>
       <c r="Y66" s="13" t="n"/>
       <c r="Z66" s="13" t="n"/>
+      <c r="AA66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -4914,6 +5073,9 @@
       </c>
       <c r="Z67" s="13" t="n">
         <v>12.84</v>
+      </c>
+      <c r="AA67" s="13" t="n">
+        <v>10.88</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -4947,6 +5109,9 @@
       <c r="Z68" s="13" t="n">
         <v>9712.48</v>
       </c>
+      <c r="AA68" s="13" t="n">
+        <v>9484.99</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -5023,6 +5188,7 @@
       </c>
       <c r="Y69" s="13" t="n"/>
       <c r="Z69" s="13" t="n"/>
+      <c r="AA69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -5102,6 +5268,9 @@
       </c>
       <c r="Z70" s="13" t="n">
         <v>24.61</v>
+      </c>
+      <c r="AA70" s="13" t="n">
+        <v>25.5</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -5135,6 +5304,9 @@
       <c r="Z71" s="13" t="n">
         <v>3112.04</v>
       </c>
+      <c r="AA71" s="13" t="n">
+        <v>3196.65</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -5211,6 +5383,7 @@
       </c>
       <c r="Y72" s="13" t="n"/>
       <c r="Z72" s="13" t="n"/>
+      <c r="AA72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -5290,6 +5463,9 @@
       </c>
       <c r="Z73" s="13" t="n">
         <v>47.87</v>
+      </c>
+      <c r="AA73" s="13" t="n">
+        <v>49.18</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -5323,6 +5499,9 @@
       <c r="Z74" s="13" t="n">
         <v>5722.24</v>
       </c>
+      <c r="AA74" s="13" t="n">
+        <v>5860.66</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -5399,6 +5578,7 @@
       </c>
       <c r="Y75" s="13" t="n"/>
       <c r="Z75" s="13" t="n"/>
+      <c r="AA75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -5478,6 +5658,9 @@
       </c>
       <c r="Z76" s="13" t="n">
         <v>26.68</v>
+      </c>
+      <c r="AA76" s="13" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -5511,6 +5694,9 @@
       <c r="Z77" s="13" t="n">
         <v>9031.110000000001</v>
       </c>
+      <c r="AA77" s="13" t="n">
+        <v>8871.82</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -5587,6 +5773,7 @@
       </c>
       <c r="Y78" s="13" t="n"/>
       <c r="Z78" s="13" t="n"/>
+      <c r="AA78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -5666,6 +5853,9 @@
       </c>
       <c r="Z79" s="13" t="n">
         <v>14.92</v>
+      </c>
+      <c r="AA79" s="13" t="n">
+        <v>16.07</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -5699,6 +5889,9 @@
       <c r="Z80" s="13" t="n">
         <v>1443.29</v>
       </c>
+      <c r="AA80" s="13" t="n">
+        <v>1480.33</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -5775,6 +5968,7 @@
       </c>
       <c r="Y81" s="13" t="n"/>
       <c r="Z81" s="13" t="n"/>
+      <c r="AA81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -5854,6 +6048,9 @@
       </c>
       <c r="Z82" s="13" t="n">
         <v>16.25</v>
+      </c>
+      <c r="AA82" s="13" t="n">
+        <v>15.75</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -5887,6 +6084,9 @@
       <c r="Z83" s="13" t="n">
         <v>15985</v>
       </c>
+      <c r="AA83" s="13" t="n">
+        <v>15668.81</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -5963,6 +6163,7 @@
       </c>
       <c r="Y84" s="13" t="n"/>
       <c r="Z84" s="13" t="n"/>
+      <c r="AA84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -6042,6 +6243,9 @@
       </c>
       <c r="Z85" s="13" t="n">
         <v>55.05</v>
+      </c>
+      <c r="AA85" s="13" t="n">
+        <v>54.05</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -6075,6 +6279,9 @@
       <c r="Z86" s="13" t="n">
         <v>3097.65</v>
       </c>
+      <c r="AA86" s="13" t="n">
+        <v>3022.69</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -6151,6 +6358,7 @@
       </c>
       <c r="Y87" s="13" t="n"/>
       <c r="Z87" s="13" t="n"/>
+      <c r="AA87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -6230,6 +6438,9 @@
       </c>
       <c r="Z88" s="13" t="n">
         <v>58.73</v>
+      </c>
+      <c r="AA88" s="13" t="n">
+        <v>58.62</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -6263,6 +6474,9 @@
       <c r="Z89" s="13" t="n">
         <v>3354.76</v>
       </c>
+      <c r="AA89" s="13" t="n">
+        <v>3317.06</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -6339,6 +6553,7 @@
       </c>
       <c r="Y90" s="13" t="n"/>
       <c r="Z90" s="13" t="n"/>
+      <c r="AA90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -6418,6 +6633,9 @@
       </c>
       <c r="Z91" s="13" t="n">
         <v>51.86</v>
+      </c>
+      <c r="AA91" s="13" t="n">
+        <v>49.96</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -6451,6 +6669,9 @@
       <c r="Z92" s="13" t="n">
         <v>3209.69</v>
       </c>
+      <c r="AA92" s="13" t="n">
+        <v>3093.96</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -6527,6 +6748,7 @@
       </c>
       <c r="Y93" s="13" t="n"/>
       <c r="Z93" s="13" t="n"/>
+      <c r="AA93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -6606,6 +6828,9 @@
       </c>
       <c r="Z94" s="13" t="n">
         <v>45.76</v>
+      </c>
+      <c r="AA94" s="13" t="n">
+        <v>44.8</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -6639,6 +6864,9 @@
       <c r="Z95" s="13" t="n">
         <v>1947.38</v>
       </c>
+      <c r="AA95" s="13" t="n">
+        <v>1908.25</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -6715,6 +6943,7 @@
       </c>
       <c r="Y96" s="13" t="n"/>
       <c r="Z96" s="13" t="n"/>
+      <c r="AA96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -6794,6 +7023,9 @@
       </c>
       <c r="Z97" s="13" t="n">
         <v>27.88</v>
+      </c>
+      <c r="AA97" s="13" t="n">
+        <v>27.31</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -6827,6 +7059,9 @@
       <c r="Z98" s="13" t="n">
         <v>10602.82</v>
       </c>
+      <c r="AA98" s="13" t="n">
+        <v>10420.47</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -6903,6 +7138,7 @@
       </c>
       <c r="Y99" s="13" t="n"/>
       <c r="Z99" s="13" t="n"/>
+      <c r="AA99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -6982,6 +7218,9 @@
       </c>
       <c r="Z100" s="13" t="n">
         <v>88.05</v>
+      </c>
+      <c r="AA100" s="13" t="n">
+        <v>88.19</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -7015,6 +7254,9 @@
       <c r="Z101" s="13" t="n">
         <v>10704.68</v>
       </c>
+      <c r="AA101" s="13" t="n">
+        <v>10827.98</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -7091,6 +7333,7 @@
       </c>
       <c r="Y102" s="13" t="n"/>
       <c r="Z102" s="13" t="n"/>
+      <c r="AA102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -7170,6 +7413,9 @@
       </c>
       <c r="Z103" s="13" t="n">
         <v>60.03</v>
+      </c>
+      <c r="AA103" s="13" t="n">
+        <v>59.57</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -7203,6 +7449,9 @@
       <c r="Z104" s="13" t="n">
         <v>15500.32</v>
       </c>
+      <c r="AA104" s="13" t="n">
+        <v>15184.31</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -7279,6 +7528,7 @@
       </c>
       <c r="Y105" s="13" t="n"/>
       <c r="Z105" s="13" t="n"/>
+      <c r="AA105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -7358,6 +7608,9 @@
       </c>
       <c r="Z106" s="13" t="n">
         <v>5.46</v>
+      </c>
+      <c r="AA106" s="13" t="n">
+        <v>5.38</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -7391,6 +7644,9 @@
       <c r="Z107" s="13" t="n">
         <v>2199.54</v>
       </c>
+      <c r="AA107" s="13" t="n">
+        <v>2226.24</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -7467,6 +7723,7 @@
       </c>
       <c r="Y108" s="13" t="n"/>
       <c r="Z108" s="13" t="n"/>
+      <c r="AA108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -7546,6 +7803,9 @@
       </c>
       <c r="Z109" s="13" t="n">
         <v>25.31</v>
+      </c>
+      <c r="AA109" s="13" t="n">
+        <v>25.23</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -7579,6 +7839,9 @@
       <c r="Z110" s="13" t="n">
         <v>853.6799999999999</v>
       </c>
+      <c r="AA110" s="13" t="n">
+        <v>833.7</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -7655,6 +7918,7 @@
       </c>
       <c r="Y111" s="13" t="n"/>
       <c r="Z111" s="13" t="n"/>
+      <c r="AA111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -7734,6 +7998,9 @@
       </c>
       <c r="Z112" s="13" t="n">
         <v>33.59</v>
+      </c>
+      <c r="AA112" s="13" t="n">
+        <v>34.09</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -7767,6 +8034,9 @@
       <c r="Z113" s="13" t="n">
         <v>3855.83</v>
       </c>
+      <c r="AA113" s="13" t="n">
+        <v>4205.38</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -7843,6 +8113,7 @@
       </c>
       <c r="Y114" s="13" t="n"/>
       <c r="Z114" s="13" t="n"/>
+      <c r="AA114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -7922,6 +8193,9 @@
       </c>
       <c r="Z115" s="13" t="n">
         <v>22.52</v>
+      </c>
+      <c r="AA115" s="13" t="n">
+        <v>22.62</v>
       </c>
     </row>
     <row r="116">
@@ -7940,6 +8214,9 @@
       <c r="Z116" s="13" t="n">
         <v>4168.32</v>
       </c>
+      <c r="AA116" s="13" t="n">
+        <v>4166.62</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -7971,6 +8248,7 @@
       </c>
       <c r="Y117" s="13" t="n"/>
       <c r="Z117" s="13" t="n"/>
+      <c r="AA117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -8006,6 +8284,9 @@
       <c r="Z118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AA118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -8013,6 +8294,9 @@
       </c>
       <c r="Z119" s="13" t="n">
         <v>3104.67</v>
+      </c>
+      <c r="AA119" s="13" t="n">
+        <v>3175.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-02 05:15:25]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA119"/>
+  <dimension ref="A1:AB119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -549,6 +549,7 @@
     <col width="15" customWidth="1" min="25" max="25"/>
     <col width="15" customWidth="1" min="26" max="26"/>
     <col width="15" customWidth="1" min="27" max="27"/>
+    <col width="15" customWidth="1" min="28" max="28"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -687,6 +688,11 @@
           <t>2026/01/29</t>
         </is>
       </c>
+      <c r="AB1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/02</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -824,6 +830,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AB2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -907,6 +918,9 @@
       <c r="AA3" s="13" t="n">
         <v>66.16</v>
       </c>
+      <c r="AB3" s="13" t="n">
+        <v>65.77</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -989,6 +1003,9 @@
       </c>
       <c r="AA4" s="13" t="n">
         <v>4147.15</v>
+      </c>
+      <c r="AB4" s="13" t="n">
+        <v>4061.63</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1019,6 +1036,7 @@
       <c r="Y5" s="13" t="n"/>
       <c r="Z5" s="13" t="n"/>
       <c r="AA5" s="13" t="n"/>
+      <c r="AB5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1096,6 +1114,7 @@
       <c r="Y6" s="13" t="n"/>
       <c r="Z6" s="13" t="n"/>
       <c r="AA6" s="13" t="n"/>
+      <c r="AB6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1178,6 +1197,9 @@
       </c>
       <c r="AA7" s="13" t="n">
         <v>51.43</v>
+      </c>
+      <c r="AB7" s="13" t="n">
+        <v>51.22</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1214,6 +1236,9 @@
       <c r="AA8" s="13" t="n">
         <v>5950.84</v>
       </c>
+      <c r="AB8" s="13" t="n">
+        <v>5809.78</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1291,6 +1316,7 @@
       <c r="Y9" s="13" t="n"/>
       <c r="Z9" s="13" t="n"/>
       <c r="AA9" s="13" t="n"/>
+      <c r="AB9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1373,6 +1399,9 @@
       </c>
       <c r="AA10" s="13" t="n">
         <v>54.62</v>
+      </c>
+      <c r="AB10" s="13" t="n">
+        <v>54.42</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1409,6 +1438,9 @@
       <c r="AA11" s="13" t="n">
         <v>4713.5</v>
       </c>
+      <c r="AB11" s="13" t="n">
+        <v>4651.63</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1486,6 +1518,7 @@
       <c r="Y12" s="13" t="n"/>
       <c r="Z12" s="13" t="n"/>
       <c r="AA12" s="13" t="n"/>
+      <c r="AB12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1568,6 +1601,9 @@
       </c>
       <c r="AA13" s="13" t="n">
         <v>61.88</v>
+      </c>
+      <c r="AB13" s="13" t="n">
+        <v>61.37</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1604,6 +1640,9 @@
       <c r="AA14" s="13" t="n">
         <v>8605.49</v>
       </c>
+      <c r="AB14" s="13" t="n">
+        <v>8178.6</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1681,6 +1720,7 @@
       <c r="Y15" s="13" t="n"/>
       <c r="Z15" s="13" t="n"/>
       <c r="AA15" s="13" t="n"/>
+      <c r="AB15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1763,6 +1803,9 @@
       </c>
       <c r="AA16" s="13" t="n">
         <v>31.7</v>
+      </c>
+      <c r="AB16" s="13" t="n">
+        <v>30.79</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1799,6 +1842,9 @@
       <c r="AA17" s="13" t="n">
         <v>2740.51</v>
       </c>
+      <c r="AB17" s="13" t="n">
+        <v>2740.51</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1876,6 +1922,7 @@
       <c r="Y18" s="13" t="n"/>
       <c r="Z18" s="13" t="n"/>
       <c r="AA18" s="13" t="n"/>
+      <c r="AB18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -1958,6 +2005,9 @@
       </c>
       <c r="AA19" s="13" t="n">
         <v>96.72</v>
+      </c>
+      <c r="AB19" s="13" t="n">
+        <v>96.53</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1994,6 +2044,9 @@
       <c r="AA20" s="13" t="n">
         <v>6978.03</v>
       </c>
+      <c r="AB20" s="13" t="n">
+        <v>6939.03</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2071,6 +2124,7 @@
       <c r="Y21" s="13" t="n"/>
       <c r="Z21" s="13" t="n"/>
       <c r="AA21" s="13" t="n"/>
+      <c r="AB21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2151,6 +2205,9 @@
       </c>
       <c r="AA22" s="13" t="n">
         <v>60.87</v>
+      </c>
+      <c r="AB22" s="13" t="n">
+        <v>60.62</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2187,6 +2244,9 @@
       <c r="AA23" s="13" t="n">
         <v>81785.89999999999</v>
       </c>
+      <c r="AB23" s="13" t="n">
+        <v>80904</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2264,6 +2324,7 @@
       <c r="Y24" s="13" t="n"/>
       <c r="Z24" s="13" t="n"/>
       <c r="AA24" s="13" t="n"/>
+      <c r="AB24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2346,6 +2407,9 @@
       </c>
       <c r="AA25" s="13" t="n">
         <v>80.98999999999999</v>
+      </c>
+      <c r="AB25" s="13" t="n">
+        <v>78.53</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2382,6 +2446,9 @@
       <c r="AA26" s="13" t="n">
         <v>24822.79</v>
       </c>
+      <c r="AB26" s="13" t="n">
+        <v>24538.81</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2459,6 +2526,7 @@
       <c r="Y27" s="13" t="n"/>
       <c r="Z27" s="13" t="n"/>
       <c r="AA27" s="13" t="n"/>
+      <c r="AB27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2541,6 +2609,9 @@
       </c>
       <c r="AA28" s="13" t="n">
         <v>75.38</v>
+      </c>
+      <c r="AB28" s="13" t="n">
+        <v>74.78</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2577,6 +2648,9 @@
       <c r="AA29" s="13" t="n">
         <v>53403.15</v>
       </c>
+      <c r="AB29" s="13" t="n">
+        <v>52809.58</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2654,6 +2728,7 @@
       <c r="Y30" s="13" t="n"/>
       <c r="Z30" s="13" t="n"/>
       <c r="AA30" s="13" t="n"/>
+      <c r="AB30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2736,6 +2811,9 @@
       </c>
       <c r="AA31" s="13" t="n">
         <v>50</v>
+      </c>
+      <c r="AB31" s="13" t="n">
+        <v>50.26</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2772,6 +2850,9 @@
       <c r="AA32" s="13" t="n">
         <v>5726.73</v>
       </c>
+      <c r="AB32" s="13" t="n">
+        <v>5584.62</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2849,6 +2930,7 @@
       <c r="Y33" s="13" t="n"/>
       <c r="Z33" s="13" t="n"/>
       <c r="AA33" s="13" t="n"/>
+      <c r="AB33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -2931,6 +3013,9 @@
       </c>
       <c r="AA34" s="13" t="n">
         <v>1.96</v>
+      </c>
+      <c r="AB34" s="13" t="n">
+        <v>2.03</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -2967,6 +3052,9 @@
       <c r="AA35" s="13" t="n">
         <v>34653.62</v>
       </c>
+      <c r="AB35" s="13" t="n">
+        <v>33792.13</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3044,6 +3132,7 @@
       <c r="Y36" s="13" t="n"/>
       <c r="Z36" s="13" t="n"/>
       <c r="AA36" s="13" t="n"/>
+      <c r="AB36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3126,6 +3215,9 @@
       </c>
       <c r="AA37" s="13" t="n">
         <v>30.94</v>
+      </c>
+      <c r="AB37" s="13" t="n">
+        <v>31.52</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3162,6 +3254,9 @@
       <c r="AA38" s="13" t="n">
         <v>3464.91</v>
       </c>
+      <c r="AB38" s="13" t="n">
+        <v>3476.54</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3239,6 +3334,7 @@
       <c r="Y39" s="13" t="n"/>
       <c r="Z39" s="13" t="n"/>
       <c r="AA39" s="13" t="n"/>
+      <c r="AB39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3321,6 +3417,9 @@
       </c>
       <c r="AA40" s="13" t="n">
         <v>54.22</v>
+      </c>
+      <c r="AB40" s="13" t="n">
+        <v>54.49</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3357,6 +3456,9 @@
       <c r="AA41" s="13" t="n">
         <v>3322</v>
       </c>
+      <c r="AB41" s="13" t="n">
+        <v>3307.31</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3434,6 +3536,7 @@
       <c r="Y42" s="13" t="n"/>
       <c r="Z42" s="13" t="n"/>
       <c r="AA42" s="13" t="n"/>
+      <c r="AB42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3516,6 +3619,9 @@
       </c>
       <c r="AA43" s="13" t="n">
         <v>18.92</v>
+      </c>
+      <c r="AB43" s="13" t="n">
+        <v>18.63</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3552,6 +3658,9 @@
       <c r="AA44" s="13" t="n">
         <v>7151.29</v>
       </c>
+      <c r="AB44" s="13" t="n">
+        <v>7039.3</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3629,6 +3738,7 @@
       <c r="Y45" s="13" t="n"/>
       <c r="Z45" s="13" t="n"/>
       <c r="AA45" s="13" t="n"/>
+      <c r="AB45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3711,6 +3821,9 @@
       </c>
       <c r="AA46" s="13" t="n">
         <v>23.61</v>
+      </c>
+      <c r="AB46" s="13" t="n">
+        <v>24.07</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3747,6 +3860,9 @@
       <c r="AA47" s="13" t="n">
         <v>8179.11</v>
       </c>
+      <c r="AB47" s="13" t="n">
+        <v>8140.03</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3824,6 +3940,7 @@
       <c r="Y48" s="13" t="n"/>
       <c r="Z48" s="13" t="n"/>
       <c r="AA48" s="13" t="n"/>
+      <c r="AB48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -3906,6 +4023,9 @@
       </c>
       <c r="AA49" s="13" t="n">
         <v>6.12</v>
+      </c>
+      <c r="AB49" s="13" t="n">
+        <v>6.79</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -3942,6 +4062,9 @@
       <c r="AA50" s="13" t="n">
         <v>12220.92</v>
       </c>
+      <c r="AB50" s="13" t="n">
+        <v>12306.88</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4019,6 +4142,7 @@
       <c r="Y51" s="13" t="n"/>
       <c r="Z51" s="13" t="n"/>
       <c r="AA51" s="13" t="n"/>
+      <c r="AB51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4101,6 +4225,9 @@
       </c>
       <c r="AA52" s="13" t="n">
         <v>27.32</v>
+      </c>
+      <c r="AB52" s="13" t="n">
+        <v>27.25</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4137,6 +4264,9 @@
       <c r="AA53" s="13" t="n">
         <v>12936.65</v>
       </c>
+      <c r="AB53" s="13" t="n">
+        <v>13442.13</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4214,6 +4344,7 @@
       <c r="Y54" s="13" t="n"/>
       <c r="Z54" s="13" t="n"/>
       <c r="AA54" s="13" t="n"/>
+      <c r="AB54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4296,6 +4427,9 @@
       </c>
       <c r="AA55" s="13" t="n">
         <v>14.99</v>
+      </c>
+      <c r="AB55" s="13" t="n">
+        <v>17.53</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4332,6 +4466,9 @@
       <c r="AA56" s="13" t="n">
         <v>8557.110000000001</v>
       </c>
+      <c r="AB56" s="13" t="n">
+        <v>8975.16</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4409,6 +4546,7 @@
       <c r="Y57" s="13" t="n"/>
       <c r="Z57" s="13" t="n"/>
       <c r="AA57" s="13" t="n"/>
+      <c r="AB57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4491,6 +4629,9 @@
       </c>
       <c r="AA58" s="13" t="n">
         <v>21.84</v>
+      </c>
+      <c r="AB58" s="13" t="n">
+        <v>23.98</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4527,6 +4668,9 @@
       <c r="AA59" s="13" t="n">
         <v>14790.28</v>
       </c>
+      <c r="AB59" s="13" t="n">
+        <v>15057.85</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4604,6 +4748,7 @@
       <c r="Y60" s="13" t="n"/>
       <c r="Z60" s="13" t="n"/>
       <c r="AA60" s="13" t="n"/>
+      <c r="AB60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4686,6 +4831,9 @@
       </c>
       <c r="AA61" s="13" t="n">
         <v>31.8</v>
+      </c>
+      <c r="AB61" s="13" t="n">
+        <v>30.86</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -4722,6 +4870,9 @@
       <c r="AA62" s="13" t="n">
         <v>15842.76</v>
       </c>
+      <c r="AB62" s="13" t="n">
+        <v>14838.1</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4799,6 +4950,7 @@
       <c r="Y63" s="13" t="n"/>
       <c r="Z63" s="13" t="n"/>
       <c r="AA63" s="13" t="n"/>
+      <c r="AB63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -4881,6 +5033,9 @@
       </c>
       <c r="AA64" s="13" t="n">
         <v>22.25</v>
+      </c>
+      <c r="AB64" s="13" t="n">
+        <v>20.77</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -4917,6 +5072,9 @@
       <c r="AA65" s="13" t="n">
         <v>9648.25</v>
       </c>
+      <c r="AB65" s="13" t="n">
+        <v>9441.42</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -4994,6 +5152,7 @@
       <c r="Y66" s="13" t="n"/>
       <c r="Z66" s="13" t="n"/>
       <c r="AA66" s="13" t="n"/>
+      <c r="AB66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -5076,6 +5235,9 @@
       </c>
       <c r="AA67" s="13" t="n">
         <v>10.88</v>
+      </c>
+      <c r="AB67" s="13" t="n">
+        <v>11.07</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -5112,6 +5274,9 @@
       <c r="AA68" s="13" t="n">
         <v>9484.99</v>
       </c>
+      <c r="AB68" s="13" t="n">
+        <v>9541.26</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -5189,6 +5354,7 @@
       <c r="Y69" s="13" t="n"/>
       <c r="Z69" s="13" t="n"/>
       <c r="AA69" s="13" t="n"/>
+      <c r="AB69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -5271,6 +5437,9 @@
       </c>
       <c r="AA70" s="13" t="n">
         <v>25.5</v>
+      </c>
+      <c r="AB70" s="13" t="n">
+        <v>24.7</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -5307,6 +5476,9 @@
       <c r="AA71" s="13" t="n">
         <v>3196.65</v>
       </c>
+      <c r="AB71" s="13" t="n">
+        <v>3020.97</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -5384,6 +5556,7 @@
       <c r="Y72" s="13" t="n"/>
       <c r="Z72" s="13" t="n"/>
       <c r="AA72" s="13" t="n"/>
+      <c r="AB72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -5466,6 +5639,9 @@
       </c>
       <c r="AA73" s="13" t="n">
         <v>49.18</v>
+      </c>
+      <c r="AB73" s="13" t="n">
+        <v>47.8</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -5502,6 +5678,9 @@
       <c r="AA74" s="13" t="n">
         <v>5860.66</v>
       </c>
+      <c r="AB74" s="13" t="n">
+        <v>5508.01</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -5579,6 +5758,7 @@
       <c r="Y75" s="13" t="n"/>
       <c r="Z75" s="13" t="n"/>
       <c r="AA75" s="13" t="n"/>
+      <c r="AB75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -5661,6 +5841,9 @@
       </c>
       <c r="AA76" s="13" t="n">
         <v>25</v>
+      </c>
+      <c r="AB76" s="13" t="n">
+        <v>24.26</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -5697,6 +5880,9 @@
       <c r="AA77" s="13" t="n">
         <v>8871.82</v>
       </c>
+      <c r="AB77" s="13" t="n">
+        <v>8758.940000000001</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -5774,6 +5960,7 @@
       <c r="Y78" s="13" t="n"/>
       <c r="Z78" s="13" t="n"/>
       <c r="AA78" s="13" t="n"/>
+      <c r="AB78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -5856,6 +6043,9 @@
       </c>
       <c r="AA79" s="13" t="n">
         <v>16.07</v>
+      </c>
+      <c r="AB79" s="13" t="n">
+        <v>17.65</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -5892,6 +6082,9 @@
       <c r="AA80" s="13" t="n">
         <v>1480.33</v>
       </c>
+      <c r="AB80" s="13" t="n">
+        <v>1522.73</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -5969,6 +6162,7 @@
       <c r="Y81" s="13" t="n"/>
       <c r="Z81" s="13" t="n"/>
       <c r="AA81" s="13" t="n"/>
+      <c r="AB81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -6051,6 +6245,9 @@
       </c>
       <c r="AA82" s="13" t="n">
         <v>15.75</v>
+      </c>
+      <c r="AB82" s="13" t="n">
+        <v>17.11</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -6087,6 +6284,9 @@
       <c r="AA83" s="13" t="n">
         <v>15668.81</v>
       </c>
+      <c r="AB83" s="13" t="n">
+        <v>16234.4</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -6164,6 +6364,7 @@
       <c r="Y84" s="13" t="n"/>
       <c r="Z84" s="13" t="n"/>
       <c r="AA84" s="13" t="n"/>
+      <c r="AB84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -6246,6 +6447,9 @@
       </c>
       <c r="AA85" s="13" t="n">
         <v>54.05</v>
+      </c>
+      <c r="AB85" s="13" t="n">
+        <v>53.16</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -6282,6 +6486,9 @@
       <c r="AA86" s="13" t="n">
         <v>3022.69</v>
       </c>
+      <c r="AB86" s="13" t="n">
+        <v>2923.23</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -6359,6 +6566,7 @@
       <c r="Y87" s="13" t="n"/>
       <c r="Z87" s="13" t="n"/>
       <c r="AA87" s="13" t="n"/>
+      <c r="AB87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -6441,6 +6649,9 @@
       </c>
       <c r="AA88" s="13" t="n">
         <v>58.62</v>
+      </c>
+      <c r="AB88" s="13" t="n">
+        <v>58.52</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -6477,6 +6688,9 @@
       <c r="AA89" s="13" t="n">
         <v>3317.06</v>
       </c>
+      <c r="AB89" s="13" t="n">
+        <v>3209.67</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -6554,6 +6768,7 @@
       <c r="Y90" s="13" t="n"/>
       <c r="Z90" s="13" t="n"/>
       <c r="AA90" s="13" t="n"/>
+      <c r="AB90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -6636,6 +6851,9 @@
       </c>
       <c r="AA91" s="13" t="n">
         <v>49.96</v>
+      </c>
+      <c r="AB91" s="13" t="n">
+        <v>49.05</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -6672,6 +6890,9 @@
       <c r="AA92" s="13" t="n">
         <v>3093.96</v>
       </c>
+      <c r="AB92" s="13" t="n">
+        <v>2973.41</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -6749,6 +6970,7 @@
       <c r="Y93" s="13" t="n"/>
       <c r="Z93" s="13" t="n"/>
       <c r="AA93" s="13" t="n"/>
+      <c r="AB93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -6831,6 +7053,9 @@
       </c>
       <c r="AA94" s="13" t="n">
         <v>44.8</v>
+      </c>
+      <c r="AB94" s="13" t="n">
+        <v>43.94</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -6867,6 +7092,9 @@
       <c r="AA95" s="13" t="n">
         <v>1908.25</v>
       </c>
+      <c r="AB95" s="13" t="n">
+        <v>1875.96</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -6944,6 +7172,7 @@
       <c r="Y96" s="13" t="n"/>
       <c r="Z96" s="13" t="n"/>
       <c r="AA96" s="13" t="n"/>
+      <c r="AB96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -7026,6 +7255,9 @@
       </c>
       <c r="AA97" s="13" t="n">
         <v>27.31</v>
+      </c>
+      <c r="AB97" s="13" t="n">
+        <v>27.05</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -7062,6 +7294,9 @@
       <c r="AA98" s="13" t="n">
         <v>10420.47</v>
       </c>
+      <c r="AB98" s="13" t="n">
+        <v>10233.75</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -7139,6 +7374,7 @@
       <c r="Y99" s="13" t="n"/>
       <c r="Z99" s="13" t="n"/>
       <c r="AA99" s="13" t="n"/>
+      <c r="AB99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -7221,6 +7457,9 @@
       </c>
       <c r="AA100" s="13" t="n">
         <v>88.19</v>
+      </c>
+      <c r="AB100" s="13" t="n">
+        <v>87.90000000000001</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -7257,6 +7496,9 @@
       <c r="AA101" s="13" t="n">
         <v>10827.98</v>
       </c>
+      <c r="AB101" s="13" t="n">
+        <v>10329.32</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -7334,6 +7576,7 @@
       <c r="Y102" s="13" t="n"/>
       <c r="Z102" s="13" t="n"/>
       <c r="AA102" s="13" t="n"/>
+      <c r="AB102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -7416,6 +7659,9 @@
       </c>
       <c r="AA103" s="13" t="n">
         <v>59.57</v>
+      </c>
+      <c r="AB103" s="13" t="n">
+        <v>58.89</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -7452,6 +7698,9 @@
       <c r="AA104" s="13" t="n">
         <v>15184.31</v>
       </c>
+      <c r="AB104" s="13" t="n">
+        <v>14672.02</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -7529,6 +7778,7 @@
       <c r="Y105" s="13" t="n"/>
       <c r="Z105" s="13" t="n"/>
       <c r="AA105" s="13" t="n"/>
+      <c r="AB105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -7611,6 +7861,9 @@
       </c>
       <c r="AA106" s="13" t="n">
         <v>5.38</v>
+      </c>
+      <c r="AB106" s="13" t="n">
+        <v>5.73</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -7647,6 +7900,9 @@
       <c r="AA107" s="13" t="n">
         <v>2226.24</v>
       </c>
+      <c r="AB107" s="13" t="n">
+        <v>2186.14</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -7724,6 +7980,7 @@
       <c r="Y108" s="13" t="n"/>
       <c r="Z108" s="13" t="n"/>
       <c r="AA108" s="13" t="n"/>
+      <c r="AB108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -7806,6 +8063,9 @@
       </c>
       <c r="AA109" s="13" t="n">
         <v>25.23</v>
+      </c>
+      <c r="AB109" s="13" t="n">
+        <v>25.21</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -7842,6 +8102,9 @@
       <c r="AA110" s="13" t="n">
         <v>833.7</v>
       </c>
+      <c r="AB110" s="13" t="n">
+        <v>838.1799999999999</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -7919,6 +8182,7 @@
       <c r="Y111" s="13" t="n"/>
       <c r="Z111" s="13" t="n"/>
       <c r="AA111" s="13" t="n"/>
+      <c r="AB111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -8001,6 +8265,9 @@
       </c>
       <c r="AA112" s="13" t="n">
         <v>34.09</v>
+      </c>
+      <c r="AB112" s="13" t="n">
+        <v>33.69</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -8037,6 +8304,9 @@
       <c r="AA113" s="13" t="n">
         <v>4205.38</v>
       </c>
+      <c r="AB113" s="13" t="n">
+        <v>3565.58</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -8114,6 +8384,7 @@
       <c r="Y114" s="13" t="n"/>
       <c r="Z114" s="13" t="n"/>
       <c r="AA114" s="13" t="n"/>
+      <c r="AB114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -8196,6 +8467,9 @@
       </c>
       <c r="AA115" s="13" t="n">
         <v>22.62</v>
+      </c>
+      <c r="AB115" s="13" t="n">
+        <v>22.34</v>
       </c>
     </row>
     <row r="116">
@@ -8217,6 +8491,9 @@
       <c r="AA116" s="13" t="n">
         <v>4166.62</v>
       </c>
+      <c r="AB116" s="13" t="n">
+        <v>4043.97</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -8249,6 +8526,7 @@
       <c r="Y117" s="13" t="n"/>
       <c r="Z117" s="13" t="n"/>
       <c r="AA117" s="13" t="n"/>
+      <c r="AB117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -8287,6 +8565,9 @@
       <c r="AA118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AB118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -8297,6 +8578,9 @@
       </c>
       <c r="AA119" s="13" t="n">
         <v>3175.26</v>
+      </c>
+      <c r="AB119" s="13" t="n">
+        <v>3173.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-05 05:07:53]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB119"/>
+  <dimension ref="A1:AC119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -550,6 +550,7 @@
     <col width="15" customWidth="1" min="26" max="26"/>
     <col width="15" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -693,6 +694,11 @@
           <t>2026/02/02</t>
         </is>
       </c>
+      <c r="AC1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/05</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -835,6 +841,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AC2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -921,6 +932,9 @@
       <c r="AB3" s="13" t="n">
         <v>65.77</v>
       </c>
+      <c r="AC3" s="13" t="n">
+        <v>65.72</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -1006,6 +1020,9 @@
       </c>
       <c r="AB4" s="13" t="n">
         <v>4061.63</v>
+      </c>
+      <c r="AC4" s="13" t="n">
+        <v>4056.88</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1037,6 +1054,7 @@
       <c r="Z5" s="13" t="n"/>
       <c r="AA5" s="13" t="n"/>
       <c r="AB5" s="13" t="n"/>
+      <c r="AC5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1115,6 +1133,7 @@
       <c r="Z6" s="13" t="n"/>
       <c r="AA6" s="13" t="n"/>
       <c r="AB6" s="13" t="n"/>
+      <c r="AC6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1200,6 +1219,9 @@
       </c>
       <c r="AB7" s="13" t="n">
         <v>51.22</v>
+      </c>
+      <c r="AC7" s="13" t="n">
+        <v>51.02</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1239,6 +1261,9 @@
       <c r="AB8" s="13" t="n">
         <v>5809.78</v>
       </c>
+      <c r="AC8" s="13" t="n">
+        <v>5792.56</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1317,6 +1342,7 @@
       <c r="Z9" s="13" t="n"/>
       <c r="AA9" s="13" t="n"/>
       <c r="AB9" s="13" t="n"/>
+      <c r="AC9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1402,6 +1428,9 @@
       </c>
       <c r="AB10" s="13" t="n">
         <v>54.42</v>
+      </c>
+      <c r="AC10" s="13" t="n">
+        <v>53.98</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1441,6 +1470,9 @@
       <c r="AB11" s="13" t="n">
         <v>4651.63</v>
       </c>
+      <c r="AC11" s="13" t="n">
+        <v>4647.78</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1519,6 +1551,7 @@
       <c r="Z12" s="13" t="n"/>
       <c r="AA12" s="13" t="n"/>
       <c r="AB12" s="13" t="n"/>
+      <c r="AC12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1604,6 +1637,9 @@
       </c>
       <c r="AB13" s="13" t="n">
         <v>61.37</v>
+      </c>
+      <c r="AC13" s="13" t="n">
+        <v>61.16</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1643,6 +1679,9 @@
       <c r="AB14" s="13" t="n">
         <v>8178.6</v>
       </c>
+      <c r="AC14" s="13" t="n">
+        <v>8110.21</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1721,6 +1760,7 @@
       <c r="Z15" s="13" t="n"/>
       <c r="AA15" s="13" t="n"/>
       <c r="AB15" s="13" t="n"/>
+      <c r="AC15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1806,6 +1846,9 @@
       </c>
       <c r="AB16" s="13" t="n">
         <v>30.79</v>
+      </c>
+      <c r="AC16" s="13" t="n">
+        <v>29.66</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1845,6 +1888,9 @@
       <c r="AB17" s="13" t="n">
         <v>2740.51</v>
       </c>
+      <c r="AC17" s="13" t="n">
+        <v>2698.8</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1923,6 +1969,7 @@
       <c r="Z18" s="13" t="n"/>
       <c r="AA18" s="13" t="n"/>
       <c r="AB18" s="13" t="n"/>
+      <c r="AC18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -2008,6 +2055,9 @@
       </c>
       <c r="AB19" s="13" t="n">
         <v>96.53</v>
+      </c>
+      <c r="AC19" s="13" t="n">
+        <v>95.59</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -2047,6 +2097,9 @@
       <c r="AB20" s="13" t="n">
         <v>6939.03</v>
       </c>
+      <c r="AC20" s="13" t="n">
+        <v>6882.72</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2125,6 +2178,7 @@
       <c r="Z21" s="13" t="n"/>
       <c r="AA21" s="13" t="n"/>
       <c r="AB21" s="13" t="n"/>
+      <c r="AC21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2208,6 +2262,9 @@
       </c>
       <c r="AB22" s="13" t="n">
         <v>60.62</v>
+      </c>
+      <c r="AC22" s="13" t="n">
+        <v>65.56</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2247,6 +2304,9 @@
       <c r="AB23" s="13" t="n">
         <v>80904</v>
       </c>
+      <c r="AC23" s="13" t="n">
+        <v>83473.86</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2325,6 +2385,7 @@
       <c r="Z24" s="13" t="n"/>
       <c r="AA24" s="13" t="n"/>
       <c r="AB24" s="13" t="n"/>
+      <c r="AC24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2410,6 +2471,9 @@
       </c>
       <c r="AB25" s="13" t="n">
         <v>78.53</v>
+      </c>
+      <c r="AC25" s="13" t="n">
+        <v>79.61</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2449,6 +2513,9 @@
       <c r="AB26" s="13" t="n">
         <v>24538.81</v>
       </c>
+      <c r="AC26" s="13" t="n">
+        <v>24603.04</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2527,6 +2594,7 @@
       <c r="Z27" s="13" t="n"/>
       <c r="AA27" s="13" t="n"/>
       <c r="AB27" s="13" t="n"/>
+      <c r="AC27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2612,6 +2680,9 @@
       </c>
       <c r="AB28" s="13" t="n">
         <v>74.78</v>
+      </c>
+      <c r="AC28" s="13" t="n">
+        <v>76.22</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2651,6 +2722,9 @@
       <c r="AB29" s="13" t="n">
         <v>52809.58</v>
       </c>
+      <c r="AC29" s="13" t="n">
+        <v>53833.48</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2729,6 +2803,7 @@
       <c r="Z30" s="13" t="n"/>
       <c r="AA30" s="13" t="n"/>
       <c r="AB30" s="13" t="n"/>
+      <c r="AC30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2814,6 +2889,9 @@
       </c>
       <c r="AB31" s="13" t="n">
         <v>50.26</v>
+      </c>
+      <c r="AC31" s="13" t="n">
+        <v>50.02</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2853,6 +2931,9 @@
       <c r="AB32" s="13" t="n">
         <v>5584.62</v>
       </c>
+      <c r="AC32" s="13" t="n">
+        <v>5666.34</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -2931,6 +3012,7 @@
       <c r="Z33" s="13" t="n"/>
       <c r="AA33" s="13" t="n"/>
       <c r="AB33" s="13" t="n"/>
+      <c r="AC33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -3016,6 +3098,9 @@
       </c>
       <c r="AB34" s="13" t="n">
         <v>2.03</v>
+      </c>
+      <c r="AC34" s="13" t="n">
+        <v>2.13</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -3055,6 +3140,9 @@
       <c r="AB35" s="13" t="n">
         <v>33792.13</v>
       </c>
+      <c r="AC35" s="13" t="n">
+        <v>33886.61</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3133,6 +3221,7 @@
       <c r="Z36" s="13" t="n"/>
       <c r="AA36" s="13" t="n"/>
       <c r="AB36" s="13" t="n"/>
+      <c r="AC36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3218,6 +3307,9 @@
       </c>
       <c r="AB37" s="13" t="n">
         <v>31.52</v>
+      </c>
+      <c r="AC37" s="13" t="n">
+        <v>31.27</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3257,6 +3349,9 @@
       <c r="AB38" s="13" t="n">
         <v>3476.54</v>
       </c>
+      <c r="AC38" s="13" t="n">
+        <v>3402.83</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3335,6 +3430,7 @@
       <c r="Z39" s="13" t="n"/>
       <c r="AA39" s="13" t="n"/>
       <c r="AB39" s="13" t="n"/>
+      <c r="AC39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3420,6 +3516,9 @@
       </c>
       <c r="AB40" s="13" t="n">
         <v>54.49</v>
+      </c>
+      <c r="AC40" s="13" t="n">
+        <v>54.11</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3459,6 +3558,9 @@
       <c r="AB41" s="13" t="n">
         <v>3307.31</v>
       </c>
+      <c r="AC41" s="13" t="n">
+        <v>3249.59</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3537,6 +3639,7 @@
       <c r="Z42" s="13" t="n"/>
       <c r="AA42" s="13" t="n"/>
       <c r="AB42" s="13" t="n"/>
+      <c r="AC42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3622,6 +3725,9 @@
       </c>
       <c r="AB43" s="13" t="n">
         <v>18.63</v>
+      </c>
+      <c r="AC43" s="13" t="n">
+        <v>19.2</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3661,6 +3767,9 @@
       <c r="AB44" s="13" t="n">
         <v>7039.3</v>
       </c>
+      <c r="AC44" s="13" t="n">
+        <v>7150.81</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3739,6 +3848,7 @@
       <c r="Z45" s="13" t="n"/>
       <c r="AA45" s="13" t="n"/>
       <c r="AB45" s="13" t="n"/>
+      <c r="AC45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3824,6 +3934,9 @@
       </c>
       <c r="AB46" s="13" t="n">
         <v>24.07</v>
+      </c>
+      <c r="AC46" s="13" t="n">
+        <v>24.87</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3863,6 +3976,9 @@
       <c r="AB47" s="13" t="n">
         <v>8140.03</v>
       </c>
+      <c r="AC47" s="13" t="n">
+        <v>8313.58</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -3941,6 +4057,7 @@
       <c r="Z48" s="13" t="n"/>
       <c r="AA48" s="13" t="n"/>
       <c r="AB48" s="13" t="n"/>
+      <c r="AC48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -4026,6 +4143,9 @@
       </c>
       <c r="AB49" s="13" t="n">
         <v>6.79</v>
+      </c>
+      <c r="AC49" s="13" t="n">
+        <v>9.58</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -4065,6 +4185,9 @@
       <c r="AB50" s="13" t="n">
         <v>12306.88</v>
       </c>
+      <c r="AC50" s="13" t="n">
+        <v>12568.02</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4143,6 +4266,7 @@
       <c r="Z51" s="13" t="n"/>
       <c r="AA51" s="13" t="n"/>
       <c r="AB51" s="13" t="n"/>
+      <c r="AC51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4228,6 +4352,9 @@
       </c>
       <c r="AB52" s="13" t="n">
         <v>27.25</v>
+      </c>
+      <c r="AC52" s="13" t="n">
+        <v>30.07</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4267,6 +4394,9 @@
       <c r="AB53" s="13" t="n">
         <v>13442.13</v>
       </c>
+      <c r="AC53" s="13" t="n">
+        <v>12875.77</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4345,6 +4475,7 @@
       <c r="Z54" s="13" t="n"/>
       <c r="AA54" s="13" t="n"/>
       <c r="AB54" s="13" t="n"/>
+      <c r="AC54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4430,6 +4561,9 @@
       </c>
       <c r="AB55" s="13" t="n">
         <v>17.53</v>
+      </c>
+      <c r="AC55" s="13" t="n">
+        <v>22.23</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4469,6 +4603,9 @@
       <c r="AB56" s="13" t="n">
         <v>8975.16</v>
       </c>
+      <c r="AC56" s="13" t="n">
+        <v>9221.23</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4547,6 +4684,7 @@
       <c r="Z57" s="13" t="n"/>
       <c r="AA57" s="13" t="n"/>
       <c r="AB57" s="13" t="n"/>
+      <c r="AC57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4632,6 +4770,9 @@
       </c>
       <c r="AB58" s="13" t="n">
         <v>23.98</v>
+      </c>
+      <c r="AC58" s="13" t="n">
+        <v>26.77</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4671,6 +4812,9 @@
       <c r="AB59" s="13" t="n">
         <v>15057.85</v>
       </c>
+      <c r="AC59" s="13" t="n">
+        <v>15511.19</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4749,6 +4893,7 @@
       <c r="Z60" s="13" t="n"/>
       <c r="AA60" s="13" t="n"/>
       <c r="AB60" s="13" t="n"/>
+      <c r="AC60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4834,6 +4979,9 @@
       </c>
       <c r="AB61" s="13" t="n">
         <v>30.86</v>
+      </c>
+      <c r="AC61" s="13" t="n">
+        <v>30.45</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -4873,6 +5021,9 @@
       <c r="AB62" s="13" t="n">
         <v>14838.1</v>
       </c>
+      <c r="AC62" s="13" t="n">
+        <v>14929.19</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -4951,6 +5102,7 @@
       <c r="Z63" s="13" t="n"/>
       <c r="AA63" s="13" t="n"/>
       <c r="AB63" s="13" t="n"/>
+      <c r="AC63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -5036,6 +5188,9 @@
       </c>
       <c r="AB64" s="13" t="n">
         <v>20.77</v>
+      </c>
+      <c r="AC64" s="13" t="n">
+        <v>18.25</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -5075,6 +5230,9 @@
       <c r="AB65" s="13" t="n">
         <v>9441.42</v>
       </c>
+      <c r="AC65" s="13" t="n">
+        <v>8928.9</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -5153,6 +5311,7 @@
       <c r="Z66" s="13" t="n"/>
       <c r="AA66" s="13" t="n"/>
       <c r="AB66" s="13" t="n"/>
+      <c r="AC66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -5238,6 +5397,9 @@
       </c>
       <c r="AB67" s="13" t="n">
         <v>11.07</v>
+      </c>
+      <c r="AC67" s="13" t="n">
+        <v>11.91</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -5277,6 +5439,9 @@
       <c r="AB68" s="13" t="n">
         <v>9541.26</v>
       </c>
+      <c r="AC68" s="13" t="n">
+        <v>9678.959999999999</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -5355,6 +5520,7 @@
       <c r="Z69" s="13" t="n"/>
       <c r="AA69" s="13" t="n"/>
       <c r="AB69" s="13" t="n"/>
+      <c r="AC69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -5440,6 +5606,9 @@
       </c>
       <c r="AB70" s="13" t="n">
         <v>24.7</v>
+      </c>
+      <c r="AC70" s="13" t="n">
+        <v>22.25</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -5479,6 +5648,9 @@
       <c r="AB71" s="13" t="n">
         <v>3020.97</v>
       </c>
+      <c r="AC71" s="13" t="n">
+        <v>2868.22</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -5557,6 +5729,7 @@
       <c r="Z72" s="13" t="n"/>
       <c r="AA72" s="13" t="n"/>
       <c r="AB72" s="13" t="n"/>
+      <c r="AC72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -5642,6 +5815,9 @@
       </c>
       <c r="AB73" s="13" t="n">
         <v>47.8</v>
+      </c>
+      <c r="AC73" s="13" t="n">
+        <v>41.86</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -5681,6 +5857,9 @@
       <c r="AB74" s="13" t="n">
         <v>5508.01</v>
       </c>
+      <c r="AC74" s="13" t="n">
+        <v>5304.35</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -5759,6 +5938,7 @@
       <c r="Z75" s="13" t="n"/>
       <c r="AA75" s="13" t="n"/>
       <c r="AB75" s="13" t="n"/>
+      <c r="AC75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -5844,6 +6024,9 @@
       </c>
       <c r="AB76" s="13" t="n">
         <v>24.26</v>
+      </c>
+      <c r="AC76" s="13" t="n">
+        <v>24.46</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -5883,6 +6066,9 @@
       <c r="AB77" s="13" t="n">
         <v>8758.940000000001</v>
       </c>
+      <c r="AC77" s="13" t="n">
+        <v>8879.33</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -5961,6 +6147,7 @@
       <c r="Z78" s="13" t="n"/>
       <c r="AA78" s="13" t="n"/>
       <c r="AB78" s="13" t="n"/>
+      <c r="AC78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -6046,6 +6233,9 @@
       </c>
       <c r="AB79" s="13" t="n">
         <v>17.65</v>
+      </c>
+      <c r="AC79" s="13" t="n">
+        <v>17.71</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -6085,6 +6275,9 @@
       <c r="AB80" s="13" t="n">
         <v>1522.73</v>
       </c>
+      <c r="AC80" s="13" t="n">
+        <v>1524.6</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -6163,6 +6356,7 @@
       <c r="Z81" s="13" t="n"/>
       <c r="AA81" s="13" t="n"/>
       <c r="AB81" s="13" t="n"/>
+      <c r="AC81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -6248,6 +6442,9 @@
       </c>
       <c r="AB82" s="13" t="n">
         <v>17.11</v>
+      </c>
+      <c r="AC82" s="13" t="n">
+        <v>19.74</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -6287,6 +6484,9 @@
       <c r="AB83" s="13" t="n">
         <v>16234.4</v>
       </c>
+      <c r="AC83" s="13" t="n">
+        <v>17031.49</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -6365,6 +6565,7 @@
       <c r="Z84" s="13" t="n"/>
       <c r="AA84" s="13" t="n"/>
       <c r="AB84" s="13" t="n"/>
+      <c r="AC84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -6450,6 +6651,9 @@
       </c>
       <c r="AB85" s="13" t="n">
         <v>53.16</v>
+      </c>
+      <c r="AC85" s="13" t="n">
+        <v>54.7</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -6489,6 +6693,9 @@
       <c r="AB86" s="13" t="n">
         <v>2923.23</v>
       </c>
+      <c r="AC86" s="13" t="n">
+        <v>2902.46</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -6567,6 +6774,7 @@
       <c r="Z87" s="13" t="n"/>
       <c r="AA87" s="13" t="n"/>
       <c r="AB87" s="13" t="n"/>
+      <c r="AC87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -6652,6 +6860,9 @@
       </c>
       <c r="AB88" s="13" t="n">
         <v>58.52</v>
+      </c>
+      <c r="AC88" s="13" t="n">
+        <v>58.73</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -6691,6 +6902,9 @@
       <c r="AB89" s="13" t="n">
         <v>3209.67</v>
       </c>
+      <c r="AC89" s="13" t="n">
+        <v>3251.46</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -6769,6 +6983,7 @@
       <c r="Z90" s="13" t="n"/>
       <c r="AA90" s="13" t="n"/>
       <c r="AB90" s="13" t="n"/>
+      <c r="AC90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -6854,6 +7069,9 @@
       </c>
       <c r="AB91" s="13" t="n">
         <v>49.05</v>
+      </c>
+      <c r="AC91" s="13" t="n">
+        <v>49.89</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -6893,6 +7111,9 @@
       <c r="AB92" s="13" t="n">
         <v>2973.41</v>
       </c>
+      <c r="AC92" s="13" t="n">
+        <v>2926.71</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -6971,6 +7192,7 @@
       <c r="Z93" s="13" t="n"/>
       <c r="AA93" s="13" t="n"/>
       <c r="AB93" s="13" t="n"/>
+      <c r="AC93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -7056,6 +7278,9 @@
       </c>
       <c r="AB94" s="13" t="n">
         <v>43.94</v>
+      </c>
+      <c r="AC94" s="13" t="n">
+        <v>43.63</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -7095,6 +7320,9 @@
       <c r="AB95" s="13" t="n">
         <v>1875.96</v>
       </c>
+      <c r="AC95" s="13" t="n">
+        <v>1892.15</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -7173,6 +7401,7 @@
       <c r="Z96" s="13" t="n"/>
       <c r="AA96" s="13" t="n"/>
       <c r="AB96" s="13" t="n"/>
+      <c r="AC96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -7258,6 +7487,9 @@
       </c>
       <c r="AB97" s="13" t="n">
         <v>27.05</v>
+      </c>
+      <c r="AC97" s="13" t="n">
+        <v>27.12</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -7297,6 +7529,9 @@
       <c r="AB98" s="13" t="n">
         <v>10233.75</v>
       </c>
+      <c r="AC98" s="13" t="n">
+        <v>10079.91</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -7375,6 +7610,7 @@
       <c r="Z99" s="13" t="n"/>
       <c r="AA99" s="13" t="n"/>
       <c r="AB99" s="13" t="n"/>
+      <c r="AC99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -7460,6 +7696,9 @@
       </c>
       <c r="AB100" s="13" t="n">
         <v>87.90000000000001</v>
+      </c>
+      <c r="AC100" s="13" t="n">
+        <v>87.03</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -7499,6 +7738,9 @@
       <c r="AB101" s="13" t="n">
         <v>10329.32</v>
       </c>
+      <c r="AC101" s="13" t="n">
+        <v>10114.57</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -7577,6 +7819,7 @@
       <c r="Z102" s="13" t="n"/>
       <c r="AA102" s="13" t="n"/>
       <c r="AB102" s="13" t="n"/>
+      <c r="AC102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -7662,6 +7905,9 @@
       </c>
       <c r="AB103" s="13" t="n">
         <v>58.89</v>
+      </c>
+      <c r="AC103" s="13" t="n">
+        <v>59.3</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -7701,6 +7947,9 @@
       <c r="AB104" s="13" t="n">
         <v>14672.02</v>
       </c>
+      <c r="AC104" s="13" t="n">
+        <v>14941.7</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -7779,6 +8028,7 @@
       <c r="Z105" s="13" t="n"/>
       <c r="AA105" s="13" t="n"/>
       <c r="AB105" s="13" t="n"/>
+      <c r="AC105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -7864,6 +8114,9 @@
       </c>
       <c r="AB106" s="13" t="n">
         <v>5.73</v>
+      </c>
+      <c r="AC106" s="13" t="n">
+        <v>5.74</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -7903,6 +8156,9 @@
       <c r="AB107" s="13" t="n">
         <v>2186.14</v>
       </c>
+      <c r="AC107" s="13" t="n">
+        <v>2188.99</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -7981,6 +8237,7 @@
       <c r="Z108" s="13" t="n"/>
       <c r="AA108" s="13" t="n"/>
       <c r="AB108" s="13" t="n"/>
+      <c r="AC108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -8066,6 +8323,9 @@
       </c>
       <c r="AB109" s="13" t="n">
         <v>25.21</v>
+      </c>
+      <c r="AC109" s="13" t="n">
+        <v>25.23</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -8105,6 +8365,9 @@
       <c r="AB110" s="13" t="n">
         <v>838.1799999999999</v>
       </c>
+      <c r="AC110" s="13" t="n">
+        <v>833.39</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -8183,6 +8446,7 @@
       <c r="Z111" s="13" t="n"/>
       <c r="AA111" s="13" t="n"/>
       <c r="AB111" s="13" t="n"/>
+      <c r="AC111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -8268,6 +8532,9 @@
       </c>
       <c r="AB112" s="13" t="n">
         <v>33.69</v>
+      </c>
+      <c r="AC112" s="13" t="n">
+        <v>33.48</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -8307,6 +8574,9 @@
       <c r="AB113" s="13" t="n">
         <v>3565.58</v>
       </c>
+      <c r="AC113" s="13" t="n">
+        <v>3410.89</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -8385,6 +8655,7 @@
       <c r="Z114" s="13" t="n"/>
       <c r="AA114" s="13" t="n"/>
       <c r="AB114" s="13" t="n"/>
+      <c r="AC114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -8470,6 +8741,9 @@
       </c>
       <c r="AB115" s="13" t="n">
         <v>22.34</v>
+      </c>
+      <c r="AC115" s="13" t="n">
+        <v>22.21</v>
       </c>
     </row>
     <row r="116">
@@ -8494,6 +8768,9 @@
       <c r="AB116" s="13" t="n">
         <v>4043.97</v>
       </c>
+      <c r="AC116" s="13" t="n">
+        <v>4052.97</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -8527,6 +8804,7 @@
       <c r="Z117" s="13" t="n"/>
       <c r="AA117" s="13" t="n"/>
       <c r="AB117" s="13" t="n"/>
+      <c r="AC117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -8568,6 +8846,9 @@
       <c r="AB118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AC118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -8581,6 +8862,9 @@
       </c>
       <c r="AB119" s="13" t="n">
         <v>3173.89</v>
+      </c>
+      <c r="AC119" s="13" t="n">
+        <v>3115.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-09 05:19:20]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC119"/>
+  <dimension ref="A1:AD119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -551,6 +551,7 @@
     <col width="15" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="15" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -699,6 +700,11 @@
           <t>2026/02/05</t>
         </is>
       </c>
+      <c r="AD1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/09</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -846,6 +852,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AD2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -935,6 +946,9 @@
       <c r="AC3" s="13" t="n">
         <v>65.72</v>
       </c>
+      <c r="AD3" s="13" t="n">
+        <v>65.3</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -1023,6 +1037,9 @@
       </c>
       <c r="AC4" s="13" t="n">
         <v>4056.88</v>
+      </c>
+      <c r="AD4" s="13" t="n">
+        <v>4111.75</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1055,6 +1072,7 @@
       <c r="AA5" s="13" t="n"/>
       <c r="AB5" s="13" t="n"/>
       <c r="AC5" s="13" t="n"/>
+      <c r="AD5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1134,6 +1152,7 @@
       <c r="AA6" s="13" t="n"/>
       <c r="AB6" s="13" t="n"/>
       <c r="AC6" s="13" t="n"/>
+      <c r="AD6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1222,6 +1241,9 @@
       </c>
       <c r="AC7" s="13" t="n">
         <v>51.02</v>
+      </c>
+      <c r="AD7" s="13" t="n">
+        <v>50.61</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1264,6 +1286,9 @@
       <c r="AC8" s="13" t="n">
         <v>5792.56</v>
       </c>
+      <c r="AD8" s="13" t="n">
+        <v>5882.73</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1343,6 +1368,7 @@
       <c r="AA9" s="13" t="n"/>
       <c r="AB9" s="13" t="n"/>
       <c r="AC9" s="13" t="n"/>
+      <c r="AD9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1431,6 +1457,9 @@
       </c>
       <c r="AC10" s="13" t="n">
         <v>53.98</v>
+      </c>
+      <c r="AD10" s="13" t="n">
+        <v>53.06</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1473,6 +1502,9 @@
       <c r="AC11" s="13" t="n">
         <v>4647.78</v>
       </c>
+      <c r="AD11" s="13" t="n">
+        <v>4708.24</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1552,6 +1584,7 @@
       <c r="AA12" s="13" t="n"/>
       <c r="AB12" s="13" t="n"/>
       <c r="AC12" s="13" t="n"/>
+      <c r="AD12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1640,6 +1673,9 @@
       </c>
       <c r="AC13" s="13" t="n">
         <v>61.16</v>
+      </c>
+      <c r="AD13" s="13" t="n">
+        <v>60.77</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1682,6 +1718,9 @@
       <c r="AC14" s="13" t="n">
         <v>8110.21</v>
       </c>
+      <c r="AD14" s="13" t="n">
+        <v>8289.950000000001</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1761,6 +1800,7 @@
       <c r="AA15" s="13" t="n"/>
       <c r="AB15" s="13" t="n"/>
       <c r="AC15" s="13" t="n"/>
+      <c r="AD15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1849,6 +1889,9 @@
       </c>
       <c r="AC16" s="13" t="n">
         <v>29.66</v>
+      </c>
+      <c r="AD16" s="13" t="n">
+        <v>28.73</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1891,6 +1934,9 @@
       <c r="AC17" s="13" t="n">
         <v>2698.8</v>
       </c>
+      <c r="AD17" s="13" t="n">
+        <v>2698.8</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -1970,6 +2016,7 @@
       <c r="AA18" s="13" t="n"/>
       <c r="AB18" s="13" t="n"/>
       <c r="AC18" s="13" t="n"/>
+      <c r="AD18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -2058,6 +2105,9 @@
       </c>
       <c r="AC19" s="13" t="n">
         <v>95.59</v>
+      </c>
+      <c r="AD19" s="13" t="n">
+        <v>95.63</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -2100,6 +2150,9 @@
       <c r="AC20" s="13" t="n">
         <v>6882.72</v>
       </c>
+      <c r="AD20" s="13" t="n">
+        <v>6932.3</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2179,6 +2232,7 @@
       <c r="AA21" s="13" t="n"/>
       <c r="AB21" s="13" t="n"/>
       <c r="AC21" s="13" t="n"/>
+      <c r="AD21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2265,6 +2319,9 @@
       </c>
       <c r="AC22" s="13" t="n">
         <v>65.56</v>
+      </c>
+      <c r="AD22" s="13" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2307,6 +2364,9 @@
       <c r="AC23" s="13" t="n">
         <v>83473.86</v>
       </c>
+      <c r="AD23" s="13" t="n">
+        <v>83935.19</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2386,6 +2446,7 @@
       <c r="AA24" s="13" t="n"/>
       <c r="AB24" s="13" t="n"/>
       <c r="AC24" s="13" t="n"/>
+      <c r="AD24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2474,6 +2535,9 @@
       </c>
       <c r="AC25" s="13" t="n">
         <v>79.61</v>
+      </c>
+      <c r="AD25" s="13" t="n">
+        <v>84.5</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2516,6 +2580,9 @@
       <c r="AC26" s="13" t="n">
         <v>24603.04</v>
       </c>
+      <c r="AD26" s="13" t="n">
+        <v>24721.46</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2595,6 +2662,7 @@
       <c r="AA27" s="13" t="n"/>
       <c r="AB27" s="13" t="n"/>
       <c r="AC27" s="13" t="n"/>
+      <c r="AD27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2683,6 +2751,9 @@
       </c>
       <c r="AC28" s="13" t="n">
         <v>76.22</v>
+      </c>
+      <c r="AD28" s="13" t="n">
+        <v>75.69</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2725,6 +2796,9 @@
       <c r="AC29" s="13" t="n">
         <v>53833.48</v>
       </c>
+      <c r="AD29" s="13" t="n">
+        <v>56598.37</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2804,6 +2878,7 @@
       <c r="AA30" s="13" t="n"/>
       <c r="AB30" s="13" t="n"/>
       <c r="AC30" s="13" t="n"/>
+      <c r="AD30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2892,6 +2967,9 @@
       </c>
       <c r="AC31" s="13" t="n">
         <v>50.02</v>
+      </c>
+      <c r="AD31" s="13" t="n">
+        <v>51.33</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -2934,6 +3012,9 @@
       <c r="AC32" s="13" t="n">
         <v>5666.34</v>
       </c>
+      <c r="AD32" s="13" t="n">
+        <v>5697.28</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -3013,6 +3094,7 @@
       <c r="AA33" s="13" t="n"/>
       <c r="AB33" s="13" t="n"/>
       <c r="AC33" s="13" t="n"/>
+      <c r="AD33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -3101,6 +3183,9 @@
       </c>
       <c r="AC34" s="13" t="n">
         <v>2.13</v>
+      </c>
+      <c r="AD34" s="13" t="n">
+        <v>2.21</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -3143,6 +3228,9 @@
       <c r="AC35" s="13" t="n">
         <v>33886.61</v>
       </c>
+      <c r="AD35" s="13" t="n">
+        <v>34500.62</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3222,6 +3310,7 @@
       <c r="AA36" s="13" t="n"/>
       <c r="AB36" s="13" t="n"/>
       <c r="AC36" s="13" t="n"/>
+      <c r="AD36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3310,6 +3399,9 @@
       </c>
       <c r="AC37" s="13" t="n">
         <v>31.27</v>
+      </c>
+      <c r="AD37" s="13" t="n">
+        <v>30.22</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3352,6 +3444,9 @@
       <c r="AC38" s="13" t="n">
         <v>3402.83</v>
       </c>
+      <c r="AD38" s="13" t="n">
+        <v>3482.87</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3431,6 +3526,7 @@
       <c r="AA39" s="13" t="n"/>
       <c r="AB39" s="13" t="n"/>
       <c r="AC39" s="13" t="n"/>
+      <c r="AD39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3519,6 +3615,9 @@
       </c>
       <c r="AC40" s="13" t="n">
         <v>54.11</v>
+      </c>
+      <c r="AD40" s="13" t="n">
+        <v>52.68</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3561,6 +3660,9 @@
       <c r="AC41" s="13" t="n">
         <v>3249.59</v>
       </c>
+      <c r="AD41" s="13" t="n">
+        <v>3325.56</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3640,6 +3742,7 @@
       <c r="AA42" s="13" t="n"/>
       <c r="AB42" s="13" t="n"/>
       <c r="AC42" s="13" t="n"/>
+      <c r="AD42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3728,6 +3831,9 @@
       </c>
       <c r="AC43" s="13" t="n">
         <v>19.2</v>
+      </c>
+      <c r="AD43" s="13" t="n">
+        <v>19.15</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3770,6 +3876,9 @@
       <c r="AC44" s="13" t="n">
         <v>7150.81</v>
       </c>
+      <c r="AD44" s="13" t="n">
+        <v>7143.84</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3849,6 +3958,7 @@
       <c r="AA45" s="13" t="n"/>
       <c r="AB45" s="13" t="n"/>
       <c r="AC45" s="13" t="n"/>
+      <c r="AD45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -3937,6 +4047,9 @@
       </c>
       <c r="AC46" s="13" t="n">
         <v>24.87</v>
+      </c>
+      <c r="AD46" s="13" t="n">
+        <v>25.62</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -3979,6 +4092,9 @@
       <c r="AC47" s="13" t="n">
         <v>8313.58</v>
       </c>
+      <c r="AD47" s="13" t="n">
+        <v>8309.629999999999</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -4058,6 +4174,7 @@
       <c r="AA48" s="13" t="n"/>
       <c r="AB48" s="13" t="n"/>
       <c r="AC48" s="13" t="n"/>
+      <c r="AD48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -4146,6 +4263,9 @@
       </c>
       <c r="AC49" s="13" t="n">
         <v>9.58</v>
+      </c>
+      <c r="AD49" s="13" t="n">
+        <v>9.18</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -4188,6 +4308,9 @@
       <c r="AC50" s="13" t="n">
         <v>12568.02</v>
       </c>
+      <c r="AD50" s="13" t="n">
+        <v>12689.18</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4267,6 +4390,7 @@
       <c r="AA51" s="13" t="n"/>
       <c r="AB51" s="13" t="n"/>
       <c r="AC51" s="13" t="n"/>
+      <c r="AD51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4355,6 +4479,9 @@
       </c>
       <c r="AC52" s="13" t="n">
         <v>30.07</v>
+      </c>
+      <c r="AD52" s="13" t="n">
+        <v>29.11</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4397,6 +4524,9 @@
       <c r="AC53" s="13" t="n">
         <v>12875.77</v>
       </c>
+      <c r="AD53" s="13" t="n">
+        <v>12951.93</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4476,6 +4606,7 @@
       <c r="AA54" s="13" t="n"/>
       <c r="AB54" s="13" t="n"/>
       <c r="AC54" s="13" t="n"/>
+      <c r="AD54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4564,6 +4695,9 @@
       </c>
       <c r="AC55" s="13" t="n">
         <v>22.23</v>
+      </c>
+      <c r="AD55" s="13" t="n">
+        <v>21.32</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4606,6 +4740,9 @@
       <c r="AC56" s="13" t="n">
         <v>9221.23</v>
       </c>
+      <c r="AD56" s="13" t="n">
+        <v>8963.790000000001</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4685,6 +4822,7 @@
       <c r="AA57" s="13" t="n"/>
       <c r="AB57" s="13" t="n"/>
       <c r="AC57" s="13" t="n"/>
+      <c r="AD57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4773,6 +4911,9 @@
       </c>
       <c r="AC58" s="13" t="n">
         <v>26.77</v>
+      </c>
+      <c r="AD58" s="13" t="n">
+        <v>26.62</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4815,6 +4956,9 @@
       <c r="AC59" s="13" t="n">
         <v>15511.19</v>
       </c>
+      <c r="AD59" s="13" t="n">
+        <v>15334.17</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -4894,6 +5038,7 @@
       <c r="AA60" s="13" t="n"/>
       <c r="AB60" s="13" t="n"/>
       <c r="AC60" s="13" t="n"/>
+      <c r="AD60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -4982,6 +5127,9 @@
       </c>
       <c r="AC61" s="13" t="n">
         <v>30.45</v>
+      </c>
+      <c r="AD61" s="13" t="n">
+        <v>30.65</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -5024,6 +5172,9 @@
       <c r="AC62" s="13" t="n">
         <v>14929.19</v>
       </c>
+      <c r="AD62" s="13" t="n">
+        <v>15471.64</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -5103,6 +5254,7 @@
       <c r="AA63" s="13" t="n"/>
       <c r="AB63" s="13" t="n"/>
       <c r="AC63" s="13" t="n"/>
+      <c r="AD63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -5191,6 +5343,9 @@
       </c>
       <c r="AC64" s="13" t="n">
         <v>18.25</v>
+      </c>
+      <c r="AD64" s="13" t="n">
+        <v>17.99</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -5233,6 +5388,9 @@
       <c r="AC65" s="13" t="n">
         <v>8928.9</v>
       </c>
+      <c r="AD65" s="13" t="n">
+        <v>9441.42</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -5312,6 +5470,7 @@
       <c r="AA66" s="13" t="n"/>
       <c r="AB66" s="13" t="n"/>
       <c r="AC66" s="13" t="n"/>
+      <c r="AD66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -5400,6 +5559,9 @@
       </c>
       <c r="AC67" s="13" t="n">
         <v>11.91</v>
+      </c>
+      <c r="AD67" s="13" t="n">
+        <v>13.95</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -5442,6 +5604,9 @@
       <c r="AC68" s="13" t="n">
         <v>9678.959999999999</v>
       </c>
+      <c r="AD68" s="13" t="n">
+        <v>9771.25</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -5521,6 +5686,7 @@
       <c r="AA69" s="13" t="n"/>
       <c r="AB69" s="13" t="n"/>
       <c r="AC69" s="13" t="n"/>
+      <c r="AD69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -5609,6 +5775,9 @@
       </c>
       <c r="AC70" s="13" t="n">
         <v>22.25</v>
+      </c>
+      <c r="AD70" s="13" t="n">
+        <v>21.67</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -5651,6 +5820,9 @@
       <c r="AC71" s="13" t="n">
         <v>2868.22</v>
       </c>
+      <c r="AD71" s="13" t="n">
+        <v>2907.74</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -5730,6 +5902,7 @@
       <c r="AA72" s="13" t="n"/>
       <c r="AB72" s="13" t="n"/>
       <c r="AC72" s="13" t="n"/>
+      <c r="AD72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -5818,6 +5991,9 @@
       </c>
       <c r="AC73" s="13" t="n">
         <v>41.86</v>
+      </c>
+      <c r="AD73" s="13" t="n">
+        <v>41.01</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -5860,6 +6036,9 @@
       <c r="AC74" s="13" t="n">
         <v>5304.35</v>
       </c>
+      <c r="AD74" s="13" t="n">
+        <v>5411.36</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -5939,6 +6118,7 @@
       <c r="AA75" s="13" t="n"/>
       <c r="AB75" s="13" t="n"/>
       <c r="AC75" s="13" t="n"/>
+      <c r="AD75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -6027,6 +6207,9 @@
       </c>
       <c r="AC76" s="13" t="n">
         <v>24.46</v>
+      </c>
+      <c r="AD76" s="13" t="n">
+        <v>24.59</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -6069,6 +6252,9 @@
       <c r="AC77" s="13" t="n">
         <v>8879.33</v>
       </c>
+      <c r="AD77" s="13" t="n">
+        <v>8905.639999999999</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -6148,6 +6334,7 @@
       <c r="AA78" s="13" t="n"/>
       <c r="AB78" s="13" t="n"/>
       <c r="AC78" s="13" t="n"/>
+      <c r="AD78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -6236,6 +6423,9 @@
       </c>
       <c r="AC79" s="13" t="n">
         <v>17.71</v>
+      </c>
+      <c r="AD79" s="13" t="n">
+        <v>17.45</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -6278,6 +6468,9 @@
       <c r="AC80" s="13" t="n">
         <v>1524.6</v>
       </c>
+      <c r="AD80" s="13" t="n">
+        <v>1511.86</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -6357,6 +6550,7 @@
       <c r="AA81" s="13" t="n"/>
       <c r="AB81" s="13" t="n"/>
       <c r="AC81" s="13" t="n"/>
+      <c r="AD81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -6445,6 +6639,9 @@
       </c>
       <c r="AC82" s="13" t="n">
         <v>19.74</v>
+      </c>
+      <c r="AD82" s="13" t="n">
+        <v>19.57</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -6487,6 +6684,9 @@
       <c r="AC83" s="13" t="n">
         <v>17031.49</v>
       </c>
+      <c r="AD83" s="13" t="n">
+        <v>16934.73</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -6566,6 +6766,7 @@
       <c r="AA84" s="13" t="n"/>
       <c r="AB84" s="13" t="n"/>
       <c r="AC84" s="13" t="n"/>
+      <c r="AD84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -6654,6 +6855,9 @@
       </c>
       <c r="AC85" s="13" t="n">
         <v>54.7</v>
+      </c>
+      <c r="AD85" s="13" t="n">
+        <v>53.92</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -6696,6 +6900,9 @@
       <c r="AC86" s="13" t="n">
         <v>2902.46</v>
       </c>
+      <c r="AD86" s="13" t="n">
+        <v>3016.72</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -6775,6 +6982,7 @@
       <c r="AA87" s="13" t="n"/>
       <c r="AB87" s="13" t="n"/>
       <c r="AC87" s="13" t="n"/>
+      <c r="AD87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -6863,6 +7071,9 @@
       </c>
       <c r="AC88" s="13" t="n">
         <v>58.73</v>
+      </c>
+      <c r="AD88" s="13" t="n">
+        <v>58.52</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -6905,6 +7116,9 @@
       <c r="AC89" s="13" t="n">
         <v>3251.46</v>
       </c>
+      <c r="AD89" s="13" t="n">
+        <v>3394.23</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -6984,6 +7198,7 @@
       <c r="AA90" s="13" t="n"/>
       <c r="AB90" s="13" t="n"/>
       <c r="AC90" s="13" t="n"/>
+      <c r="AD90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -7072,6 +7287,9 @@
       </c>
       <c r="AC91" s="13" t="n">
         <v>49.89</v>
+      </c>
+      <c r="AD91" s="13" t="n">
+        <v>49.97</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -7114,6 +7332,9 @@
       <c r="AC92" s="13" t="n">
         <v>2926.71</v>
       </c>
+      <c r="AD92" s="13" t="n">
+        <v>3018.49</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -7193,6 +7414,7 @@
       <c r="AA93" s="13" t="n"/>
       <c r="AB93" s="13" t="n"/>
       <c r="AC93" s="13" t="n"/>
+      <c r="AD93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -7281,6 +7503,9 @@
       </c>
       <c r="AC94" s="13" t="n">
         <v>43.63</v>
+      </c>
+      <c r="AD94" s="13" t="n">
+        <v>43.5</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -7323,6 +7548,9 @@
       <c r="AC95" s="13" t="n">
         <v>1892.15</v>
       </c>
+      <c r="AD95" s="13" t="n">
+        <v>1900.15</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -7402,6 +7630,7 @@
       <c r="AA96" s="13" t="n"/>
       <c r="AB96" s="13" t="n"/>
       <c r="AC96" s="13" t="n"/>
+      <c r="AD96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -7490,6 +7719,9 @@
       </c>
       <c r="AC97" s="13" t="n">
         <v>27.12</v>
+      </c>
+      <c r="AD97" s="13" t="n">
+        <v>27.06</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -7532,6 +7764,9 @@
       <c r="AC98" s="13" t="n">
         <v>10079.91</v>
       </c>
+      <c r="AD98" s="13" t="n">
+        <v>10373.06</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -7611,6 +7846,7 @@
       <c r="AA99" s="13" t="n"/>
       <c r="AB99" s="13" t="n"/>
       <c r="AC99" s="13" t="n"/>
+      <c r="AD99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -7699,6 +7935,9 @@
       </c>
       <c r="AC100" s="13" t="n">
         <v>87.03</v>
+      </c>
+      <c r="AD100" s="13" t="n">
+        <v>86.77</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -7741,6 +7980,9 @@
       <c r="AC101" s="13" t="n">
         <v>10114.57</v>
       </c>
+      <c r="AD101" s="13" t="n">
+        <v>10211.03</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -7820,6 +8062,7 @@
       <c r="AA102" s="13" t="n"/>
       <c r="AB102" s="13" t="n"/>
       <c r="AC102" s="13" t="n"/>
+      <c r="AD102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -7908,6 +8151,9 @@
       </c>
       <c r="AC103" s="13" t="n">
         <v>59.3</v>
+      </c>
+      <c r="AD103" s="13" t="n">
+        <v>58.73</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -7950,6 +8196,9 @@
       <c r="AC104" s="13" t="n">
         <v>14941.7</v>
       </c>
+      <c r="AD104" s="13" t="n">
+        <v>14951.54</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -8029,6 +8278,7 @@
       <c r="AA105" s="13" t="n"/>
       <c r="AB105" s="13" t="n"/>
       <c r="AC105" s="13" t="n"/>
+      <c r="AD105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -8117,6 +8367,9 @@
       </c>
       <c r="AC106" s="13" t="n">
         <v>5.74</v>
+      </c>
+      <c r="AD106" s="13" t="n">
+        <v>5.67</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -8159,6 +8412,9 @@
       <c r="AC107" s="13" t="n">
         <v>2188.99</v>
       </c>
+      <c r="AD107" s="13" t="n">
+        <v>2197.1</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -8238,6 +8494,7 @@
       <c r="AA108" s="13" t="n"/>
       <c r="AB108" s="13" t="n"/>
       <c r="AC108" s="13" t="n"/>
+      <c r="AD108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -8326,6 +8583,9 @@
       </c>
       <c r="AC109" s="13" t="n">
         <v>25.23</v>
+      </c>
+      <c r="AD109" s="13" t="n">
+        <v>25.2</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -8368,6 +8628,9 @@
       <c r="AC110" s="13" t="n">
         <v>833.39</v>
       </c>
+      <c r="AD110" s="13" t="n">
+        <v>841.3099999999999</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -8447,6 +8710,7 @@
       <c r="AA111" s="13" t="n"/>
       <c r="AB111" s="13" t="n"/>
       <c r="AC111" s="13" t="n"/>
+      <c r="AD111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -8535,6 +8799,9 @@
       </c>
       <c r="AC112" s="13" t="n">
         <v>33.48</v>
+      </c>
+      <c r="AD112" s="13" t="n">
+        <v>32.69</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -8577,6 +8844,9 @@
       <c r="AC113" s="13" t="n">
         <v>3410.89</v>
       </c>
+      <c r="AD113" s="13" t="n">
+        <v>3526.49</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -8656,6 +8926,7 @@
       <c r="AA114" s="13" t="n"/>
       <c r="AB114" s="13" t="n"/>
       <c r="AC114" s="13" t="n"/>
+      <c r="AD114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -8744,6 +9015,9 @@
       </c>
       <c r="AC115" s="13" t="n">
         <v>22.21</v>
+      </c>
+      <c r="AD115" s="13" t="n">
+        <v>21.46</v>
       </c>
     </row>
     <row r="116">
@@ -8771,6 +9045,9 @@
       <c r="AC116" s="13" t="n">
         <v>4052.97</v>
       </c>
+      <c r="AD116" s="13" t="n">
+        <v>4067.21</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -8805,6 +9082,7 @@
       <c r="AA117" s="13" t="n"/>
       <c r="AB117" s="13" t="n"/>
       <c r="AC117" s="13" t="n"/>
+      <c r="AD117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -8849,6 +9127,9 @@
       <c r="AC118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AD118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -8865,6 +9146,9 @@
       </c>
       <c r="AC119" s="13" t="n">
         <v>3115.12</v>
+      </c>
+      <c r="AD119" s="13" t="n">
+        <v>3127.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-12 05:15:54]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD119"/>
+  <dimension ref="A1:AE119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -552,6 +552,7 @@
     <col width="15" customWidth="1" min="28" max="28"/>
     <col width="15" customWidth="1" min="29" max="29"/>
     <col width="15" customWidth="1" min="30" max="30"/>
+    <col width="15" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -705,6 +706,11 @@
           <t>2026/02/09</t>
         </is>
       </c>
+      <c r="AE1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/12</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -857,6 +863,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AE2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -949,6 +960,9 @@
       <c r="AD3" s="13" t="n">
         <v>65.3</v>
       </c>
+      <c r="AE3" s="13" t="n">
+        <v>69.33</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -1040,6 +1054,9 @@
       </c>
       <c r="AD4" s="13" t="n">
         <v>4111.75</v>
+      </c>
+      <c r="AE4" s="13" t="n">
+        <v>4133.82</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1073,6 +1090,7 @@
       <c r="AB5" s="13" t="n"/>
       <c r="AC5" s="13" t="n"/>
       <c r="AD5" s="13" t="n"/>
+      <c r="AE5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1153,6 +1171,7 @@
       <c r="AB6" s="13" t="n"/>
       <c r="AC6" s="13" t="n"/>
       <c r="AD6" s="13" t="n"/>
+      <c r="AE6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1244,6 +1263,9 @@
       </c>
       <c r="AD7" s="13" t="n">
         <v>50.61</v>
+      </c>
+      <c r="AE7" s="13" t="n">
+        <v>51.3</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1289,6 +1311,9 @@
       <c r="AD8" s="13" t="n">
         <v>5882.73</v>
       </c>
+      <c r="AE8" s="13" t="n">
+        <v>5916.6</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1369,6 +1394,7 @@
       <c r="AB9" s="13" t="n"/>
       <c r="AC9" s="13" t="n"/>
       <c r="AD9" s="13" t="n"/>
+      <c r="AE9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1460,6 +1486,9 @@
       </c>
       <c r="AD10" s="13" t="n">
         <v>53.06</v>
+      </c>
+      <c r="AE10" s="13" t="n">
+        <v>54.86</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1505,6 +1534,9 @@
       <c r="AD11" s="13" t="n">
         <v>4708.24</v>
       </c>
+      <c r="AE11" s="13" t="n">
+        <v>4717.25</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1585,6 +1617,7 @@
       <c r="AB12" s="13" t="n"/>
       <c r="AC12" s="13" t="n"/>
       <c r="AD12" s="13" t="n"/>
+      <c r="AE12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1676,6 +1709,9 @@
       </c>
       <c r="AD13" s="13" t="n">
         <v>60.77</v>
+      </c>
+      <c r="AE13" s="13" t="n">
+        <v>61.25</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1721,6 +1757,9 @@
       <c r="AD14" s="13" t="n">
         <v>8289.950000000001</v>
       </c>
+      <c r="AE14" s="13" t="n">
+        <v>8411.370000000001</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1801,6 +1840,7 @@
       <c r="AB15" s="13" t="n"/>
       <c r="AC15" s="13" t="n"/>
       <c r="AD15" s="13" t="n"/>
+      <c r="AE15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1892,6 +1932,9 @@
       </c>
       <c r="AD16" s="13" t="n">
         <v>28.73</v>
+      </c>
+      <c r="AE16" s="13" t="n">
+        <v>31.02</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1937,6 +1980,9 @@
       <c r="AD17" s="13" t="n">
         <v>2698.8</v>
       </c>
+      <c r="AE17" s="13" t="n">
+        <v>2730.77</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -2017,6 +2063,7 @@
       <c r="AB18" s="13" t="n"/>
       <c r="AC18" s="13" t="n"/>
       <c r="AD18" s="13" t="n"/>
+      <c r="AE18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -2108,6 +2155,9 @@
       </c>
       <c r="AD19" s="13" t="n">
         <v>95.63</v>
+      </c>
+      <c r="AE19" s="13" t="n">
+        <v>95.97</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -2153,6 +2203,9 @@
       <c r="AD20" s="13" t="n">
         <v>6932.3</v>
       </c>
+      <c r="AE20" s="13" t="n">
+        <v>6941.47</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2233,6 +2286,7 @@
       <c r="AB21" s="13" t="n"/>
       <c r="AC21" s="13" t="n"/>
       <c r="AD21" s="13" t="n"/>
+      <c r="AE21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2322,6 +2376,9 @@
       </c>
       <c r="AD22" s="13" t="n">
         <v>67</v>
+      </c>
+      <c r="AE22" s="13" t="n">
+        <v>67.15000000000001</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2367,6 +2424,9 @@
       <c r="AD23" s="13" t="n">
         <v>83935.19</v>
       </c>
+      <c r="AE23" s="13" t="n">
+        <v>83920.96000000001</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2447,6 +2507,7 @@
       <c r="AB24" s="13" t="n"/>
       <c r="AC24" s="13" t="n"/>
       <c r="AD24" s="13" t="n"/>
+      <c r="AE24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2538,6 +2599,9 @@
       </c>
       <c r="AD25" s="13" t="n">
         <v>84.5</v>
+      </c>
+      <c r="AE25" s="13" t="n">
+        <v>80.55</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2583,6 +2647,9 @@
       <c r="AD26" s="13" t="n">
         <v>24721.46</v>
       </c>
+      <c r="AE26" s="13" t="n">
+        <v>24856.15</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2663,6 +2730,7 @@
       <c r="AB27" s="13" t="n"/>
       <c r="AC27" s="13" t="n"/>
       <c r="AD27" s="13" t="n"/>
+      <c r="AE27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2754,6 +2822,9 @@
       </c>
       <c r="AD28" s="13" t="n">
         <v>75.69</v>
+      </c>
+      <c r="AE28" s="13" t="n">
+        <v>83.88</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2799,6 +2870,9 @@
       <c r="AD29" s="13" t="n">
         <v>56598.37</v>
       </c>
+      <c r="AE29" s="13" t="n">
+        <v>57798.82</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2879,6 +2953,7 @@
       <c r="AB30" s="13" t="n"/>
       <c r="AC30" s="13" t="n"/>
       <c r="AD30" s="13" t="n"/>
+      <c r="AE30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -2970,6 +3045,9 @@
       </c>
       <c r="AD31" s="13" t="n">
         <v>51.33</v>
+      </c>
+      <c r="AE31" s="13" t="n">
+        <v>51.57</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -3015,6 +3093,9 @@
       <c r="AD32" s="13" t="n">
         <v>5697.28</v>
       </c>
+      <c r="AE32" s="13" t="n">
+        <v>5747.82</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -3095,6 +3176,7 @@
       <c r="AB33" s="13" t="n"/>
       <c r="AC33" s="13" t="n"/>
       <c r="AD33" s="13" t="n"/>
+      <c r="AE33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -3186,6 +3268,9 @@
       </c>
       <c r="AD34" s="13" t="n">
         <v>2.21</v>
+      </c>
+      <c r="AE34" s="13" t="n">
+        <v>2.34</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -3231,6 +3316,9 @@
       <c r="AD35" s="13" t="n">
         <v>34500.62</v>
       </c>
+      <c r="AE35" s="13" t="n">
+        <v>34579.87</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3311,6 +3399,7 @@
       <c r="AB36" s="13" t="n"/>
       <c r="AC36" s="13" t="n"/>
       <c r="AD36" s="13" t="n"/>
+      <c r="AE36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3402,6 +3491,9 @@
       </c>
       <c r="AD37" s="13" t="n">
         <v>30.22</v>
+      </c>
+      <c r="AE37" s="13" t="n">
+        <v>30.84</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3447,6 +3539,9 @@
       <c r="AD38" s="13" t="n">
         <v>3482.87</v>
       </c>
+      <c r="AE38" s="13" t="n">
+        <v>3476</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3527,6 +3622,7 @@
       <c r="AB39" s="13" t="n"/>
       <c r="AC39" s="13" t="n"/>
       <c r="AD39" s="13" t="n"/>
+      <c r="AE39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3618,6 +3714,9 @@
       </c>
       <c r="AD40" s="13" t="n">
         <v>52.68</v>
+      </c>
+      <c r="AE40" s="13" t="n">
+        <v>53.55</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3663,6 +3762,9 @@
       <c r="AD41" s="13" t="n">
         <v>3325.56</v>
       </c>
+      <c r="AE41" s="13" t="n">
+        <v>3323.8</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3743,6 +3845,7 @@
       <c r="AB42" s="13" t="n"/>
       <c r="AC42" s="13" t="n"/>
       <c r="AD42" s="13" t="n"/>
+      <c r="AE42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3834,6 +3937,9 @@
       </c>
       <c r="AD43" s="13" t="n">
         <v>19.15</v>
+      </c>
+      <c r="AE43" s="13" t="n">
+        <v>19.52</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3879,6 +3985,9 @@
       <c r="AD44" s="13" t="n">
         <v>7143.84</v>
       </c>
+      <c r="AE44" s="13" t="n">
+        <v>7154.47</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -3959,6 +4068,7 @@
       <c r="AB45" s="13" t="n"/>
       <c r="AC45" s="13" t="n"/>
       <c r="AD45" s="13" t="n"/>
+      <c r="AE45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -4050,6 +4160,9 @@
       </c>
       <c r="AD46" s="13" t="n">
         <v>25.62</v>
+      </c>
+      <c r="AE46" s="13" t="n">
+        <v>25.89</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -4095,6 +4208,9 @@
       <c r="AD47" s="13" t="n">
         <v>8309.629999999999</v>
       </c>
+      <c r="AE47" s="13" t="n">
+        <v>8426.450000000001</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -4175,6 +4291,7 @@
       <c r="AB48" s="13" t="n"/>
       <c r="AC48" s="13" t="n"/>
       <c r="AD48" s="13" t="n"/>
+      <c r="AE48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -4266,6 +4383,9 @@
       </c>
       <c r="AD49" s="13" t="n">
         <v>9.18</v>
+      </c>
+      <c r="AE49" s="13" t="n">
+        <v>9.56</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -4311,6 +4431,9 @@
       <c r="AD50" s="13" t="n">
         <v>12689.18</v>
       </c>
+      <c r="AE50" s="13" t="n">
+        <v>12692.55</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4391,6 +4514,7 @@
       <c r="AB51" s="13" t="n"/>
       <c r="AC51" s="13" t="n"/>
       <c r="AD51" s="13" t="n"/>
+      <c r="AE51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4482,6 +4606,9 @@
       </c>
       <c r="AD52" s="13" t="n">
         <v>29.11</v>
+      </c>
+      <c r="AE52" s="13" t="n">
+        <v>30.54</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4527,6 +4654,9 @@
       <c r="AD53" s="13" t="n">
         <v>12951.93</v>
       </c>
+      <c r="AE53" s="13" t="n">
+        <v>12886.7</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4607,6 +4737,7 @@
       <c r="AB54" s="13" t="n"/>
       <c r="AC54" s="13" t="n"/>
       <c r="AD54" s="13" t="n"/>
+      <c r="AE54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4698,6 +4829,9 @@
       </c>
       <c r="AD55" s="13" t="n">
         <v>21.32</v>
+      </c>
+      <c r="AE55" s="13" t="n">
+        <v>20.55</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4743,6 +4877,9 @@
       <c r="AD56" s="13" t="n">
         <v>8963.790000000001</v>
       </c>
+      <c r="AE56" s="13" t="n">
+        <v>8676.040000000001</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4823,6 +4960,7 @@
       <c r="AB57" s="13" t="n"/>
       <c r="AC57" s="13" t="n"/>
       <c r="AD57" s="13" t="n"/>
+      <c r="AE57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -4914,6 +5052,9 @@
       </c>
       <c r="AD58" s="13" t="n">
         <v>26.62</v>
+      </c>
+      <c r="AE58" s="13" t="n">
+        <v>26.42</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -4959,6 +5100,9 @@
       <c r="AD59" s="13" t="n">
         <v>15334.17</v>
       </c>
+      <c r="AE59" s="13" t="n">
+        <v>15022.27</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -5039,6 +5183,7 @@
       <c r="AB60" s="13" t="n"/>
       <c r="AC60" s="13" t="n"/>
       <c r="AD60" s="13" t="n"/>
+      <c r="AE60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -5130,6 +5275,9 @@
       </c>
       <c r="AD61" s="13" t="n">
         <v>30.65</v>
+      </c>
+      <c r="AE61" s="13" t="n">
+        <v>32.05</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -5175,6 +5323,9 @@
       <c r="AD62" s="13" t="n">
         <v>15471.64</v>
       </c>
+      <c r="AE62" s="13" t="n">
+        <v>15934.99</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -5255,6 +5406,7 @@
       <c r="AB63" s="13" t="n"/>
       <c r="AC63" s="13" t="n"/>
       <c r="AD63" s="13" t="n"/>
+      <c r="AE63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -5346,6 +5498,9 @@
       </c>
       <c r="AD64" s="13" t="n">
         <v>17.99</v>
+      </c>
+      <c r="AE64" s="13" t="n">
+        <v>18.45</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -5391,6 +5546,9 @@
       <c r="AD65" s="13" t="n">
         <v>9441.42</v>
       </c>
+      <c r="AE65" s="13" t="n">
+        <v>8874.879999999999</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -5471,6 +5629,7 @@
       <c r="AB66" s="13" t="n"/>
       <c r="AC66" s="13" t="n"/>
       <c r="AD66" s="13" t="n"/>
+      <c r="AE66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -5562,6 +5721,9 @@
       </c>
       <c r="AD67" s="13" t="n">
         <v>13.95</v>
+      </c>
+      <c r="AE67" s="13" t="n">
+        <v>11.49</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -5607,6 +5769,9 @@
       <c r="AD68" s="13" t="n">
         <v>9771.25</v>
       </c>
+      <c r="AE68" s="13" t="n">
+        <v>9637.360000000001</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -5687,6 +5852,7 @@
       <c r="AB69" s="13" t="n"/>
       <c r="AC69" s="13" t="n"/>
       <c r="AD69" s="13" t="n"/>
+      <c r="AE69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -5778,6 +5944,9 @@
       </c>
       <c r="AD70" s="13" t="n">
         <v>21.67</v>
+      </c>
+      <c r="AE70" s="13" t="n">
+        <v>22.5</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -5823,6 +5992,9 @@
       <c r="AD71" s="13" t="n">
         <v>2907.74</v>
       </c>
+      <c r="AE71" s="13" t="n">
+        <v>2884.47</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -5903,6 +6075,7 @@
       <c r="AB72" s="13" t="n"/>
       <c r="AC72" s="13" t="n"/>
       <c r="AD72" s="13" t="n"/>
+      <c r="AE72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -5994,6 +6167,9 @@
       </c>
       <c r="AD73" s="13" t="n">
         <v>41.01</v>
+      </c>
+      <c r="AE73" s="13" t="n">
+        <v>42.87</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -6039,6 +6215,9 @@
       <c r="AD74" s="13" t="n">
         <v>5411.36</v>
       </c>
+      <c r="AE74" s="13" t="n">
+        <v>5398.24</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -6119,6 +6298,7 @@
       <c r="AB75" s="13" t="n"/>
       <c r="AC75" s="13" t="n"/>
       <c r="AD75" s="13" t="n"/>
+      <c r="AE75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -6210,6 +6390,9 @@
       </c>
       <c r="AD76" s="13" t="n">
         <v>24.59</v>
+      </c>
+      <c r="AE76" s="13" t="n">
+        <v>25.27</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -6255,6 +6438,9 @@
       <c r="AD77" s="13" t="n">
         <v>8905.639999999999</v>
       </c>
+      <c r="AE77" s="13" t="n">
+        <v>8957.67</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -6335,6 +6521,7 @@
       <c r="AB78" s="13" t="n"/>
       <c r="AC78" s="13" t="n"/>
       <c r="AD78" s="13" t="n"/>
+      <c r="AE78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -6426,6 +6613,9 @@
       </c>
       <c r="AD79" s="13" t="n">
         <v>17.45</v>
+      </c>
+      <c r="AE79" s="13" t="n">
+        <v>20.09</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -6471,6 +6661,9 @@
       <c r="AD80" s="13" t="n">
         <v>1511.86</v>
       </c>
+      <c r="AE80" s="13" t="n">
+        <v>1522.4</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -6551,6 +6744,7 @@
       <c r="AB81" s="13" t="n"/>
       <c r="AC81" s="13" t="n"/>
       <c r="AD81" s="13" t="n"/>
+      <c r="AE81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -6642,6 +6836,9 @@
       </c>
       <c r="AD82" s="13" t="n">
         <v>19.57</v>
+      </c>
+      <c r="AE82" s="13" t="n">
+        <v>17.19</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -6687,6 +6884,9 @@
       <c r="AD83" s="13" t="n">
         <v>16934.73</v>
       </c>
+      <c r="AE83" s="13" t="n">
+        <v>16757.72</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -6767,6 +6967,7 @@
       <c r="AB84" s="13" t="n"/>
       <c r="AC84" s="13" t="n"/>
       <c r="AD84" s="13" t="n"/>
+      <c r="AE84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -6858,6 +7059,9 @@
       </c>
       <c r="AD85" s="13" t="n">
         <v>53.92</v>
+      </c>
+      <c r="AE85" s="13" t="n">
+        <v>54.5</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -6903,6 +7107,9 @@
       <c r="AD86" s="13" t="n">
         <v>3016.72</v>
       </c>
+      <c r="AE86" s="13" t="n">
+        <v>3053.93</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -6983,6 +7190,7 @@
       <c r="AB87" s="13" t="n"/>
       <c r="AC87" s="13" t="n"/>
       <c r="AD87" s="13" t="n"/>
+      <c r="AE87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -7074,6 +7282,9 @@
       </c>
       <c r="AD88" s="13" t="n">
         <v>58.52</v>
+      </c>
+      <c r="AE88" s="13" t="n">
+        <v>58.49</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -7119,6 +7330,9 @@
       <c r="AD89" s="13" t="n">
         <v>3394.23</v>
       </c>
+      <c r="AE89" s="13" t="n">
+        <v>3348.69</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -7199,6 +7413,7 @@
       <c r="AB90" s="13" t="n"/>
       <c r="AC90" s="13" t="n"/>
       <c r="AD90" s="13" t="n"/>
+      <c r="AE90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -7290,6 +7505,9 @@
       </c>
       <c r="AD91" s="13" t="n">
         <v>49.97</v>
+      </c>
+      <c r="AE91" s="13" t="n">
+        <v>50.84</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -7335,6 +7553,9 @@
       <c r="AD92" s="13" t="n">
         <v>3018.49</v>
       </c>
+      <c r="AE92" s="13" t="n">
+        <v>3077.81</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -7415,6 +7636,7 @@
       <c r="AB93" s="13" t="n"/>
       <c r="AC93" s="13" t="n"/>
       <c r="AD93" s="13" t="n"/>
+      <c r="AE93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -7506,6 +7728,9 @@
       </c>
       <c r="AD94" s="13" t="n">
         <v>43.5</v>
+      </c>
+      <c r="AE94" s="13" t="n">
+        <v>45.15</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -7551,6 +7776,9 @@
       <c r="AD95" s="13" t="n">
         <v>1900.15</v>
       </c>
+      <c r="AE95" s="13" t="n">
+        <v>1924.96</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -7631,6 +7859,7 @@
       <c r="AB96" s="13" t="n"/>
       <c r="AC96" s="13" t="n"/>
       <c r="AD96" s="13" t="n"/>
+      <c r="AE96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -7722,6 +7951,9 @@
       </c>
       <c r="AD97" s="13" t="n">
         <v>27.06</v>
+      </c>
+      <c r="AE97" s="13" t="n">
+        <v>27.18</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -7767,6 +7999,9 @@
       <c r="AD98" s="13" t="n">
         <v>10373.06</v>
       </c>
+      <c r="AE98" s="13" t="n">
+        <v>10286.58</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -7847,6 +8082,7 @@
       <c r="AB99" s="13" t="n"/>
       <c r="AC99" s="13" t="n"/>
       <c r="AD99" s="13" t="n"/>
+      <c r="AE99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -7938,6 +8174,9 @@
       </c>
       <c r="AD100" s="13" t="n">
         <v>86.77</v>
+      </c>
+      <c r="AE100" s="13" t="n">
+        <v>87.04000000000001</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -7983,6 +8222,9 @@
       <c r="AD101" s="13" t="n">
         <v>10211.03</v>
       </c>
+      <c r="AE101" s="13" t="n">
+        <v>10284.64</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -8063,6 +8305,7 @@
       <c r="AB102" s="13" t="n"/>
       <c r="AC102" s="13" t="n"/>
       <c r="AD102" s="13" t="n"/>
+      <c r="AE102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -8154,6 +8397,9 @@
       </c>
       <c r="AD103" s="13" t="n">
         <v>58.73</v>
+      </c>
+      <c r="AE103" s="13" t="n">
+        <v>59.21</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -8199,6 +8445,9 @@
       <c r="AD104" s="13" t="n">
         <v>14951.54</v>
       </c>
+      <c r="AE104" s="13" t="n">
+        <v>15091.44</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -8279,6 +8528,7 @@
       <c r="AB105" s="13" t="n"/>
       <c r="AC105" s="13" t="n"/>
       <c r="AD105" s="13" t="n"/>
+      <c r="AE105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -8370,6 +8620,9 @@
       </c>
       <c r="AD106" s="13" t="n">
         <v>5.67</v>
+      </c>
+      <c r="AE106" s="13" t="n">
+        <v>6.26</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -8415,6 +8668,9 @@
       <c r="AD107" s="13" t="n">
         <v>2197.1</v>
       </c>
+      <c r="AE107" s="13" t="n">
+        <v>2183.55</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -8495,6 +8751,7 @@
       <c r="AB108" s="13" t="n"/>
       <c r="AC108" s="13" t="n"/>
       <c r="AD108" s="13" t="n"/>
+      <c r="AE108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -8586,6 +8843,9 @@
       </c>
       <c r="AD109" s="13" t="n">
         <v>25.2</v>
+      </c>
+      <c r="AE109" s="13" t="n">
+        <v>25.26</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -8631,6 +8891,9 @@
       <c r="AD110" s="13" t="n">
         <v>841.3099999999999</v>
       </c>
+      <c r="AE110" s="13" t="n">
+        <v>833.08</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -8711,6 +8974,7 @@
       <c r="AB111" s="13" t="n"/>
       <c r="AC111" s="13" t="n"/>
       <c r="AD111" s="13" t="n"/>
+      <c r="AE111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -8802,6 +9066,9 @@
       </c>
       <c r="AD112" s="13" t="n">
         <v>32.69</v>
+      </c>
+      <c r="AE112" s="13" t="n">
+        <v>33.38</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -8847,6 +9114,9 @@
       <c r="AD113" s="13" t="n">
         <v>3526.49</v>
       </c>
+      <c r="AE113" s="13" t="n">
+        <v>3634.16</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -8927,6 +9197,7 @@
       <c r="AB114" s="13" t="n"/>
       <c r="AC114" s="13" t="n"/>
       <c r="AD114" s="13" t="n"/>
+      <c r="AE114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -9018,6 +9289,9 @@
       </c>
       <c r="AD115" s="13" t="n">
         <v>21.46</v>
+      </c>
+      <c r="AE115" s="13" t="n">
+        <v>21.63</v>
       </c>
     </row>
     <row r="116">
@@ -9048,6 +9322,9 @@
       <c r="AD116" s="13" t="n">
         <v>4067.21</v>
       </c>
+      <c r="AE116" s="13" t="n">
+        <v>4064.43</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -9083,6 +9360,7 @@
       <c r="AB117" s="13" t="n"/>
       <c r="AC117" s="13" t="n"/>
       <c r="AD117" s="13" t="n"/>
+      <c r="AE117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -9130,6 +9408,9 @@
       <c r="AD118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AE118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -9149,6 +9430,9 @@
       </c>
       <c r="AD119" s="13" t="n">
         <v>3127.86</v>
+      </c>
+      <c r="AE119" s="13" t="n">
+        <v>3086.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-19 05:12:32]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE119"/>
+  <dimension ref="A1:AF119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -553,6 +553,7 @@
     <col width="15" customWidth="1" min="29" max="29"/>
     <col width="15" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -711,6 +712,11 @@
           <t>2026/02/12</t>
         </is>
       </c>
+      <c r="AF1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/19</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -868,6 +874,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AF2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -963,6 +974,9 @@
       <c r="AE3" s="13" t="n">
         <v>69.33</v>
       </c>
+      <c r="AF3" s="13" t="n">
+        <v>68.91</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -1057,6 +1071,9 @@
       </c>
       <c r="AE4" s="13" t="n">
         <v>4133.82</v>
+      </c>
+      <c r="AF4" s="13" t="n">
+        <v>4082.07</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1091,6 +1108,7 @@
       <c r="AC5" s="13" t="n"/>
       <c r="AD5" s="13" t="n"/>
       <c r="AE5" s="13" t="n"/>
+      <c r="AF5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1172,6 +1190,7 @@
       <c r="AC6" s="13" t="n"/>
       <c r="AD6" s="13" t="n"/>
       <c r="AE6" s="13" t="n"/>
+      <c r="AF6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1266,6 +1285,9 @@
       </c>
       <c r="AE7" s="13" t="n">
         <v>51.3</v>
+      </c>
+      <c r="AF7" s="13" t="n">
+        <v>50.67</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1314,6 +1336,9 @@
       <c r="AE8" s="13" t="n">
         <v>5916.6</v>
       </c>
+      <c r="AF8" s="13" t="n">
+        <v>5840.73</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1395,6 +1420,7 @@
       <c r="AC9" s="13" t="n"/>
       <c r="AD9" s="13" t="n"/>
       <c r="AE9" s="13" t="n"/>
+      <c r="AF9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1489,6 +1515,9 @@
       </c>
       <c r="AE10" s="13" t="n">
         <v>54.86</v>
+      </c>
+      <c r="AF10" s="13" t="n">
+        <v>52.88</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1537,6 +1566,9 @@
       <c r="AE11" s="13" t="n">
         <v>4717.25</v>
       </c>
+      <c r="AF11" s="13" t="n">
+        <v>4660.41</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1618,6 +1650,7 @@
       <c r="AC12" s="13" t="n"/>
       <c r="AD12" s="13" t="n"/>
       <c r="AE12" s="13" t="n"/>
+      <c r="AF12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1712,6 +1745,9 @@
       </c>
       <c r="AE13" s="13" t="n">
         <v>61.25</v>
+      </c>
+      <c r="AF13" s="13" t="n">
+        <v>61.11</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1760,6 +1796,9 @@
       <c r="AE14" s="13" t="n">
         <v>8411.370000000001</v>
       </c>
+      <c r="AF14" s="13" t="n">
+        <v>8299.59</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1841,6 +1880,7 @@
       <c r="AC15" s="13" t="n"/>
       <c r="AD15" s="13" t="n"/>
       <c r="AE15" s="13" t="n"/>
+      <c r="AF15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1935,6 +1975,9 @@
       </c>
       <c r="AE16" s="13" t="n">
         <v>31.02</v>
+      </c>
+      <c r="AF16" s="13" t="n">
+        <v>28.58</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1983,6 +2026,9 @@
       <c r="AE17" s="13" t="n">
         <v>2730.77</v>
       </c>
+      <c r="AF17" s="13" t="n">
+        <v>2699.25</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -2064,6 +2110,7 @@
       <c r="AC18" s="13" t="n"/>
       <c r="AD18" s="13" t="n"/>
       <c r="AE18" s="13" t="n"/>
+      <c r="AF18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -2158,6 +2205,9 @@
       </c>
       <c r="AE19" s="13" t="n">
         <v>95.97</v>
+      </c>
+      <c r="AF19" s="13" t="n">
+        <v>95.25</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -2206,6 +2256,9 @@
       <c r="AE20" s="13" t="n">
         <v>6941.47</v>
       </c>
+      <c r="AF20" s="13" t="n">
+        <v>6881.31</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2287,6 +2340,7 @@
       <c r="AC21" s="13" t="n"/>
       <c r="AD21" s="13" t="n"/>
       <c r="AE21" s="13" t="n"/>
+      <c r="AF21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2379,6 +2433,9 @@
       </c>
       <c r="AE22" s="13" t="n">
         <v>67.15000000000001</v>
+      </c>
+      <c r="AF22" s="13" t="n">
+        <v>61.28</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2427,6 +2484,9 @@
       <c r="AE23" s="13" t="n">
         <v>83920.96000000001</v>
       </c>
+      <c r="AF23" s="13" t="n">
+        <v>83518.11</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2508,6 +2568,7 @@
       <c r="AC24" s="13" t="n"/>
       <c r="AD24" s="13" t="n"/>
       <c r="AE24" s="13" t="n"/>
+      <c r="AF24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2602,6 +2663,9 @@
       </c>
       <c r="AE25" s="13" t="n">
         <v>80.55</v>
+      </c>
+      <c r="AF25" s="13" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2650,6 +2714,9 @@
       <c r="AE26" s="13" t="n">
         <v>24856.15</v>
       </c>
+      <c r="AF26" s="13" t="n">
+        <v>25278.21</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2731,6 +2798,7 @@
       <c r="AC27" s="13" t="n"/>
       <c r="AD27" s="13" t="n"/>
       <c r="AE27" s="13" t="n"/>
+      <c r="AF27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2825,6 +2893,9 @@
       </c>
       <c r="AE28" s="13" t="n">
         <v>83.88</v>
+      </c>
+      <c r="AF28" s="13" t="n">
+        <v>78.11</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -2873,6 +2944,9 @@
       <c r="AE29" s="13" t="n">
         <v>57798.82</v>
       </c>
+      <c r="AF29" s="13" t="n">
+        <v>57563.42</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -2954,6 +3028,7 @@
       <c r="AC30" s="13" t="n"/>
       <c r="AD30" s="13" t="n"/>
       <c r="AE30" s="13" t="n"/>
+      <c r="AF30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -3048,6 +3123,9 @@
       </c>
       <c r="AE31" s="13" t="n">
         <v>51.57</v>
+      </c>
+      <c r="AF31" s="13" t="n">
+        <v>50.9</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -3096,6 +3174,9 @@
       <c r="AE32" s="13" t="n">
         <v>5747.82</v>
       </c>
+      <c r="AF32" s="13" t="n">
+        <v>5668.22</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -3177,6 +3258,7 @@
       <c r="AC33" s="13" t="n"/>
       <c r="AD33" s="13" t="n"/>
       <c r="AE33" s="13" t="n"/>
+      <c r="AF33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -3271,6 +3353,9 @@
       </c>
       <c r="AE34" s="13" t="n">
         <v>2.34</v>
+      </c>
+      <c r="AF34" s="13" t="n">
+        <v>2.06</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -3319,6 +3404,9 @@
       <c r="AE35" s="13" t="n">
         <v>34579.87</v>
       </c>
+      <c r="AF35" s="13" t="n">
+        <v>34125.79</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3400,6 +3488,7 @@
       <c r="AC36" s="13" t="n"/>
       <c r="AD36" s="13" t="n"/>
       <c r="AE36" s="13" t="n"/>
+      <c r="AF36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3494,6 +3583,9 @@
       </c>
       <c r="AE37" s="13" t="n">
         <v>30.84</v>
+      </c>
+      <c r="AF37" s="13" t="n">
+        <v>30.77</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3542,6 +3634,9 @@
       <c r="AE38" s="13" t="n">
         <v>3476</v>
       </c>
+      <c r="AF38" s="13" t="n">
+        <v>3423.05</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3623,6 +3718,7 @@
       <c r="AC39" s="13" t="n"/>
       <c r="AD39" s="13" t="n"/>
       <c r="AE39" s="13" t="n"/>
+      <c r="AF39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3717,6 +3813,9 @@
       </c>
       <c r="AE40" s="13" t="n">
         <v>53.55</v>
+      </c>
+      <c r="AF40" s="13" t="n">
+        <v>53.45</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3765,6 +3864,9 @@
       <c r="AE41" s="13" t="n">
         <v>3323.8</v>
       </c>
+      <c r="AF41" s="13" t="n">
+        <v>3275.96</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3846,6 +3948,7 @@
       <c r="AC42" s="13" t="n"/>
       <c r="AD42" s="13" t="n"/>
       <c r="AE42" s="13" t="n"/>
+      <c r="AF42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -3940,6 +4043,9 @@
       </c>
       <c r="AE43" s="13" t="n">
         <v>19.52</v>
+      </c>
+      <c r="AF43" s="13" t="n">
+        <v>18.43</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -3988,6 +4094,9 @@
       <c r="AE44" s="13" t="n">
         <v>7154.47</v>
       </c>
+      <c r="AF44" s="13" t="n">
+        <v>7020.65</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -4069,6 +4178,7 @@
       <c r="AC45" s="13" t="n"/>
       <c r="AD45" s="13" t="n"/>
       <c r="AE45" s="13" t="n"/>
+      <c r="AF45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -4163,6 +4273,9 @@
       </c>
       <c r="AE46" s="13" t="n">
         <v>25.89</v>
+      </c>
+      <c r="AF46" s="13" t="n">
+        <v>23.8</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -4211,6 +4324,9 @@
       <c r="AE47" s="13" t="n">
         <v>8426.450000000001</v>
       </c>
+      <c r="AF47" s="13" t="n">
+        <v>8295.26</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -4292,6 +4408,7 @@
       <c r="AC48" s="13" t="n"/>
       <c r="AD48" s="13" t="n"/>
       <c r="AE48" s="13" t="n"/>
+      <c r="AF48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -4386,6 +4503,9 @@
       </c>
       <c r="AE49" s="13" t="n">
         <v>9.56</v>
+      </c>
+      <c r="AF49" s="13" t="n">
+        <v>8.220000000000001</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -4434,6 +4554,9 @@
       <c r="AE50" s="13" t="n">
         <v>12692.55</v>
       </c>
+      <c r="AF50" s="13" t="n">
+        <v>12530.04</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4515,6 +4638,7 @@
       <c r="AC51" s="13" t="n"/>
       <c r="AD51" s="13" t="n"/>
       <c r="AE51" s="13" t="n"/>
+      <c r="AF51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4609,6 +4733,9 @@
       </c>
       <c r="AE52" s="13" t="n">
         <v>30.54</v>
+      </c>
+      <c r="AF52" s="13" t="n">
+        <v>29.32</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4657,6 +4784,9 @@
       <c r="AE53" s="13" t="n">
         <v>12886.7</v>
       </c>
+      <c r="AF53" s="13" t="n">
+        <v>12947.59</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4738,6 +4868,7 @@
       <c r="AC54" s="13" t="n"/>
       <c r="AD54" s="13" t="n"/>
       <c r="AE54" s="13" t="n"/>
+      <c r="AF54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4832,6 +4963,9 @@
       </c>
       <c r="AE55" s="13" t="n">
         <v>20.55</v>
+      </c>
+      <c r="AF55" s="13" t="n">
+        <v>19.63</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -4880,6 +5014,9 @@
       <c r="AE56" s="13" t="n">
         <v>8676.040000000001</v>
       </c>
+      <c r="AF56" s="13" t="n">
+        <v>8655.870000000001</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -4961,6 +5098,7 @@
       <c r="AC57" s="13" t="n"/>
       <c r="AD57" s="13" t="n"/>
       <c r="AE57" s="13" t="n"/>
+      <c r="AF57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -5055,6 +5193,9 @@
       </c>
       <c r="AE58" s="13" t="n">
         <v>26.42</v>
+      </c>
+      <c r="AF58" s="13" t="n">
+        <v>25.62</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -5103,6 +5244,9 @@
       <c r="AE59" s="13" t="n">
         <v>15022.27</v>
       </c>
+      <c r="AF59" s="13" t="n">
+        <v>14952.52</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -5184,6 +5328,7 @@
       <c r="AC60" s="13" t="n"/>
       <c r="AD60" s="13" t="n"/>
       <c r="AE60" s="13" t="n"/>
+      <c r="AF60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -5278,6 +5423,9 @@
       </c>
       <c r="AE61" s="13" t="n">
         <v>32.05</v>
+      </c>
+      <c r="AF61" s="13" t="n">
+        <v>31.43</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -5326,6 +5474,9 @@
       <c r="AE62" s="13" t="n">
         <v>15934.99</v>
       </c>
+      <c r="AF62" s="13" t="n">
+        <v>15797.64</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -5407,6 +5558,7 @@
       <c r="AC63" s="13" t="n"/>
       <c r="AD63" s="13" t="n"/>
       <c r="AE63" s="13" t="n"/>
+      <c r="AF63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -5501,6 +5653,9 @@
       </c>
       <c r="AE64" s="13" t="n">
         <v>18.45</v>
+      </c>
+      <c r="AF64" s="13" t="n">
+        <v>17.73</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -5549,6 +5704,9 @@
       <c r="AE65" s="13" t="n">
         <v>8874.879999999999</v>
       </c>
+      <c r="AF65" s="13" t="n">
+        <v>8772.110000000001</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -5630,6 +5788,7 @@
       <c r="AC66" s="13" t="n"/>
       <c r="AD66" s="13" t="n"/>
       <c r="AE66" s="13" t="n"/>
+      <c r="AF66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -5724,6 +5883,9 @@
       </c>
       <c r="AE67" s="13" t="n">
         <v>11.49</v>
+      </c>
+      <c r="AF67" s="13" t="n">
+        <v>10.07</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -5772,6 +5934,9 @@
       <c r="AE68" s="13" t="n">
         <v>9637.360000000001</v>
       </c>
+      <c r="AF68" s="13" t="n">
+        <v>9563.01</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -5853,6 +6018,7 @@
       <c r="AC69" s="13" t="n"/>
       <c r="AD69" s="13" t="n"/>
       <c r="AE69" s="13" t="n"/>
+      <c r="AF69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -5947,6 +6113,9 @@
       </c>
       <c r="AE70" s="13" t="n">
         <v>22.5</v>
+      </c>
+      <c r="AF70" s="13" t="n">
+        <v>21.43</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -5995,6 +6164,9 @@
       <c r="AE71" s="13" t="n">
         <v>2884.47</v>
       </c>
+      <c r="AF71" s="13" t="n">
+        <v>2868.34</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -6076,6 +6248,7 @@
       <c r="AC72" s="13" t="n"/>
       <c r="AD72" s="13" t="n"/>
       <c r="AE72" s="13" t="n"/>
+      <c r="AF72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -6170,6 +6343,9 @@
       </c>
       <c r="AE73" s="13" t="n">
         <v>42.87</v>
+      </c>
+      <c r="AF73" s="13" t="n">
+        <v>40.86</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -6218,6 +6394,9 @@
       <c r="AE74" s="13" t="n">
         <v>5398.24</v>
       </c>
+      <c r="AF74" s="13" t="n">
+        <v>5367.52</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -6299,6 +6478,7 @@
       <c r="AC75" s="13" t="n"/>
       <c r="AD75" s="13" t="n"/>
       <c r="AE75" s="13" t="n"/>
+      <c r="AF75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -6393,6 +6573,9 @@
       </c>
       <c r="AE76" s="13" t="n">
         <v>25.27</v>
+      </c>
+      <c r="AF76" s="13" t="n">
+        <v>23.61</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -6441,6 +6624,9 @@
       <c r="AE77" s="13" t="n">
         <v>8957.67</v>
       </c>
+      <c r="AF77" s="13" t="n">
+        <v>8820.860000000001</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -6522,6 +6708,7 @@
       <c r="AC78" s="13" t="n"/>
       <c r="AD78" s="13" t="n"/>
       <c r="AE78" s="13" t="n"/>
+      <c r="AF78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -6616,6 +6803,9 @@
       </c>
       <c r="AE79" s="13" t="n">
         <v>20.09</v>
+      </c>
+      <c r="AF79" s="13" t="n">
+        <v>18.25</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -6664,6 +6854,9 @@
       <c r="AE80" s="13" t="n">
         <v>1522.4</v>
       </c>
+      <c r="AF80" s="13" t="n">
+        <v>1474.31</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -6745,6 +6938,7 @@
       <c r="AC81" s="13" t="n"/>
       <c r="AD81" s="13" t="n"/>
       <c r="AE81" s="13" t="n"/>
+      <c r="AF81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -6839,6 +7033,9 @@
       </c>
       <c r="AE82" s="13" t="n">
         <v>17.19</v>
+      </c>
+      <c r="AF82" s="13" t="n">
+        <v>16.38</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -6887,6 +7084,9 @@
       <c r="AE83" s="13" t="n">
         <v>16757.72</v>
       </c>
+      <c r="AF83" s="13" t="n">
+        <v>16509.82</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -6968,6 +7168,7 @@
       <c r="AC84" s="13" t="n"/>
       <c r="AD84" s="13" t="n"/>
       <c r="AE84" s="13" t="n"/>
+      <c r="AF84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -7062,6 +7263,9 @@
       </c>
       <c r="AE85" s="13" t="n">
         <v>54.5</v>
+      </c>
+      <c r="AF85" s="13" t="n">
+        <v>54.2</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -7110,6 +7314,9 @@
       <c r="AE86" s="13" t="n">
         <v>3053.93</v>
       </c>
+      <c r="AF86" s="13" t="n">
+        <v>2994.14</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -7191,6 +7398,7 @@
       <c r="AC87" s="13" t="n"/>
       <c r="AD87" s="13" t="n"/>
       <c r="AE87" s="13" t="n"/>
+      <c r="AF87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -7285,6 +7493,9 @@
       </c>
       <c r="AE88" s="13" t="n">
         <v>58.49</v>
+      </c>
+      <c r="AF88" s="13" t="n">
+        <v>58.36</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -7333,6 +7544,9 @@
       <c r="AE89" s="13" t="n">
         <v>3348.69</v>
       </c>
+      <c r="AF89" s="13" t="n">
+        <v>3251.43</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -7414,6 +7628,7 @@
       <c r="AC90" s="13" t="n"/>
       <c r="AD90" s="13" t="n"/>
       <c r="AE90" s="13" t="n"/>
+      <c r="AF90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -7508,6 +7723,9 @@
       </c>
       <c r="AE91" s="13" t="n">
         <v>50.84</v>
+      </c>
+      <c r="AF91" s="13" t="n">
+        <v>50.72</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -7556,6 +7774,9 @@
       <c r="AE92" s="13" t="n">
         <v>3077.81</v>
       </c>
+      <c r="AF92" s="13" t="n">
+        <v>3056.18</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -7637,6 +7858,7 @@
       <c r="AC93" s="13" t="n"/>
       <c r="AD93" s="13" t="n"/>
       <c r="AE93" s="13" t="n"/>
+      <c r="AF93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -7731,6 +7953,9 @@
       </c>
       <c r="AE94" s="13" t="n">
         <v>45.15</v>
+      </c>
+      <c r="AF94" s="13" t="n">
+        <v>43.69</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -7779,6 +8004,9 @@
       <c r="AE95" s="13" t="n">
         <v>1924.96</v>
       </c>
+      <c r="AF95" s="13" t="n">
+        <v>1891.58</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -7860,6 +8088,7 @@
       <c r="AC96" s="13" t="n"/>
       <c r="AD96" s="13" t="n"/>
       <c r="AE96" s="13" t="n"/>
+      <c r="AF96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -7954,6 +8183,9 @@
       </c>
       <c r="AE97" s="13" t="n">
         <v>27.18</v>
+      </c>
+      <c r="AF97" s="13" t="n">
+        <v>26.77</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -8002,6 +8234,9 @@
       <c r="AE98" s="13" t="n">
         <v>10286.58</v>
       </c>
+      <c r="AF98" s="13" t="n">
+        <v>10406.57</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -8083,6 +8318,7 @@
       <c r="AC99" s="13" t="n"/>
       <c r="AD99" s="13" t="n"/>
       <c r="AE99" s="13" t="n"/>
+      <c r="AF99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -8177,6 +8413,9 @@
       </c>
       <c r="AE100" s="13" t="n">
         <v>87.04000000000001</v>
+      </c>
+      <c r="AF100" s="13" t="n">
+        <v>87.48999999999999</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -8225,6 +8464,9 @@
       <c r="AE101" s="13" t="n">
         <v>10284.64</v>
       </c>
+      <c r="AF101" s="13" t="n">
+        <v>10413.72</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -8306,6 +8548,7 @@
       <c r="AC102" s="13" t="n"/>
       <c r="AD102" s="13" t="n"/>
       <c r="AE102" s="13" t="n"/>
+      <c r="AF102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -8400,6 +8643,9 @@
       </c>
       <c r="AE103" s="13" t="n">
         <v>59.21</v>
+      </c>
+      <c r="AF103" s="13" t="n">
+        <v>59.65</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -8448,6 +8694,9 @@
       <c r="AE104" s="13" t="n">
         <v>15091.44</v>
       </c>
+      <c r="AF104" s="13" t="n">
+        <v>15127.96</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -8529,6 +8778,7 @@
       <c r="AC105" s="13" t="n"/>
       <c r="AD105" s="13" t="n"/>
       <c r="AE105" s="13" t="n"/>
+      <c r="AF105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -8623,6 +8873,9 @@
       </c>
       <c r="AE106" s="13" t="n">
         <v>6.26</v>
+      </c>
+      <c r="AF106" s="13" t="n">
+        <v>5.64</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -8671,6 +8924,9 @@
       <c r="AE107" s="13" t="n">
         <v>2183.55</v>
       </c>
+      <c r="AF107" s="13" t="n">
+        <v>2156.61</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -8752,6 +9008,7 @@
       <c r="AC108" s="13" t="n"/>
       <c r="AD108" s="13" t="n"/>
       <c r="AE108" s="13" t="n"/>
+      <c r="AF108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -8846,6 +9103,9 @@
       </c>
       <c r="AE109" s="13" t="n">
         <v>25.26</v>
+      </c>
+      <c r="AF109" s="13" t="n">
+        <v>24.99</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -8894,6 +9154,9 @@
       <c r="AE110" s="13" t="n">
         <v>833.08</v>
       </c>
+      <c r="AF110" s="13" t="n">
+        <v>823.65</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -8975,6 +9238,7 @@
       <c r="AC111" s="13" t="n"/>
       <c r="AD111" s="13" t="n"/>
       <c r="AE111" s="13" t="n"/>
+      <c r="AF111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -9069,6 +9333,9 @@
       </c>
       <c r="AE112" s="13" t="n">
         <v>33.38</v>
+      </c>
+      <c r="AF112" s="13" t="n">
+        <v>32.9</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -9117,6 +9384,9 @@
       <c r="AE113" s="13" t="n">
         <v>3634.16</v>
       </c>
+      <c r="AF113" s="13" t="n">
+        <v>3513.48</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -9198,6 +9468,7 @@
       <c r="AC114" s="13" t="n"/>
       <c r="AD114" s="13" t="n"/>
       <c r="AE114" s="13" t="n"/>
+      <c r="AF114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -9292,6 +9563,9 @@
       </c>
       <c r="AE115" s="13" t="n">
         <v>21.63</v>
+      </c>
+      <c r="AF115" s="13" t="n">
+        <v>21.34</v>
       </c>
     </row>
     <row r="116">
@@ -9325,6 +9599,9 @@
       <c r="AE116" s="13" t="n">
         <v>4064.43</v>
       </c>
+      <c r="AF116" s="13" t="n">
+        <v>4024.89</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -9361,6 +9638,7 @@
       <c r="AC117" s="13" t="n"/>
       <c r="AD117" s="13" t="n"/>
       <c r="AE117" s="13" t="n"/>
+      <c r="AF117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -9411,6 +9689,9 @@
       <c r="AE118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AF118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -9433,6 +9714,9 @@
       </c>
       <c r="AE119" s="13" t="n">
         <v>3086.27</v>
+      </c>
+      <c r="AF119" s="13" t="n">
+        <v>3062.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-23 05:16:38]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF119"/>
+  <dimension ref="A1:AG119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -554,6 +554,7 @@
     <col width="15" customWidth="1" min="30" max="30"/>
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="15" customWidth="1" min="33" max="33"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -717,6 +718,11 @@
           <t>2026/02/19</t>
         </is>
       </c>
+      <c r="AG1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/23</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -879,6 +885,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AG2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -977,6 +988,9 @@
       <c r="AF3" s="13" t="n">
         <v>68.91</v>
       </c>
+      <c r="AG3" s="13" t="n">
+        <v>68.91</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -1073,6 +1087,9 @@
         <v>4133.82</v>
       </c>
       <c r="AF4" s="13" t="n">
+        <v>4082.07</v>
+      </c>
+      <c r="AG4" s="13" t="n">
         <v>4082.07</v>
       </c>
     </row>
@@ -1109,6 +1126,7 @@
       <c r="AD5" s="13" t="n"/>
       <c r="AE5" s="13" t="n"/>
       <c r="AF5" s="13" t="n"/>
+      <c r="AG5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1191,6 +1209,7 @@
       <c r="AD6" s="13" t="n"/>
       <c r="AE6" s="13" t="n"/>
       <c r="AF6" s="13" t="n"/>
+      <c r="AG6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1287,6 +1306,9 @@
         <v>51.3</v>
       </c>
       <c r="AF7" s="13" t="n">
+        <v>50.67</v>
+      </c>
+      <c r="AG7" s="13" t="n">
         <v>50.67</v>
       </c>
     </row>
@@ -1339,6 +1361,9 @@
       <c r="AF8" s="13" t="n">
         <v>5840.73</v>
       </c>
+      <c r="AG8" s="13" t="n">
+        <v>5840.73</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1421,6 +1446,7 @@
       <c r="AD9" s="13" t="n"/>
       <c r="AE9" s="13" t="n"/>
       <c r="AF9" s="13" t="n"/>
+      <c r="AG9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1517,6 +1543,9 @@
         <v>54.86</v>
       </c>
       <c r="AF10" s="13" t="n">
+        <v>52.88</v>
+      </c>
+      <c r="AG10" s="13" t="n">
         <v>52.88</v>
       </c>
     </row>
@@ -1569,6 +1598,9 @@
       <c r="AF11" s="13" t="n">
         <v>4660.41</v>
       </c>
+      <c r="AG11" s="13" t="n">
+        <v>4660.41</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1651,6 +1683,7 @@
       <c r="AD12" s="13" t="n"/>
       <c r="AE12" s="13" t="n"/>
       <c r="AF12" s="13" t="n"/>
+      <c r="AG12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1747,6 +1780,9 @@
         <v>61.25</v>
       </c>
       <c r="AF13" s="13" t="n">
+        <v>61.11</v>
+      </c>
+      <c r="AG13" s="13" t="n">
         <v>61.11</v>
       </c>
     </row>
@@ -1799,6 +1835,9 @@
       <c r="AF14" s="13" t="n">
         <v>8299.59</v>
       </c>
+      <c r="AG14" s="13" t="n">
+        <v>8299.59</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1881,6 +1920,7 @@
       <c r="AD15" s="13" t="n"/>
       <c r="AE15" s="13" t="n"/>
       <c r="AF15" s="13" t="n"/>
+      <c r="AG15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -1977,6 +2017,9 @@
         <v>31.02</v>
       </c>
       <c r="AF16" s="13" t="n">
+        <v>28.58</v>
+      </c>
+      <c r="AG16" s="13" t="n">
         <v>28.58</v>
       </c>
     </row>
@@ -2029,6 +2072,9 @@
       <c r="AF17" s="13" t="n">
         <v>2699.25</v>
       </c>
+      <c r="AG17" s="13" t="n">
+        <v>2699.25</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -2111,6 +2157,7 @@
       <c r="AD18" s="13" t="n"/>
       <c r="AE18" s="13" t="n"/>
       <c r="AF18" s="13" t="n"/>
+      <c r="AG18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -2207,6 +2254,9 @@
         <v>95.97</v>
       </c>
       <c r="AF19" s="13" t="n">
+        <v>95.25</v>
+      </c>
+      <c r="AG19" s="13" t="n">
         <v>95.25</v>
       </c>
     </row>
@@ -2259,6 +2309,9 @@
       <c r="AF20" s="13" t="n">
         <v>6881.31</v>
       </c>
+      <c r="AG20" s="13" t="n">
+        <v>6909.51</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2341,6 +2394,7 @@
       <c r="AD21" s="13" t="n"/>
       <c r="AE21" s="13" t="n"/>
       <c r="AF21" s="13" t="n"/>
+      <c r="AG21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2435,6 +2489,9 @@
         <v>67.15000000000001</v>
       </c>
       <c r="AF22" s="13" t="n">
+        <v>61.28</v>
+      </c>
+      <c r="AG22" s="13" t="n">
         <v>61.28</v>
       </c>
     </row>
@@ -2487,6 +2544,9 @@
       <c r="AF23" s="13" t="n">
         <v>83518.11</v>
       </c>
+      <c r="AG23" s="13" t="n">
+        <v>83233.38</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2569,6 +2629,7 @@
       <c r="AD24" s="13" t="n"/>
       <c r="AE24" s="13" t="n"/>
       <c r="AF24" s="13" t="n"/>
+      <c r="AG24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2665,6 +2726,9 @@
         <v>80.55</v>
       </c>
       <c r="AF25" s="13" t="n">
+        <v>80</v>
+      </c>
+      <c r="AG25" s="13" t="n">
         <v>80</v>
       </c>
     </row>
@@ -2717,6 +2781,9 @@
       <c r="AF26" s="13" t="n">
         <v>25278.21</v>
       </c>
+      <c r="AG26" s="13" t="n">
+        <v>25260.69</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2799,6 +2866,7 @@
       <c r="AD27" s="13" t="n"/>
       <c r="AE27" s="13" t="n"/>
       <c r="AF27" s="13" t="n"/>
+      <c r="AG27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2895,6 +2963,9 @@
         <v>83.88</v>
       </c>
       <c r="AF28" s="13" t="n">
+        <v>78.11</v>
+      </c>
+      <c r="AG28" s="13" t="n">
         <v>78.11</v>
       </c>
     </row>
@@ -2947,6 +3018,9 @@
       <c r="AF29" s="13" t="n">
         <v>57563.42</v>
       </c>
+      <c r="AG29" s="13" t="n">
+        <v>56825.7</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -3029,6 +3103,7 @@
       <c r="AD30" s="13" t="n"/>
       <c r="AE30" s="13" t="n"/>
       <c r="AF30" s="13" t="n"/>
+      <c r="AG30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -3125,6 +3200,9 @@
         <v>51.57</v>
       </c>
       <c r="AF31" s="13" t="n">
+        <v>50.9</v>
+      </c>
+      <c r="AG31" s="13" t="n">
         <v>50.9</v>
       </c>
     </row>
@@ -3177,6 +3255,9 @@
       <c r="AF32" s="13" t="n">
         <v>5668.22</v>
       </c>
+      <c r="AG32" s="13" t="n">
+        <v>5668.22</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -3259,6 +3340,7 @@
       <c r="AD33" s="13" t="n"/>
       <c r="AE33" s="13" t="n"/>
       <c r="AF33" s="13" t="n"/>
+      <c r="AG33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -3355,6 +3437,9 @@
         <v>2.34</v>
       </c>
       <c r="AF34" s="13" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="AG34" s="13" t="n">
         <v>2.06</v>
       </c>
     </row>
@@ -3407,6 +3492,9 @@
       <c r="AF35" s="13" t="n">
         <v>34125.79</v>
       </c>
+      <c r="AG35" s="13" t="n">
+        <v>34125.79</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3489,6 +3577,7 @@
       <c r="AD36" s="13" t="n"/>
       <c r="AE36" s="13" t="n"/>
       <c r="AF36" s="13" t="n"/>
+      <c r="AG36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3585,6 +3674,9 @@
         <v>30.84</v>
       </c>
       <c r="AF37" s="13" t="n">
+        <v>30.77</v>
+      </c>
+      <c r="AG37" s="13" t="n">
         <v>30.77</v>
       </c>
     </row>
@@ -3637,6 +3729,9 @@
       <c r="AF38" s="13" t="n">
         <v>3423.05</v>
       </c>
+      <c r="AG38" s="13" t="n">
+        <v>3423.05</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3719,6 +3814,7 @@
       <c r="AD39" s="13" t="n"/>
       <c r="AE39" s="13" t="n"/>
       <c r="AF39" s="13" t="n"/>
+      <c r="AG39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3815,6 +3911,9 @@
         <v>53.55</v>
       </c>
       <c r="AF40" s="13" t="n">
+        <v>53.45</v>
+      </c>
+      <c r="AG40" s="13" t="n">
         <v>53.45</v>
       </c>
     </row>
@@ -3867,6 +3966,9 @@
       <c r="AF41" s="13" t="n">
         <v>3275.96</v>
       </c>
+      <c r="AG41" s="13" t="n">
+        <v>3275.96</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -3949,6 +4051,7 @@
       <c r="AD42" s="13" t="n"/>
       <c r="AE42" s="13" t="n"/>
       <c r="AF42" s="13" t="n"/>
+      <c r="AG42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -4045,6 +4148,9 @@
         <v>19.52</v>
       </c>
       <c r="AF43" s="13" t="n">
+        <v>18.43</v>
+      </c>
+      <c r="AG43" s="13" t="n">
         <v>18.43</v>
       </c>
     </row>
@@ -4097,6 +4203,9 @@
       <c r="AF44" s="13" t="n">
         <v>7020.65</v>
       </c>
+      <c r="AG44" s="13" t="n">
+        <v>7020.65</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -4179,6 +4288,7 @@
       <c r="AD45" s="13" t="n"/>
       <c r="AE45" s="13" t="n"/>
       <c r="AF45" s="13" t="n"/>
+      <c r="AG45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -4275,6 +4385,9 @@
         <v>25.89</v>
       </c>
       <c r="AF46" s="13" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="AG46" s="13" t="n">
         <v>23.8</v>
       </c>
     </row>
@@ -4327,6 +4440,9 @@
       <c r="AF47" s="13" t="n">
         <v>8295.26</v>
       </c>
+      <c r="AG47" s="13" t="n">
+        <v>8295.26</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -4409,6 +4525,7 @@
       <c r="AD48" s="13" t="n"/>
       <c r="AE48" s="13" t="n"/>
       <c r="AF48" s="13" t="n"/>
+      <c r="AG48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -4505,6 +4622,9 @@
         <v>9.56</v>
       </c>
       <c r="AF49" s="13" t="n">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="AG49" s="13" t="n">
         <v>8.220000000000001</v>
       </c>
     </row>
@@ -4557,6 +4677,9 @@
       <c r="AF50" s="13" t="n">
         <v>12530.04</v>
       </c>
+      <c r="AG50" s="13" t="n">
+        <v>12530.04</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4639,6 +4762,7 @@
       <c r="AD51" s="13" t="n"/>
       <c r="AE51" s="13" t="n"/>
       <c r="AF51" s="13" t="n"/>
+      <c r="AG51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4735,6 +4859,9 @@
         <v>30.54</v>
       </c>
       <c r="AF52" s="13" t="n">
+        <v>29.32</v>
+      </c>
+      <c r="AG52" s="13" t="n">
         <v>29.32</v>
       </c>
     </row>
@@ -4787,6 +4914,9 @@
       <c r="AF53" s="13" t="n">
         <v>12947.59</v>
       </c>
+      <c r="AG53" s="13" t="n">
+        <v>13013.04</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -4869,6 +4999,7 @@
       <c r="AD54" s="13" t="n"/>
       <c r="AE54" s="13" t="n"/>
       <c r="AF54" s="13" t="n"/>
+      <c r="AG54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -4965,6 +5096,9 @@
         <v>20.55</v>
       </c>
       <c r="AF55" s="13" t="n">
+        <v>19.63</v>
+      </c>
+      <c r="AG55" s="13" t="n">
         <v>19.63</v>
       </c>
     </row>
@@ -5017,6 +5151,9 @@
       <c r="AF56" s="13" t="n">
         <v>8655.870000000001</v>
       </c>
+      <c r="AG56" s="13" t="n">
+        <v>8655.870000000001</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -5099,6 +5236,7 @@
       <c r="AD57" s="13" t="n"/>
       <c r="AE57" s="13" t="n"/>
       <c r="AF57" s="13" t="n"/>
+      <c r="AG57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -5195,6 +5333,9 @@
         <v>26.42</v>
       </c>
       <c r="AF58" s="13" t="n">
+        <v>25.62</v>
+      </c>
+      <c r="AG58" s="13" t="n">
         <v>25.62</v>
       </c>
     </row>
@@ -5247,6 +5388,9 @@
       <c r="AF59" s="13" t="n">
         <v>14952.52</v>
       </c>
+      <c r="AG59" s="13" t="n">
+        <v>14952.52</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -5329,6 +5473,7 @@
       <c r="AD60" s="13" t="n"/>
       <c r="AE60" s="13" t="n"/>
       <c r="AF60" s="13" t="n"/>
+      <c r="AG60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -5425,6 +5570,9 @@
         <v>32.05</v>
       </c>
       <c r="AF61" s="13" t="n">
+        <v>31.43</v>
+      </c>
+      <c r="AG61" s="13" t="n">
         <v>31.43</v>
       </c>
     </row>
@@ -5477,6 +5625,9 @@
       <c r="AF62" s="13" t="n">
         <v>15797.64</v>
       </c>
+      <c r="AG62" s="13" t="n">
+        <v>16186.92</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -5559,6 +5710,7 @@
       <c r="AD63" s="13" t="n"/>
       <c r="AE63" s="13" t="n"/>
       <c r="AF63" s="13" t="n"/>
+      <c r="AG63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -5655,6 +5807,9 @@
         <v>18.45</v>
       </c>
       <c r="AF64" s="13" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="AG64" s="13" t="n">
         <v>17.73</v>
       </c>
     </row>
@@ -5707,6 +5862,9 @@
       <c r="AF65" s="13" t="n">
         <v>8772.110000000001</v>
       </c>
+      <c r="AG65" s="13" t="n">
+        <v>8772.110000000001</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -5789,6 +5947,7 @@
       <c r="AD66" s="13" t="n"/>
       <c r="AE66" s="13" t="n"/>
       <c r="AF66" s="13" t="n"/>
+      <c r="AG66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -5885,6 +6044,9 @@
         <v>11.49</v>
       </c>
       <c r="AF67" s="13" t="n">
+        <v>10.07</v>
+      </c>
+      <c r="AG67" s="13" t="n">
         <v>10.07</v>
       </c>
     </row>
@@ -5937,6 +6099,9 @@
       <c r="AF68" s="13" t="n">
         <v>9563.01</v>
       </c>
+      <c r="AG68" s="13" t="n">
+        <v>9563.01</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -6019,6 +6184,7 @@
       <c r="AD69" s="13" t="n"/>
       <c r="AE69" s="13" t="n"/>
       <c r="AF69" s="13" t="n"/>
+      <c r="AG69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -6115,6 +6281,9 @@
         <v>22.5</v>
       </c>
       <c r="AF70" s="13" t="n">
+        <v>21.43</v>
+      </c>
+      <c r="AG70" s="13" t="n">
         <v>21.43</v>
       </c>
     </row>
@@ -6167,6 +6336,9 @@
       <c r="AF71" s="13" t="n">
         <v>2868.34</v>
       </c>
+      <c r="AG71" s="13" t="n">
+        <v>2863.88</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -6249,6 +6421,7 @@
       <c r="AD72" s="13" t="n"/>
       <c r="AE72" s="13" t="n"/>
       <c r="AF72" s="13" t="n"/>
+      <c r="AG72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -6345,6 +6518,9 @@
         <v>42.87</v>
       </c>
       <c r="AF73" s="13" t="n">
+        <v>40.86</v>
+      </c>
+      <c r="AG73" s="13" t="n">
         <v>40.86</v>
       </c>
     </row>
@@ -6397,6 +6573,9 @@
       <c r="AF74" s="13" t="n">
         <v>5367.52</v>
       </c>
+      <c r="AG74" s="13" t="n">
+        <v>5361.58</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -6479,6 +6658,7 @@
       <c r="AD75" s="13" t="n"/>
       <c r="AE75" s="13" t="n"/>
       <c r="AF75" s="13" t="n"/>
+      <c r="AG75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -6575,6 +6755,9 @@
         <v>25.27</v>
       </c>
       <c r="AF76" s="13" t="n">
+        <v>23.61</v>
+      </c>
+      <c r="AG76" s="13" t="n">
         <v>23.61</v>
       </c>
     </row>
@@ -6627,6 +6810,9 @@
       <c r="AF77" s="13" t="n">
         <v>8820.860000000001</v>
       </c>
+      <c r="AG77" s="13" t="n">
+        <v>8820.860000000001</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -6709,6 +6895,7 @@
       <c r="AD78" s="13" t="n"/>
       <c r="AE78" s="13" t="n"/>
       <c r="AF78" s="13" t="n"/>
+      <c r="AG78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -6805,6 +6992,9 @@
         <v>20.09</v>
       </c>
       <c r="AF79" s="13" t="n">
+        <v>18.25</v>
+      </c>
+      <c r="AG79" s="13" t="n">
         <v>18.25</v>
       </c>
     </row>
@@ -6857,6 +7047,9 @@
       <c r="AF80" s="13" t="n">
         <v>1474.31</v>
       </c>
+      <c r="AG80" s="13" t="n">
+        <v>1474.31</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -6939,6 +7132,7 @@
       <c r="AD81" s="13" t="n"/>
       <c r="AE81" s="13" t="n"/>
       <c r="AF81" s="13" t="n"/>
+      <c r="AG81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -7035,6 +7229,9 @@
         <v>17.19</v>
       </c>
       <c r="AF82" s="13" t="n">
+        <v>16.38</v>
+      </c>
+      <c r="AG82" s="13" t="n">
         <v>16.38</v>
       </c>
     </row>
@@ -7087,6 +7284,9 @@
       <c r="AF83" s="13" t="n">
         <v>16509.82</v>
       </c>
+      <c r="AG83" s="13" t="n">
+        <v>16509.82</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -7169,6 +7369,7 @@
       <c r="AD84" s="13" t="n"/>
       <c r="AE84" s="13" t="n"/>
       <c r="AF84" s="13" t="n"/>
+      <c r="AG84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -7265,6 +7466,9 @@
         <v>54.5</v>
       </c>
       <c r="AF85" s="13" t="n">
+        <v>54.2</v>
+      </c>
+      <c r="AG85" s="13" t="n">
         <v>54.2</v>
       </c>
     </row>
@@ -7317,6 +7521,9 @@
       <c r="AF86" s="13" t="n">
         <v>2994.14</v>
       </c>
+      <c r="AG86" s="13" t="n">
+        <v>2994.14</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -7399,6 +7606,7 @@
       <c r="AD87" s="13" t="n"/>
       <c r="AE87" s="13" t="n"/>
       <c r="AF87" s="13" t="n"/>
+      <c r="AG87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -7495,6 +7703,9 @@
         <v>58.49</v>
       </c>
       <c r="AF88" s="13" t="n">
+        <v>58.36</v>
+      </c>
+      <c r="AG88" s="13" t="n">
         <v>58.36</v>
       </c>
     </row>
@@ -7547,6 +7758,9 @@
       <c r="AF89" s="13" t="n">
         <v>3251.43</v>
       </c>
+      <c r="AG89" s="13" t="n">
+        <v>3251.43</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -7629,6 +7843,7 @@
       <c r="AD90" s="13" t="n"/>
       <c r="AE90" s="13" t="n"/>
       <c r="AF90" s="13" t="n"/>
+      <c r="AG90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -7725,6 +7940,9 @@
         <v>50.84</v>
       </c>
       <c r="AF91" s="13" t="n">
+        <v>50.72</v>
+      </c>
+      <c r="AG91" s="13" t="n">
         <v>50.72</v>
       </c>
     </row>
@@ -7777,6 +7995,9 @@
       <c r="AF92" s="13" t="n">
         <v>3056.18</v>
       </c>
+      <c r="AG92" s="13" t="n">
+        <v>3056.18</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -7859,6 +8080,7 @@
       <c r="AD93" s="13" t="n"/>
       <c r="AE93" s="13" t="n"/>
       <c r="AF93" s="13" t="n"/>
+      <c r="AG93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -7955,6 +8177,9 @@
         <v>45.15</v>
       </c>
       <c r="AF94" s="13" t="n">
+        <v>43.69</v>
+      </c>
+      <c r="AG94" s="13" t="n">
         <v>43.69</v>
       </c>
     </row>
@@ -8007,6 +8232,9 @@
       <c r="AF95" s="13" t="n">
         <v>1891.58</v>
       </c>
+      <c r="AG95" s="13" t="n">
+        <v>1891.58</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -8089,6 +8317,7 @@
       <c r="AD96" s="13" t="n"/>
       <c r="AE96" s="13" t="n"/>
       <c r="AF96" s="13" t="n"/>
+      <c r="AG96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -8185,6 +8414,9 @@
         <v>27.18</v>
       </c>
       <c r="AF97" s="13" t="n">
+        <v>26.77</v>
+      </c>
+      <c r="AG97" s="13" t="n">
         <v>26.77</v>
       </c>
     </row>
@@ -8237,6 +8469,9 @@
       <c r="AF98" s="13" t="n">
         <v>10406.57</v>
       </c>
+      <c r="AG98" s="13" t="n">
+        <v>10184.4</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -8319,6 +8554,7 @@
       <c r="AD99" s="13" t="n"/>
       <c r="AE99" s="13" t="n"/>
       <c r="AF99" s="13" t="n"/>
+      <c r="AG99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -8415,6 +8651,9 @@
         <v>87.04000000000001</v>
       </c>
       <c r="AF100" s="13" t="n">
+        <v>87.48999999999999</v>
+      </c>
+      <c r="AG100" s="13" t="n">
         <v>87.48999999999999</v>
       </c>
     </row>
@@ -8467,6 +8706,9 @@
       <c r="AF101" s="13" t="n">
         <v>10413.72</v>
       </c>
+      <c r="AG101" s="13" t="n">
+        <v>10413.72</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -8549,6 +8791,7 @@
       <c r="AD102" s="13" t="n"/>
       <c r="AE102" s="13" t="n"/>
       <c r="AF102" s="13" t="n"/>
+      <c r="AG102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -8645,6 +8888,9 @@
         <v>59.21</v>
       </c>
       <c r="AF103" s="13" t="n">
+        <v>59.65</v>
+      </c>
+      <c r="AG103" s="13" t="n">
         <v>59.65</v>
       </c>
     </row>
@@ -8697,6 +8943,9 @@
       <c r="AF104" s="13" t="n">
         <v>15127.96</v>
       </c>
+      <c r="AG104" s="13" t="n">
+        <v>15127.96</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -8779,6 +9028,7 @@
       <c r="AD105" s="13" t="n"/>
       <c r="AE105" s="13" t="n"/>
       <c r="AF105" s="13" t="n"/>
+      <c r="AG105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -8875,6 +9125,9 @@
         <v>6.26</v>
       </c>
       <c r="AF106" s="13" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="AG106" s="13" t="n">
         <v>5.64</v>
       </c>
     </row>
@@ -8927,6 +9180,9 @@
       <c r="AF107" s="13" t="n">
         <v>2156.61</v>
       </c>
+      <c r="AG107" s="13" t="n">
+        <v>2156.61</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -9009,6 +9265,7 @@
       <c r="AD108" s="13" t="n"/>
       <c r="AE108" s="13" t="n"/>
       <c r="AF108" s="13" t="n"/>
+      <c r="AG108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -9105,6 +9362,9 @@
         <v>25.26</v>
       </c>
       <c r="AF109" s="13" t="n">
+        <v>24.99</v>
+      </c>
+      <c r="AG109" s="13" t="n">
         <v>24.99</v>
       </c>
     </row>
@@ -9157,6 +9417,9 @@
       <c r="AF110" s="13" t="n">
         <v>823.65</v>
       </c>
+      <c r="AG110" s="13" t="n">
+        <v>823.65</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -9239,6 +9502,7 @@
       <c r="AD111" s="13" t="n"/>
       <c r="AE111" s="13" t="n"/>
       <c r="AF111" s="13" t="n"/>
+      <c r="AG111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -9335,6 +9599,9 @@
         <v>33.38</v>
       </c>
       <c r="AF112" s="13" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="AG112" s="13" t="n">
         <v>32.9</v>
       </c>
     </row>
@@ -9387,6 +9654,9 @@
       <c r="AF113" s="13" t="n">
         <v>3513.48</v>
       </c>
+      <c r="AG113" s="13" t="n">
+        <v>3513.48</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -9469,6 +9739,7 @@
       <c r="AD114" s="13" t="n"/>
       <c r="AE114" s="13" t="n"/>
       <c r="AF114" s="13" t="n"/>
+      <c r="AG114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -9565,6 +9836,9 @@
         <v>21.63</v>
       </c>
       <c r="AF115" s="13" t="n">
+        <v>21.34</v>
+      </c>
+      <c r="AG115" s="13" t="n">
         <v>21.34</v>
       </c>
     </row>
@@ -9602,6 +9876,9 @@
       <c r="AF116" s="13" t="n">
         <v>4024.89</v>
       </c>
+      <c r="AG116" s="13" t="n">
+        <v>4024.89</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -9639,6 +9916,7 @@
       <c r="AD117" s="13" t="n"/>
       <c r="AE117" s="13" t="n"/>
       <c r="AF117" s="13" t="n"/>
+      <c r="AG117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -9692,6 +9970,9 @@
       <c r="AF118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AG118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -9716,6 +9997,9 @@
         <v>3086.27</v>
       </c>
       <c r="AF119" s="13" t="n">
+        <v>3062.87</v>
+      </c>
+      <c r="AG119" s="13" t="n">
         <v>3062.87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update stocks_data.xlsx [2026-02-26 05:10:44]
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG119"/>
+  <dimension ref="A1:AH119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
@@ -555,6 +555,7 @@
     <col width="15" customWidth="1" min="31" max="31"/>
     <col width="15" customWidth="1" min="32" max="32"/>
     <col width="15" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -723,6 +724,11 @@
           <t>2026/02/23</t>
         </is>
       </c>
+      <c r="AH1" s="13" t="inlineStr">
+        <is>
+          <t>2026/02/26</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -890,6 +896,11 @@
           <t>上证</t>
         </is>
       </c>
+      <c r="AH2" s="14" t="inlineStr">
+        <is>
+          <t>上证</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="n">
@@ -991,6 +1002,9 @@
       <c r="AG3" s="13" t="n">
         <v>68.91</v>
       </c>
+      <c r="AH3" s="13" t="n">
+        <v>69.66</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="n">
@@ -1091,6 +1105,9 @@
       </c>
       <c r="AG4" s="13" t="n">
         <v>4082.07</v>
+      </c>
+      <c r="AH4" s="13" t="n">
+        <v>4147.93</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -1127,6 +1144,7 @@
       <c r="AE5" s="13" t="n"/>
       <c r="AF5" s="13" t="n"/>
       <c r="AG5" s="13" t="n"/>
+      <c r="AH5" s="13" t="n"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="n">
@@ -1210,6 +1228,7 @@
       <c r="AE6" s="13" t="n"/>
       <c r="AF6" s="13" t="n"/>
       <c r="AG6" s="13" t="n"/>
+      <c r="AH6" s="13" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="n">
@@ -1310,6 +1329,9 @@
       </c>
       <c r="AG7" s="13" t="n">
         <v>50.67</v>
+      </c>
+      <c r="AH7" s="13" t="n">
+        <v>51.5</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -1364,6 +1386,9 @@
       <c r="AG8" s="13" t="n">
         <v>5840.73</v>
       </c>
+      <c r="AH8" s="13" t="n">
+        <v>5970.65</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="n">
@@ -1447,6 +1472,7 @@
       <c r="AE9" s="13" t="n"/>
       <c r="AF9" s="13" t="n"/>
       <c r="AG9" s="13" t="n"/>
+      <c r="AH9" s="13" t="n"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="3" t="n">
@@ -1547,6 +1573,9 @@
       </c>
       <c r="AG10" s="13" t="n">
         <v>52.88</v>
+      </c>
+      <c r="AH10" s="13" t="n">
+        <v>54.67</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -1601,6 +1630,9 @@
       <c r="AG11" s="13" t="n">
         <v>4660.41</v>
       </c>
+      <c r="AH11" s="13" t="n">
+        <v>4731.98</v>
+      </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="n">
@@ -1684,6 +1716,7 @@
       <c r="AE12" s="13" t="n"/>
       <c r="AF12" s="13" t="n"/>
       <c r="AG12" s="13" t="n"/>
+      <c r="AH12" s="13" t="n"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="3" t="n">
@@ -1784,6 +1817,9 @@
       </c>
       <c r="AG13" s="13" t="n">
         <v>61.11</v>
+      </c>
+      <c r="AH13" s="13" t="n">
+        <v>61.68</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -1838,6 +1874,9 @@
       <c r="AG14" s="13" t="n">
         <v>8299.59</v>
       </c>
+      <c r="AH14" s="13" t="n">
+        <v>8575.25</v>
+      </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="3" t="n">
@@ -1921,6 +1960,7 @@
       <c r="AE15" s="13" t="n"/>
       <c r="AF15" s="13" t="n"/>
       <c r="AG15" s="13" t="n"/>
+      <c r="AH15" s="13" t="n"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="n">
@@ -2021,6 +2061,9 @@
       </c>
       <c r="AG16" s="13" t="n">
         <v>28.58</v>
+      </c>
+      <c r="AH16" s="13" t="n">
+        <v>29.81</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -2075,6 +2118,9 @@
       <c r="AG17" s="13" t="n">
         <v>2699.25</v>
       </c>
+      <c r="AH17" s="13" t="n">
+        <v>2748.51</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="n">
@@ -2158,6 +2204,7 @@
       <c r="AE18" s="13" t="n"/>
       <c r="AF18" s="13" t="n"/>
       <c r="AG18" s="13" t="n"/>
+      <c r="AH18" s="13" t="n"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="n">
@@ -2258,6 +2305,9 @@
       </c>
       <c r="AG19" s="13" t="n">
         <v>95.25</v>
+      </c>
+      <c r="AH19" s="13" t="n">
+        <v>95.75</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -2312,6 +2362,9 @@
       <c r="AG20" s="13" t="n">
         <v>6909.51</v>
       </c>
+      <c r="AH20" s="13" t="n">
+        <v>6946.13</v>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="3" t="n">
@@ -2395,6 +2448,7 @@
       <c r="AE21" s="13" t="n"/>
       <c r="AF21" s="13" t="n"/>
       <c r="AG21" s="13" t="n"/>
+      <c r="AH21" s="13" t="n"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="n">
@@ -2493,6 +2547,9 @@
       </c>
       <c r="AG22" s="13" t="n">
         <v>61.28</v>
+      </c>
+      <c r="AH22" s="13" t="n">
+        <v>60.13</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -2547,6 +2604,9 @@
       <c r="AG23" s="13" t="n">
         <v>83233.38</v>
       </c>
+      <c r="AH23" s="13" t="n">
+        <v>82443.33</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="n">
@@ -2630,6 +2690,7 @@
       <c r="AE24" s="13" t="n"/>
       <c r="AF24" s="13" t="n"/>
       <c r="AG24" s="13" t="n"/>
+      <c r="AH24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="n">
@@ -2730,6 +2791,9 @@
       </c>
       <c r="AG25" s="13" t="n">
         <v>80</v>
+      </c>
+      <c r="AH25" s="13" t="n">
+        <v>81.65000000000001</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -2784,6 +2848,9 @@
       <c r="AG26" s="13" t="n">
         <v>25260.69</v>
       </c>
+      <c r="AH26" s="13" t="n">
+        <v>25175.94</v>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3" t="n">
@@ -2867,6 +2934,7 @@
       <c r="AE27" s="13" t="n"/>
       <c r="AF27" s="13" t="n"/>
       <c r="AG27" s="13" t="n"/>
+      <c r="AH27" s="13" t="n"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="n">
@@ -2967,6 +3035,9 @@
       </c>
       <c r="AG28" s="13" t="n">
         <v>78.11</v>
+      </c>
+      <c r="AH28" s="13" t="n">
+        <v>77.40000000000001</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -3021,6 +3092,9 @@
       <c r="AG29" s="13" t="n">
         <v>56825.7</v>
       </c>
+      <c r="AH29" s="13" t="n">
+        <v>58662.72</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="3" t="n">
@@ -3104,6 +3178,7 @@
       <c r="AE30" s="13" t="n"/>
       <c r="AF30" s="13" t="n"/>
       <c r="AG30" s="13" t="n"/>
+      <c r="AH30" s="13" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="n">
@@ -3204,6 +3279,9 @@
       </c>
       <c r="AG31" s="13" t="n">
         <v>50.9</v>
+      </c>
+      <c r="AH31" s="13" t="n">
+        <v>51.42</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -3258,6 +3336,9 @@
       <c r="AG32" s="13" t="n">
         <v>5668.22</v>
       </c>
+      <c r="AH32" s="13" t="n">
+        <v>5765.52</v>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="n">
@@ -3341,6 +3422,7 @@
       <c r="AE33" s="13" t="n"/>
       <c r="AF33" s="13" t="n"/>
       <c r="AG33" s="13" t="n"/>
+      <c r="AH33" s="13" t="n"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="n">
@@ -3441,6 +3523,9 @@
       </c>
       <c r="AG34" s="13" t="n">
         <v>2.06</v>
+      </c>
+      <c r="AH34" s="13" t="n">
+        <v>2.27</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -3495,6 +3580,9 @@
       <c r="AG35" s="13" t="n">
         <v>34125.79</v>
       </c>
+      <c r="AH35" s="13" t="n">
+        <v>34383.02</v>
+      </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="n">
@@ -3578,6 +3666,7 @@
       <c r="AE36" s="13" t="n"/>
       <c r="AF36" s="13" t="n"/>
       <c r="AG36" s="13" t="n"/>
+      <c r="AH36" s="13" t="n"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="n">
@@ -3678,6 +3767,9 @@
       </c>
       <c r="AG37" s="13" t="n">
         <v>30.77</v>
+      </c>
+      <c r="AH37" s="13" t="n">
+        <v>32.22</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -3732,6 +3824,9 @@
       <c r="AG38" s="13" t="n">
         <v>3423.05</v>
       </c>
+      <c r="AH38" s="13" t="n">
+        <v>3502.92</v>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="n">
@@ -3815,6 +3910,7 @@
       <c r="AE39" s="13" t="n"/>
       <c r="AF39" s="13" t="n"/>
       <c r="AG39" s="13" t="n"/>
+      <c r="AH39" s="13" t="n"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="n">
@@ -3915,6 +4011,9 @@
       </c>
       <c r="AG40" s="13" t="n">
         <v>53.45</v>
+      </c>
+      <c r="AH40" s="13" t="n">
+        <v>55.73</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -3969,6 +4068,9 @@
       <c r="AG41" s="13" t="n">
         <v>3275.96</v>
       </c>
+      <c r="AH41" s="13" t="n">
+        <v>3347.54</v>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="3" t="n">
@@ -4052,6 +4154,7 @@
       <c r="AE42" s="13" t="n"/>
       <c r="AF42" s="13" t="n"/>
       <c r="AG42" s="13" t="n"/>
+      <c r="AH42" s="13" t="n"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="3" t="n">
@@ -4152,6 +4255,9 @@
       </c>
       <c r="AG43" s="13" t="n">
         <v>18.43</v>
+      </c>
+      <c r="AH43" s="13" t="n">
+        <v>18.91</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -4206,6 +4312,9 @@
       <c r="AG44" s="13" t="n">
         <v>7020.65</v>
       </c>
+      <c r="AH44" s="13" t="n">
+        <v>7037.7</v>
+      </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="3" t="n">
@@ -4289,6 +4398,7 @@
       <c r="AE45" s="13" t="n"/>
       <c r="AF45" s="13" t="n"/>
       <c r="AG45" s="13" t="n"/>
+      <c r="AH45" s="13" t="n"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="3" t="n">
@@ -4389,6 +4499,9 @@
       </c>
       <c r="AG46" s="13" t="n">
         <v>23.8</v>
+      </c>
+      <c r="AH46" s="13" t="n">
+        <v>23.97</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -4443,6 +4556,9 @@
       <c r="AG47" s="13" t="n">
         <v>8295.26</v>
       </c>
+      <c r="AH47" s="13" t="n">
+        <v>8262.309999999999</v>
+      </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="3" t="n">
@@ -4526,6 +4642,7 @@
       <c r="AE48" s="13" t="n"/>
       <c r="AF48" s="13" t="n"/>
       <c r="AG48" s="13" t="n"/>
+      <c r="AH48" s="13" t="n"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="3" t="n">
@@ -4626,6 +4743,9 @@
       </c>
       <c r="AG49" s="13" t="n">
         <v>8.220000000000001</v>
+      </c>
+      <c r="AH49" s="13" t="n">
+        <v>8.82</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -4680,6 +4800,9 @@
       <c r="AG50" s="13" t="n">
         <v>12530.04</v>
       </c>
+      <c r="AH50" s="13" t="n">
+        <v>12530.04</v>
+      </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="n">
@@ -4763,6 +4886,7 @@
       <c r="AE51" s="13" t="n"/>
       <c r="AF51" s="13" t="n"/>
       <c r="AG51" s="13" t="n"/>
+      <c r="AH51" s="13" t="n"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="3" t="n">
@@ -4863,6 +4987,9 @@
       </c>
       <c r="AG52" s="13" t="n">
         <v>29.32</v>
+      </c>
+      <c r="AH52" s="13" t="n">
+        <v>30.71</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -4917,6 +5044,9 @@
       <c r="AG53" s="13" t="n">
         <v>13013.04</v>
       </c>
+      <c r="AH53" s="13" t="n">
+        <v>12997.41</v>
+      </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="n">
@@ -5000,6 +5130,7 @@
       <c r="AE54" s="13" t="n"/>
       <c r="AF54" s="13" t="n"/>
       <c r="AG54" s="13" t="n"/>
+      <c r="AH54" s="13" t="n"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="n">
@@ -5100,6 +5231,9 @@
       </c>
       <c r="AG55" s="13" t="n">
         <v>19.63</v>
+      </c>
+      <c r="AH55" s="13" t="n">
+        <v>19.46</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -5154,6 +5288,9 @@
       <c r="AG56" s="13" t="n">
         <v>8655.870000000001</v>
       </c>
+      <c r="AH56" s="13" t="n">
+        <v>8453.26</v>
+      </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="n">
@@ -5237,6 +5374,7 @@
       <c r="AE57" s="13" t="n"/>
       <c r="AF57" s="13" t="n"/>
       <c r="AG57" s="13" t="n"/>
+      <c r="AH57" s="13" t="n"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="n">
@@ -5337,6 +5475,9 @@
       </c>
       <c r="AG58" s="13" t="n">
         <v>25.62</v>
+      </c>
+      <c r="AH58" s="13" t="n">
+        <v>26.3</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -5391,6 +5532,9 @@
       <c r="AG59" s="13" t="n">
         <v>14952.52</v>
       </c>
+      <c r="AH59" s="13" t="n">
+        <v>14835.13</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="3" t="n">
@@ -5474,6 +5618,7 @@
       <c r="AE60" s="13" t="n"/>
       <c r="AF60" s="13" t="n"/>
       <c r="AG60" s="13" t="n"/>
+      <c r="AH60" s="13" t="n"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="n">
@@ -5574,6 +5719,9 @@
       </c>
       <c r="AG61" s="13" t="n">
         <v>31.43</v>
+      </c>
+      <c r="AH61" s="13" t="n">
+        <v>30.84</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -5628,6 +5776,9 @@
       <c r="AG62" s="13" t="n">
         <v>16186.92</v>
       </c>
+      <c r="AH62" s="13" t="n">
+        <v>15377.58</v>
+      </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="n">
@@ -5711,6 +5862,7 @@
       <c r="AE63" s="13" t="n"/>
       <c r="AF63" s="13" t="n"/>
       <c r="AG63" s="13" t="n"/>
+      <c r="AH63" s="13" t="n"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="3" t="n">
@@ -5811,6 +5963,9 @@
       </c>
       <c r="AG64" s="13" t="n">
         <v>17.73</v>
+      </c>
+      <c r="AH64" s="13" t="n">
+        <v>16.7</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -5865,6 +6020,9 @@
       <c r="AG65" s="13" t="n">
         <v>8772.110000000001</v>
       </c>
+      <c r="AH65" s="13" t="n">
+        <v>8421.98</v>
+      </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3" t="n">
@@ -5948,6 +6106,7 @@
       <c r="AE66" s="13" t="n"/>
       <c r="AF66" s="13" t="n"/>
       <c r="AG66" s="13" t="n"/>
+      <c r="AH66" s="13" t="n"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3" t="n">
@@ -6048,6 +6207,9 @@
       </c>
       <c r="AG67" s="13" t="n">
         <v>10.07</v>
+      </c>
+      <c r="AH67" s="13" t="n">
+        <v>10.75</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -6102,6 +6264,9 @@
       <c r="AG68" s="13" t="n">
         <v>9563.01</v>
       </c>
+      <c r="AH68" s="13" t="n">
+        <v>9582.959999999999</v>
+      </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3" t="n">
@@ -6185,6 +6350,7 @@
       <c r="AE69" s="13" t="n"/>
       <c r="AF69" s="13" t="n"/>
       <c r="AG69" s="13" t="n"/>
+      <c r="AH69" s="13" t="n"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="n">
@@ -6285,6 +6451,9 @@
       </c>
       <c r="AG70" s="13" t="n">
         <v>21.43</v>
+      </c>
+      <c r="AH70" s="13" t="n">
+        <v>20.15</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -6339,6 +6508,9 @@
       <c r="AG71" s="13" t="n">
         <v>2863.88</v>
       </c>
+      <c r="AH71" s="13" t="n">
+        <v>2731.91</v>
+      </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="n">
@@ -6422,6 +6594,7 @@
       <c r="AE72" s="13" t="n"/>
       <c r="AF72" s="13" t="n"/>
       <c r="AG72" s="13" t="n"/>
+      <c r="AH72" s="13" t="n"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="n">
@@ -6522,6 +6695,9 @@
       </c>
       <c r="AG73" s="13" t="n">
         <v>40.86</v>
+      </c>
+      <c r="AH73" s="13" t="n">
+        <v>39.39</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -6576,6 +6752,9 @@
       <c r="AG74" s="13" t="n">
         <v>5361.58</v>
       </c>
+      <c r="AH74" s="13" t="n">
+        <v>5167.11</v>
+      </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="n">
@@ -6659,6 +6838,7 @@
       <c r="AE75" s="13" t="n"/>
       <c r="AF75" s="13" t="n"/>
       <c r="AG75" s="13" t="n"/>
+      <c r="AH75" s="13" t="n"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="n">
@@ -6759,6 +6939,9 @@
       </c>
       <c r="AG76" s="13" t="n">
         <v>23.61</v>
+      </c>
+      <c r="AH76" s="13" t="n">
+        <v>22.99</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -6813,6 +6996,9 @@
       <c r="AG77" s="13" t="n">
         <v>8820.860000000001</v>
       </c>
+      <c r="AH77" s="13" t="n">
+        <v>8813.01</v>
+      </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="n">
@@ -6896,6 +7082,7 @@
       <c r="AE78" s="13" t="n"/>
       <c r="AF78" s="13" t="n"/>
       <c r="AG78" s="13" t="n"/>
+      <c r="AH78" s="13" t="n"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="n">
@@ -6996,6 +7183,9 @@
       </c>
       <c r="AG79" s="13" t="n">
         <v>18.25</v>
+      </c>
+      <c r="AH79" s="13" t="n">
+        <v>17.66</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -7050,6 +7240,9 @@
       <c r="AG80" s="13" t="n">
         <v>1474.31</v>
       </c>
+      <c r="AH80" s="13" t="n">
+        <v>1462.19</v>
+      </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="3" t="n">
@@ -7133,6 +7326,7 @@
       <c r="AE81" s="13" t="n"/>
       <c r="AF81" s="13" t="n"/>
       <c r="AG81" s="13" t="n"/>
+      <c r="AH81" s="13" t="n"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="3" t="n">
@@ -7233,6 +7427,9 @@
       </c>
       <c r="AG82" s="13" t="n">
         <v>16.38</v>
+      </c>
+      <c r="AH82" s="13" t="n">
+        <v>16.34</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -7287,6 +7484,9 @@
       <c r="AG83" s="13" t="n">
         <v>16509.82</v>
       </c>
+      <c r="AH83" s="13" t="n">
+        <v>16497.29</v>
+      </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="3" t="n">
@@ -7370,6 +7570,7 @@
       <c r="AE84" s="13" t="n"/>
       <c r="AF84" s="13" t="n"/>
       <c r="AG84" s="13" t="n"/>
+      <c r="AH84" s="13" t="n"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="3" t="n">
@@ -7470,6 +7671,9 @@
       </c>
       <c r="AG85" s="13" t="n">
         <v>54.2</v>
+      </c>
+      <c r="AH85" s="13" t="n">
+        <v>55.06</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -7524,6 +7728,9 @@
       <c r="AG86" s="13" t="n">
         <v>2994.14</v>
       </c>
+      <c r="AH86" s="13" t="n">
+        <v>3055.67</v>
+      </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="n">
@@ -7607,6 +7814,7 @@
       <c r="AE87" s="13" t="n"/>
       <c r="AF87" s="13" t="n"/>
       <c r="AG87" s="13" t="n"/>
+      <c r="AH87" s="13" t="n"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="3" t="n">
@@ -7707,6 +7915,9 @@
       </c>
       <c r="AG88" s="13" t="n">
         <v>58.36</v>
+      </c>
+      <c r="AH88" s="13" t="n">
+        <v>58.66</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -7761,6 +7972,9 @@
       <c r="AG89" s="13" t="n">
         <v>3251.43</v>
       </c>
+      <c r="AH89" s="13" t="n">
+        <v>3325.49</v>
+      </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="n">
@@ -7844,6 +8058,7 @@
       <c r="AE90" s="13" t="n"/>
       <c r="AF90" s="13" t="n"/>
       <c r="AG90" s="13" t="n"/>
+      <c r="AH90" s="13" t="n"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="3" t="n">
@@ -7944,6 +8159,9 @@
       </c>
       <c r="AG91" s="13" t="n">
         <v>50.72</v>
+      </c>
+      <c r="AH91" s="13" t="n">
+        <v>51.62</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -7998,6 +8216,9 @@
       <c r="AG92" s="13" t="n">
         <v>3056.18</v>
       </c>
+      <c r="AH92" s="13" t="n">
+        <v>3096.89</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="3" t="n">
@@ -8081,6 +8302,7 @@
       <c r="AE93" s="13" t="n"/>
       <c r="AF93" s="13" t="n"/>
       <c r="AG93" s="13" t="n"/>
+      <c r="AH93" s="13" t="n"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="n">
@@ -8181,6 +8403,9 @@
       </c>
       <c r="AG94" s="13" t="n">
         <v>43.69</v>
+      </c>
+      <c r="AH94" s="13" t="n">
+        <v>40.96</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -8235,6 +8460,9 @@
       <c r="AG95" s="13" t="n">
         <v>1891.58</v>
       </c>
+      <c r="AH95" s="13" t="n">
+        <v>1879.37</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="n">
@@ -8318,6 +8546,7 @@
       <c r="AE96" s="13" t="n"/>
       <c r="AF96" s="13" t="n"/>
       <c r="AG96" s="13" t="n"/>
+      <c r="AH96" s="13" t="n"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="n">
@@ -8418,6 +8647,9 @@
       </c>
       <c r="AG97" s="13" t="n">
         <v>26.77</v>
+      </c>
+      <c r="AH97" s="13" t="n">
+        <v>27.08</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -8472,6 +8704,9 @@
       <c r="AG98" s="13" t="n">
         <v>10184.4</v>
       </c>
+      <c r="AH98" s="13" t="n">
+        <v>10184.4</v>
+      </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="n">
@@ -8555,6 +8790,7 @@
       <c r="AE99" s="13" t="n"/>
       <c r="AF99" s="13" t="n"/>
       <c r="AG99" s="13" t="n"/>
+      <c r="AH99" s="13" t="n"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="n">
@@ -8655,6 +8891,9 @@
       </c>
       <c r="AG100" s="13" t="n">
         <v>87.48999999999999</v>
+      </c>
+      <c r="AH100" s="13" t="n">
+        <v>87.61</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -8709,6 +8948,9 @@
       <c r="AG101" s="13" t="n">
         <v>10413.72</v>
       </c>
+      <c r="AH101" s="13" t="n">
+        <v>10690.49</v>
+      </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="n">
@@ -8792,6 +9034,7 @@
       <c r="AE102" s="13" t="n"/>
       <c r="AF102" s="13" t="n"/>
       <c r="AG102" s="13" t="n"/>
+      <c r="AH102" s="13" t="n"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="n">
@@ -8892,6 +9135,9 @@
       </c>
       <c r="AG103" s="13" t="n">
         <v>59.65</v>
+      </c>
+      <c r="AH103" s="13" t="n">
+        <v>59.91</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -8946,6 +9192,9 @@
       <c r="AG104" s="13" t="n">
         <v>15127.96</v>
       </c>
+      <c r="AH104" s="13" t="n">
+        <v>15852.73</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="n">
@@ -9029,6 +9278,7 @@
       <c r="AE105" s="13" t="n"/>
       <c r="AF105" s="13" t="n"/>
       <c r="AG105" s="13" t="n"/>
+      <c r="AH105" s="13" t="n"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="3" t="n">
@@ -9129,6 +9379,9 @@
       </c>
       <c r="AG106" s="13" t="n">
         <v>5.64</v>
+      </c>
+      <c r="AH106" s="13" t="n">
+        <v>7.81</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -9183,6 +9436,9 @@
       <c r="AG107" s="13" t="n">
         <v>2156.61</v>
       </c>
+      <c r="AH107" s="13" t="n">
+        <v>2199.65</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="n">
@@ -9266,6 +9522,7 @@
       <c r="AE108" s="13" t="n"/>
       <c r="AF108" s="13" t="n"/>
       <c r="AG108" s="13" t="n"/>
+      <c r="AH108" s="13" t="n"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="n">
@@ -9366,6 +9623,9 @@
       </c>
       <c r="AG109" s="13" t="n">
         <v>24.99</v>
+      </c>
+      <c r="AH109" s="13" t="n">
+        <v>25.03</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -9420,6 +9680,9 @@
       <c r="AG110" s="13" t="n">
         <v>823.65</v>
       </c>
+      <c r="AH110" s="13" t="n">
+        <v>819.92</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="3" t="n">
@@ -9503,6 +9766,7 @@
       <c r="AE111" s="13" t="n"/>
       <c r="AF111" s="13" t="n"/>
       <c r="AG111" s="13" t="n"/>
+      <c r="AH111" s="13" t="n"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="3" t="n">
@@ -9603,6 +9867,9 @@
       </c>
       <c r="AG112" s="13" t="n">
         <v>32.9</v>
+      </c>
+      <c r="AH112" s="13" t="n">
+        <v>33.73</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -9657,6 +9924,9 @@
       <c r="AG113" s="13" t="n">
         <v>3513.48</v>
       </c>
+      <c r="AH113" s="13" t="n">
+        <v>3760.14</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="3" t="n">
@@ -9740,6 +10010,7 @@
       <c r="AE114" s="13" t="n"/>
       <c r="AF114" s="13" t="n"/>
       <c r="AG114" s="13" t="n"/>
+      <c r="AH114" s="13" t="n"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="3" t="n">
@@ -9840,6 +10111,9 @@
       </c>
       <c r="AG115" s="13" t="n">
         <v>21.34</v>
+      </c>
+      <c r="AH115" s="13" t="n">
+        <v>22.57</v>
       </c>
     </row>
     <row r="116">
@@ -9879,6 +10153,9 @@
       <c r="AG116" s="13" t="n">
         <v>4024.89</v>
       </c>
+      <c r="AH116" s="13" t="n">
+        <v>4172.56</v>
+      </c>
     </row>
     <row r="117">
       <c r="P117" s="13" t="n">
@@ -9917,6 +10194,7 @@
       <c r="AE117" s="13" t="n"/>
       <c r="AF117" s="13" t="n"/>
       <c r="AG117" s="13" t="n"/>
+      <c r="AH117" s="13" t="n"/>
     </row>
     <row r="118">
       <c r="P118" s="13" t="n">
@@ -9973,6 +10251,9 @@
       <c r="AG118" s="13" t="n">
         <v>29.02</v>
       </c>
+      <c r="AH118" s="13" t="n">
+        <v>29.02</v>
+      </c>
     </row>
     <row r="119">
       <c r="Y119" s="13" t="n">
@@ -10001,6 +10282,9 @@
       </c>
       <c r="AG119" s="13" t="n">
         <v>3062.87</v>
+      </c>
+      <c r="AH119" s="13" t="n">
+        <v>3083.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>